<commit_message>
Bug fixes; different-colored text for IO
</commit_message>
<xml_diff>
--- a/config/phone_list.xlsx
+++ b/config/phone_list.xlsx
@@ -1746,11 +1746,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:J206"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A123" sqref="A123"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1799,7 +1798,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10" hidden="1">
+    <row r="2" spans="1:10">
       <c r="A2" s="1" t="s">
         <v>315</v>
       </c>
@@ -1816,7 +1815,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:10" hidden="1">
+    <row r="3" spans="1:10">
       <c r="A3" s="1" t="s">
         <v>313</v>
       </c>
@@ -1833,7 +1832,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:10" hidden="1">
+    <row r="4" spans="1:10">
       <c r="A4" s="1" t="s">
         <v>312</v>
       </c>
@@ -1850,7 +1849,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:10" hidden="1">
+    <row r="5" spans="1:10">
       <c r="A5" s="1" t="s">
         <v>311</v>
       </c>
@@ -1867,7 +1866,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:10" hidden="1">
+    <row r="6" spans="1:10">
       <c r="A6" s="1" t="s">
         <v>314</v>
       </c>
@@ -1884,7 +1883,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:10" hidden="1">
+    <row r="7" spans="1:10">
       <c r="A7" s="1" t="s">
         <v>316</v>
       </c>
@@ -1901,7 +1900,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:10" hidden="1">
+    <row r="8" spans="1:10">
       <c r="A8" s="1" t="s">
         <v>317</v>
       </c>
@@ -1918,7 +1917,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:10" hidden="1">
+    <row r="9" spans="1:10">
       <c r="A9" s="1" t="s">
         <v>391</v>
       </c>
@@ -1935,7 +1934,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:10" hidden="1">
+    <row r="10" spans="1:10">
       <c r="A10" s="1" t="s">
         <v>371</v>
       </c>
@@ -1952,7 +1951,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:10" hidden="1">
+    <row r="11" spans="1:10">
       <c r="A11" s="1" t="s">
         <v>361</v>
       </c>
@@ -1969,7 +1968,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:10" hidden="1">
+    <row r="12" spans="1:10">
       <c r="A12" s="1" t="s">
         <v>366</v>
       </c>
@@ -1986,7 +1985,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:10" hidden="1">
+    <row r="13" spans="1:10">
       <c r="A13" s="1" t="s">
         <v>365</v>
       </c>
@@ -2003,7 +2002,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:10" hidden="1">
+    <row r="14" spans="1:10">
       <c r="A14" s="1" t="s">
         <v>364</v>
       </c>
@@ -2020,7 +2019,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:10" hidden="1">
+    <row r="15" spans="1:10">
       <c r="A15" s="1" t="s">
         <v>360</v>
       </c>
@@ -2037,7 +2036,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:10" hidden="1">
+    <row r="16" spans="1:10">
       <c r="A16" s="1" t="s">
         <v>363</v>
       </c>
@@ -2054,7 +2053,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:9" hidden="1">
+    <row r="17" spans="1:9">
       <c r="A17" s="1" t="s">
         <v>362</v>
       </c>
@@ -2071,7 +2070,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:9" hidden="1">
+    <row r="18" spans="1:9">
       <c r="A18" s="1" t="s">
         <v>367</v>
       </c>
@@ -2088,7 +2087,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:9" hidden="1">
+    <row r="19" spans="1:9">
       <c r="A19" s="1" t="s">
         <v>368</v>
       </c>
@@ -2105,7 +2104,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:9" hidden="1">
+    <row r="20" spans="1:9">
       <c r="A20" s="1" t="s">
         <v>370</v>
       </c>
@@ -2122,7 +2121,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:9" hidden="1">
+    <row r="21" spans="1:9">
       <c r="A21" s="1" t="s">
         <v>369</v>
       </c>
@@ -2139,7 +2138,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:9" hidden="1">
+    <row r="22" spans="1:9">
       <c r="A22" s="1" t="s">
         <v>379</v>
       </c>
@@ -2156,7 +2155,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:9" hidden="1">
+    <row r="23" spans="1:9">
       <c r="A23" s="1" t="s">
         <v>381</v>
       </c>
@@ -2173,7 +2172,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:9" hidden="1">
+    <row r="24" spans="1:9">
       <c r="A24" s="1" t="s">
         <v>395</v>
       </c>
@@ -2190,7 +2189,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:9" hidden="1">
+    <row r="25" spans="1:9">
       <c r="A25" s="1" t="s">
         <v>398</v>
       </c>
@@ -2207,7 +2206,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:9" hidden="1">
+    <row r="26" spans="1:9">
       <c r="A26" s="1" t="s">
         <v>382</v>
       </c>
@@ -2224,7 +2223,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:9" hidden="1">
+    <row r="27" spans="1:9">
       <c r="A27" s="1" t="s">
         <v>380</v>
       </c>
@@ -2241,7 +2240,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:9" hidden="1">
+    <row r="28" spans="1:9">
       <c r="A28" s="1" t="s">
         <v>397</v>
       </c>
@@ -2258,7 +2257,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:9" hidden="1">
+    <row r="29" spans="1:9">
       <c r="A29" s="1" t="s">
         <v>290</v>
       </c>
@@ -2275,7 +2274,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:9" hidden="1">
+    <row r="30" spans="1:9">
       <c r="A30" s="1" t="s">
         <v>334</v>
       </c>
@@ -2292,7 +2291,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:9" hidden="1">
+    <row r="31" spans="1:9">
       <c r="A31" s="1" t="s">
         <v>388</v>
       </c>
@@ -2309,7 +2308,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:9" hidden="1">
+    <row r="32" spans="1:9">
       <c r="A32" s="1" t="s">
         <v>385</v>
       </c>
@@ -2326,7 +2325,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:10" hidden="1">
+    <row r="33" spans="1:10">
       <c r="A33" s="1" t="s">
         <v>383</v>
       </c>
@@ -2343,7 +2342,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:10" hidden="1">
+    <row r="34" spans="1:10">
       <c r="A34" s="1" t="s">
         <v>390</v>
       </c>
@@ -2363,7 +2362,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="35" spans="1:10" hidden="1">
+    <row r="35" spans="1:10">
       <c r="A35" s="1" t="s">
         <v>386</v>
       </c>
@@ -2380,7 +2379,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:10" hidden="1">
+    <row r="36" spans="1:10">
       <c r="A36" s="1" t="s">
         <v>387</v>
       </c>
@@ -2397,7 +2396,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:10" hidden="1">
+    <row r="37" spans="1:10">
       <c r="A37" s="1" t="s">
         <v>389</v>
       </c>
@@ -2414,7 +2413,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:10" hidden="1">
+    <row r="38" spans="1:10">
       <c r="A38" s="1" t="s">
         <v>384</v>
       </c>
@@ -2431,7 +2430,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:10" hidden="1">
+    <row r="39" spans="1:10">
       <c r="A39" s="1" t="s">
         <v>396</v>
       </c>
@@ -2448,7 +2447,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:10" hidden="1">
+    <row r="40" spans="1:10">
       <c r="A40" s="1" t="s">
         <v>337</v>
       </c>
@@ -2465,7 +2464,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:10" hidden="1">
+    <row r="41" spans="1:10">
       <c r="A41" s="1" t="s">
         <v>335</v>
       </c>
@@ -2482,7 +2481,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:10" hidden="1">
+    <row r="42" spans="1:10">
       <c r="A42" s="1" t="s">
         <v>376</v>
       </c>
@@ -2499,7 +2498,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:10" hidden="1">
+    <row r="43" spans="1:10">
       <c r="A43" s="1" t="s">
         <v>377</v>
       </c>
@@ -2516,7 +2515,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:10" hidden="1">
+    <row r="44" spans="1:10">
       <c r="A44" s="1" t="s">
         <v>378</v>
       </c>
@@ -2533,7 +2532,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:10" hidden="1">
+    <row r="45" spans="1:10">
       <c r="A45" s="1" t="s">
         <v>296</v>
       </c>
@@ -2550,7 +2549,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:10" hidden="1">
+    <row r="46" spans="1:10">
       <c r="A46" s="1" t="s">
         <v>297</v>
       </c>
@@ -2567,7 +2566,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:10" hidden="1">
+    <row r="47" spans="1:10">
       <c r="A47" s="1" t="s">
         <v>294</v>
       </c>
@@ -2584,7 +2583,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:10" hidden="1">
+    <row r="48" spans="1:10">
       <c r="A48" s="1" t="s">
         <v>295</v>
       </c>
@@ -2601,7 +2600,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:9" hidden="1">
+    <row r="49" spans="1:9">
       <c r="A49" s="1" t="s">
         <v>303</v>
       </c>
@@ -2618,7 +2617,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:9" hidden="1">
+    <row r="50" spans="1:9">
       <c r="A50" s="1" t="s">
         <v>304</v>
       </c>
@@ -2635,7 +2634,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:9" hidden="1">
+    <row r="51" spans="1:9">
       <c r="A51" s="1" t="s">
         <v>375</v>
       </c>
@@ -2652,7 +2651,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:9" hidden="1">
+    <row r="52" spans="1:9">
       <c r="A52" s="1" t="s">
         <v>393</v>
       </c>
@@ -2669,7 +2668,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:9" hidden="1">
+    <row r="53" spans="1:9">
       <c r="A53" s="1" t="s">
         <v>392</v>
       </c>
@@ -2686,7 +2685,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:9" hidden="1">
+    <row r="54" spans="1:9">
       <c r="A54" s="1" t="s">
         <v>394</v>
       </c>
@@ -2703,7 +2702,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:9" hidden="1">
+    <row r="55" spans="1:9">
       <c r="A55" s="1" t="s">
         <v>372</v>
       </c>
@@ -2720,7 +2719,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:9" hidden="1">
+    <row r="56" spans="1:9">
       <c r="A56" s="1" t="s">
         <v>374</v>
       </c>
@@ -2737,7 +2736,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:9" hidden="1">
+    <row r="57" spans="1:9">
       <c r="A57" s="1" t="s">
         <v>373</v>
       </c>
@@ -2754,7 +2753,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:9" hidden="1">
+    <row r="58" spans="1:9">
       <c r="A58" s="1" t="s">
         <v>301</v>
       </c>
@@ -2771,7 +2770,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:9" hidden="1">
+    <row r="59" spans="1:9">
       <c r="A59" s="1" t="s">
         <v>302</v>
       </c>
@@ -2788,7 +2787,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:9" hidden="1">
+    <row r="60" spans="1:9">
       <c r="A60" s="1" t="s">
         <v>291</v>
       </c>
@@ -2805,7 +2804,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:9" hidden="1">
+    <row r="61" spans="1:9">
       <c r="A61" s="1" t="s">
         <v>292</v>
       </c>
@@ -2822,7 +2821,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:9" hidden="1">
+    <row r="62" spans="1:9">
       <c r="A62" s="1" t="s">
         <v>298</v>
       </c>
@@ -2839,7 +2838,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:9" hidden="1">
+    <row r="63" spans="1:9">
       <c r="A63" s="1" t="s">
         <v>299</v>
       </c>
@@ -2856,7 +2855,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:9" hidden="1">
+    <row r="64" spans="1:9">
       <c r="A64" s="1" t="s">
         <v>300</v>
       </c>
@@ -2873,7 +2872,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:9" hidden="1">
+    <row r="65" spans="1:9">
       <c r="A65" s="1" t="s">
         <v>338</v>
       </c>
@@ -2890,7 +2889,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:9" hidden="1">
+    <row r="66" spans="1:9">
       <c r="A66" s="1" t="s">
         <v>340</v>
       </c>
@@ -2907,7 +2906,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:9" hidden="1">
+    <row r="67" spans="1:9">
       <c r="A67" s="1" t="s">
         <v>339</v>
       </c>
@@ -2924,7 +2923,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:9" hidden="1">
+    <row r="68" spans="1:9">
       <c r="A68" s="1" t="s">
         <v>333</v>
       </c>
@@ -2941,7 +2940,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:9" hidden="1">
+    <row r="69" spans="1:9">
       <c r="A69" s="1" t="s">
         <v>332</v>
       </c>
@@ -2958,7 +2957,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:9" hidden="1">
+    <row r="70" spans="1:9">
       <c r="A70" s="1" t="s">
         <v>293</v>
       </c>
@@ -2975,7 +2974,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:9" hidden="1">
+    <row r="71" spans="1:9">
       <c r="A71" s="1" t="s">
         <v>403</v>
       </c>
@@ -2992,7 +2991,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:9" hidden="1">
+    <row r="72" spans="1:9">
       <c r="A72" s="1" t="s">
         <v>399</v>
       </c>
@@ -3009,7 +3008,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:9" hidden="1">
+    <row r="73" spans="1:9">
       <c r="A73" s="1" t="s">
         <v>401</v>
       </c>
@@ -3026,7 +3025,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:9" hidden="1">
+    <row r="74" spans="1:9">
       <c r="A74" s="1" t="s">
         <v>402</v>
       </c>
@@ -3043,7 +3042,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:9" hidden="1">
+    <row r="75" spans="1:9">
       <c r="A75" s="1" t="s">
         <v>400</v>
       </c>
@@ -3060,7 +3059,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:9" hidden="1">
+    <row r="76" spans="1:9">
       <c r="A76" s="1" t="s">
         <v>404</v>
       </c>
@@ -3077,7 +3076,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:9" hidden="1">
+    <row r="77" spans="1:9">
       <c r="A77" s="1" t="s">
         <v>341</v>
       </c>
@@ -3094,7 +3093,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:9" hidden="1">
+    <row r="78" spans="1:9">
       <c r="A78" s="1" t="s">
         <v>336</v>
       </c>
@@ -3111,7 +3110,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:9" hidden="1">
+    <row r="79" spans="1:9">
       <c r="A79" s="1" t="s">
         <v>441</v>
       </c>
@@ -3128,7 +3127,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:9" hidden="1">
+    <row r="80" spans="1:9">
       <c r="A80" s="1" t="s">
         <v>442</v>
       </c>
@@ -3145,7 +3144,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="1:10" hidden="1">
+    <row r="81" spans="1:10">
       <c r="A81" s="1" t="s">
         <v>440</v>
       </c>
@@ -3162,7 +3161,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:10" hidden="1">
+    <row r="82" spans="1:10">
       <c r="A82" s="1" t="s">
         <v>443</v>
       </c>
@@ -3179,7 +3178,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:10" hidden="1">
+    <row r="83" spans="1:10">
       <c r="A83" s="1" t="s">
         <v>444</v>
       </c>
@@ -3196,7 +3195,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:10" hidden="1">
+    <row r="84" spans="1:10">
       <c r="A84" s="1" t="s">
         <v>319</v>
       </c>
@@ -3213,7 +3212,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:10" hidden="1">
+    <row r="85" spans="1:10">
       <c r="A85" s="1" t="s">
         <v>318</v>
       </c>
@@ -3230,7 +3229,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:10" hidden="1">
+    <row r="86" spans="1:10">
       <c r="A86" s="1" t="s">
         <v>450</v>
       </c>
@@ -3247,7 +3246,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:10" hidden="1">
+    <row r="87" spans="1:10">
       <c r="A87" s="1" t="s">
         <v>449</v>
       </c>
@@ -3264,7 +3263,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:10" hidden="1">
+    <row r="88" spans="1:10">
       <c r="A88" s="1" t="s">
         <v>451</v>
       </c>
@@ -3281,7 +3280,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:10" hidden="1">
+    <row r="89" spans="1:10">
       <c r="A89" s="1" t="s">
         <v>446</v>
       </c>
@@ -3298,7 +3297,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:10" hidden="1">
+    <row r="90" spans="1:10">
       <c r="A90" s="1" t="s">
         <v>445</v>
       </c>
@@ -3315,7 +3314,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="1:10" hidden="1">
+    <row r="91" spans="1:10">
       <c r="A91" s="1" t="s">
         <v>447</v>
       </c>
@@ -3332,7 +3331,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="1:10" hidden="1">
+    <row r="92" spans="1:10">
       <c r="A92" s="1" t="s">
         <v>448</v>
       </c>
@@ -3349,7 +3348,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="1:10" hidden="1">
+    <row r="93" spans="1:10">
       <c r="A93" s="1" t="s">
         <v>320</v>
       </c>
@@ -3366,7 +3365,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="1:10" hidden="1">
+    <row r="94" spans="1:10">
       <c r="A94" s="1" t="s">
         <v>347</v>
       </c>
@@ -3456,7 +3455,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="97" spans="1:10" hidden="1">
+    <row r="97" spans="1:10">
       <c r="A97" s="1" t="s">
         <v>414</v>
       </c>
@@ -3488,7 +3487,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="98" spans="1:10" hidden="1">
+    <row r="98" spans="1:10">
       <c r="A98" s="1" t="s">
         <v>415</v>
       </c>
@@ -3520,7 +3519,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="99" spans="1:10" hidden="1">
+    <row r="99" spans="1:10">
       <c r="A99" s="1" t="s">
         <v>416</v>
       </c>
@@ -3552,7 +3551,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="100" spans="1:10" hidden="1">
+    <row r="100" spans="1:10">
       <c r="A100" s="1" t="s">
         <v>429</v>
       </c>
@@ -3584,7 +3583,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="101" spans="1:10" hidden="1">
+    <row r="101" spans="1:10">
       <c r="A101" s="1" t="s">
         <v>328</v>
       </c>
@@ -3616,7 +3615,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="102" spans="1:10" hidden="1">
+    <row r="102" spans="1:10">
       <c r="A102" s="1" t="s">
         <v>330</v>
       </c>
@@ -3648,7 +3647,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="103" spans="1:10" hidden="1">
+    <row r="103" spans="1:10">
       <c r="A103" s="1" t="s">
         <v>426</v>
       </c>
@@ -3680,7 +3679,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="104" spans="1:10" hidden="1">
+    <row r="104" spans="1:10">
       <c r="A104" s="1" t="s">
         <v>329</v>
       </c>
@@ -3712,7 +3711,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="105" spans="1:10" hidden="1">
+    <row r="105" spans="1:10">
       <c r="A105" s="1" t="s">
         <v>331</v>
       </c>
@@ -3744,7 +3743,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="106" spans="1:10" hidden="1">
+    <row r="106" spans="1:10">
       <c r="A106" s="1" t="s">
         <v>413</v>
       </c>
@@ -3776,7 +3775,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="107" spans="1:10" hidden="1">
+    <row r="107" spans="1:10">
       <c r="A107" s="1" t="s">
         <v>310</v>
       </c>
@@ -3808,7 +3807,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="108" spans="1:10" hidden="1">
+    <row r="108" spans="1:10">
       <c r="A108" s="1" t="s">
         <v>321</v>
       </c>
@@ -3840,7 +3839,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="109" spans="1:10" hidden="1">
+    <row r="109" spans="1:10">
       <c r="A109" s="1" t="s">
         <v>458</v>
       </c>
@@ -3872,7 +3871,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="110" spans="1:10" hidden="1">
+    <row r="110" spans="1:10">
       <c r="A110" s="1" t="s">
         <v>309</v>
       </c>
@@ -3904,7 +3903,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="111" spans="1:10" hidden="1">
+    <row r="111" spans="1:10">
       <c r="B111" t="s">
         <v>79</v>
       </c>
@@ -3930,7 +3929,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="112" spans="1:10" hidden="1">
+    <row r="112" spans="1:10">
       <c r="B112" t="s">
         <v>80</v>
       </c>
@@ -3956,7 +3955,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="113" spans="1:10" hidden="1">
+    <row r="113" spans="1:10">
       <c r="A113" s="1" t="s">
         <v>322</v>
       </c>
@@ -3988,7 +3987,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="114" spans="1:10" hidden="1">
+    <row r="114" spans="1:10">
       <c r="A114" s="1" t="s">
         <v>323</v>
       </c>
@@ -4020,7 +4019,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="115" spans="1:10" hidden="1">
+    <row r="115" spans="1:10">
       <c r="A115" s="1" t="s">
         <v>288</v>
       </c>
@@ -4052,7 +4051,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="116" spans="1:10" hidden="1">
+    <row r="116" spans="1:10">
       <c r="A116" s="1" t="s">
         <v>289</v>
       </c>
@@ -4084,7 +4083,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="117" spans="1:10" hidden="1">
+    <row r="117" spans="1:10">
       <c r="A117" s="1" t="s">
         <v>342</v>
       </c>
@@ -4116,7 +4115,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="118" spans="1:10" hidden="1">
+    <row r="118" spans="1:10">
       <c r="A118" s="1" t="s">
         <v>343</v>
       </c>
@@ -4180,7 +4179,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="120" spans="1:10" hidden="1">
+    <row r="120" spans="1:10">
       <c r="A120" s="1" t="s">
         <v>417</v>
       </c>
@@ -4212,7 +4211,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="121" spans="1:10" hidden="1">
+    <row r="121" spans="1:10">
       <c r="A121" s="1" t="s">
         <v>307</v>
       </c>
@@ -4244,7 +4243,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="122" spans="1:10" hidden="1">
+    <row r="122" spans="1:10">
       <c r="A122" s="1" t="s">
         <v>308</v>
       </c>
@@ -4340,7 +4339,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="125" spans="1:10" hidden="1">
+    <row r="125" spans="1:10">
       <c r="B125" t="s">
         <v>267</v>
       </c>
@@ -4366,7 +4365,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="126" spans="1:10" hidden="1">
+    <row r="126" spans="1:10">
       <c r="B126" t="s">
         <v>266</v>
       </c>
@@ -4392,7 +4391,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="127" spans="1:10" hidden="1">
+    <row r="127" spans="1:10">
       <c r="A127" s="1" t="s">
         <v>456</v>
       </c>
@@ -4424,7 +4423,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="128" spans="1:10" hidden="1">
+    <row r="128" spans="1:10">
       <c r="A128" s="1" t="s">
         <v>344</v>
       </c>
@@ -4456,7 +4455,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="129" spans="1:10" hidden="1">
+    <row r="129" spans="1:10">
       <c r="A129" s="1" t="s">
         <v>345</v>
       </c>
@@ -4488,7 +4487,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="130" spans="1:10" hidden="1">
+    <row r="130" spans="1:10">
       <c r="A130" s="1" t="s">
         <v>283</v>
       </c>
@@ -4520,7 +4519,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="131" spans="1:10" hidden="1">
+    <row r="131" spans="1:10">
       <c r="A131" s="1" t="s">
         <v>284</v>
       </c>
@@ -4700,7 +4699,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="137" spans="1:10" hidden="1">
+    <row r="137" spans="1:10">
       <c r="A137" s="1" t="s">
         <v>423</v>
       </c>
@@ -4732,7 +4731,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="138" spans="1:10" hidden="1">
+    <row r="138" spans="1:10">
       <c r="A138" s="1" t="s">
         <v>424</v>
       </c>
@@ -4764,7 +4763,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="139" spans="1:10" hidden="1">
+    <row r="139" spans="1:10">
       <c r="A139" s="1" t="s">
         <v>325</v>
       </c>
@@ -4796,7 +4795,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="140" spans="1:10" hidden="1">
+    <row r="140" spans="1:10">
       <c r="A140" s="1" t="s">
         <v>327</v>
       </c>
@@ -4828,7 +4827,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="141" spans="1:10" hidden="1">
+    <row r="141" spans="1:10">
       <c r="A141" s="1" t="s">
         <v>425</v>
       </c>
@@ -4860,7 +4859,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="142" spans="1:10" hidden="1">
+    <row r="142" spans="1:10">
       <c r="A142" s="1" t="s">
         <v>281</v>
       </c>
@@ -4892,7 +4891,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="143" spans="1:10" hidden="1">
+    <row r="143" spans="1:10">
       <c r="A143" s="1" t="s">
         <v>282</v>
       </c>
@@ -4924,7 +4923,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="144" spans="1:10" hidden="1">
+    <row r="144" spans="1:10">
       <c r="A144" s="1" t="s">
         <v>355</v>
       </c>
@@ -4956,7 +4955,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="145" spans="1:10" hidden="1">
+    <row r="145" spans="1:10">
       <c r="A145" s="1" t="s">
         <v>357</v>
       </c>
@@ -4988,7 +4987,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="146" spans="1:10" hidden="1">
+    <row r="146" spans="1:10">
       <c r="A146" s="1" t="s">
         <v>353</v>
       </c>
@@ -5020,7 +5019,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="147" spans="1:10" hidden="1">
+    <row r="147" spans="1:10">
       <c r="A147" s="1" t="s">
         <v>354</v>
       </c>
@@ -5052,7 +5051,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="148" spans="1:10" hidden="1">
+    <row r="148" spans="1:10">
       <c r="A148" s="1" t="s">
         <v>356</v>
       </c>
@@ -5084,7 +5083,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="149" spans="1:10" hidden="1">
+    <row r="149" spans="1:10">
       <c r="A149" s="1" t="s">
         <v>410</v>
       </c>
@@ -5116,7 +5115,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="150" spans="1:10" hidden="1">
+    <row r="150" spans="1:10">
       <c r="A150" s="1" t="s">
         <v>411</v>
       </c>
@@ -5148,7 +5147,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="151" spans="1:10" hidden="1">
+    <row r="151" spans="1:10">
       <c r="A151" s="1" t="s">
         <v>409</v>
       </c>
@@ -5180,7 +5179,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="152" spans="1:10" hidden="1">
+    <row r="152" spans="1:10">
       <c r="A152" s="1" t="s">
         <v>412</v>
       </c>
@@ -5212,7 +5211,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="153" spans="1:10" hidden="1">
+    <row r="153" spans="1:10">
       <c r="A153" s="1" t="s">
         <v>406</v>
       </c>
@@ -5244,7 +5243,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="154" spans="1:10" hidden="1">
+    <row r="154" spans="1:10">
       <c r="A154" s="1" t="s">
         <v>405</v>
       </c>
@@ -5276,7 +5275,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="155" spans="1:10" hidden="1">
+    <row r="155" spans="1:10">
       <c r="A155" s="1" t="s">
         <v>407</v>
       </c>
@@ -5308,7 +5307,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="156" spans="1:10" hidden="1">
+    <row r="156" spans="1:10">
       <c r="A156" s="1" t="s">
         <v>408</v>
       </c>
@@ -5340,7 +5339,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="157" spans="1:10" hidden="1">
+    <row r="157" spans="1:10">
       <c r="A157" s="1" t="s">
         <v>326</v>
       </c>
@@ -5372,7 +5371,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="158" spans="1:10" hidden="1">
+    <row r="158" spans="1:10">
       <c r="A158" s="1" t="s">
         <v>324</v>
       </c>
@@ -5404,7 +5403,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="159" spans="1:10" hidden="1">
+    <row r="159" spans="1:10">
       <c r="B159" t="s">
         <v>90</v>
       </c>
@@ -5424,7 +5423,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="160" spans="1:10" hidden="1">
+    <row r="160" spans="1:10">
       <c r="A160" s="1" t="s">
         <v>455</v>
       </c>
@@ -5485,7 +5484,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="162" spans="1:10" hidden="1">
+    <row r="162" spans="1:10">
       <c r="B162" t="s">
         <v>199</v>
       </c>
@@ -5511,7 +5510,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="163" spans="1:10" hidden="1">
+    <row r="163" spans="1:10">
       <c r="B163" t="s">
         <v>199</v>
       </c>
@@ -5537,7 +5536,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="164" spans="1:10" hidden="1">
+    <row r="164" spans="1:10">
       <c r="B164" t="s">
         <v>219</v>
       </c>
@@ -5563,7 +5562,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="165" spans="1:10" hidden="1">
+    <row r="165" spans="1:10">
       <c r="B165" t="s">
         <v>219</v>
       </c>
@@ -5589,7 +5588,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="166" spans="1:10" hidden="1">
+    <row r="166" spans="1:10">
       <c r="A166" s="1" t="s">
         <v>421</v>
       </c>
@@ -5621,7 +5620,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="167" spans="1:10" hidden="1">
+    <row r="167" spans="1:10">
       <c r="A167" s="1" t="s">
         <v>422</v>
       </c>
@@ -5769,7 +5768,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="172" spans="1:10" hidden="1">
+    <row r="172" spans="1:10">
       <c r="B172" t="s">
         <v>257</v>
       </c>
@@ -5795,7 +5794,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="173" spans="1:10" hidden="1">
+    <row r="173" spans="1:10">
       <c r="B173" t="s">
         <v>258</v>
       </c>
@@ -5821,7 +5820,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="174" spans="1:10" hidden="1">
+    <row r="174" spans="1:10">
       <c r="A174" s="1" t="s">
         <v>454</v>
       </c>
@@ -5882,7 +5881,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="176" spans="1:10" hidden="1">
+    <row r="176" spans="1:10">
       <c r="A176" s="1" t="s">
         <v>428</v>
       </c>
@@ -5914,7 +5913,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="177" spans="1:10" hidden="1">
+    <row r="177" spans="1:10">
       <c r="A177" s="1" t="s">
         <v>346</v>
       </c>
@@ -5946,7 +5945,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="178" spans="1:10" hidden="1">
+    <row r="178" spans="1:10">
       <c r="A178" s="1" t="s">
         <v>348</v>
       </c>
@@ -5978,7 +5977,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="179" spans="1:10" hidden="1">
+    <row r="179" spans="1:10">
       <c r="A179" s="1" t="s">
         <v>427</v>
       </c>
@@ -6010,7 +6009,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="180" spans="1:10" hidden="1">
+    <row r="180" spans="1:10">
       <c r="B180" t="s">
         <v>218</v>
       </c>
@@ -6036,7 +6035,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="181" spans="1:10" hidden="1">
+    <row r="181" spans="1:10">
       <c r="A181" s="1" t="s">
         <v>431</v>
       </c>
@@ -6068,7 +6067,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="182" spans="1:10" hidden="1">
+    <row r="182" spans="1:10">
       <c r="A182" s="1" t="s">
         <v>432</v>
       </c>
@@ -6100,7 +6099,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="183" spans="1:10" hidden="1">
+    <row r="183" spans="1:10">
       <c r="A183" s="1" t="s">
         <v>430</v>
       </c>
@@ -6132,7 +6131,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="184" spans="1:10" hidden="1">
+    <row r="184" spans="1:10">
       <c r="A184" s="1" t="s">
         <v>433</v>
       </c>
@@ -6164,7 +6163,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="185" spans="1:10" hidden="1">
+    <row r="185" spans="1:10">
       <c r="A185" s="1" t="s">
         <v>285</v>
       </c>
@@ -6196,7 +6195,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="186" spans="1:10" hidden="1">
+    <row r="186" spans="1:10">
       <c r="A186" s="1" t="s">
         <v>286</v>
       </c>
@@ -6228,7 +6227,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="187" spans="1:10" hidden="1">
+    <row r="187" spans="1:10">
       <c r="A187" s="1" t="s">
         <v>287</v>
       </c>
@@ -6260,7 +6259,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="188" spans="1:10" hidden="1">
+    <row r="188" spans="1:10">
       <c r="A188" s="1" t="s">
         <v>305</v>
       </c>
@@ -6292,7 +6291,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="189" spans="1:10" hidden="1">
+    <row r="189" spans="1:10">
       <c r="A189" s="1" t="s">
         <v>306</v>
       </c>
@@ -6324,7 +6323,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="190" spans="1:10" hidden="1">
+    <row r="190" spans="1:10">
       <c r="A190" s="1" t="s">
         <v>352</v>
       </c>
@@ -6356,7 +6355,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="191" spans="1:10" hidden="1">
+    <row r="191" spans="1:10">
       <c r="A191" s="1" t="s">
         <v>358</v>
       </c>
@@ -6388,7 +6387,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="192" spans="1:10" hidden="1">
+    <row r="192" spans="1:10">
       <c r="A192" s="1" t="s">
         <v>359</v>
       </c>
@@ -6420,7 +6419,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="193" spans="1:10" hidden="1">
+    <row r="193" spans="1:10">
       <c r="A193" s="1" t="s">
         <v>349</v>
       </c>
@@ -6452,7 +6451,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="194" spans="1:10" hidden="1">
+    <row r="194" spans="1:10">
       <c r="A194" s="1" t="s">
         <v>350</v>
       </c>
@@ -6484,7 +6483,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="195" spans="1:10" hidden="1">
+    <row r="195" spans="1:10">
       <c r="A195" s="1" t="s">
         <v>351</v>
       </c>
@@ -6516,7 +6515,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="196" spans="1:10" hidden="1">
+    <row r="196" spans="1:10">
       <c r="A196" s="1" t="s">
         <v>418</v>
       </c>
@@ -6548,7 +6547,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="197" spans="1:10" hidden="1">
+    <row r="197" spans="1:10">
       <c r="A197" s="1" t="s">
         <v>419</v>
       </c>
@@ -6580,7 +6579,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="198" spans="1:10" hidden="1">
+    <row r="198" spans="1:10">
       <c r="A198" s="1" t="s">
         <v>420</v>
       </c>
@@ -6612,7 +6611,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="199" spans="1:10" hidden="1">
+    <row r="199" spans="1:10">
       <c r="A199" s="1" t="s">
         <v>437</v>
       </c>
@@ -6644,7 +6643,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="200" spans="1:10" hidden="1">
+    <row r="200" spans="1:10">
       <c r="A200" s="1" t="s">
         <v>436</v>
       </c>
@@ -6676,7 +6675,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="201" spans="1:10" hidden="1">
+    <row r="201" spans="1:10">
       <c r="A201" s="1" t="s">
         <v>435</v>
       </c>
@@ -6708,7 +6707,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="202" spans="1:10" hidden="1">
+    <row r="202" spans="1:10">
       <c r="A202" s="1" t="s">
         <v>434</v>
       </c>
@@ -6740,7 +6739,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="203" spans="1:10" hidden="1">
+    <row r="203" spans="1:10">
       <c r="A203" s="1" t="s">
         <v>438</v>
       </c>
@@ -6772,7 +6771,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="204" spans="1:10" hidden="1">
+    <row r="204" spans="1:10">
       <c r="A204" s="1" t="s">
         <v>439</v>
       </c>
@@ -6804,7 +6803,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="205" spans="1:10" hidden="1">
+    <row r="205" spans="1:10">
       <c r="A205" s="1" t="s">
         <v>453</v>
       </c>
@@ -6836,7 +6835,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="206" spans="1:10" hidden="1">
+    <row r="206" spans="1:10">
       <c r="A206" s="1" t="s">
         <v>452</v>
       </c>
@@ -6870,11 +6869,6 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:J206">
-    <filterColumn colId="3">
-      <filters>
-        <filter val="CENTRAL"/>
-      </filters>
-    </filterColumn>
     <sortState ref="A2:J206">
       <sortCondition ref="B1:B206"/>
     </sortState>

</xml_diff>

<commit_message>
Data and modifications to phone list, etc.
</commit_message>
<xml_diff>
--- a/config/phone_list.xlsx
+++ b/config/phone_list.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1063" uniqueCount="463">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1070" uniqueCount="465">
   <si>
     <t>PH_NUMBER</t>
   </si>
@@ -1416,6 +1416,12 @@
   </si>
   <si>
     <t>GAOXIONG,TAIZHONG_SOUTH,南區，YANCHENG,GUSHAN,ZUOYING,NANZI,SANMIN,XINXING,QIANJIN,LINGYA,QIANZHEN,QIJIN,XIAOGANG,FENGSHAN,LINYUAN,DALIAO,DASHU,DASHE,RENWU,NIAOSONG,GANGSHAN,QIAOTOU,YANCHAO,TIANLIAO,ALIAN,GAOXIONG_LUZHU,HUNEI,QIEDING,YONGAN,MITUO,ZIGUAN,QISHAN,MEINONG,LIUGUI,JIAXIAN,SHANLIN,NEIMEN,MAOLIN,GAOXIONG_TAOYUAN,NAMAXIA,JIAYI,TAIBAO,PUZI,BUDAI,DALIN,MINXIONG,XIKOU,XINGANG,LIUJIAO,JIAYI_DONGSHI,YIZHU,LUCAO,SHUISHANG,ZHONGPU,ZHUQI,MEISHAN,FANLU,DAPU,ALISHAN,NANTOU,NANTOU_CITY,PULI,CAOTUN,ZHUSHAN,JIJI,MINGJIAN,LUGU,ZHONGLIAO,YUCHI,GUOXING,SHUILI,NANYOU_XINYI,NANYOU_RENAI,PENGHU,MAGONG,HUXI,BAISHA,XIYU,WANGAN,QIMEI,PINGDONG,PINGDONG_CITY,CHAZHOU,DONGANG,DONGGANG,HENGCHUN,WANDAN,CHANGZHI,LINLUO,JIURU,LIGANG,YANPU,GAOSHU,WANLUAN,NEIPU,ZHUTIAN,XINPI,FANGLIAO,XINYUAN,KANDING,LINBIAN,NANZHOU,JIADONG,LIUQIU,CHECHENG,MANZHOU,FANGSHAN,SANDIMEN,WUTAI,MAJIA,TAIWU,LAIYI,CHUNRI,SHIZI,MUDAN,TAINAN,XINYING,YANSHUI,BAIHE,LIUYING,HOUBI,DONGSHAN,MADOU,XIAYING,LIUJIA,GUANTIAN,DANEI,JIALI,XUEJIA,XIGANG,QIGU,JIANGJUN,BEIMEN,XINHUA,SHANHUA,XINSHI,ANDING,SHANSHANGQU,YUJING,NANXI,NANHUA,ZUOZHEN,RENDE,GUIREN,GUANMIAO,LONGQI,YONGKANG,TAINAN_EAST,TAINAN_SOUTH,TAINAN_NORTH,ANNAN,ANPING,WEST_CENTRAL,TAIZHONG,NANTUN,BEITUN,FENGYUAN,TAIZHONG_DONGSHI,DAJIA,QINGSHUI,SHALU,WUQI,HOULI,SHENGANG,TANZI,DAYA,XINSHE,SHIGANG,WAIPU,TAIZHONG_DAAN,WURI,DADU,LONGJING,WUFENG,TAIPING,DALI,HEPING,TAIZHONG_WEST,TAIZHONG_EAST,XITUN,TAIZHONG_CENTRAL,TAIZHONG_NORTH,TAIZHONG_SOUTH,YUNLIN,DOULIU,DOUNAN,HUWEI,XILUO,TUKU,BEIGANG,GUKENG,DAPI,CITONG,LINNEI,ERLUN,LUNBEI,MAILIAO,YULIN_DONGSHI,BAOZHONG,TAIXI,YUANCHANG,SIHU,KOUHU,SHUILIN,ZHANGHUA,ZHANGHUA_CITY,YUANLIN,LUGANG,HEMEI,BEIDOU,ZHANGHUA_XIHU,TIANZHONG,ERLIN,XIANXI,SHENGANG,ZHANGHUA_FUXING,XIUSHUI,HUATAN,FENYUAN,DACUN,PUYAN,PUXIN,YONGJING,SHETOU,ERSHUI,TIANWEI,PITOU,FANGYUAN,DACHENG,ZHUTANG,XIZHOU,高雄,高雄市,鹽埕區,鼓山區,左營區,楠梓區,三民區,新興區,前金區,苓雅區,前鎮區,旗津區,小港區,鳳山區,林園區,大寮區,大樹區,大社區,仁武區,鳥松區,岡山區,橋頭區,燕巢區,田寮區,阿蓮區,路竹區,湖內區,茄萣區,永安區,彌陀區,梓官區,旗山區,美濃區,六龜區,甲仙區,杉林區,內門區,茂林區,桃源區,那瑪夏區,嘉義,太保市,朴子市,布袋鎮,大林鎮,民雄鄉,溪口鄉,新港鄉,六腳鄉,東石鄉,義竹鄉,鹿草鄉,水上鄉,中埔鄉,竹崎鄉,梅山鄉,番路鄉,大埔鄉,阿里山鄉,南投,南投市,埔里鎮,草屯鎮,竹山鎮,集集鎮,名間鄉,鹿谷鄉,中寮鄉,魚池鄉,國姓鄉,水里鄉,信義鄉,仁愛鄉,澎湖,馬公市,湖西鄉,白沙鄉,西嶼鄉,望安鄉,七美鄉,屏東,屏東市,潮州鎮,東港鎮,恆春鎮,萬丹鄉,長治鄉,麟洛鄉,九如鄉,里港鄉,鹽埔鄉,高樹鄉,萬巒鄉,內埔鄉,竹田鄉,新埤鄉,枋寮鄉,新園鄉,崁頂鄉,林邊鄉,南州鄉,佳冬鄉,琉球鄉,車城鄉,滿州鄉,枋山鄉,三地門鄉,霧臺鄉,瑪家鄉,泰武鄉,來義鄉,春日鄉,獅子鄉,牡丹鄉,台南,臺南,新營區,鹽水區,白河區,柳營區,後壁區,東山區,麻豆區,下營區,六甲區,官田區,大內區,佳里區,學甲區,西港區,七股區,將軍區,北門區,新化區,善化區,新市區,安定區,山上區,玉井區,楠西區,南化區,左鎮區,仁德區,歸仁區,關廟區,龍崎區,永康區,台南東區,臺南東區,台南南區,臺南南區,台南北區,臺南北區,安南區,安平區,中西區,台中,臺中,南屯區,北屯區,豐原區,東勢區,大甲區,清水區,沙鹿區,梧棲區,后里區,神岡區,潭子區,大雅區,新社區,石岡區,外埔區,台中大安區,臺中大安區,烏日區,大肚區,龍井區,霧峰區,太平區,大里區,和平區,台中西區,臺中西區,台中東區,臺中東區,西屯區,台中中區,臺中中區,台中北區,臺中北區,台中南區,臺中南區,雲林,斗六市,斗南鎮,虎尾鎮,西螺鎮,土庫鎮,北港鎮,古坑鄉,大埤鄉,莿桐鄉,林內鄉,二崙鄉,崙背鄉,麥寮鄉,東勢鄉,褒忠鄉,臺西鄉,元長鄉,四湖鄉,口湖鄉,水林鄉,彰化,彰化市,員林市,鹿港鎮,和美鎮,北斗鎮,溪湖鎮,田中鎮,二林鎮,線西鄉,伸港鄉,彰化福興鄉,秀水鄉,花壇鄉,芬園鄉,大村鄉,埔鹽鄉,埔心鄉,永靖鄉,社頭鄉,二水鄉,田尾鄉,埤頭鄉,芳苑鄉,大城鄉,竹塘鄉,溪州鄉</t>
+  </si>
+  <si>
+    <t>0988128506</t>
+  </si>
+  <si>
+    <t>SENIOR_COUPLE</t>
   </si>
 </sst>
 </file>
@@ -1746,10 +1752,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J206"/>
+  <dimension ref="A1:J207"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView tabSelected="1" topLeftCell="G129" workbookViewId="0">
+      <selection activeCell="H147" sqref="H147"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3897,7 +3903,7 @@
         <v>1</v>
       </c>
       <c r="I110">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J110" t="s">
         <v>69</v>
@@ -3981,7 +3987,7 @@
         <v>1</v>
       </c>
       <c r="I113">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J113" t="s">
         <v>77</v>
@@ -4173,7 +4179,7 @@
         <v>1</v>
       </c>
       <c r="I119">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J119" t="s">
         <v>30</v>
@@ -5013,7 +5019,7 @@
         <v>1</v>
       </c>
       <c r="I146">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J146" t="s">
         <v>131</v>
@@ -5205,7 +5211,7 @@
         <v>1</v>
       </c>
       <c r="I152">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J152" t="s">
         <v>164</v>
@@ -6317,7 +6323,7 @@
         <v>1</v>
       </c>
       <c r="I189">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J189" t="s">
         <v>61</v>
@@ -6865,6 +6871,35 @@
       </c>
       <c r="J206" t="s">
         <v>249</v>
+      </c>
+    </row>
+    <row r="207" spans="1:10">
+      <c r="A207" s="1" t="s">
+        <v>463</v>
+      </c>
+      <c r="B207" t="s">
+        <v>464</v>
+      </c>
+      <c r="C207" t="s">
+        <v>13</v>
+      </c>
+      <c r="D207" t="s">
+        <v>12</v>
+      </c>
+      <c r="E207" t="s">
+        <v>13</v>
+      </c>
+      <c r="F207" t="s">
+        <v>12</v>
+      </c>
+      <c r="G207" t="s">
+        <v>11</v>
+      </c>
+      <c r="H207">
+        <v>0</v>
+      </c>
+      <c r="I207">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
t addData update; remove unnecessary files
</commit_message>
<xml_diff>
--- a/config/phone_list.xlsx
+++ b/config/phone_list.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Toon Town\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="J:\ARPS\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -17,7 +17,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$Q$204</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="152511" calcMode="manual" calcCompleted="0" calcOnSave="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -1620,12 +1620,6 @@
   </si>
   <si>
     <t>E. McNeil ZL/ Hansen ZL</t>
-  </si>
-  <si>
-    <t>E. Elliott Operations Assistant</t>
-  </si>
-  <si>
-    <t>E. Smith Recorder</t>
   </si>
   <si>
     <t>E. Luther DL/ Smith</t>
@@ -2449,6 +2443,12 @@
   </si>
   <si>
     <t>Senior Couple</t>
+  </si>
+  <si>
+    <t>E. Elliott</t>
+  </si>
+  <si>
+    <t>E. Smith DL</t>
   </si>
 </sst>
 </file>
@@ -2789,8 +2789,8 @@
   <dimension ref="A1:Q205"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A177" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C207" sqref="C207"/>
+      <pane ySplit="1" topLeftCell="A118" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G128" sqref="G128"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2816,7 +2816,7 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>571</v>
+        <v>569</v>
       </c>
       <c r="D1" t="s">
         <v>456</v>
@@ -4436,10 +4436,10 @@
         <v>110</v>
       </c>
       <c r="C94" t="s">
-        <v>572</v>
+        <v>570</v>
       </c>
       <c r="D94" t="s">
-        <v>682</v>
+        <v>680</v>
       </c>
       <c r="E94" t="s">
         <v>506</v>
@@ -4477,10 +4477,10 @@
         <v>31</v>
       </c>
       <c r="C95" t="s">
-        <v>573</v>
+        <v>571</v>
       </c>
       <c r="D95" t="s">
-        <v>688</v>
+        <v>686</v>
       </c>
       <c r="E95" t="s">
         <v>508</v>
@@ -4515,10 +4515,10 @@
         <v>31</v>
       </c>
       <c r="C96" t="s">
-        <v>573</v>
+        <v>571</v>
       </c>
       <c r="D96" t="s">
-        <v>688</v>
+        <v>686</v>
       </c>
       <c r="E96" t="s">
         <v>507</v>
@@ -4553,10 +4553,10 @@
         <v>167</v>
       </c>
       <c r="C97" t="s">
-        <v>574</v>
+        <v>572</v>
       </c>
       <c r="D97" t="s">
-        <v>689</v>
+        <v>687</v>
       </c>
       <c r="E97" t="s">
         <v>462</v>
@@ -4594,10 +4594,10 @@
         <v>170</v>
       </c>
       <c r="C98" t="s">
-        <v>575</v>
+        <v>573</v>
       </c>
       <c r="D98" t="s">
-        <v>690</v>
+        <v>688</v>
       </c>
       <c r="E98" t="s">
         <v>463</v>
@@ -4635,10 +4635,10 @@
         <v>172</v>
       </c>
       <c r="C99" t="s">
-        <v>576</v>
+        <v>574</v>
       </c>
       <c r="D99" t="s">
-        <v>683</v>
+        <v>681</v>
       </c>
       <c r="E99" t="s">
         <v>509</v>
@@ -4676,10 +4676,10 @@
         <v>207</v>
       </c>
       <c r="C100" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="D100" t="s">
-        <v>691</v>
+        <v>689</v>
       </c>
       <c r="E100" t="s">
         <v>510</v>
@@ -4717,10 +4717,10 @@
         <v>89</v>
       </c>
       <c r="C101" t="s">
-        <v>578</v>
+        <v>576</v>
       </c>
       <c r="D101" t="s">
-        <v>684</v>
+        <v>682</v>
       </c>
       <c r="E101" t="s">
         <v>511</v>
@@ -4758,10 +4758,10 @@
         <v>95</v>
       </c>
       <c r="C102" t="s">
-        <v>579</v>
+        <v>577</v>
       </c>
       <c r="D102" t="s">
-        <v>685</v>
+        <v>683</v>
       </c>
       <c r="E102" t="s">
         <v>464</v>
@@ -4799,10 +4799,10 @@
         <v>198</v>
       </c>
       <c r="C103" t="s">
-        <v>580</v>
+        <v>578</v>
       </c>
       <c r="D103" t="s">
-        <v>686</v>
+        <v>684</v>
       </c>
       <c r="E103" t="s">
         <v>512</v>
@@ -4840,10 +4840,10 @@
         <v>92</v>
       </c>
       <c r="C104" t="s">
-        <v>587</v>
+        <v>585</v>
       </c>
       <c r="D104" t="s">
-        <v>736</v>
+        <v>734</v>
       </c>
       <c r="E104" t="s">
         <v>513</v>
@@ -4881,10 +4881,10 @@
         <v>96</v>
       </c>
       <c r="C105" t="s">
-        <v>586</v>
+        <v>584</v>
       </c>
       <c r="D105" t="s">
-        <v>737</v>
+        <v>735</v>
       </c>
       <c r="E105" t="s">
         <v>465</v>
@@ -4922,10 +4922,10 @@
         <v>164</v>
       </c>
       <c r="C106" t="s">
-        <v>581</v>
+        <v>579</v>
       </c>
       <c r="D106" t="s">
-        <v>687</v>
+        <v>685</v>
       </c>
       <c r="E106" t="s">
         <v>514</v>
@@ -4963,10 +4963,10 @@
         <v>68</v>
       </c>
       <c r="C107" t="s">
-        <v>585</v>
+        <v>583</v>
       </c>
       <c r="D107" t="s">
-        <v>753</v>
+        <v>751</v>
       </c>
       <c r="E107" t="s">
         <v>515</v>
@@ -5004,10 +5004,10 @@
         <v>72</v>
       </c>
       <c r="C108" t="s">
-        <v>584</v>
+        <v>582</v>
       </c>
       <c r="D108" t="s">
-        <v>754</v>
+        <v>752</v>
       </c>
       <c r="E108" t="s">
         <v>516</v>
@@ -5045,10 +5045,10 @@
         <v>448</v>
       </c>
       <c r="C109" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="D109" t="s">
-        <v>755</v>
+        <v>753</v>
       </c>
       <c r="E109" t="s">
         <v>466</v>
@@ -5086,10 +5086,10 @@
         <v>446</v>
       </c>
       <c r="C110" t="s">
-        <v>582</v>
+        <v>580</v>
       </c>
       <c r="D110" t="s">
-        <v>756</v>
+        <v>754</v>
       </c>
       <c r="E110" t="s">
         <v>517</v>
@@ -5124,10 +5124,10 @@
         <v>76</v>
       </c>
       <c r="C111" t="s">
-        <v>591</v>
+        <v>589</v>
       </c>
       <c r="D111" t="s">
-        <v>783</v>
+        <v>781</v>
       </c>
       <c r="J111" t="s">
         <v>64</v>
@@ -5156,10 +5156,10 @@
         <v>77</v>
       </c>
       <c r="C112" t="s">
-        <v>592</v>
+        <v>590</v>
       </c>
       <c r="D112" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="J112" t="s">
         <v>64</v>
@@ -5191,10 +5191,10 @@
         <v>73</v>
       </c>
       <c r="C113" t="s">
-        <v>588</v>
+        <v>586</v>
       </c>
       <c r="D113" t="s">
-        <v>757</v>
+        <v>755</v>
       </c>
       <c r="E113" t="s">
         <v>518</v>
@@ -5232,10 +5232,10 @@
         <v>78</v>
       </c>
       <c r="C114" t="s">
-        <v>595</v>
+        <v>593</v>
       </c>
       <c r="D114" t="s">
-        <v>758</v>
+        <v>756</v>
       </c>
       <c r="E114" t="s">
         <v>519</v>
@@ -5273,10 +5273,10 @@
         <v>48</v>
       </c>
       <c r="C115" t="s">
-        <v>593</v>
+        <v>591</v>
       </c>
       <c r="D115" t="s">
-        <v>738</v>
+        <v>736</v>
       </c>
       <c r="E115" t="s">
         <v>520</v>
@@ -5314,10 +5314,10 @@
         <v>51</v>
       </c>
       <c r="C116" t="s">
-        <v>594</v>
+        <v>592</v>
       </c>
       <c r="D116" t="s">
-        <v>739</v>
+        <v>737</v>
       </c>
       <c r="E116" t="s">
         <v>467</v>
@@ -5355,10 +5355,10 @@
         <v>468</v>
       </c>
       <c r="C117" t="s">
-        <v>607</v>
+        <v>605</v>
       </c>
       <c r="D117" t="s">
-        <v>692</v>
+        <v>690</v>
       </c>
       <c r="E117" t="s">
         <v>521</v>
@@ -5396,10 +5396,10 @@
         <v>103</v>
       </c>
       <c r="C118" t="s">
-        <v>608</v>
+        <v>606</v>
       </c>
       <c r="D118" t="s">
-        <v>695</v>
+        <v>693</v>
       </c>
       <c r="E118" t="s">
         <v>469</v>
@@ -5437,10 +5437,10 @@
         <v>450</v>
       </c>
       <c r="C119" t="s">
-        <v>609</v>
+        <v>607</v>
       </c>
       <c r="D119" t="s">
-        <v>710</v>
+        <v>708</v>
       </c>
       <c r="E119" t="s">
         <v>470</v>
@@ -5478,10 +5478,10 @@
         <v>174</v>
       </c>
       <c r="C120" t="s">
-        <v>610</v>
+        <v>608</v>
       </c>
       <c r="D120" t="s">
-        <v>716</v>
+        <v>714</v>
       </c>
       <c r="E120" t="s">
         <v>522</v>
@@ -5519,10 +5519,10 @@
         <v>60</v>
       </c>
       <c r="C121" t="s">
-        <v>611</v>
+        <v>609</v>
       </c>
       <c r="D121" t="s">
-        <v>785</v>
+        <v>783</v>
       </c>
       <c r="E121" t="s">
         <v>523</v>
@@ -5560,10 +5560,10 @@
         <v>62</v>
       </c>
       <c r="C122" t="s">
-        <v>612</v>
+        <v>610</v>
       </c>
       <c r="D122" t="s">
-        <v>786</v>
+        <v>784</v>
       </c>
       <c r="E122" t="s">
         <v>471</v>
@@ -5601,10 +5601,10 @@
         <v>25</v>
       </c>
       <c r="C123" t="s">
-        <v>589</v>
+        <v>587</v>
       </c>
       <c r="D123" t="s">
-        <v>740</v>
+        <v>738</v>
       </c>
       <c r="E123" t="s">
         <v>472</v>
@@ -5642,10 +5642,10 @@
         <v>30</v>
       </c>
       <c r="C124" t="s">
-        <v>590</v>
+        <v>588</v>
       </c>
       <c r="D124" t="s">
-        <v>741</v>
+        <v>739</v>
       </c>
       <c r="E124" t="s">
         <v>524</v>
@@ -5680,10 +5680,10 @@
         <v>256</v>
       </c>
       <c r="C125" t="s">
-        <v>613</v>
+        <v>611</v>
       </c>
       <c r="D125" t="s">
-        <v>742</v>
+        <v>740</v>
       </c>
       <c r="J125" t="s">
         <v>249</v>
@@ -5712,10 +5712,10 @@
         <v>255</v>
       </c>
       <c r="C126" t="s">
-        <v>614</v>
+        <v>612</v>
       </c>
       <c r="D126" t="s">
-        <v>743</v>
+        <v>741</v>
       </c>
       <c r="J126" t="s">
         <v>249</v>
@@ -5747,10 +5747,10 @@
         <v>252</v>
       </c>
       <c r="C127" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
       <c r="D127" t="s">
-        <v>717</v>
+        <v>715</v>
       </c>
       <c r="E127" t="s">
         <v>525</v>
@@ -5788,10 +5788,10 @@
         <v>104</v>
       </c>
       <c r="C128" t="s">
-        <v>616</v>
+        <v>614</v>
       </c>
       <c r="D128" t="s">
-        <v>718</v>
+        <v>716</v>
       </c>
       <c r="E128" t="s">
         <v>526</v>
@@ -5829,10 +5829,10 @@
         <v>107</v>
       </c>
       <c r="C129" t="s">
-        <v>617</v>
+        <v>615</v>
       </c>
       <c r="D129" t="s">
-        <v>719</v>
+        <v>717</v>
       </c>
       <c r="E129" t="s">
         <v>527</v>
@@ -5870,10 +5870,10 @@
         <v>39</v>
       </c>
       <c r="C130" t="s">
-        <v>618</v>
+        <v>616</v>
       </c>
       <c r="D130" t="s">
-        <v>720</v>
+        <v>718</v>
       </c>
       <c r="E130" t="s">
         <v>528</v>
@@ -5911,10 +5911,10 @@
         <v>42</v>
       </c>
       <c r="C131" t="s">
-        <v>619</v>
+        <v>617</v>
       </c>
       <c r="D131" t="s">
-        <v>721</v>
+        <v>719</v>
       </c>
       <c r="E131" t="s">
         <v>529</v>
@@ -5952,10 +5952,10 @@
         <v>473</v>
       </c>
       <c r="C132" t="s">
-        <v>620</v>
+        <v>618</v>
       </c>
       <c r="D132" t="s">
-        <v>697</v>
+        <v>695</v>
       </c>
       <c r="E132" t="s">
         <v>530</v>
@@ -5993,13 +5993,13 @@
         <v>33</v>
       </c>
       <c r="C133" t="s">
-        <v>621</v>
+        <v>619</v>
       </c>
       <c r="D133" t="s">
-        <v>734</v>
+        <v>732</v>
       </c>
       <c r="E133" t="s">
-        <v>531</v>
+        <v>790</v>
       </c>
       <c r="J133" t="s">
         <v>12</v>
@@ -6028,13 +6028,13 @@
         <v>33</v>
       </c>
       <c r="C134" t="s">
-        <v>621</v>
+        <v>619</v>
       </c>
       <c r="D134" t="s">
-        <v>734</v>
+        <v>732</v>
       </c>
       <c r="E134" t="s">
-        <v>532</v>
+        <v>791</v>
       </c>
       <c r="J134" t="s">
         <v>12</v>
@@ -6063,13 +6063,13 @@
         <v>21</v>
       </c>
       <c r="C135" t="s">
-        <v>622</v>
+        <v>620</v>
       </c>
       <c r="D135" t="s">
-        <v>694</v>
+        <v>692</v>
       </c>
       <c r="E135" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="J135" t="s">
         <v>22</v>
@@ -6104,10 +6104,10 @@
         <v>24</v>
       </c>
       <c r="C136" t="s">
-        <v>623</v>
+        <v>621</v>
       </c>
       <c r="D136" t="s">
-        <v>711</v>
+        <v>709</v>
       </c>
       <c r="E136" t="s">
         <v>474</v>
@@ -6145,13 +6145,13 @@
         <v>475</v>
       </c>
       <c r="C137" t="s">
-        <v>596</v>
+        <v>594</v>
       </c>
       <c r="D137" t="s">
-        <v>744</v>
+        <v>742</v>
       </c>
       <c r="E137" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
       <c r="J137" t="s">
         <v>186</v>
@@ -6186,13 +6186,13 @@
         <v>476</v>
       </c>
       <c r="C138" t="s">
-        <v>597</v>
+        <v>595</v>
       </c>
       <c r="D138" t="s">
-        <v>745</v>
+        <v>743</v>
       </c>
       <c r="E138" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
       <c r="J138" t="s">
         <v>186</v>
@@ -6227,13 +6227,13 @@
         <v>477</v>
       </c>
       <c r="C139" t="s">
-        <v>606</v>
+        <v>604</v>
       </c>
       <c r="D139" t="s">
-        <v>698</v>
+        <v>696</v>
       </c>
       <c r="E139" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
       <c r="J139" t="s">
         <v>80</v>
@@ -6268,10 +6268,10 @@
         <v>87</v>
       </c>
       <c r="C140" t="s">
-        <v>624</v>
+        <v>622</v>
       </c>
       <c r="D140" t="s">
-        <v>712</v>
+        <v>710</v>
       </c>
       <c r="E140" t="s">
         <v>478</v>
@@ -6309,10 +6309,10 @@
         <v>194</v>
       </c>
       <c r="C141" t="s">
-        <v>625</v>
+        <v>623</v>
       </c>
       <c r="D141" t="s">
-        <v>722</v>
+        <v>720</v>
       </c>
       <c r="E141" t="s">
         <v>479</v>
@@ -6350,13 +6350,13 @@
         <v>480</v>
       </c>
       <c r="C142" t="s">
-        <v>626</v>
+        <v>624</v>
       </c>
       <c r="D142" t="s">
-        <v>699</v>
+        <v>697</v>
       </c>
       <c r="E142" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="J142" t="s">
         <v>34</v>
@@ -6391,13 +6391,13 @@
         <v>37</v>
       </c>
       <c r="C143" t="s">
-        <v>627</v>
+        <v>625</v>
       </c>
       <c r="D143" t="s">
-        <v>696</v>
+        <v>694</v>
       </c>
       <c r="E143" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="J143" t="s">
         <v>34</v>
@@ -6432,10 +6432,10 @@
         <v>129</v>
       </c>
       <c r="C144" t="s">
-        <v>628</v>
+        <v>626</v>
       </c>
       <c r="D144" t="s">
-        <v>759</v>
+        <v>757</v>
       </c>
       <c r="E144" t="s">
         <v>481</v>
@@ -6473,10 +6473,10 @@
         <v>136</v>
       </c>
       <c r="C145" t="s">
-        <v>629</v>
+        <v>627</v>
       </c>
       <c r="D145" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="E145" t="s">
         <v>482</v>
@@ -6514,13 +6514,13 @@
         <v>483</v>
       </c>
       <c r="C146" t="s">
-        <v>630</v>
+        <v>628</v>
       </c>
       <c r="D146" t="s">
-        <v>761</v>
+        <v>759</v>
       </c>
       <c r="E146" t="s">
-        <v>539</v>
+        <v>537</v>
       </c>
       <c r="J146" t="s">
         <v>124</v>
@@ -6555,13 +6555,13 @@
         <v>127</v>
       </c>
       <c r="C147" t="s">
-        <v>631</v>
+        <v>629</v>
       </c>
       <c r="D147" t="s">
-        <v>762</v>
+        <v>760</v>
       </c>
       <c r="E147" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
       <c r="J147" t="s">
         <v>124</v>
@@ -6596,13 +6596,13 @@
         <v>133</v>
       </c>
       <c r="C148" t="s">
-        <v>632</v>
+        <v>630</v>
       </c>
       <c r="D148" t="s">
-        <v>763</v>
+        <v>761</v>
       </c>
       <c r="E148" t="s">
-        <v>541</v>
+        <v>539</v>
       </c>
       <c r="J148" t="s">
         <v>130</v>
@@ -6637,10 +6637,10 @@
         <v>160</v>
       </c>
       <c r="C149" t="s">
-        <v>633</v>
+        <v>631</v>
       </c>
       <c r="D149" t="s">
-        <v>788</v>
+        <v>786</v>
       </c>
       <c r="E149" t="s">
         <v>484</v>
@@ -6678,10 +6678,10 @@
         <v>162</v>
       </c>
       <c r="C150" t="s">
-        <v>634</v>
+        <v>632</v>
       </c>
       <c r="D150" t="s">
-        <v>787</v>
+        <v>785</v>
       </c>
       <c r="E150" t="s">
         <v>485</v>
@@ -6719,10 +6719,10 @@
         <v>156</v>
       </c>
       <c r="C151" t="s">
-        <v>598</v>
+        <v>596</v>
       </c>
       <c r="D151" t="s">
-        <v>764</v>
+        <v>762</v>
       </c>
       <c r="E151" t="s">
         <v>486</v>
@@ -6760,13 +6760,13 @@
         <v>163</v>
       </c>
       <c r="C152" t="s">
-        <v>635</v>
+        <v>633</v>
       </c>
       <c r="D152" t="s">
-        <v>765</v>
+        <v>763</v>
       </c>
       <c r="E152" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="J152" t="s">
         <v>157</v>
@@ -6801,10 +6801,10 @@
         <v>150</v>
       </c>
       <c r="C153" t="s">
-        <v>636</v>
+        <v>634</v>
       </c>
       <c r="D153" t="s">
-        <v>766</v>
+        <v>764</v>
       </c>
       <c r="E153" t="s">
         <v>487</v>
@@ -6842,13 +6842,13 @@
         <v>146</v>
       </c>
       <c r="C154" t="s">
-        <v>637</v>
+        <v>635</v>
       </c>
       <c r="D154" t="s">
-        <v>789</v>
+        <v>787</v>
       </c>
       <c r="E154" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="J154" t="s">
         <v>147</v>
@@ -6883,13 +6883,13 @@
         <v>152</v>
       </c>
       <c r="C155" t="s">
-        <v>638</v>
+        <v>636</v>
       </c>
       <c r="D155" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
       <c r="E155" t="s">
-        <v>544</v>
+        <v>542</v>
       </c>
       <c r="J155" t="s">
         <v>147</v>
@@ -6924,13 +6924,13 @@
         <v>155</v>
       </c>
       <c r="C156" t="s">
-        <v>639</v>
+        <v>637</v>
       </c>
       <c r="D156" t="s">
-        <v>768</v>
+        <v>766</v>
       </c>
       <c r="E156" t="s">
-        <v>545</v>
+        <v>543</v>
       </c>
       <c r="J156" t="s">
         <v>147</v>
@@ -6965,13 +6965,13 @@
         <v>85</v>
       </c>
       <c r="C157" t="s">
-        <v>599</v>
+        <v>597</v>
       </c>
       <c r="D157" t="s">
-        <v>746</v>
+        <v>744</v>
       </c>
       <c r="E157" t="s">
-        <v>546</v>
+        <v>544</v>
       </c>
       <c r="J157" t="s">
         <v>80</v>
@@ -7006,10 +7006,10 @@
         <v>79</v>
       </c>
       <c r="C158" t="s">
-        <v>600</v>
+        <v>598</v>
       </c>
       <c r="D158" t="s">
-        <v>790</v>
+        <v>788</v>
       </c>
       <c r="E158" t="s">
         <v>488</v>
@@ -7044,10 +7044,10 @@
         <v>86</v>
       </c>
       <c r="C159" t="s">
-        <v>640</v>
+        <v>638</v>
       </c>
       <c r="D159" t="s">
-        <v>723</v>
+        <v>721</v>
       </c>
       <c r="J159" t="s">
         <v>80</v>
@@ -7073,13 +7073,13 @@
         <v>248</v>
       </c>
       <c r="C160" t="s">
-        <v>641</v>
+        <v>639</v>
       </c>
       <c r="D160" t="s">
-        <v>724</v>
+        <v>722</v>
       </c>
       <c r="E160" t="s">
-        <v>547</v>
+        <v>545</v>
       </c>
       <c r="J160" t="s">
         <v>249</v>
@@ -7114,10 +7114,10 @@
         <v>28</v>
       </c>
       <c r="C161" t="s">
-        <v>642</v>
+        <v>640</v>
       </c>
       <c r="D161" t="s">
-        <v>735</v>
+        <v>733</v>
       </c>
       <c r="E161" t="s">
         <v>489</v>
@@ -7149,10 +7149,10 @@
         <v>191</v>
       </c>
       <c r="C162" t="s">
-        <v>643</v>
+        <v>641</v>
       </c>
       <c r="D162" t="s">
-        <v>747</v>
+        <v>745</v>
       </c>
       <c r="J162" t="s">
         <v>186</v>
@@ -7181,10 +7181,10 @@
         <v>209</v>
       </c>
       <c r="C163" t="s">
-        <v>644</v>
+        <v>642</v>
       </c>
       <c r="D163" t="s">
-        <v>748</v>
+        <v>746</v>
       </c>
       <c r="J163" t="s">
         <v>186</v>
@@ -7216,13 +7216,13 @@
         <v>490</v>
       </c>
       <c r="C164" t="s">
-        <v>646</v>
+        <v>644</v>
       </c>
       <c r="D164" t="s">
-        <v>700</v>
+        <v>698</v>
       </c>
       <c r="E164" t="s">
-        <v>548</v>
+        <v>546</v>
       </c>
       <c r="J164" t="s">
         <v>186</v>
@@ -7257,13 +7257,13 @@
         <v>189</v>
       </c>
       <c r="C165" t="s">
-        <v>645</v>
+        <v>643</v>
       </c>
       <c r="D165" t="s">
-        <v>701</v>
+        <v>699</v>
       </c>
       <c r="E165" t="s">
-        <v>549</v>
+        <v>547</v>
       </c>
       <c r="J165" t="s">
         <v>186</v>
@@ -7295,10 +7295,10 @@
         <v>16</v>
       </c>
       <c r="C166" t="s">
-        <v>647</v>
+        <v>645</v>
       </c>
       <c r="D166" t="s">
-        <v>749</v>
+        <v>747</v>
       </c>
       <c r="J166" t="s">
         <v>19</v>
@@ -7327,10 +7327,10 @@
         <v>17</v>
       </c>
       <c r="C167" t="s">
-        <v>648</v>
+        <v>646</v>
       </c>
       <c r="D167" t="s">
-        <v>750</v>
+        <v>748</v>
       </c>
       <c r="J167" t="s">
         <v>19</v>
@@ -7362,13 +7362,13 @@
         <v>14</v>
       </c>
       <c r="C168" t="s">
-        <v>650</v>
+        <v>648</v>
       </c>
       <c r="D168" t="s">
-        <v>725</v>
+        <v>723</v>
       </c>
       <c r="E168" t="s">
-        <v>550</v>
+        <v>548</v>
       </c>
       <c r="J168" t="s">
         <v>19</v>
@@ -7403,10 +7403,10 @@
         <v>449</v>
       </c>
       <c r="C169" t="s">
-        <v>649</v>
+        <v>647</v>
       </c>
       <c r="D169" t="s">
-        <v>726</v>
+        <v>724</v>
       </c>
       <c r="E169" t="s">
         <v>491</v>
@@ -7441,10 +7441,10 @@
         <v>246</v>
       </c>
       <c r="C170" t="s">
-        <v>651</v>
+        <v>649</v>
       </c>
       <c r="D170" t="s">
-        <v>727</v>
+        <v>725</v>
       </c>
       <c r="J170" t="s">
         <v>239</v>
@@ -7473,10 +7473,10 @@
         <v>247</v>
       </c>
       <c r="C171" t="s">
-        <v>652</v>
+        <v>650</v>
       </c>
       <c r="D171" t="s">
-        <v>728</v>
+        <v>726</v>
       </c>
       <c r="J171" t="s">
         <v>239</v>
@@ -7508,13 +7508,13 @@
         <v>243</v>
       </c>
       <c r="C172" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
       <c r="D172" t="s">
-        <v>729</v>
+        <v>727</v>
       </c>
       <c r="E172" t="s">
-        <v>551</v>
+        <v>549</v>
       </c>
       <c r="J172" t="s">
         <v>239</v>
@@ -7549,10 +7549,10 @@
         <v>18</v>
       </c>
       <c r="C173" t="s">
-        <v>654</v>
+        <v>652</v>
       </c>
       <c r="D173" t="s">
-        <v>713</v>
+        <v>711</v>
       </c>
       <c r="E173" t="s">
         <v>492</v>
@@ -7587,10 +7587,10 @@
         <v>206</v>
       </c>
       <c r="C174" t="s">
-        <v>655</v>
+        <v>653</v>
       </c>
       <c r="D174" t="s">
-        <v>730</v>
+        <v>728</v>
       </c>
       <c r="E174" t="s">
         <v>493</v>
@@ -7628,13 +7628,13 @@
         <v>108</v>
       </c>
       <c r="C175" t="s">
-        <v>656</v>
+        <v>654</v>
       </c>
       <c r="D175" t="s">
-        <v>702</v>
+        <v>700</v>
       </c>
       <c r="E175" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
       <c r="J175" t="s">
         <v>101</v>
@@ -7669,13 +7669,13 @@
         <v>113</v>
       </c>
       <c r="C176" t="s">
-        <v>657</v>
+        <v>655</v>
       </c>
       <c r="D176" t="s">
-        <v>703</v>
+        <v>701</v>
       </c>
       <c r="E176" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="J176" t="s">
         <v>101</v>
@@ -7710,13 +7710,13 @@
         <v>201</v>
       </c>
       <c r="C177" t="s">
-        <v>658</v>
+        <v>656</v>
       </c>
       <c r="D177" t="s">
-        <v>731</v>
+        <v>729</v>
       </c>
       <c r="E177" t="s">
-        <v>554</v>
+        <v>552</v>
       </c>
       <c r="J177" t="s">
         <v>202</v>
@@ -7748,10 +7748,10 @@
         <v>208</v>
       </c>
       <c r="C178" t="s">
-        <v>659</v>
+        <v>657</v>
       </c>
       <c r="D178" t="s">
-        <v>732</v>
+        <v>730</v>
       </c>
       <c r="J178" t="s">
         <v>202</v>
@@ -7783,13 +7783,13 @@
         <v>214</v>
       </c>
       <c r="C179" t="s">
-        <v>660</v>
+        <v>658</v>
       </c>
       <c r="D179" t="s">
-        <v>769</v>
+        <v>767</v>
       </c>
       <c r="E179" t="s">
-        <v>555</v>
+        <v>553</v>
       </c>
       <c r="J179" t="s">
         <v>210</v>
@@ -7824,13 +7824,13 @@
         <v>217</v>
       </c>
       <c r="C180" t="s">
-        <v>661</v>
+        <v>659</v>
       </c>
       <c r="D180" t="s">
-        <v>770</v>
+        <v>768</v>
       </c>
       <c r="E180" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="J180" t="s">
         <v>210</v>
@@ -7865,13 +7865,13 @@
         <v>494</v>
       </c>
       <c r="C181" t="s">
-        <v>662</v>
+        <v>660</v>
       </c>
       <c r="D181" t="s">
-        <v>771</v>
+        <v>769</v>
       </c>
       <c r="E181" t="s">
-        <v>557</v>
+        <v>555</v>
       </c>
       <c r="J181" t="s">
         <v>210</v>
@@ -7906,10 +7906,10 @@
         <v>218</v>
       </c>
       <c r="C182" t="s">
-        <v>663</v>
+        <v>661</v>
       </c>
       <c r="D182" t="s">
-        <v>772</v>
+        <v>770</v>
       </c>
       <c r="E182" t="s">
         <v>495</v>
@@ -7947,13 +7947,13 @@
         <v>43</v>
       </c>
       <c r="C183" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
       <c r="D183" t="s">
-        <v>751</v>
+        <v>749</v>
       </c>
       <c r="E183" t="s">
-        <v>558</v>
+        <v>556</v>
       </c>
       <c r="J183" t="s">
         <v>44</v>
@@ -7988,10 +7988,10 @@
         <v>46</v>
       </c>
       <c r="C184" t="s">
-        <v>602</v>
+        <v>600</v>
       </c>
       <c r="D184" t="s">
-        <v>752</v>
+        <v>750</v>
       </c>
       <c r="E184" t="s">
         <v>496</v>
@@ -8029,13 +8029,13 @@
         <v>47</v>
       </c>
       <c r="C185" t="s">
-        <v>664</v>
+        <v>662</v>
       </c>
       <c r="D185" t="s">
-        <v>704</v>
+        <v>702</v>
       </c>
       <c r="E185" t="s">
-        <v>559</v>
+        <v>557</v>
       </c>
       <c r="J185" t="s">
         <v>44</v>
@@ -8070,10 +8070,10 @@
         <v>55</v>
       </c>
       <c r="C186" t="s">
-        <v>665</v>
+        <v>663</v>
       </c>
       <c r="D186" t="s">
-        <v>693</v>
+        <v>691</v>
       </c>
       <c r="E186" t="s">
         <v>497</v>
@@ -8111,10 +8111,10 @@
         <v>58</v>
       </c>
       <c r="C187" t="s">
-        <v>666</v>
+        <v>664</v>
       </c>
       <c r="D187" t="s">
-        <v>714</v>
+        <v>712</v>
       </c>
       <c r="E187" t="s">
         <v>498</v>
@@ -8152,13 +8152,13 @@
         <v>121</v>
       </c>
       <c r="C188" t="s">
-        <v>667</v>
+        <v>665</v>
       </c>
       <c r="D188" t="s">
-        <v>733</v>
+        <v>731</v>
       </c>
       <c r="E188" t="s">
-        <v>560</v>
+        <v>558</v>
       </c>
       <c r="J188" t="s">
         <v>115</v>
@@ -8193,13 +8193,13 @@
         <v>137</v>
       </c>
       <c r="C189" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
       <c r="D189" t="s">
-        <v>705</v>
+        <v>703</v>
       </c>
       <c r="E189" t="s">
-        <v>561</v>
+        <v>559</v>
       </c>
       <c r="J189" t="s">
         <v>138</v>
@@ -8234,13 +8234,13 @@
         <v>140</v>
       </c>
       <c r="C190" t="s">
-        <v>669</v>
+        <v>667</v>
       </c>
       <c r="D190" t="s">
-        <v>706</v>
+        <v>704</v>
       </c>
       <c r="E190" t="s">
-        <v>562</v>
+        <v>560</v>
       </c>
       <c r="J190" t="s">
         <v>138</v>
@@ -8275,10 +8275,10 @@
         <v>114</v>
       </c>
       <c r="C191" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="D191" t="s">
-        <v>773</v>
+        <v>771</v>
       </c>
       <c r="E191" t="s">
         <v>499</v>
@@ -8316,13 +8316,13 @@
         <v>118</v>
       </c>
       <c r="C192" t="s">
-        <v>604</v>
+        <v>602</v>
       </c>
       <c r="D192" t="s">
-        <v>774</v>
+        <v>772</v>
       </c>
       <c r="E192" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
       <c r="J192" t="s">
         <v>115</v>
@@ -8357,13 +8357,13 @@
         <v>120</v>
       </c>
       <c r="C193" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
       <c r="D193" t="s">
-        <v>775</v>
+        <v>773</v>
       </c>
       <c r="E193" t="s">
-        <v>564</v>
+        <v>562</v>
       </c>
       <c r="J193" t="s">
         <v>115</v>
@@ -8398,10 +8398,10 @@
         <v>177</v>
       </c>
       <c r="C194" t="s">
-        <v>671</v>
+        <v>669</v>
       </c>
       <c r="D194" t="s">
-        <v>776</v>
+        <v>774</v>
       </c>
       <c r="E194" t="s">
         <v>500</v>
@@ -8439,10 +8439,10 @@
         <v>181</v>
       </c>
       <c r="C195" t="s">
-        <v>672</v>
+        <v>670</v>
       </c>
       <c r="D195" t="s">
-        <v>777</v>
+        <v>775</v>
       </c>
       <c r="E195" t="s">
         <v>501</v>
@@ -8480,13 +8480,13 @@
         <v>183</v>
       </c>
       <c r="C196" t="s">
-        <v>673</v>
+        <v>671</v>
       </c>
       <c r="D196" t="s">
-        <v>778</v>
+        <v>776</v>
       </c>
       <c r="E196" t="s">
-        <v>565</v>
+        <v>563</v>
       </c>
       <c r="J196" t="s">
         <v>178</v>
@@ -8521,10 +8521,10 @@
         <v>229</v>
       </c>
       <c r="C197" t="s">
-        <v>674</v>
+        <v>672</v>
       </c>
       <c r="D197" t="s">
-        <v>779</v>
+        <v>777</v>
       </c>
       <c r="E197" t="s">
         <v>502</v>
@@ -8562,10 +8562,10 @@
         <v>227</v>
       </c>
       <c r="C198" t="s">
-        <v>675</v>
+        <v>673</v>
       </c>
       <c r="D198" t="s">
-        <v>780</v>
+        <v>778</v>
       </c>
       <c r="E198" t="s">
         <v>503</v>
@@ -8603,13 +8603,13 @@
         <v>224</v>
       </c>
       <c r="C199" t="s">
-        <v>676</v>
+        <v>674</v>
       </c>
       <c r="D199" t="s">
-        <v>781</v>
+        <v>779</v>
       </c>
       <c r="E199" t="s">
-        <v>566</v>
+        <v>564</v>
       </c>
       <c r="J199" t="s">
         <v>221</v>
@@ -8644,13 +8644,13 @@
         <v>220</v>
       </c>
       <c r="C200" t="s">
-        <v>605</v>
+        <v>603</v>
       </c>
       <c r="D200" t="s">
-        <v>782</v>
+        <v>780</v>
       </c>
       <c r="E200" t="s">
-        <v>567</v>
+        <v>565</v>
       </c>
       <c r="J200" t="s">
         <v>221</v>
@@ -8685,13 +8685,13 @@
         <v>232</v>
       </c>
       <c r="C201" t="s">
-        <v>677</v>
+        <v>675</v>
       </c>
       <c r="D201" t="s">
-        <v>707</v>
+        <v>705</v>
       </c>
       <c r="E201" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
       <c r="J201" t="s">
         <v>233</v>
@@ -8726,13 +8726,13 @@
         <v>235</v>
       </c>
       <c r="C202" t="s">
-        <v>678</v>
+        <v>676</v>
       </c>
       <c r="D202" t="s">
-        <v>708</v>
+        <v>706</v>
       </c>
       <c r="E202" t="s">
-        <v>569</v>
+        <v>567</v>
       </c>
       <c r="J202" t="s">
         <v>233</v>
@@ -8767,10 +8767,10 @@
         <v>241</v>
       </c>
       <c r="C203" t="s">
-        <v>679</v>
+        <v>677</v>
       </c>
       <c r="D203" t="s">
-        <v>715</v>
+        <v>713</v>
       </c>
       <c r="E203" t="s">
         <v>504</v>
@@ -8808,13 +8808,13 @@
         <v>238</v>
       </c>
       <c r="C204" t="s">
-        <v>680</v>
+        <v>678</v>
       </c>
       <c r="D204" t="s">
-        <v>709</v>
+        <v>707</v>
       </c>
       <c r="E204" t="s">
-        <v>570</v>
+        <v>568</v>
       </c>
       <c r="J204" t="s">
         <v>239</v>
@@ -8849,10 +8849,10 @@
         <v>455</v>
       </c>
       <c r="C205" t="s">
-        <v>681</v>
+        <v>679</v>
       </c>
       <c r="D205" t="s">
-        <v>791</v>
+        <v>789</v>
       </c>
       <c r="E205" t="s">
         <v>505</v>

</xml_diff>

<commit_message>
Phone list and config update
</commit_message>
<xml_diff>
--- a/config/phone_list.xlsx
+++ b/config/phone_list.xlsx
@@ -17,7 +17,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">PHONE_LIST!$A$1:$N$101</definedName>
   </definedNames>
-  <calcPr calcId="152511" calcMode="manual"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1200" uniqueCount="717">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1200" uniqueCount="719">
   <si>
     <t>AREA_NAME</t>
   </si>
@@ -1133,9 +1133,6 @@
     <t>0963537337</t>
   </si>
   <si>
-    <t>Tuanmu B E</t>
-  </si>
-  <si>
     <t>天母 B 長老</t>
   </si>
   <si>
@@ -2226,6 +2223,15 @@
   </si>
   <si>
     <t>E. Lindahl / Dorius ZL</t>
+  </si>
+  <si>
+    <t>ZHUNAN_ZHENGNAN</t>
+  </si>
+  <si>
+    <t>LUZHOU_XINYI</t>
+  </si>
+  <si>
+    <t>Tianmu B E</t>
   </si>
 </sst>
 </file>
@@ -2573,7 +2579,7 @@
   <dimension ref="A1:N104"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2598,7 +2604,7 @@
         <v>3</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>4</v>
@@ -2642,10 +2648,10 @@
         <v>19</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
       <c r="G2" s="2" t="s">
         <v>20</v>
@@ -2686,10 +2692,10 @@
         <v>27</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
       <c r="G3" s="3" t="s">
         <v>28</v>
@@ -2711,7 +2717,7 @@
         <v>0</v>
       </c>
       <c r="N3" s="3" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
     </row>
     <row r="4" spans="1:14">
@@ -2728,10 +2734,10 @@
         <v>27</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
       <c r="G4" s="2" t="s">
         <v>28</v>
@@ -2753,7 +2759,7 @@
         <v>0</v>
       </c>
       <c r="N4" s="3" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
     </row>
     <row r="5" spans="1:14">
@@ -2770,10 +2776,10 @@
         <v>34</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>35</v>
@@ -2814,7 +2820,7 @@
         <v>41</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="F6" s="3" t="s">
         <v>42</v>
@@ -2858,10 +2864,10 @@
         <v>47</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
       <c r="G7" s="2" t="s">
         <v>35</v>
@@ -2902,10 +2908,10 @@
         <v>56</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
       <c r="G8" s="2" t="s">
         <v>57</v>
@@ -2946,7 +2952,7 @@
         <v>63</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="F9" s="3" t="s">
         <v>64</v>
@@ -2990,10 +2996,10 @@
         <v>68</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
       <c r="G10" s="2" t="s">
         <v>69</v>
@@ -3034,10 +3040,10 @@
         <v>75</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="G11" s="2" t="s">
         <v>57</v>
@@ -3078,7 +3084,7 @@
         <v>81</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="F12" s="2" t="s">
         <v>82</v>
@@ -3166,7 +3172,7 @@
         <v>95</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="F14" s="3" t="s">
         <v>96</v>
@@ -3210,10 +3216,10 @@
         <v>105</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
       <c r="G15" s="2" t="s">
         <v>97</v>
@@ -3254,7 +3260,7 @@
         <v>109</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="F16" s="2" t="s">
         <v>110</v>
@@ -3298,7 +3304,7 @@
         <v>116</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="F17" s="2" t="s">
         <v>117</v>
@@ -3342,10 +3348,10 @@
         <v>122</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
       <c r="G18" s="2" t="s">
         <v>98</v>
@@ -3386,10 +3392,10 @@
         <v>127</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
       <c r="G19" s="2" t="s">
         <v>98</v>
@@ -3433,7 +3439,7 @@
         <v>132</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
       <c r="G20" s="2" t="s">
         <v>132</v>
@@ -3477,7 +3483,7 @@
         <v>132</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
       <c r="G21" s="2" t="s">
         <v>132</v>
@@ -3518,10 +3524,10 @@
         <v>150</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="G22" s="2" t="s">
         <v>145</v>
@@ -3562,7 +3568,7 @@
         <v>143</v>
       </c>
       <c r="E23" s="4" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="F23" s="2" t="s">
         <v>144</v>
@@ -3606,7 +3612,7 @@
         <v>154</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="F24" s="2" t="s">
         <v>155</v>
@@ -3633,7 +3639,7 @@
         <v>0</v>
       </c>
       <c r="N24" s="3" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
     </row>
     <row r="25" spans="1:14">
@@ -3650,10 +3656,10 @@
         <v>217</v>
       </c>
       <c r="E25" s="4" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="F25" s="3" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
       <c r="G25" s="2" t="s">
         <v>156</v>
@@ -3697,7 +3703,7 @@
         <v>162</v>
       </c>
       <c r="F26" s="3" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="G26" s="2" t="s">
         <v>35</v>
@@ -3738,10 +3744,10 @@
         <v>167</v>
       </c>
       <c r="E27" s="4" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="F27" s="3" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
       <c r="G27" s="2" t="s">
         <v>168</v>
@@ -3782,10 +3788,10 @@
         <v>173</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="F28" s="3" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="G28" s="2" t="s">
         <v>168</v>
@@ -3826,10 +3832,10 @@
         <v>177</v>
       </c>
       <c r="E29" s="4" t="s">
-        <v>179</v>
+        <v>717</v>
       </c>
       <c r="F29" s="3" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="G29" s="2" t="s">
         <v>178</v>
@@ -3870,10 +3876,10 @@
         <v>184</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>179</v>
+        <v>717</v>
       </c>
       <c r="F30" s="3" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="G30" s="2" t="s">
         <v>178</v>
@@ -3917,7 +3923,7 @@
         <v>187</v>
       </c>
       <c r="F31" s="3" t="s">
-        <v>713</v>
+        <v>712</v>
       </c>
       <c r="G31" s="2" t="s">
         <v>185</v>
@@ -3958,10 +3964,10 @@
         <v>197</v>
       </c>
       <c r="E32" s="4" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="F32" s="3" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="G32" s="2" t="s">
         <v>145</v>
@@ -3985,7 +3991,7 @@
         <v>1</v>
       </c>
       <c r="N32" s="3" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
     </row>
     <row r="33" spans="1:14">
@@ -4002,10 +4008,10 @@
         <v>202</v>
       </c>
       <c r="E33" s="4" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="F33" s="3" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
       <c r="G33" s="2" t="s">
         <v>145</v>
@@ -4029,7 +4035,7 @@
         <v>1</v>
       </c>
       <c r="N33" s="3" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
     </row>
     <row r="34" spans="1:14">
@@ -4046,10 +4052,10 @@
         <v>206</v>
       </c>
       <c r="E34" s="4" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="F34" s="3" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="G34" s="2" t="s">
         <v>207</v>
@@ -4090,10 +4096,10 @@
         <v>213</v>
       </c>
       <c r="E35" s="4" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="F35" s="3" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="G35" s="2" t="s">
         <v>207</v>
@@ -4134,10 +4140,10 @@
         <v>222</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="F36" s="3" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
       <c r="G36" s="2" t="s">
         <v>156</v>
@@ -4159,7 +4165,7 @@
         <v>0</v>
       </c>
       <c r="N36" s="3" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
     </row>
     <row r="37" spans="1:14">
@@ -4176,10 +4182,10 @@
         <v>222</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="F37" s="3" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
       <c r="G37" s="2" t="s">
         <v>156</v>
@@ -4201,7 +4207,7 @@
         <v>0</v>
       </c>
       <c r="N37" s="3" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
     </row>
     <row r="38" spans="1:14">
@@ -4218,10 +4224,10 @@
         <v>227</v>
       </c>
       <c r="E38" s="4" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="F38" s="3" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
       <c r="G38" s="2" t="s">
         <v>178</v>
@@ -4262,10 +4268,10 @@
         <v>232</v>
       </c>
       <c r="E39" s="4" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="F39" s="3" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
       <c r="G39" s="2" t="s">
         <v>178</v>
@@ -4306,7 +4312,7 @@
         <v>236</v>
       </c>
       <c r="E40" s="4" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="F40" s="3" t="s">
         <v>237</v>
@@ -4350,10 +4356,10 @@
         <v>244</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="F41" s="3" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="G41" s="2" t="s">
         <v>238</v>
@@ -4382,22 +4388,22 @@
     </row>
     <row r="42" spans="1:14">
       <c r="A42" s="2" t="s">
+        <v>556</v>
+      </c>
+      <c r="B42" s="2" t="s">
         <v>557</v>
       </c>
-      <c r="B42" s="2" t="s">
+      <c r="C42" s="1" t="s">
         <v>558</v>
       </c>
-      <c r="C42" s="1" t="s">
+      <c r="D42" s="1" t="s">
         <v>559</v>
       </c>
-      <c r="D42" s="1" t="s">
+      <c r="E42" s="1" t="s">
+        <v>637</v>
+      </c>
+      <c r="F42" s="2" t="s">
         <v>560</v>
-      </c>
-      <c r="E42" s="1" t="s">
-        <v>638</v>
-      </c>
-      <c r="F42" s="2" t="s">
-        <v>561</v>
       </c>
       <c r="G42" s="2" t="s">
         <v>156</v>
@@ -4436,10 +4442,10 @@
         <v>254</v>
       </c>
       <c r="E43" s="4" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="F43" s="3" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="G43" s="2" t="s">
         <v>249</v>
@@ -4480,10 +4486,10 @@
         <v>248</v>
       </c>
       <c r="E44" s="4" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="F44" s="3" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="G44" s="2" t="s">
         <v>249</v>
@@ -4524,10 +4530,10 @@
         <v>259</v>
       </c>
       <c r="E45" s="4" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="F45" s="3" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="G45" s="2" t="s">
         <v>69</v>
@@ -4568,10 +4574,10 @@
         <v>270</v>
       </c>
       <c r="E46" s="4" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="F46" s="3" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="G46" s="2" t="s">
         <v>207</v>
@@ -4595,7 +4601,7 @@
         <v>1</v>
       </c>
       <c r="N46" s="3" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
     </row>
     <row r="47" spans="1:14">
@@ -4612,10 +4618,10 @@
         <v>265</v>
       </c>
       <c r="E47" s="4" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="F47" s="3" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="G47" s="2" t="s">
         <v>207</v>
@@ -4656,7 +4662,7 @@
         <v>274</v>
       </c>
       <c r="E48" s="4" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="F48" s="2" t="s">
         <v>275</v>
@@ -4700,10 +4706,10 @@
         <v>283</v>
       </c>
       <c r="E49" s="4" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="F49" s="3" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="G49" s="2" t="s">
         <v>276</v>
@@ -4744,10 +4750,10 @@
         <v>293</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="F50" s="3" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
       <c r="G50" s="2" t="s">
         <v>288</v>
@@ -4788,10 +4794,10 @@
         <v>287</v>
       </c>
       <c r="E51" s="4" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="F51" s="3" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
       <c r="G51" s="2" t="s">
         <v>288</v>
@@ -4832,10 +4838,10 @@
         <v>298</v>
       </c>
       <c r="E52" s="4" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="F52" s="3" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
       <c r="G52" s="2" t="s">
         <v>276</v>
@@ -4864,7 +4870,7 @@
     </row>
     <row r="53" spans="1:14">
       <c r="A53" s="3" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="B53" s="2" t="s">
         <v>14</v>
@@ -4873,7 +4879,7 @@
         <v>435</v>
       </c>
       <c r="D53" s="3" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="E53" s="4"/>
       <c r="F53" s="2"/>
@@ -4908,7 +4914,7 @@
         <v>304</v>
       </c>
       <c r="E54" s="4" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="F54" s="2" t="s">
         <v>305</v>
@@ -4952,10 +4958,10 @@
         <v>311</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="F55" s="3" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="G55" s="2" t="s">
         <v>89</v>
@@ -4996,7 +5002,7 @@
         <v>315</v>
       </c>
       <c r="E56" s="4" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="F56" s="3" t="s">
         <v>316</v>
@@ -5040,10 +5046,10 @@
         <v>321</v>
       </c>
       <c r="E57" s="4" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="F57" s="3" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
       <c r="G57" s="2" t="s">
         <v>89</v>
@@ -5084,10 +5090,10 @@
         <v>325</v>
       </c>
       <c r="E58" s="4" t="s">
-        <v>607</v>
+        <v>608</v>
       </c>
       <c r="F58" s="3" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="G58" s="2" t="s">
         <v>326</v>
@@ -5128,10 +5134,10 @@
         <v>331</v>
       </c>
       <c r="E59" s="4" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="F59" s="3" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="G59" s="2" t="s">
         <v>326</v>
@@ -5172,10 +5178,10 @@
         <v>336</v>
       </c>
       <c r="E60" s="4" t="s">
-        <v>609</v>
+        <v>606</v>
       </c>
       <c r="F60" s="3" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
       <c r="G60" s="2" t="s">
         <v>326</v>
@@ -5216,7 +5222,7 @@
         <v>342</v>
       </c>
       <c r="E61" s="4" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="F61" s="3" t="s">
         <v>343</v>
@@ -5260,10 +5266,10 @@
         <v>347</v>
       </c>
       <c r="E62" s="4" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="F62" s="3" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="G62" s="2" t="s">
         <v>249</v>
@@ -5298,16 +5304,16 @@
         <v>351</v>
       </c>
       <c r="C63" s="1" t="s">
+        <v>718</v>
+      </c>
+      <c r="D63" s="1" t="s">
         <v>352</v>
       </c>
-      <c r="D63" s="1" t="s">
+      <c r="E63" s="1" t="s">
+        <v>610</v>
+      </c>
+      <c r="F63" s="3" t="s">
         <v>353</v>
-      </c>
-      <c r="E63" s="1" t="s">
-        <v>611</v>
-      </c>
-      <c r="F63" s="3" t="s">
-        <v>354</v>
       </c>
       <c r="G63" s="2" t="s">
         <v>249</v>
@@ -5336,22 +5342,22 @@
     </row>
     <row r="64" spans="1:14">
       <c r="A64" s="2" t="s">
+        <v>354</v>
+      </c>
+      <c r="B64" s="2" t="s">
         <v>355</v>
       </c>
-      <c r="B64" s="2" t="s">
+      <c r="C64" s="1" t="s">
         <v>356</v>
       </c>
-      <c r="C64" s="1" t="s">
+      <c r="D64" s="1" t="s">
         <v>357</v>
       </c>
-      <c r="D64" s="1" t="s">
+      <c r="E64" s="4" t="s">
         <v>358</v>
       </c>
-      <c r="E64" s="4" t="s">
-        <v>359</v>
-      </c>
       <c r="F64" s="3" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
       <c r="G64" s="2" t="s">
         <v>185</v>
@@ -5360,42 +5366,42 @@
         <v>186</v>
       </c>
       <c r="I64" s="2" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="J64" s="2" t="s">
         <v>188</v>
       </c>
       <c r="K64" s="2" t="s">
+        <v>358</v>
+      </c>
+      <c r="L64" s="2">
+        <v>1</v>
+      </c>
+      <c r="M64" s="2">
+        <v>1</v>
+      </c>
+      <c r="N64" s="2" t="s">
         <v>359</v>
-      </c>
-      <c r="L64" s="2">
-        <v>1</v>
-      </c>
-      <c r="M64" s="2">
-        <v>1</v>
-      </c>
-      <c r="N64" s="2" t="s">
-        <v>360</v>
       </c>
     </row>
     <row r="65" spans="1:14">
       <c r="A65" s="2" t="s">
+        <v>360</v>
+      </c>
+      <c r="B65" s="2" t="s">
         <v>361</v>
       </c>
-      <c r="B65" s="2" t="s">
+      <c r="C65" s="1" t="s">
         <v>362</v>
       </c>
-      <c r="C65" s="1" t="s">
+      <c r="D65" s="1" t="s">
         <v>363</v>
       </c>
-      <c r="D65" s="1" t="s">
-        <v>364</v>
-      </c>
       <c r="E65" s="4" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="F65" s="3" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
       <c r="G65" s="2" t="s">
         <v>156</v>
@@ -5417,27 +5423,27 @@
         <v>0</v>
       </c>
       <c r="N65" s="3" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
     </row>
     <row r="66" spans="1:14">
       <c r="A66" s="2" t="s">
+        <v>369</v>
+      </c>
+      <c r="B66" s="2" t="s">
         <v>370</v>
       </c>
-      <c r="B66" s="2" t="s">
+      <c r="C66" s="1" t="s">
         <v>371</v>
       </c>
-      <c r="C66" s="1" t="s">
+      <c r="D66" s="1" t="s">
         <v>372</v>
       </c>
-      <c r="D66" s="1" t="s">
-        <v>373</v>
-      </c>
       <c r="E66" s="4" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="F66" s="3" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
       <c r="G66" s="2" t="s">
         <v>238</v>
@@ -5461,27 +5467,27 @@
         <v>1</v>
       </c>
       <c r="N66" s="2" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
     </row>
     <row r="67" spans="1:14">
       <c r="A67" s="2" t="s">
+        <v>364</v>
+      </c>
+      <c r="B67" s="2" t="s">
         <v>365</v>
       </c>
-      <c r="B67" s="2" t="s">
+      <c r="C67" s="1" t="s">
         <v>366</v>
       </c>
-      <c r="C67" s="1" t="s">
+      <c r="D67" s="1" t="s">
         <v>367</v>
       </c>
-      <c r="D67" s="1" t="s">
-        <v>368</v>
-      </c>
       <c r="E67" s="4" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="F67" s="3" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="G67" s="2" t="s">
         <v>238</v>
@@ -5505,27 +5511,27 @@
         <v>1</v>
       </c>
       <c r="N67" s="2" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
     </row>
     <row r="68" spans="1:14">
       <c r="A68" s="2" t="s">
+        <v>374</v>
+      </c>
+      <c r="B68" s="2" t="s">
         <v>375</v>
       </c>
-      <c r="B68" s="2" t="s">
+      <c r="C68" s="1" t="s">
         <v>376</v>
       </c>
-      <c r="C68" s="1" t="s">
+      <c r="D68" s="1" t="s">
         <v>377</v>
       </c>
-      <c r="D68" s="1" t="s">
-        <v>378</v>
-      </c>
       <c r="E68" s="4" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="F68" s="3" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
       <c r="G68" s="2" t="s">
         <v>28</v>
@@ -5549,27 +5555,27 @@
         <v>1</v>
       </c>
       <c r="N68" s="3" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
     </row>
     <row r="69" spans="1:14">
       <c r="A69" s="2" t="s">
+        <v>378</v>
+      </c>
+      <c r="B69" s="2" t="s">
         <v>379</v>
       </c>
-      <c r="B69" s="2" t="s">
+      <c r="C69" s="1" t="s">
         <v>380</v>
       </c>
-      <c r="C69" s="1" t="s">
+      <c r="D69" s="1" t="s">
         <v>381</v>
       </c>
-      <c r="D69" s="1" t="s">
+      <c r="E69" s="4" t="s">
+        <v>615</v>
+      </c>
+      <c r="F69" s="3" t="s">
         <v>382</v>
-      </c>
-      <c r="E69" s="4" t="s">
-        <v>616</v>
-      </c>
-      <c r="F69" s="3" t="s">
-        <v>383</v>
       </c>
       <c r="G69" s="2" t="s">
         <v>28</v>
@@ -5593,27 +5599,27 @@
         <v>1</v>
       </c>
       <c r="N69" s="3" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
     </row>
     <row r="70" spans="1:14">
       <c r="A70" s="2" t="s">
+        <v>384</v>
+      </c>
+      <c r="B70" s="2" t="s">
         <v>385</v>
       </c>
-      <c r="B70" s="2" t="s">
+      <c r="C70" s="1" t="s">
         <v>386</v>
       </c>
-      <c r="C70" s="1" t="s">
+      <c r="D70" s="1" t="s">
         <v>387</v>
       </c>
-      <c r="D70" s="1" t="s">
-        <v>388</v>
-      </c>
       <c r="E70" s="4" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="F70" s="3" t="s">
-        <v>715</v>
+        <v>714</v>
       </c>
       <c r="G70" s="2" t="s">
         <v>186</v>
@@ -5622,7 +5628,7 @@
         <v>186</v>
       </c>
       <c r="I70" s="2" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="J70" s="2" t="s">
         <v>188</v>
@@ -5637,27 +5643,27 @@
         <v>1</v>
       </c>
       <c r="N70" s="2" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
     </row>
     <row r="71" spans="1:14">
       <c r="A71" s="2" t="s">
+        <v>389</v>
+      </c>
+      <c r="B71" s="2" t="s">
         <v>390</v>
       </c>
-      <c r="B71" s="2" t="s">
+      <c r="C71" s="1" t="s">
         <v>391</v>
       </c>
-      <c r="C71" s="1" t="s">
+      <c r="D71" s="1" t="s">
         <v>392</v>
       </c>
-      <c r="D71" s="1" t="s">
-        <v>393</v>
-      </c>
       <c r="E71" s="4" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="F71" s="3" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
       <c r="G71" s="2" t="s">
         <v>28</v>
@@ -5679,27 +5685,27 @@
         <v>0</v>
       </c>
       <c r="N71" s="2" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
     </row>
     <row r="72" spans="1:14">
       <c r="A72" s="2" t="s">
+        <v>394</v>
+      </c>
+      <c r="B72" s="2" t="s">
         <v>395</v>
       </c>
-      <c r="B72" s="2" t="s">
+      <c r="C72" s="1" t="s">
         <v>396</v>
       </c>
-      <c r="C72" s="1" t="s">
+      <c r="D72" s="1" t="s">
         <v>397</v>
       </c>
-      <c r="D72" s="1" t="s">
-        <v>398</v>
-      </c>
       <c r="E72" s="4" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="F72" s="3" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
       <c r="G72" s="2" t="s">
         <v>49</v>
@@ -5728,22 +5734,22 @@
     </row>
     <row r="73" spans="1:14">
       <c r="A73" s="2" t="s">
+        <v>398</v>
+      </c>
+      <c r="B73" s="2" t="s">
         <v>399</v>
       </c>
-      <c r="B73" s="2" t="s">
+      <c r="C73" s="1" t="s">
         <v>400</v>
       </c>
-      <c r="C73" s="1" t="s">
+      <c r="D73" s="1" t="s">
         <v>401</v>
       </c>
-      <c r="D73" s="1" t="s">
-        <v>402</v>
-      </c>
       <c r="E73" s="1" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="F73" s="3" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="G73" s="2" t="s">
         <v>20</v>
@@ -5767,27 +5773,27 @@
         <v>1</v>
       </c>
       <c r="N73" s="2" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
     </row>
     <row r="74" spans="1:14">
       <c r="A74" s="2" t="s">
+        <v>403</v>
+      </c>
+      <c r="B74" s="2" t="s">
         <v>404</v>
       </c>
-      <c r="B74" s="2" t="s">
+      <c r="C74" s="1" t="s">
         <v>405</v>
       </c>
-      <c r="C74" s="1" t="s">
+      <c r="D74" s="1" t="s">
         <v>406</v>
       </c>
-      <c r="D74" s="1" t="s">
-        <v>407</v>
-      </c>
       <c r="E74" s="4" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="F74" s="3" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
       <c r="G74" s="2" t="s">
         <v>20</v>
@@ -5811,27 +5817,27 @@
         <v>1</v>
       </c>
       <c r="N74" s="2" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
     </row>
     <row r="75" spans="1:14">
       <c r="A75" s="2" t="s">
+        <v>407</v>
+      </c>
+      <c r="B75" s="2" t="s">
         <v>408</v>
       </c>
-      <c r="B75" s="2" t="s">
+      <c r="C75" s="1" t="s">
         <v>409</v>
       </c>
-      <c r="C75" s="1" t="s">
+      <c r="D75" s="1" t="s">
         <v>410</v>
       </c>
-      <c r="D75" s="1" t="s">
-        <v>411</v>
-      </c>
       <c r="E75" s="1" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="F75" s="3" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
       <c r="G75" s="2" t="s">
         <v>49</v>
@@ -5840,7 +5846,7 @@
         <v>50</v>
       </c>
       <c r="I75" s="2" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="J75" s="2" t="s">
         <v>50</v>
@@ -5860,37 +5866,37 @@
     </row>
     <row r="76" spans="1:14">
       <c r="A76" s="2" t="s">
+        <v>412</v>
+      </c>
+      <c r="B76" s="2" t="s">
         <v>413</v>
       </c>
-      <c r="B76" s="2" t="s">
+      <c r="C76" s="1" t="s">
         <v>414</v>
       </c>
-      <c r="C76" s="1" t="s">
+      <c r="D76" s="1" t="s">
         <v>415</v>
       </c>
-      <c r="D76" s="1" t="s">
+      <c r="E76" s="4" t="s">
+        <v>619</v>
+      </c>
+      <c r="F76" s="3" t="s">
+        <v>704</v>
+      </c>
+      <c r="G76" s="2" t="s">
         <v>416</v>
       </c>
-      <c r="E76" s="4" t="s">
-        <v>620</v>
-      </c>
-      <c r="F76" s="3" t="s">
-        <v>705</v>
-      </c>
-      <c r="G76" s="2" t="s">
+      <c r="H76" s="2" t="s">
+        <v>416</v>
+      </c>
+      <c r="I76" s="2" t="s">
         <v>417</v>
-      </c>
-      <c r="H76" s="2" t="s">
-        <v>417</v>
-      </c>
-      <c r="I76" s="2" t="s">
-        <v>418</v>
       </c>
       <c r="J76" s="2" t="s">
         <v>188</v>
       </c>
       <c r="K76" s="2" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="L76" s="2">
         <v>1</v>
@@ -5899,42 +5905,42 @@
         <v>1</v>
       </c>
       <c r="N76" s="2" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
     </row>
     <row r="77" spans="1:14">
       <c r="A77" s="2" t="s">
+        <v>419</v>
+      </c>
+      <c r="B77" s="2" t="s">
         <v>420</v>
       </c>
-      <c r="B77" s="2" t="s">
+      <c r="C77" s="1" t="s">
         <v>421</v>
       </c>
-      <c r="C77" s="1" t="s">
+      <c r="D77" s="1" t="s">
         <v>422</v>
       </c>
-      <c r="D77" s="1" t="s">
-        <v>423</v>
-      </c>
       <c r="E77" s="4" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="F77" s="3" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
       <c r="G77" s="2" t="s">
+        <v>416</v>
+      </c>
+      <c r="H77" s="2" t="s">
+        <v>416</v>
+      </c>
+      <c r="I77" s="2" t="s">
         <v>417</v>
-      </c>
-      <c r="H77" s="2" t="s">
-        <v>417</v>
-      </c>
-      <c r="I77" s="2" t="s">
-        <v>418</v>
       </c>
       <c r="J77" s="2" t="s">
         <v>188</v>
       </c>
       <c r="K77" s="2" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="L77" s="2">
         <v>1</v>
@@ -5943,42 +5949,42 @@
         <v>1</v>
       </c>
       <c r="N77" s="2" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
     </row>
     <row r="78" spans="1:14">
       <c r="A78" s="2" t="s">
+        <v>429</v>
+      </c>
+      <c r="B78" s="2" t="s">
         <v>430</v>
       </c>
-      <c r="B78" s="2" t="s">
+      <c r="C78" s="1" t="s">
         <v>431</v>
       </c>
-      <c r="C78" s="1" t="s">
+      <c r="D78" s="1" t="s">
         <v>432</v>
       </c>
-      <c r="D78" s="1" t="s">
+      <c r="E78" s="1" t="s">
+        <v>620</v>
+      </c>
+      <c r="F78" s="3" t="s">
         <v>433</v>
       </c>
-      <c r="E78" s="1" t="s">
-        <v>621</v>
-      </c>
-      <c r="F78" s="3" t="s">
-        <v>434</v>
-      </c>
       <c r="G78" s="2" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="H78" s="2" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="I78" s="2" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="J78" s="2" t="s">
         <v>188</v>
       </c>
       <c r="K78" s="2" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="L78" s="2">
         <v>1</v>
@@ -5987,42 +5993,42 @@
         <v>1</v>
       </c>
       <c r="N78" s="2" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
     </row>
     <row r="79" spans="1:14">
       <c r="A79" s="2" t="s">
+        <v>423</v>
+      </c>
+      <c r="B79" s="2" t="s">
         <v>424</v>
       </c>
-      <c r="B79" s="2" t="s">
+      <c r="C79" s="1" t="s">
         <v>425</v>
       </c>
-      <c r="C79" s="1" t="s">
+      <c r="D79" s="1" t="s">
         <v>426</v>
       </c>
-      <c r="D79" s="1" t="s">
+      <c r="E79" s="4" t="s">
+        <v>621</v>
+      </c>
+      <c r="F79" s="3" t="s">
+        <v>706</v>
+      </c>
+      <c r="G79" s="2" t="s">
+        <v>416</v>
+      </c>
+      <c r="H79" s="2" t="s">
+        <v>416</v>
+      </c>
+      <c r="I79" s="2" t="s">
         <v>427</v>
-      </c>
-      <c r="E79" s="4" t="s">
-        <v>622</v>
-      </c>
-      <c r="F79" s="3" t="s">
-        <v>707</v>
-      </c>
-      <c r="G79" s="2" t="s">
-        <v>417</v>
-      </c>
-      <c r="H79" s="2" t="s">
-        <v>417</v>
-      </c>
-      <c r="I79" s="2" t="s">
-        <v>428</v>
       </c>
       <c r="J79" s="2" t="s">
         <v>188</v>
       </c>
       <c r="K79" s="2" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="L79" s="2">
         <v>1</v>
@@ -6031,159 +6037,159 @@
         <v>1</v>
       </c>
       <c r="N79" s="2" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="80" spans="1:14">
       <c r="A80" s="2" t="s">
+        <v>435</v>
+      </c>
+      <c r="B80" s="2" t="s">
         <v>436</v>
       </c>
-      <c r="B80" s="2" t="s">
+      <c r="C80" s="1" t="s">
         <v>437</v>
       </c>
-      <c r="C80" s="1" t="s">
+      <c r="D80" s="1" t="s">
         <v>438</v>
       </c>
-      <c r="D80" s="1" t="s">
+      <c r="E80" s="4" t="s">
+        <v>622</v>
+      </c>
+      <c r="F80" s="3" t="s">
+        <v>662</v>
+      </c>
+      <c r="G80" s="2" t="s">
         <v>439</v>
-      </c>
-      <c r="E80" s="4" t="s">
-        <v>623</v>
-      </c>
-      <c r="F80" s="3" t="s">
-        <v>663</v>
-      </c>
-      <c r="G80" s="2" t="s">
-        <v>440</v>
       </c>
       <c r="H80" s="2" t="s">
         <v>133</v>
       </c>
       <c r="I80" s="2" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="J80" s="2" t="s">
         <v>133</v>
       </c>
       <c r="K80" s="2" t="s">
+        <v>439</v>
+      </c>
+      <c r="L80" s="2">
+        <v>1</v>
+      </c>
+      <c r="M80" s="2">
+        <v>1</v>
+      </c>
+      <c r="N80" s="2" t="s">
         <v>440</v>
-      </c>
-      <c r="L80" s="2">
-        <v>1</v>
-      </c>
-      <c r="M80" s="2">
-        <v>1</v>
-      </c>
-      <c r="N80" s="2" t="s">
-        <v>441</v>
       </c>
     </row>
     <row r="81" spans="1:14">
       <c r="A81" s="2" t="s">
+        <v>441</v>
+      </c>
+      <c r="B81" s="2" t="s">
         <v>442</v>
       </c>
-      <c r="B81" s="2" t="s">
+      <c r="C81" s="1" t="s">
         <v>443</v>
       </c>
-      <c r="C81" s="1" t="s">
+      <c r="D81" s="1" t="s">
         <v>444</v>
       </c>
-      <c r="D81" s="1" t="s">
+      <c r="E81" s="4" t="s">
+        <v>622</v>
+      </c>
+      <c r="F81" s="3" t="s">
         <v>445</v>
       </c>
-      <c r="E81" s="4" t="s">
-        <v>623</v>
-      </c>
-      <c r="F81" s="3" t="s">
-        <v>446</v>
-      </c>
       <c r="G81" s="2" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="H81" s="2" t="s">
         <v>133</v>
       </c>
       <c r="I81" s="2" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="J81" s="2" t="s">
         <v>133</v>
       </c>
       <c r="K81" s="2" t="s">
+        <v>439</v>
+      </c>
+      <c r="L81" s="2">
+        <v>1</v>
+      </c>
+      <c r="M81" s="2">
+        <v>1</v>
+      </c>
+      <c r="N81" s="2" t="s">
         <v>440</v>
-      </c>
-      <c r="L81" s="2">
-        <v>1</v>
-      </c>
-      <c r="M81" s="2">
-        <v>1</v>
-      </c>
-      <c r="N81" s="2" t="s">
-        <v>441</v>
       </c>
     </row>
     <row r="82" spans="1:14">
       <c r="A82" s="2" t="s">
+        <v>446</v>
+      </c>
+      <c r="B82" s="2" t="s">
         <v>447</v>
       </c>
-      <c r="B82" s="2" t="s">
+      <c r="C82" s="1" t="s">
         <v>448</v>
       </c>
-      <c r="C82" s="1" t="s">
+      <c r="D82" s="1" t="s">
         <v>449</v>
       </c>
-      <c r="D82" s="1" t="s">
-        <v>450</v>
-      </c>
       <c r="E82" s="4" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="F82" s="3" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
       <c r="G82" s="2" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="H82" s="2" t="s">
         <v>133</v>
       </c>
       <c r="I82" s="2" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="J82" s="2" t="s">
         <v>133</v>
       </c>
       <c r="K82" s="2" t="s">
+        <v>439</v>
+      </c>
+      <c r="L82" s="2">
+        <v>1</v>
+      </c>
+      <c r="M82" s="2">
+        <v>1</v>
+      </c>
+      <c r="N82" s="2" t="s">
         <v>440</v>
-      </c>
-      <c r="L82" s="2">
-        <v>1</v>
-      </c>
-      <c r="M82" s="2">
-        <v>1</v>
-      </c>
-      <c r="N82" s="2" t="s">
-        <v>441</v>
       </c>
     </row>
     <row r="83" spans="1:14">
       <c r="A83" s="2" t="s">
+        <v>450</v>
+      </c>
+      <c r="B83" s="2" t="s">
         <v>451</v>
       </c>
-      <c r="B83" s="2" t="s">
+      <c r="C83" s="1" t="s">
         <v>452</v>
       </c>
-      <c r="C83" s="1" t="s">
+      <c r="D83" s="1" t="s">
         <v>453</v>
-      </c>
-      <c r="D83" s="1" t="s">
-        <v>454</v>
       </c>
       <c r="E83" s="4" t="s">
         <v>168</v>
       </c>
       <c r="F83" s="3" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="G83" s="2" t="s">
         <v>168</v>
@@ -6207,27 +6213,27 @@
         <v>1</v>
       </c>
       <c r="N83" s="2" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
     </row>
     <row r="84" spans="1:14">
       <c r="A84" s="2" t="s">
+        <v>455</v>
+      </c>
+      <c r="B84" s="2" t="s">
         <v>456</v>
       </c>
-      <c r="B84" s="2" t="s">
+      <c r="C84" s="1" t="s">
         <v>457</v>
       </c>
-      <c r="C84" s="1" t="s">
+      <c r="D84" s="1" t="s">
         <v>458</v>
       </c>
-      <c r="D84" s="1" t="s">
+      <c r="E84" s="4" t="s">
+        <v>624</v>
+      </c>
+      <c r="F84" s="3" t="s">
         <v>459</v>
-      </c>
-      <c r="E84" s="4" t="s">
-        <v>625</v>
-      </c>
-      <c r="F84" s="3" t="s">
-        <v>460</v>
       </c>
       <c r="G84" s="2" t="s">
         <v>168</v>
@@ -6251,42 +6257,42 @@
         <v>0</v>
       </c>
       <c r="N84" s="2" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
     </row>
     <row r="85" spans="1:14">
       <c r="A85" s="2" t="s">
+        <v>461</v>
+      </c>
+      <c r="B85" s="2" t="s">
         <v>462</v>
       </c>
-      <c r="B85" s="2" t="s">
+      <c r="C85" s="1" t="s">
         <v>463</v>
       </c>
-      <c r="C85" s="1" t="s">
+      <c r="D85" s="1" t="s">
         <v>464</v>
       </c>
-      <c r="D85" s="1" t="s">
+      <c r="E85" s="4" t="s">
+        <v>466</v>
+      </c>
+      <c r="F85" s="3" t="s">
+        <v>679</v>
+      </c>
+      <c r="G85" s="2" t="s">
         <v>465</v>
-      </c>
-      <c r="E85" s="4" t="s">
-        <v>467</v>
-      </c>
-      <c r="F85" s="3" t="s">
-        <v>680</v>
-      </c>
-      <c r="G85" s="2" t="s">
-        <v>466</v>
       </c>
       <c r="H85" s="2" t="s">
         <v>21</v>
       </c>
       <c r="I85" s="2" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="J85" s="2" t="s">
         <v>21</v>
       </c>
       <c r="K85" s="2" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="L85" s="2">
         <v>1</v>
@@ -6295,86 +6301,86 @@
         <v>1</v>
       </c>
       <c r="N85" s="2" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
     </row>
     <row r="86" spans="1:14">
       <c r="A86" s="2" t="s">
+        <v>468</v>
+      </c>
+      <c r="B86" s="2" t="s">
         <v>469</v>
       </c>
-      <c r="B86" s="2" t="s">
+      <c r="C86" s="1" t="s">
         <v>470</v>
       </c>
-      <c r="C86" s="1" t="s">
+      <c r="D86" s="1" t="s">
         <v>471</v>
       </c>
-      <c r="D86" s="1" t="s">
+      <c r="E86" s="4" t="s">
+        <v>625</v>
+      </c>
+      <c r="F86" s="3" t="s">
+        <v>685</v>
+      </c>
+      <c r="G86" s="2" t="s">
         <v>472</v>
-      </c>
-      <c r="E86" s="4" t="s">
-        <v>626</v>
-      </c>
-      <c r="F86" s="3" t="s">
-        <v>686</v>
-      </c>
-      <c r="G86" s="2" t="s">
-        <v>473</v>
       </c>
       <c r="H86" s="2" t="s">
         <v>277</v>
       </c>
       <c r="I86" s="2" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="J86" s="2" t="s">
         <v>100</v>
       </c>
       <c r="K86" s="2" t="s">
+        <v>472</v>
+      </c>
+      <c r="L86" s="2">
+        <v>1</v>
+      </c>
+      <c r="M86" s="2">
+        <v>1</v>
+      </c>
+      <c r="N86" s="2" t="s">
         <v>473</v>
-      </c>
-      <c r="L86" s="2">
-        <v>1</v>
-      </c>
-      <c r="M86" s="2">
-        <v>1</v>
-      </c>
-      <c r="N86" s="2" t="s">
-        <v>474</v>
       </c>
     </row>
     <row r="87" spans="1:14">
       <c r="A87" s="2" t="s">
+        <v>474</v>
+      </c>
+      <c r="B87" s="2" t="s">
         <v>475</v>
       </c>
-      <c r="B87" s="2" t="s">
+      <c r="C87" s="1" t="s">
         <v>476</v>
       </c>
-      <c r="C87" s="1" t="s">
+      <c r="D87" s="1" t="s">
         <v>477</v>
       </c>
-      <c r="D87" s="1" t="s">
-        <v>478</v>
-      </c>
       <c r="E87" s="4" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="F87" s="3" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
       <c r="G87" s="2" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="H87" s="2" t="s">
         <v>277</v>
       </c>
       <c r="I87" s="2" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="J87" s="2" t="s">
         <v>100</v>
       </c>
       <c r="K87" s="2" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="L87" s="2">
         <v>1</v>
@@ -6383,42 +6389,42 @@
         <v>1</v>
       </c>
       <c r="N87" s="2" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
     </row>
     <row r="88" spans="1:14">
       <c r="A88" s="2" t="s">
+        <v>479</v>
+      </c>
+      <c r="B88" s="2" t="s">
         <v>480</v>
       </c>
-      <c r="B88" s="2" t="s">
+      <c r="C88" s="1" t="s">
         <v>481</v>
       </c>
-      <c r="C88" s="1" t="s">
+      <c r="D88" s="1" t="s">
         <v>482</v>
       </c>
-      <c r="D88" s="1" t="s">
+      <c r="E88" s="4" t="s">
+        <v>627</v>
+      </c>
+      <c r="F88" s="2" t="s">
         <v>483</v>
       </c>
-      <c r="E88" s="4" t="s">
-        <v>628</v>
-      </c>
-      <c r="F88" s="2" t="s">
-        <v>484</v>
-      </c>
       <c r="G88" s="2" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="H88" s="2" t="s">
         <v>21</v>
       </c>
       <c r="I88" s="2" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="J88" s="2" t="s">
         <v>21</v>
       </c>
       <c r="K88" s="2" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="L88" s="2">
         <v>1</v>
@@ -6427,42 +6433,42 @@
         <v>1</v>
       </c>
       <c r="N88" s="2" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
     </row>
     <row r="89" spans="1:14">
       <c r="A89" s="2" t="s">
+        <v>486</v>
+      </c>
+      <c r="B89" s="2" t="s">
         <v>487</v>
       </c>
-      <c r="B89" s="2" t="s">
+      <c r="C89" s="1" t="s">
         <v>488</v>
       </c>
-      <c r="C89" s="1" t="s">
+      <c r="D89" s="1" t="s">
         <v>489</v>
       </c>
-      <c r="D89" s="1" t="s">
+      <c r="E89" s="4" t="s">
+        <v>627</v>
+      </c>
+      <c r="F89" s="2" t="s">
         <v>490</v>
       </c>
-      <c r="E89" s="4" t="s">
-        <v>628</v>
-      </c>
-      <c r="F89" s="2" t="s">
-        <v>491</v>
-      </c>
       <c r="G89" s="2" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="H89" s="2" t="s">
         <v>21</v>
       </c>
       <c r="I89" s="2" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="J89" s="2" t="s">
         <v>21</v>
       </c>
       <c r="K89" s="2" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="L89" s="2">
         <v>1</v>
@@ -6471,42 +6477,42 @@
         <v>1</v>
       </c>
       <c r="N89" s="2" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
     </row>
     <row r="90" spans="1:14">
       <c r="A90" s="2" t="s">
+        <v>492</v>
+      </c>
+      <c r="B90" s="2" t="s">
         <v>493</v>
       </c>
-      <c r="B90" s="2" t="s">
+      <c r="C90" s="1" t="s">
         <v>494</v>
       </c>
-      <c r="C90" s="1" t="s">
+      <c r="D90" s="1" t="s">
         <v>495</v>
       </c>
-      <c r="D90" s="1" t="s">
-        <v>496</v>
-      </c>
       <c r="E90" s="1" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="F90" s="3" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
       <c r="G90" s="2" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="H90" s="2" t="s">
         <v>21</v>
       </c>
       <c r="I90" s="2" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="J90" s="2" t="s">
         <v>21</v>
       </c>
       <c r="K90" s="2" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="L90" s="2">
         <v>1</v>
@@ -6515,42 +6521,42 @@
         <v>1</v>
       </c>
       <c r="N90" s="2" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
     </row>
     <row r="91" spans="1:14">
       <c r="A91" s="2" t="s">
+        <v>496</v>
+      </c>
+      <c r="B91" s="3" t="s">
         <v>497</v>
       </c>
-      <c r="B91" s="2" t="s">
+      <c r="C91" s="1" t="s">
         <v>498</v>
       </c>
-      <c r="C91" s="1" t="s">
+      <c r="D91" s="1" t="s">
         <v>499</v>
       </c>
-      <c r="D91" s="1" t="s">
+      <c r="E91" s="4" t="s">
+        <v>628</v>
+      </c>
+      <c r="F91" s="3" t="s">
+        <v>695</v>
+      </c>
+      <c r="G91" s="2" t="s">
         <v>500</v>
-      </c>
-      <c r="E91" s="4" t="s">
-        <v>629</v>
-      </c>
-      <c r="F91" s="3" t="s">
-        <v>696</v>
-      </c>
-      <c r="G91" s="2" t="s">
-        <v>501</v>
       </c>
       <c r="H91" s="2" t="s">
         <v>36</v>
       </c>
       <c r="I91" s="2" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="J91" s="2" t="s">
         <v>36</v>
       </c>
       <c r="K91" s="2" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="L91" s="2">
         <v>1</v>
@@ -6559,42 +6565,42 @@
         <v>1</v>
       </c>
       <c r="N91" s="2" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
     </row>
     <row r="92" spans="1:14">
       <c r="A92" s="2" t="s">
+        <v>503</v>
+      </c>
+      <c r="B92" s="2" t="s">
         <v>504</v>
       </c>
-      <c r="B92" s="2" t="s">
+      <c r="C92" s="1" t="s">
         <v>505</v>
       </c>
-      <c r="C92" s="1" t="s">
+      <c r="D92" s="1" t="s">
         <v>506</v>
       </c>
-      <c r="D92" s="1" t="s">
+      <c r="E92" s="4" t="s">
+        <v>629</v>
+      </c>
+      <c r="F92" s="3" t="s">
         <v>507</v>
       </c>
-      <c r="E92" s="4" t="s">
-        <v>630</v>
-      </c>
-      <c r="F92" s="3" t="s">
-        <v>508</v>
-      </c>
       <c r="G92" s="2" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="H92" s="2" t="s">
         <v>36</v>
       </c>
       <c r="I92" s="2" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="J92" s="2" t="s">
         <v>36</v>
       </c>
       <c r="K92" s="2" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="L92" s="2">
         <v>1</v>
@@ -6603,42 +6609,42 @@
         <v>1</v>
       </c>
       <c r="N92" s="2" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
     </row>
     <row r="93" spans="1:14">
       <c r="A93" s="2" t="s">
+        <v>509</v>
+      </c>
+      <c r="B93" s="2" t="s">
         <v>510</v>
       </c>
-      <c r="B93" s="2" t="s">
+      <c r="C93" s="1" t="s">
         <v>511</v>
       </c>
-      <c r="C93" s="1" t="s">
+      <c r="D93" s="1" t="s">
         <v>512</v>
       </c>
-      <c r="D93" s="1" t="s">
-        <v>513</v>
-      </c>
       <c r="E93" s="4" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="F93" s="3" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
       <c r="G93" s="2" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="H93" s="2" t="s">
         <v>36</v>
       </c>
       <c r="I93" s="2" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="J93" s="2" t="s">
         <v>36</v>
       </c>
       <c r="K93" s="2" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="L93" s="2">
         <v>1</v>
@@ -6647,42 +6653,42 @@
         <v>1</v>
       </c>
       <c r="N93" s="2" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
     </row>
     <row r="94" spans="1:14">
       <c r="A94" s="3" t="s">
-        <v>639</v>
-      </c>
-      <c r="B94" s="2" t="s">
-        <v>516</v>
+        <v>638</v>
+      </c>
+      <c r="B94" s="3" t="s">
+        <v>531</v>
       </c>
       <c r="C94" s="1" t="s">
+        <v>640</v>
+      </c>
+      <c r="D94" s="1" t="s">
         <v>641</v>
       </c>
-      <c r="D94" s="1" t="s">
-        <v>642</v>
-      </c>
       <c r="E94" s="4" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="F94" s="3" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="G94" s="2" t="s">
+        <v>517</v>
+      </c>
+      <c r="H94" s="2" t="s">
+        <v>416</v>
+      </c>
+      <c r="I94" s="2" t="s">
         <v>518</v>
-      </c>
-      <c r="H94" s="2" t="s">
-        <v>417</v>
-      </c>
-      <c r="I94" s="2" t="s">
-        <v>519</v>
       </c>
       <c r="J94" s="2" t="s">
         <v>188</v>
       </c>
       <c r="K94" s="2" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="L94" s="2">
         <v>1</v>
@@ -6691,42 +6697,42 @@
         <v>1</v>
       </c>
       <c r="N94" s="2" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
     </row>
     <row r="95" spans="1:14">
       <c r="A95" s="2" t="s">
+        <v>520</v>
+      </c>
+      <c r="B95" s="2" t="s">
         <v>521</v>
       </c>
-      <c r="B95" s="2" t="s">
+      <c r="C95" s="1" t="s">
         <v>522</v>
       </c>
-      <c r="C95" s="1" t="s">
+      <c r="D95" s="1" t="s">
         <v>523</v>
       </c>
-      <c r="D95" s="1" t="s">
+      <c r="E95" s="4" t="s">
+        <v>631</v>
+      </c>
+      <c r="F95" s="3" t="s">
+        <v>708</v>
+      </c>
+      <c r="G95" s="2" t="s">
+        <v>517</v>
+      </c>
+      <c r="H95" s="2" t="s">
+        <v>416</v>
+      </c>
+      <c r="I95" s="2" t="s">
         <v>524</v>
-      </c>
-      <c r="E95" s="4" t="s">
-        <v>632</v>
-      </c>
-      <c r="F95" s="3" t="s">
-        <v>709</v>
-      </c>
-      <c r="G95" s="2" t="s">
-        <v>518</v>
-      </c>
-      <c r="H95" s="2" t="s">
-        <v>417</v>
-      </c>
-      <c r="I95" s="2" t="s">
-        <v>525</v>
       </c>
       <c r="J95" s="2" t="s">
         <v>188</v>
       </c>
       <c r="K95" s="2" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="L95" s="2">
         <v>1</v>
@@ -6735,42 +6741,42 @@
         <v>1</v>
       </c>
       <c r="N95" s="2" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
     </row>
     <row r="96" spans="1:14">
       <c r="A96" s="2" t="s">
+        <v>526</v>
+      </c>
+      <c r="B96" s="2" t="s">
         <v>527</v>
       </c>
-      <c r="B96" s="2" t="s">
+      <c r="C96" s="1" t="s">
         <v>528</v>
       </c>
-      <c r="C96" s="1" t="s">
+      <c r="D96" s="1" t="s">
         <v>529</v>
       </c>
-      <c r="D96" s="1" t="s">
-        <v>530</v>
-      </c>
       <c r="E96" s="1" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="F96" s="3" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
       <c r="G96" s="2" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="H96" s="2" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="I96" s="2" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="J96" s="2" t="s">
         <v>188</v>
       </c>
       <c r="K96" s="2" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="L96" s="2">
         <v>1</v>
@@ -6779,42 +6785,42 @@
         <v>1</v>
       </c>
       <c r="N96" s="2" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
     </row>
     <row r="97" spans="1:14">
       <c r="A97" s="3" t="s">
-        <v>640</v>
-      </c>
-      <c r="B97" s="2" t="s">
+        <v>639</v>
+      </c>
+      <c r="B97" s="3" t="s">
+        <v>515</v>
+      </c>
+      <c r="C97" s="1" t="s">
+        <v>642</v>
+      </c>
+      <c r="D97" s="1" t="s">
+        <v>643</v>
+      </c>
+      <c r="E97" s="4" t="s">
+        <v>630</v>
+      </c>
+      <c r="F97" s="3" t="s">
+        <v>516</v>
+      </c>
+      <c r="G97" s="2" t="s">
+        <v>517</v>
+      </c>
+      <c r="H97" s="2" t="s">
+        <v>416</v>
+      </c>
+      <c r="I97" s="2" t="s">
         <v>532</v>
-      </c>
-      <c r="C97" s="1" t="s">
-        <v>643</v>
-      </c>
-      <c r="D97" s="1" t="s">
-        <v>644</v>
-      </c>
-      <c r="E97" s="4" t="s">
-        <v>631</v>
-      </c>
-      <c r="F97" s="3" t="s">
-        <v>517</v>
-      </c>
-      <c r="G97" s="2" t="s">
-        <v>518</v>
-      </c>
-      <c r="H97" s="2" t="s">
-        <v>417</v>
-      </c>
-      <c r="I97" s="2" t="s">
-        <v>533</v>
       </c>
       <c r="J97" s="2" t="s">
         <v>188</v>
       </c>
       <c r="K97" s="2" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="L97" s="2">
         <v>1</v>
@@ -6823,86 +6829,86 @@
         <v>1</v>
       </c>
       <c r="N97" s="2" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
     </row>
     <row r="98" spans="1:14">
       <c r="A98" s="2" t="s">
+        <v>534</v>
+      </c>
+      <c r="B98" s="2" t="s">
         <v>535</v>
       </c>
-      <c r="B98" s="2" t="s">
+      <c r="C98" s="1" t="s">
         <v>536</v>
       </c>
-      <c r="C98" s="1" t="s">
+      <c r="D98" s="1" t="s">
         <v>537</v>
       </c>
-      <c r="D98" s="1" t="s">
+      <c r="E98" s="4" t="s">
+        <v>633</v>
+      </c>
+      <c r="F98" s="3" t="s">
+        <v>710</v>
+      </c>
+      <c r="G98" s="2" t="s">
         <v>538</v>
       </c>
-      <c r="E98" s="4" t="s">
-        <v>634</v>
-      </c>
-      <c r="F98" s="3" t="s">
-        <v>711</v>
-      </c>
-      <c r="G98" s="2" t="s">
-        <v>539</v>
-      </c>
       <c r="H98" s="2" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="I98" s="2" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="J98" s="2" t="s">
         <v>188</v>
       </c>
       <c r="K98" s="2" t="s">
+        <v>538</v>
+      </c>
+      <c r="L98" s="2">
+        <v>1</v>
+      </c>
+      <c r="M98" s="2">
+        <v>1</v>
+      </c>
+      <c r="N98" s="2" t="s">
         <v>539</v>
-      </c>
-      <c r="L98" s="2">
-        <v>1</v>
-      </c>
-      <c r="M98" s="2">
-        <v>1</v>
-      </c>
-      <c r="N98" s="2" t="s">
-        <v>540</v>
       </c>
     </row>
     <row r="99" spans="1:14">
       <c r="A99" s="2" t="s">
+        <v>540</v>
+      </c>
+      <c r="B99" s="2" t="s">
         <v>541</v>
       </c>
-      <c r="B99" s="2" t="s">
+      <c r="C99" s="1" t="s">
         <v>542</v>
       </c>
-      <c r="C99" s="1" t="s">
+      <c r="D99" s="1" t="s">
         <v>543</v>
       </c>
-      <c r="D99" s="1" t="s">
-        <v>544</v>
-      </c>
       <c r="E99" s="4" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="F99" s="3" t="s">
-        <v>712</v>
+        <v>711</v>
       </c>
       <c r="G99" s="2" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="H99" s="2" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="I99" s="2" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="J99" s="2" t="s">
         <v>188</v>
       </c>
       <c r="K99" s="2" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="L99" s="2">
         <v>1</v>
@@ -6911,27 +6917,27 @@
         <v>1</v>
       </c>
       <c r="N99" s="2" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
     </row>
     <row r="100" spans="1:14">
       <c r="A100" s="2" t="s">
+        <v>545</v>
+      </c>
+      <c r="B100" s="2" t="s">
         <v>546</v>
       </c>
-      <c r="B100" s="2" t="s">
+      <c r="C100" s="1" t="s">
         <v>547</v>
       </c>
-      <c r="C100" s="1" t="s">
+      <c r="D100" s="1" t="s">
         <v>548</v>
       </c>
-      <c r="D100" s="1" t="s">
+      <c r="E100" s="4" t="s">
+        <v>716</v>
+      </c>
+      <c r="F100" s="2" t="s">
         <v>549</v>
-      </c>
-      <c r="E100" s="4" t="s">
-        <v>186</v>
-      </c>
-      <c r="F100" s="2" t="s">
-        <v>550</v>
       </c>
       <c r="G100" s="2" t="s">
         <v>186</v>
@@ -6955,27 +6961,27 @@
         <v>1</v>
       </c>
       <c r="N100" s="2" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
     </row>
     <row r="101" spans="1:14">
       <c r="A101" s="2" t="s">
+        <v>551</v>
+      </c>
+      <c r="B101" s="2" t="s">
         <v>552</v>
       </c>
-      <c r="B101" s="2" t="s">
+      <c r="C101" s="1" t="s">
         <v>553</v>
       </c>
-      <c r="C101" s="1" t="s">
+      <c r="D101" s="1" t="s">
         <v>554</v>
       </c>
-      <c r="D101" s="1" t="s">
-        <v>555</v>
-      </c>
       <c r="E101" s="4" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="F101" s="3" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
       <c r="G101" s="2" t="s">
         <v>186</v>
@@ -6999,7 +7005,7 @@
         <v>1</v>
       </c>
       <c r="N101" s="2" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
     </row>
     <row r="104" spans="1:14">
@@ -7011,6 +7017,9 @@
       <sortCondition ref="A1"/>
     </sortState>
   </autoFilter>
+  <sortState ref="A2:N104">
+    <sortCondition ref="A82"/>
+  </sortState>
   <conditionalFormatting sqref="B1:B101">
     <cfRule type="duplicateValues" dxfId="0" priority="11"/>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Update geographical areas in phone list
</commit_message>
<xml_diff>
--- a/config/phone_list.xlsx
+++ b/config/phone_list.xlsx
@@ -17,7 +17,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">PHONE_LIST!$A$1:$N$101</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="152511" calcMode="manual"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -1676,9 +1676,6 @@
     <t>ZHUBEI_3</t>
   </si>
   <si>
-    <t>GUANXI,HSINCHU_XINPU,ZHUBEI,關西鎮,新埔鎮,竹北市</t>
-  </si>
-  <si>
     <t>ZHUDONG_E</t>
   </si>
   <si>
@@ -1760,9 +1757,6 @@
     <t>McOmbers</t>
   </si>
   <si>
-    <t>SHENKENG,SHIDING,PINGLIN,WENSHAN,深坑區,石碇區,坪林區,文山區,木柵,木柵區</t>
-  </si>
-  <si>
     <t>ZHONGZHENG,WANHUA,中正區,萬華區,萬華</t>
   </si>
   <si>
@@ -1823,9 +1817,6 @@
     <t>HUALIAN_ZHONGMEI</t>
   </si>
   <si>
-    <t>HUALIAN_JIAN</t>
-  </si>
-  <si>
     <t>HUALIAN_DEAN</t>
   </si>
   <si>
@@ -1862,9 +1853,6 @@
     <t>SHILIN_SHUANGXI</t>
   </si>
   <si>
-    <t>SHILIN_RENYONG</t>
-  </si>
-  <si>
     <t>XINZHUANG_ZHONGZHENG</t>
   </si>
   <si>
@@ -1883,9 +1871,6 @@
     <t>TAIDONG_CHANGSHA_8</t>
   </si>
   <si>
-    <t>TAIDONG_NANWANG</t>
-  </si>
-  <si>
     <t>TAOYUAN_DAYOU</t>
   </si>
   <si>
@@ -1940,9 +1925,6 @@
     <t>XINZHU_DONGDA</t>
   </si>
   <si>
-    <t>XINZHU_LUSHUI</t>
-  </si>
-  <si>
     <t>XIZHI_LONGAN</t>
   </si>
   <si>
@@ -1952,9 +1934,6 @@
     <t>LUODONG_ZHANDONG</t>
   </si>
   <si>
-    <t>YULI_QIMO</t>
-  </si>
-  <si>
     <t>YULI_GUANGFU</t>
   </si>
   <si>
@@ -1976,21 +1955,12 @@
     <t>ZHUBEI_BOAI</t>
   </si>
   <si>
-    <t>ZHUDONG_1</t>
-  </si>
-  <si>
-    <t>ZHUDONG_21</t>
-  </si>
-  <si>
     <t>ZHUNAN_YANPING</t>
   </si>
   <si>
     <t>LUODONG_GONGZHENG</t>
   </si>
   <si>
-    <t>ZHONGZHENG_NANCHANG</t>
-  </si>
-  <si>
     <t>ZHUBEI_1_E</t>
   </si>
   <si>
@@ -2225,13 +2195,43 @@
     <t>E. Lindahl / Dorius ZL</t>
   </si>
   <si>
-    <t>ZHUNAN_ZHENGNAN</t>
-  </si>
-  <si>
     <t>LUZHOU_XINYI</t>
   </si>
   <si>
     <t>Tianmu B E</t>
+  </si>
+  <si>
+    <t>ZHUDONG_XINGFU_1</t>
+  </si>
+  <si>
+    <t>ZHUDONG_XINGFU_21</t>
+  </si>
+  <si>
+    <t>HUALIAN_ZHONGHE</t>
+  </si>
+  <si>
+    <t>YULI_XINGGUO</t>
+  </si>
+  <si>
+    <t>SHILIN_DABEI</t>
+  </si>
+  <si>
+    <t>TAIDONG_GENGSHENG</t>
+  </si>
+  <si>
+    <t>XINZHU_SHIPIN</t>
+  </si>
+  <si>
+    <t>ZHONGZHENG_NANCHANG_2_COUPLE</t>
+  </si>
+  <si>
+    <t>ZHUNAN_ZHONGZHENG</t>
+  </si>
+  <si>
+    <t>SHENKENG,SHIDING,PINGLIN,WENSHAN,MUZHA,深坑區,石碇區,坪林區,文山區,木柵,木柵區</t>
+  </si>
+  <si>
+    <t>GUANXI,XINZHU_XINPU,ZHUBEI,關西鎮,新埔鎮,竹北市</t>
   </si>
 </sst>
 </file>
@@ -2578,8 +2578,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:N104"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" topLeftCell="B80" workbookViewId="0">
+      <selection activeCell="N97" sqref="N97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2604,7 +2604,7 @@
         <v>3</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>570</v>
+        <v>568</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>4</v>
@@ -2648,10 +2648,10 @@
         <v>19</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>571</v>
+        <v>569</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>673</v>
+        <v>663</v>
       </c>
       <c r="G2" s="2" t="s">
         <v>20</v>
@@ -2692,10 +2692,10 @@
         <v>27</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>572</v>
+        <v>570</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>644</v>
+        <v>634</v>
       </c>
       <c r="G3" s="3" t="s">
         <v>28</v>
@@ -2717,7 +2717,7 @@
         <v>0</v>
       </c>
       <c r="N3" s="3" t="s">
-        <v>567</v>
+        <v>565</v>
       </c>
     </row>
     <row r="4" spans="1:14">
@@ -2734,10 +2734,10 @@
         <v>27</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>572</v>
+        <v>570</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>644</v>
+        <v>634</v>
       </c>
       <c r="G4" s="2" t="s">
         <v>28</v>
@@ -2759,7 +2759,7 @@
         <v>0</v>
       </c>
       <c r="N4" s="3" t="s">
-        <v>567</v>
+        <v>565</v>
       </c>
     </row>
     <row r="5" spans="1:14">
@@ -2776,10 +2776,10 @@
         <v>34</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>573</v>
+        <v>571</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>687</v>
+        <v>677</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>35</v>
@@ -2820,7 +2820,7 @@
         <v>41</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>574</v>
+        <v>572</v>
       </c>
       <c r="F6" s="3" t="s">
         <v>42</v>
@@ -2864,10 +2864,10 @@
         <v>47</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>575</v>
+        <v>573</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>688</v>
+        <v>678</v>
       </c>
       <c r="G7" s="2" t="s">
         <v>35</v>
@@ -2908,10 +2908,10 @@
         <v>56</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>576</v>
+        <v>574</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>668</v>
+        <v>658</v>
       </c>
       <c r="G8" s="2" t="s">
         <v>57</v>
@@ -2952,7 +2952,7 @@
         <v>63</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="F9" s="3" t="s">
         <v>64</v>
@@ -2996,10 +2996,10 @@
         <v>68</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>578</v>
+        <v>576</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>697</v>
+        <v>687</v>
       </c>
       <c r="G10" s="2" t="s">
         <v>69</v>
@@ -3040,10 +3040,10 @@
         <v>75</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>579</v>
+        <v>577</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>669</v>
+        <v>659</v>
       </c>
       <c r="G11" s="2" t="s">
         <v>57</v>
@@ -3084,7 +3084,7 @@
         <v>81</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>580</v>
+        <v>578</v>
       </c>
       <c r="F12" s="2" t="s">
         <v>82</v>
@@ -3172,7 +3172,7 @@
         <v>95</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>581</v>
+        <v>579</v>
       </c>
       <c r="F14" s="3" t="s">
         <v>96</v>
@@ -3216,10 +3216,10 @@
         <v>105</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>582</v>
+        <v>710</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>665</v>
+        <v>655</v>
       </c>
       <c r="G15" s="2" t="s">
         <v>97</v>
@@ -3260,7 +3260,7 @@
         <v>109</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>583</v>
+        <v>580</v>
       </c>
       <c r="F16" s="2" t="s">
         <v>110</v>
@@ -3304,7 +3304,7 @@
         <v>116</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>583</v>
+        <v>580</v>
       </c>
       <c r="F17" s="2" t="s">
         <v>117</v>
@@ -3348,10 +3348,10 @@
         <v>122</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>584</v>
+        <v>581</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>666</v>
+        <v>656</v>
       </c>
       <c r="G18" s="2" t="s">
         <v>98</v>
@@ -3392,10 +3392,10 @@
         <v>127</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>582</v>
+        <v>710</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>667</v>
+        <v>657</v>
       </c>
       <c r="G19" s="2" t="s">
         <v>98</v>
@@ -3439,7 +3439,7 @@
         <v>132</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>654</v>
+        <v>644</v>
       </c>
       <c r="G20" s="2" t="s">
         <v>132</v>
@@ -3483,7 +3483,7 @@
         <v>132</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>655</v>
+        <v>645</v>
       </c>
       <c r="G21" s="2" t="s">
         <v>132</v>
@@ -3524,10 +3524,10 @@
         <v>150</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>618</v>
+        <v>613</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>674</v>
+        <v>664</v>
       </c>
       <c r="G22" s="2" t="s">
         <v>145</v>
@@ -3568,7 +3568,7 @@
         <v>143</v>
       </c>
       <c r="E23" s="4" t="s">
-        <v>585</v>
+        <v>582</v>
       </c>
       <c r="F23" s="2" t="s">
         <v>144</v>
@@ -3612,7 +3612,7 @@
         <v>154</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>611</v>
+        <v>606</v>
       </c>
       <c r="F24" s="2" t="s">
         <v>155</v>
@@ -3639,7 +3639,7 @@
         <v>0</v>
       </c>
       <c r="N24" s="3" t="s">
-        <v>564</v>
+        <v>562</v>
       </c>
     </row>
     <row r="25" spans="1:14">
@@ -3656,10 +3656,10 @@
         <v>217</v>
       </c>
       <c r="E25" s="4" t="s">
-        <v>586</v>
+        <v>583</v>
       </c>
       <c r="F25" s="3" t="s">
-        <v>645</v>
+        <v>635</v>
       </c>
       <c r="G25" s="2" t="s">
         <v>156</v>
@@ -3703,7 +3703,7 @@
         <v>162</v>
       </c>
       <c r="F26" s="3" t="s">
-        <v>689</v>
+        <v>679</v>
       </c>
       <c r="G26" s="2" t="s">
         <v>35</v>
@@ -3744,10 +3744,10 @@
         <v>167</v>
       </c>
       <c r="E27" s="4" t="s">
-        <v>636</v>
+        <v>627</v>
       </c>
       <c r="F27" s="3" t="s">
-        <v>656</v>
+        <v>646</v>
       </c>
       <c r="G27" s="2" t="s">
         <v>168</v>
@@ -3788,10 +3788,10 @@
         <v>173</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>636</v>
+        <v>627</v>
       </c>
       <c r="F28" s="3" t="s">
-        <v>657</v>
+        <v>647</v>
       </c>
       <c r="G28" s="2" t="s">
         <v>168</v>
@@ -3832,10 +3832,10 @@
         <v>177</v>
       </c>
       <c r="E29" s="4" t="s">
-        <v>717</v>
+        <v>706</v>
       </c>
       <c r="F29" s="3" t="s">
-        <v>646</v>
+        <v>636</v>
       </c>
       <c r="G29" s="2" t="s">
         <v>178</v>
@@ -3876,10 +3876,10 @@
         <v>184</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>717</v>
+        <v>706</v>
       </c>
       <c r="F30" s="3" t="s">
-        <v>647</v>
+        <v>637</v>
       </c>
       <c r="G30" s="2" t="s">
         <v>178</v>
@@ -3923,7 +3923,7 @@
         <v>187</v>
       </c>
       <c r="F31" s="3" t="s">
-        <v>712</v>
+        <v>702</v>
       </c>
       <c r="G31" s="2" t="s">
         <v>185</v>
@@ -3964,10 +3964,10 @@
         <v>197</v>
       </c>
       <c r="E32" s="4" t="s">
-        <v>587</v>
+        <v>584</v>
       </c>
       <c r="F32" s="3" t="s">
-        <v>675</v>
+        <v>665</v>
       </c>
       <c r="G32" s="2" t="s">
         <v>145</v>
@@ -3991,7 +3991,7 @@
         <v>1</v>
       </c>
       <c r="N32" s="3" t="s">
-        <v>561</v>
+        <v>717</v>
       </c>
     </row>
     <row r="33" spans="1:14">
@@ -4008,10 +4008,10 @@
         <v>202</v>
       </c>
       <c r="E33" s="4" t="s">
-        <v>588</v>
+        <v>585</v>
       </c>
       <c r="F33" s="3" t="s">
-        <v>676</v>
+        <v>666</v>
       </c>
       <c r="G33" s="2" t="s">
         <v>145</v>
@@ -4035,7 +4035,7 @@
         <v>1</v>
       </c>
       <c r="N33" s="3" t="s">
-        <v>561</v>
+        <v>717</v>
       </c>
     </row>
     <row r="34" spans="1:14">
@@ -4052,10 +4052,10 @@
         <v>206</v>
       </c>
       <c r="E34" s="4" t="s">
-        <v>589</v>
+        <v>586</v>
       </c>
       <c r="F34" s="3" t="s">
-        <v>658</v>
+        <v>648</v>
       </c>
       <c r="G34" s="2" t="s">
         <v>207</v>
@@ -4096,10 +4096,10 @@
         <v>213</v>
       </c>
       <c r="E35" s="4" t="s">
-        <v>590</v>
+        <v>587</v>
       </c>
       <c r="F35" s="3" t="s">
-        <v>659</v>
+        <v>649</v>
       </c>
       <c r="G35" s="2" t="s">
         <v>207</v>
@@ -4140,10 +4140,10 @@
         <v>222</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>572</v>
+        <v>570</v>
       </c>
       <c r="F36" s="3" t="s">
-        <v>648</v>
+        <v>638</v>
       </c>
       <c r="G36" s="2" t="s">
         <v>156</v>
@@ -4165,7 +4165,7 @@
         <v>0</v>
       </c>
       <c r="N36" s="3" t="s">
-        <v>565</v>
+        <v>563</v>
       </c>
     </row>
     <row r="37" spans="1:14">
@@ -4182,10 +4182,10 @@
         <v>222</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>572</v>
+        <v>570</v>
       </c>
       <c r="F37" s="3" t="s">
-        <v>648</v>
+        <v>638</v>
       </c>
       <c r="G37" s="2" t="s">
         <v>156</v>
@@ -4207,7 +4207,7 @@
         <v>0</v>
       </c>
       <c r="N37" s="3" t="s">
-        <v>565</v>
+        <v>563</v>
       </c>
     </row>
     <row r="38" spans="1:14">
@@ -4224,10 +4224,10 @@
         <v>227</v>
       </c>
       <c r="E38" s="4" t="s">
-        <v>591</v>
+        <v>588</v>
       </c>
       <c r="F38" s="3" t="s">
-        <v>649</v>
+        <v>639</v>
       </c>
       <c r="G38" s="2" t="s">
         <v>178</v>
@@ -4268,10 +4268,10 @@
         <v>232</v>
       </c>
       <c r="E39" s="4" t="s">
-        <v>592</v>
+        <v>589</v>
       </c>
       <c r="F39" s="3" t="s">
-        <v>650</v>
+        <v>640</v>
       </c>
       <c r="G39" s="2" t="s">
         <v>178</v>
@@ -4312,7 +4312,7 @@
         <v>236</v>
       </c>
       <c r="E40" s="4" t="s">
-        <v>593</v>
+        <v>590</v>
       </c>
       <c r="F40" s="3" t="s">
         <v>237</v>
@@ -4356,10 +4356,10 @@
         <v>244</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>593</v>
+        <v>590</v>
       </c>
       <c r="F41" s="3" t="s">
-        <v>698</v>
+        <v>688</v>
       </c>
       <c r="G41" s="2" t="s">
         <v>238</v>
@@ -4388,22 +4388,22 @@
     </row>
     <row r="42" spans="1:14">
       <c r="A42" s="2" t="s">
+        <v>555</v>
+      </c>
+      <c r="B42" s="2" t="s">
         <v>556</v>
       </c>
-      <c r="B42" s="2" t="s">
+      <c r="C42" s="1" t="s">
         <v>557</v>
       </c>
-      <c r="C42" s="1" t="s">
+      <c r="D42" s="1" t="s">
         <v>558</v>
       </c>
-      <c r="D42" s="1" t="s">
+      <c r="E42" s="1" t="s">
+        <v>715</v>
+      </c>
+      <c r="F42" s="2" t="s">
         <v>559</v>
-      </c>
-      <c r="E42" s="1" t="s">
-        <v>637</v>
-      </c>
-      <c r="F42" s="2" t="s">
-        <v>560</v>
       </c>
       <c r="G42" s="2" t="s">
         <v>156</v>
@@ -4442,10 +4442,10 @@
         <v>254</v>
       </c>
       <c r="E43" s="4" t="s">
-        <v>594</v>
+        <v>591</v>
       </c>
       <c r="F43" s="3" t="s">
-        <v>670</v>
+        <v>660</v>
       </c>
       <c r="G43" s="2" t="s">
         <v>249</v>
@@ -4486,10 +4486,10 @@
         <v>248</v>
       </c>
       <c r="E44" s="4" t="s">
-        <v>595</v>
+        <v>712</v>
       </c>
       <c r="F44" s="3" t="s">
-        <v>671</v>
+        <v>661</v>
       </c>
       <c r="G44" s="2" t="s">
         <v>249</v>
@@ -4530,10 +4530,10 @@
         <v>259</v>
       </c>
       <c r="E45" s="4" t="s">
-        <v>596</v>
+        <v>592</v>
       </c>
       <c r="F45" s="3" t="s">
-        <v>699</v>
+        <v>689</v>
       </c>
       <c r="G45" s="2" t="s">
         <v>69</v>
@@ -4574,10 +4574,10 @@
         <v>270</v>
       </c>
       <c r="E46" s="4" t="s">
-        <v>597</v>
+        <v>593</v>
       </c>
       <c r="F46" s="3" t="s">
-        <v>660</v>
+        <v>650</v>
       </c>
       <c r="G46" s="2" t="s">
         <v>207</v>
@@ -4601,7 +4601,7 @@
         <v>1</v>
       </c>
       <c r="N46" s="3" t="s">
-        <v>566</v>
+        <v>564</v>
       </c>
     </row>
     <row r="47" spans="1:14">
@@ -4618,10 +4618,10 @@
         <v>265</v>
       </c>
       <c r="E47" s="4" t="s">
-        <v>598</v>
+        <v>594</v>
       </c>
       <c r="F47" s="3" t="s">
-        <v>661</v>
+        <v>651</v>
       </c>
       <c r="G47" s="2" t="s">
         <v>207</v>
@@ -4662,7 +4662,7 @@
         <v>274</v>
       </c>
       <c r="E48" s="4" t="s">
-        <v>599</v>
+        <v>595</v>
       </c>
       <c r="F48" s="2" t="s">
         <v>275</v>
@@ -4706,10 +4706,10 @@
         <v>283</v>
       </c>
       <c r="E49" s="4" t="s">
-        <v>600</v>
+        <v>596</v>
       </c>
       <c r="F49" s="3" t="s">
-        <v>681</v>
+        <v>671</v>
       </c>
       <c r="G49" s="2" t="s">
         <v>276</v>
@@ -4750,10 +4750,10 @@
         <v>293</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>600</v>
+        <v>596</v>
       </c>
       <c r="F50" s="3" t="s">
-        <v>682</v>
+        <v>672</v>
       </c>
       <c r="G50" s="2" t="s">
         <v>288</v>
@@ -4794,10 +4794,10 @@
         <v>287</v>
       </c>
       <c r="E51" s="4" t="s">
-        <v>601</v>
+        <v>597</v>
       </c>
       <c r="F51" s="3" t="s">
-        <v>683</v>
+        <v>673</v>
       </c>
       <c r="G51" s="2" t="s">
         <v>288</v>
@@ -4838,10 +4838,10 @@
         <v>298</v>
       </c>
       <c r="E52" s="4" t="s">
-        <v>602</v>
+        <v>713</v>
       </c>
       <c r="F52" s="3" t="s">
-        <v>684</v>
+        <v>674</v>
       </c>
       <c r="G52" s="2" t="s">
         <v>276</v>
@@ -4870,7 +4870,7 @@
     </row>
     <row r="53" spans="1:14">
       <c r="A53" s="3" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
       <c r="B53" s="2" t="s">
         <v>14</v>
@@ -4879,7 +4879,7 @@
         <v>435</v>
       </c>
       <c r="D53" s="3" t="s">
-        <v>569</v>
+        <v>567</v>
       </c>
       <c r="E53" s="4"/>
       <c r="F53" s="2"/>
@@ -4914,7 +4914,7 @@
         <v>304</v>
       </c>
       <c r="E54" s="4" t="s">
-        <v>603</v>
+        <v>598</v>
       </c>
       <c r="F54" s="2" t="s">
         <v>305</v>
@@ -4958,10 +4958,10 @@
         <v>311</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>603</v>
+        <v>598</v>
       </c>
       <c r="F55" s="3" t="s">
-        <v>690</v>
+        <v>680</v>
       </c>
       <c r="G55" s="2" t="s">
         <v>89</v>
@@ -5002,7 +5002,7 @@
         <v>315</v>
       </c>
       <c r="E56" s="4" t="s">
-        <v>604</v>
+        <v>599</v>
       </c>
       <c r="F56" s="3" t="s">
         <v>316</v>
@@ -5046,10 +5046,10 @@
         <v>321</v>
       </c>
       <c r="E57" s="4" t="s">
-        <v>605</v>
+        <v>600</v>
       </c>
       <c r="F57" s="3" t="s">
-        <v>691</v>
+        <v>681</v>
       </c>
       <c r="G57" s="2" t="s">
         <v>89</v>
@@ -5090,10 +5090,10 @@
         <v>325</v>
       </c>
       <c r="E58" s="4" t="s">
-        <v>608</v>
+        <v>603</v>
       </c>
       <c r="F58" s="3" t="s">
-        <v>692</v>
+        <v>682</v>
       </c>
       <c r="G58" s="2" t="s">
         <v>326</v>
@@ -5134,10 +5134,10 @@
         <v>331</v>
       </c>
       <c r="E59" s="4" t="s">
-        <v>607</v>
+        <v>602</v>
       </c>
       <c r="F59" s="3" t="s">
-        <v>693</v>
+        <v>683</v>
       </c>
       <c r="G59" s="2" t="s">
         <v>326</v>
@@ -5178,10 +5178,10 @@
         <v>336</v>
       </c>
       <c r="E60" s="4" t="s">
-        <v>606</v>
+        <v>601</v>
       </c>
       <c r="F60" s="3" t="s">
-        <v>694</v>
+        <v>684</v>
       </c>
       <c r="G60" s="2" t="s">
         <v>326</v>
@@ -5222,7 +5222,7 @@
         <v>342</v>
       </c>
       <c r="E61" s="4" t="s">
-        <v>609</v>
+        <v>604</v>
       </c>
       <c r="F61" s="3" t="s">
         <v>343</v>
@@ -5266,10 +5266,10 @@
         <v>347</v>
       </c>
       <c r="E62" s="4" t="s">
-        <v>610</v>
+        <v>605</v>
       </c>
       <c r="F62" s="3" t="s">
-        <v>672</v>
+        <v>662</v>
       </c>
       <c r="G62" s="2" t="s">
         <v>249</v>
@@ -5304,13 +5304,13 @@
         <v>351</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>718</v>
+        <v>707</v>
       </c>
       <c r="D63" s="1" t="s">
         <v>352</v>
       </c>
       <c r="E63" s="1" t="s">
-        <v>610</v>
+        <v>605</v>
       </c>
       <c r="F63" s="3" t="s">
         <v>353</v>
@@ -5357,7 +5357,7 @@
         <v>358</v>
       </c>
       <c r="F64" s="3" t="s">
-        <v>713</v>
+        <v>703</v>
       </c>
       <c r="G64" s="2" t="s">
         <v>185</v>
@@ -5398,10 +5398,10 @@
         <v>363</v>
       </c>
       <c r="E65" s="4" t="s">
-        <v>611</v>
+        <v>606</v>
       </c>
       <c r="F65" s="3" t="s">
-        <v>651</v>
+        <v>641</v>
       </c>
       <c r="G65" s="2" t="s">
         <v>156</v>
@@ -5423,7 +5423,7 @@
         <v>0</v>
       </c>
       <c r="N65" s="3" t="s">
-        <v>564</v>
+        <v>562</v>
       </c>
     </row>
     <row r="66" spans="1:14">
@@ -5440,10 +5440,10 @@
         <v>372</v>
       </c>
       <c r="E66" s="4" t="s">
-        <v>612</v>
+        <v>607</v>
       </c>
       <c r="F66" s="3" t="s">
-        <v>700</v>
+        <v>690</v>
       </c>
       <c r="G66" s="2" t="s">
         <v>238</v>
@@ -5484,10 +5484,10 @@
         <v>367</v>
       </c>
       <c r="E67" s="4" t="s">
-        <v>613</v>
+        <v>608</v>
       </c>
       <c r="F67" s="3" t="s">
-        <v>701</v>
+        <v>691</v>
       </c>
       <c r="G67" s="2" t="s">
         <v>238</v>
@@ -5528,10 +5528,10 @@
         <v>377</v>
       </c>
       <c r="E68" s="4" t="s">
-        <v>614</v>
+        <v>609</v>
       </c>
       <c r="F68" s="3" t="s">
-        <v>652</v>
+        <v>642</v>
       </c>
       <c r="G68" s="2" t="s">
         <v>28</v>
@@ -5555,7 +5555,7 @@
         <v>1</v>
       </c>
       <c r="N68" s="3" t="s">
-        <v>562</v>
+        <v>560</v>
       </c>
     </row>
     <row r="69" spans="1:14">
@@ -5572,7 +5572,7 @@
         <v>381</v>
       </c>
       <c r="E69" s="4" t="s">
-        <v>615</v>
+        <v>610</v>
       </c>
       <c r="F69" s="3" t="s">
         <v>382</v>
@@ -5599,7 +5599,7 @@
         <v>1</v>
       </c>
       <c r="N69" s="3" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
     </row>
     <row r="70" spans="1:14">
@@ -5619,7 +5619,7 @@
         <v>383</v>
       </c>
       <c r="F70" s="3" t="s">
-        <v>714</v>
+        <v>704</v>
       </c>
       <c r="G70" s="2" t="s">
         <v>186</v>
@@ -5660,10 +5660,10 @@
         <v>392</v>
       </c>
       <c r="E71" s="4" t="s">
-        <v>616</v>
+        <v>611</v>
       </c>
       <c r="F71" s="3" t="s">
-        <v>653</v>
+        <v>643</v>
       </c>
       <c r="G71" s="2" t="s">
         <v>28</v>
@@ -5702,10 +5702,10 @@
         <v>397</v>
       </c>
       <c r="E72" s="4" t="s">
-        <v>617</v>
+        <v>612</v>
       </c>
       <c r="F72" s="3" t="s">
-        <v>702</v>
+        <v>692</v>
       </c>
       <c r="G72" s="2" t="s">
         <v>49</v>
@@ -5746,10 +5746,10 @@
         <v>401</v>
       </c>
       <c r="E73" s="1" t="s">
-        <v>585</v>
+        <v>582</v>
       </c>
       <c r="F73" s="3" t="s">
-        <v>677</v>
+        <v>667</v>
       </c>
       <c r="G73" s="2" t="s">
         <v>20</v>
@@ -5790,10 +5790,10 @@
         <v>406</v>
       </c>
       <c r="E74" s="4" t="s">
-        <v>618</v>
+        <v>613</v>
       </c>
       <c r="F74" s="3" t="s">
-        <v>678</v>
+        <v>668</v>
       </c>
       <c r="G74" s="2" t="s">
         <v>20</v>
@@ -5834,10 +5834,10 @@
         <v>410</v>
       </c>
       <c r="E75" s="1" t="s">
-        <v>617</v>
+        <v>49</v>
       </c>
       <c r="F75" s="3" t="s">
-        <v>703</v>
+        <v>693</v>
       </c>
       <c r="G75" s="2" t="s">
         <v>49</v>
@@ -5878,10 +5878,10 @@
         <v>415</v>
       </c>
       <c r="E76" s="4" t="s">
-        <v>619</v>
+        <v>614</v>
       </c>
       <c r="F76" s="3" t="s">
-        <v>704</v>
+        <v>694</v>
       </c>
       <c r="G76" s="2" t="s">
         <v>416</v>
@@ -5922,10 +5922,10 @@
         <v>422</v>
       </c>
       <c r="E77" s="4" t="s">
-        <v>620</v>
+        <v>615</v>
       </c>
       <c r="F77" s="3" t="s">
-        <v>705</v>
+        <v>695</v>
       </c>
       <c r="G77" s="2" t="s">
         <v>416</v>
@@ -5966,7 +5966,7 @@
         <v>432</v>
       </c>
       <c r="E78" s="1" t="s">
-        <v>620</v>
+        <v>615</v>
       </c>
       <c r="F78" s="3" t="s">
         <v>433</v>
@@ -6010,10 +6010,10 @@
         <v>426</v>
       </c>
       <c r="E79" s="4" t="s">
-        <v>621</v>
+        <v>714</v>
       </c>
       <c r="F79" s="3" t="s">
-        <v>706</v>
+        <v>696</v>
       </c>
       <c r="G79" s="2" t="s">
         <v>416</v>
@@ -6054,10 +6054,10 @@
         <v>438</v>
       </c>
       <c r="E80" s="4" t="s">
-        <v>622</v>
+        <v>616</v>
       </c>
       <c r="F80" s="3" t="s">
-        <v>662</v>
+        <v>652</v>
       </c>
       <c r="G80" s="2" t="s">
         <v>439</v>
@@ -6098,7 +6098,7 @@
         <v>444</v>
       </c>
       <c r="E81" s="4" t="s">
-        <v>622</v>
+        <v>616</v>
       </c>
       <c r="F81" s="3" t="s">
         <v>445</v>
@@ -6142,10 +6142,10 @@
         <v>449</v>
       </c>
       <c r="E82" s="4" t="s">
-        <v>623</v>
+        <v>617</v>
       </c>
       <c r="F82" s="3" t="s">
-        <v>663</v>
+        <v>653</v>
       </c>
       <c r="G82" s="2" t="s">
         <v>439</v>
@@ -6189,7 +6189,7 @@
         <v>168</v>
       </c>
       <c r="F83" s="3" t="s">
-        <v>664</v>
+        <v>654</v>
       </c>
       <c r="G83" s="2" t="s">
         <v>168</v>
@@ -6230,7 +6230,7 @@
         <v>458</v>
       </c>
       <c r="E84" s="4" t="s">
-        <v>624</v>
+        <v>618</v>
       </c>
       <c r="F84" s="3" t="s">
         <v>459</v>
@@ -6277,7 +6277,7 @@
         <v>466</v>
       </c>
       <c r="F85" s="3" t="s">
-        <v>679</v>
+        <v>669</v>
       </c>
       <c r="G85" s="2" t="s">
         <v>465</v>
@@ -6318,10 +6318,10 @@
         <v>471</v>
       </c>
       <c r="E86" s="4" t="s">
-        <v>625</v>
+        <v>711</v>
       </c>
       <c r="F86" s="3" t="s">
-        <v>685</v>
+        <v>675</v>
       </c>
       <c r="G86" s="2" t="s">
         <v>472</v>
@@ -6362,10 +6362,10 @@
         <v>477</v>
       </c>
       <c r="E87" s="4" t="s">
-        <v>626</v>
+        <v>619</v>
       </c>
       <c r="F87" s="3" t="s">
-        <v>686</v>
+        <v>676</v>
       </c>
       <c r="G87" s="2" t="s">
         <v>472</v>
@@ -6406,7 +6406,7 @@
         <v>482</v>
       </c>
       <c r="E88" s="4" t="s">
-        <v>627</v>
+        <v>620</v>
       </c>
       <c r="F88" s="2" t="s">
         <v>483</v>
@@ -6450,7 +6450,7 @@
         <v>489</v>
       </c>
       <c r="E89" s="4" t="s">
-        <v>627</v>
+        <v>620</v>
       </c>
       <c r="F89" s="2" t="s">
         <v>490</v>
@@ -6497,7 +6497,7 @@
         <v>466</v>
       </c>
       <c r="F90" s="3" t="s">
-        <v>680</v>
+        <v>670</v>
       </c>
       <c r="G90" s="2" t="s">
         <v>465</v>
@@ -6538,10 +6538,10 @@
         <v>499</v>
       </c>
       <c r="E91" s="4" t="s">
-        <v>628</v>
+        <v>621</v>
       </c>
       <c r="F91" s="3" t="s">
-        <v>695</v>
+        <v>685</v>
       </c>
       <c r="G91" s="2" t="s">
         <v>500</v>
@@ -6582,7 +6582,7 @@
         <v>506</v>
       </c>
       <c r="E92" s="4" t="s">
-        <v>629</v>
+        <v>622</v>
       </c>
       <c r="F92" s="3" t="s">
         <v>507</v>
@@ -6626,10 +6626,10 @@
         <v>512</v>
       </c>
       <c r="E93" s="4" t="s">
-        <v>628</v>
+        <v>621</v>
       </c>
       <c r="F93" s="3" t="s">
-        <v>696</v>
+        <v>686</v>
       </c>
       <c r="G93" s="2" t="s">
         <v>500</v>
@@ -6658,22 +6658,22 @@
     </row>
     <row r="94" spans="1:14">
       <c r="A94" s="3" t="s">
-        <v>638</v>
+        <v>628</v>
       </c>
       <c r="B94" s="3" t="s">
         <v>531</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>640</v>
+        <v>630</v>
       </c>
       <c r="D94" s="1" t="s">
-        <v>641</v>
+        <v>631</v>
       </c>
       <c r="E94" s="4" t="s">
-        <v>632</v>
+        <v>625</v>
       </c>
       <c r="F94" s="3" t="s">
-        <v>707</v>
+        <v>697</v>
       </c>
       <c r="G94" s="2" t="s">
         <v>517</v>
@@ -6714,10 +6714,10 @@
         <v>523</v>
       </c>
       <c r="E95" s="4" t="s">
-        <v>631</v>
+        <v>624</v>
       </c>
       <c r="F95" s="3" t="s">
-        <v>708</v>
+        <v>698</v>
       </c>
       <c r="G95" s="2" t="s">
         <v>517</v>
@@ -6758,10 +6758,10 @@
         <v>529</v>
       </c>
       <c r="E96" s="1" t="s">
-        <v>630</v>
+        <v>623</v>
       </c>
       <c r="F96" s="3" t="s">
-        <v>709</v>
+        <v>699</v>
       </c>
       <c r="G96" s="2" t="s">
         <v>517</v>
@@ -6790,19 +6790,19 @@
     </row>
     <row r="97" spans="1:14">
       <c r="A97" s="3" t="s">
-        <v>639</v>
+        <v>629</v>
       </c>
       <c r="B97" s="3" t="s">
         <v>515</v>
       </c>
       <c r="C97" s="1" t="s">
-        <v>642</v>
+        <v>632</v>
       </c>
       <c r="D97" s="1" t="s">
-        <v>643</v>
+        <v>633</v>
       </c>
       <c r="E97" s="4" t="s">
-        <v>630</v>
+        <v>623</v>
       </c>
       <c r="F97" s="3" t="s">
         <v>516</v>
@@ -6828,87 +6828,87 @@
       <c r="M97" s="2">
         <v>1</v>
       </c>
-      <c r="N97" s="2" t="s">
-        <v>533</v>
+      <c r="N97" s="3" t="s">
+        <v>718</v>
       </c>
     </row>
     <row r="98" spans="1:14">
       <c r="A98" s="2" t="s">
+        <v>533</v>
+      </c>
+      <c r="B98" s="2" t="s">
         <v>534</v>
       </c>
-      <c r="B98" s="2" t="s">
+      <c r="C98" s="1" t="s">
         <v>535</v>
       </c>
-      <c r="C98" s="1" t="s">
+      <c r="D98" s="1" t="s">
         <v>536</v>
       </c>
-      <c r="D98" s="1" t="s">
+      <c r="E98" s="4" t="s">
+        <v>708</v>
+      </c>
+      <c r="F98" s="3" t="s">
+        <v>700</v>
+      </c>
+      <c r="G98" s="2" t="s">
         <v>537</v>
-      </c>
-      <c r="E98" s="4" t="s">
-        <v>633</v>
-      </c>
-      <c r="F98" s="3" t="s">
-        <v>710</v>
-      </c>
-      <c r="G98" s="2" t="s">
-        <v>538</v>
       </c>
       <c r="H98" s="2" t="s">
         <v>416</v>
       </c>
       <c r="I98" s="2" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="J98" s="2" t="s">
         <v>188</v>
       </c>
       <c r="K98" s="2" t="s">
+        <v>537</v>
+      </c>
+      <c r="L98" s="2">
+        <v>1</v>
+      </c>
+      <c r="M98" s="2">
+        <v>1</v>
+      </c>
+      <c r="N98" s="2" t="s">
         <v>538</v>
-      </c>
-      <c r="L98" s="2">
-        <v>1</v>
-      </c>
-      <c r="M98" s="2">
-        <v>1</v>
-      </c>
-      <c r="N98" s="2" t="s">
-        <v>539</v>
       </c>
     </row>
     <row r="99" spans="1:14">
       <c r="A99" s="2" t="s">
+        <v>539</v>
+      </c>
+      <c r="B99" s="2" t="s">
         <v>540</v>
       </c>
-      <c r="B99" s="2" t="s">
+      <c r="C99" s="1" t="s">
         <v>541</v>
       </c>
-      <c r="C99" s="1" t="s">
+      <c r="D99" s="1" t="s">
         <v>542</v>
       </c>
-      <c r="D99" s="1" t="s">
-        <v>543</v>
-      </c>
       <c r="E99" s="4" t="s">
-        <v>634</v>
+        <v>709</v>
       </c>
       <c r="F99" s="3" t="s">
-        <v>711</v>
+        <v>701</v>
       </c>
       <c r="G99" s="2" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="H99" s="2" t="s">
         <v>416</v>
       </c>
       <c r="I99" s="2" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="J99" s="2" t="s">
         <v>188</v>
       </c>
       <c r="K99" s="2" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="L99" s="2">
         <v>1</v>
@@ -6917,27 +6917,27 @@
         <v>1</v>
       </c>
       <c r="N99" s="2" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
     </row>
     <row r="100" spans="1:14">
       <c r="A100" s="2" t="s">
+        <v>544</v>
+      </c>
+      <c r="B100" s="2" t="s">
         <v>545</v>
       </c>
-      <c r="B100" s="2" t="s">
+      <c r="C100" s="1" t="s">
         <v>546</v>
       </c>
-      <c r="C100" s="1" t="s">
+      <c r="D100" s="1" t="s">
         <v>547</v>
-      </c>
-      <c r="D100" s="1" t="s">
-        <v>548</v>
       </c>
       <c r="E100" s="4" t="s">
         <v>716</v>
       </c>
       <c r="F100" s="2" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="G100" s="2" t="s">
         <v>186</v>
@@ -6961,27 +6961,27 @@
         <v>1</v>
       </c>
       <c r="N100" s="2" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
     </row>
     <row r="101" spans="1:14">
       <c r="A101" s="2" t="s">
+        <v>550</v>
+      </c>
+      <c r="B101" s="2" t="s">
         <v>551</v>
       </c>
-      <c r="B101" s="2" t="s">
+      <c r="C101" s="1" t="s">
         <v>552</v>
       </c>
-      <c r="C101" s="1" t="s">
+      <c r="D101" s="1" t="s">
         <v>553</v>
       </c>
-      <c r="D101" s="1" t="s">
-        <v>554</v>
-      </c>
       <c r="E101" s="4" t="s">
-        <v>635</v>
+        <v>626</v>
       </c>
       <c r="F101" s="3" t="s">
-        <v>715</v>
+        <v>705</v>
       </c>
       <c r="G101" s="2" t="s">
         <v>186</v>
@@ -7005,7 +7005,7 @@
         <v>1</v>
       </c>
       <c r="N101" s="2" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
     </row>
     <row r="104" spans="1:14">

</xml_diff>

<commit_message>
Add six-week history for individual companionships
</commit_message>
<xml_diff>
--- a/config/phone_list.xlsx
+++ b/config/phone_list.xlsx
@@ -5,7 +5,7 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="J:\ARPS\config\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="J:\arps\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1200" uniqueCount="719">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1200" uniqueCount="720">
   <si>
     <t>AREA_NAME</t>
   </si>
@@ -998,9 +998,6 @@
     <t>TAOYUAN_1</t>
   </si>
   <si>
-    <t>TAOYUAN,TAOYUAN_AREA,桃園區</t>
-  </si>
-  <si>
     <t>TAO_1_B</t>
   </si>
   <si>
@@ -1058,9 +1055,6 @@
     <t>TAOYUAN_3</t>
   </si>
   <si>
-    <t>DAYUAN,大園,大園區</t>
-  </si>
-  <si>
     <t>TAO_3_E_ZL</t>
   </si>
   <si>
@@ -1073,9 +1067,6 @@
     <t>桃園3 ZL</t>
   </si>
   <si>
-    <t>TAOYUAN,桃園縣,桃園</t>
-  </si>
-  <si>
     <t>TAO_4_E</t>
   </si>
   <si>
@@ -1091,9 +1082,6 @@
     <t>TAOYUAN_4</t>
   </si>
   <si>
-    <t>LUZHU,蘆竹,蘆竹區</t>
-  </si>
-  <si>
     <t>TAO_4_S</t>
   </si>
   <si>
@@ -1583,9 +1571,6 @@
     <t>ZHONGLI_1</t>
   </si>
   <si>
-    <t>ZHONGLI,GUANYIN,中壢,中壢區,觀音區</t>
-  </si>
-  <si>
     <t>ZHONGLI_1_S</t>
   </si>
   <si>
@@ -1601,9 +1586,6 @@
     <t>S. Komatsu / Clawson</t>
   </si>
   <si>
-    <t>ZHONGLI,中壢, 中壢區</t>
-  </si>
-  <si>
     <t>ZHONGLI_2_E</t>
   </si>
   <si>
@@ -1757,12 +1739,6 @@
     <t>McOmbers</t>
   </si>
   <si>
-    <t>ZHONGZHENG,WANHUA,中正區,萬華區,萬華</t>
-  </si>
-  <si>
-    <t>DATONG,大同區,大同,ENGLISH_WARD,ENGLISH,ENGLISHWARD,英文,英文支會</t>
-  </si>
-  <si>
     <t>ZHONGZHENG,DAAN,大安區,中正區</t>
   </si>
   <si>
@@ -2232,6 +2208,33 @@
   </si>
   <si>
     <t>GUANXI,XINZHU_XINPU,ZHUBEI,關西鎮,新埔鎮,竹北市</t>
+  </si>
+  <si>
+    <t>ZHONGZHENG,WANHUA,中正區,萬華區,萬華,WANDA,萬大,萬大區</t>
+  </si>
+  <si>
+    <t>DATONG,大同區,大同,ENGLISH_WARD,ENGLISH,ENGLISHWARD,英文,英文支會,WANDA,萬大,萬大區</t>
+  </si>
+  <si>
+    <t>LUZHU,蘆竹,蘆竹區,南崁,NANKAN,NANKANG</t>
+  </si>
+  <si>
+    <t>BANQIAO,板橋,板橋區,板橋市</t>
+  </si>
+  <si>
+    <t>TAOYUAN,桃園縣,桃園,桃園市,桃園市區</t>
+  </si>
+  <si>
+    <t>TAOYUAN,TAOYUAN_AREA,桃園區,桃園市區</t>
+  </si>
+  <si>
+    <t>DAYUAN,大園,大園區,DAZHU</t>
+  </si>
+  <si>
+    <t>ZHONGLI,GUANYIN,中壢,中壢區,觀音區,中歷,中歷區,NEILI,內壢,內壢區</t>
+  </si>
+  <si>
+    <t>ZHONGLI,中壢, 中壢區,中歷,中歷區,NEILI,內壢,內壢區</t>
   </si>
 </sst>
 </file>
@@ -2578,8 +2581,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:N104"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B80" workbookViewId="0">
-      <selection activeCell="N97" sqref="N97"/>
+    <sheetView tabSelected="1" topLeftCell="B19" workbookViewId="0">
+      <selection activeCell="P35" sqref="P35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2604,7 +2607,7 @@
         <v>3</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>568</v>
+        <v>560</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>4</v>
@@ -2648,10 +2651,10 @@
         <v>19</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>569</v>
+        <v>561</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>663</v>
+        <v>655</v>
       </c>
       <c r="G2" s="2" t="s">
         <v>20</v>
@@ -2692,10 +2695,10 @@
         <v>27</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>570</v>
+        <v>562</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>634</v>
+        <v>626</v>
       </c>
       <c r="G3" s="3" t="s">
         <v>28</v>
@@ -2717,7 +2720,7 @@
         <v>0</v>
       </c>
       <c r="N3" s="3" t="s">
-        <v>565</v>
+        <v>557</v>
       </c>
     </row>
     <row r="4" spans="1:14">
@@ -2734,10 +2737,10 @@
         <v>27</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>570</v>
+        <v>562</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>634</v>
+        <v>626</v>
       </c>
       <c r="G4" s="2" t="s">
         <v>28</v>
@@ -2759,7 +2762,7 @@
         <v>0</v>
       </c>
       <c r="N4" s="3" t="s">
-        <v>565</v>
+        <v>557</v>
       </c>
     </row>
     <row r="5" spans="1:14">
@@ -2776,10 +2779,10 @@
         <v>34</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>571</v>
+        <v>563</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>677</v>
+        <v>669</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>35</v>
@@ -2820,7 +2823,7 @@
         <v>41</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>572</v>
+        <v>564</v>
       </c>
       <c r="F6" s="3" t="s">
         <v>42</v>
@@ -2864,10 +2867,10 @@
         <v>47</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>573</v>
+        <v>565</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>678</v>
+        <v>670</v>
       </c>
       <c r="G7" s="2" t="s">
         <v>35</v>
@@ -2908,10 +2911,10 @@
         <v>56</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>574</v>
+        <v>566</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>658</v>
+        <v>650</v>
       </c>
       <c r="G8" s="2" t="s">
         <v>57</v>
@@ -2952,7 +2955,7 @@
         <v>63</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>575</v>
+        <v>567</v>
       </c>
       <c r="F9" s="3" t="s">
         <v>64</v>
@@ -2996,10 +2999,10 @@
         <v>68</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>576</v>
+        <v>568</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>687</v>
+        <v>679</v>
       </c>
       <c r="G10" s="2" t="s">
         <v>69</v>
@@ -3040,10 +3043,10 @@
         <v>75</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>577</v>
+        <v>569</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>659</v>
+        <v>651</v>
       </c>
       <c r="G11" s="2" t="s">
         <v>57</v>
@@ -3084,7 +3087,7 @@
         <v>81</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>578</v>
+        <v>570</v>
       </c>
       <c r="F12" s="2" t="s">
         <v>82</v>
@@ -3172,7 +3175,7 @@
         <v>95</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>579</v>
+        <v>571</v>
       </c>
       <c r="F14" s="3" t="s">
         <v>96</v>
@@ -3216,10 +3219,10 @@
         <v>105</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>710</v>
+        <v>702</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>655</v>
+        <v>647</v>
       </c>
       <c r="G15" s="2" t="s">
         <v>97</v>
@@ -3260,7 +3263,7 @@
         <v>109</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>580</v>
+        <v>572</v>
       </c>
       <c r="F16" s="2" t="s">
         <v>110</v>
@@ -3304,7 +3307,7 @@
         <v>116</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>580</v>
+        <v>572</v>
       </c>
       <c r="F17" s="2" t="s">
         <v>117</v>
@@ -3348,10 +3351,10 @@
         <v>122</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>581</v>
+        <v>573</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>656</v>
+        <v>648</v>
       </c>
       <c r="G18" s="2" t="s">
         <v>98</v>
@@ -3392,10 +3395,10 @@
         <v>127</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>710</v>
+        <v>702</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>657</v>
+        <v>649</v>
       </c>
       <c r="G19" s="2" t="s">
         <v>98</v>
@@ -3439,7 +3442,7 @@
         <v>132</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>644</v>
+        <v>636</v>
       </c>
       <c r="G20" s="2" t="s">
         <v>132</v>
@@ -3483,7 +3486,7 @@
         <v>132</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>645</v>
+        <v>637</v>
       </c>
       <c r="G21" s="2" t="s">
         <v>132</v>
@@ -3524,10 +3527,10 @@
         <v>150</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>613</v>
+        <v>605</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>664</v>
+        <v>656</v>
       </c>
       <c r="G22" s="2" t="s">
         <v>145</v>
@@ -3568,7 +3571,7 @@
         <v>143</v>
       </c>
       <c r="E23" s="4" t="s">
-        <v>582</v>
+        <v>574</v>
       </c>
       <c r="F23" s="2" t="s">
         <v>144</v>
@@ -3612,7 +3615,7 @@
         <v>154</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>606</v>
+        <v>598</v>
       </c>
       <c r="F24" s="2" t="s">
         <v>155</v>
@@ -3639,7 +3642,7 @@
         <v>0</v>
       </c>
       <c r="N24" s="3" t="s">
-        <v>562</v>
+        <v>554</v>
       </c>
     </row>
     <row r="25" spans="1:14">
@@ -3656,10 +3659,10 @@
         <v>217</v>
       </c>
       <c r="E25" s="4" t="s">
-        <v>583</v>
+        <v>575</v>
       </c>
       <c r="F25" s="3" t="s">
-        <v>635</v>
+        <v>627</v>
       </c>
       <c r="G25" s="2" t="s">
         <v>156</v>
@@ -3703,7 +3706,7 @@
         <v>162</v>
       </c>
       <c r="F26" s="3" t="s">
-        <v>679</v>
+        <v>671</v>
       </c>
       <c r="G26" s="2" t="s">
         <v>35</v>
@@ -3744,10 +3747,10 @@
         <v>167</v>
       </c>
       <c r="E27" s="4" t="s">
-        <v>627</v>
+        <v>619</v>
       </c>
       <c r="F27" s="3" t="s">
-        <v>646</v>
+        <v>638</v>
       </c>
       <c r="G27" s="2" t="s">
         <v>168</v>
@@ -3788,10 +3791,10 @@
         <v>173</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>627</v>
+        <v>619</v>
       </c>
       <c r="F28" s="3" t="s">
-        <v>647</v>
+        <v>639</v>
       </c>
       <c r="G28" s="2" t="s">
         <v>168</v>
@@ -3832,10 +3835,10 @@
         <v>177</v>
       </c>
       <c r="E29" s="4" t="s">
-        <v>706</v>
+        <v>698</v>
       </c>
       <c r="F29" s="3" t="s">
-        <v>636</v>
+        <v>628</v>
       </c>
       <c r="G29" s="2" t="s">
         <v>178</v>
@@ -3876,10 +3879,10 @@
         <v>184</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>706</v>
+        <v>698</v>
       </c>
       <c r="F30" s="3" t="s">
-        <v>637</v>
+        <v>629</v>
       </c>
       <c r="G30" s="2" t="s">
         <v>178</v>
@@ -3923,7 +3926,7 @@
         <v>187</v>
       </c>
       <c r="F31" s="3" t="s">
-        <v>702</v>
+        <v>694</v>
       </c>
       <c r="G31" s="2" t="s">
         <v>185</v>
@@ -3964,10 +3967,10 @@
         <v>197</v>
       </c>
       <c r="E32" s="4" t="s">
-        <v>584</v>
+        <v>576</v>
       </c>
       <c r="F32" s="3" t="s">
-        <v>665</v>
+        <v>657</v>
       </c>
       <c r="G32" s="2" t="s">
         <v>145</v>
@@ -3991,7 +3994,7 @@
         <v>1</v>
       </c>
       <c r="N32" s="3" t="s">
-        <v>717</v>
+        <v>709</v>
       </c>
     </row>
     <row r="33" spans="1:14">
@@ -4008,10 +4011,10 @@
         <v>202</v>
       </c>
       <c r="E33" s="4" t="s">
-        <v>585</v>
+        <v>577</v>
       </c>
       <c r="F33" s="3" t="s">
-        <v>666</v>
+        <v>658</v>
       </c>
       <c r="G33" s="2" t="s">
         <v>145</v>
@@ -4035,7 +4038,7 @@
         <v>1</v>
       </c>
       <c r="N33" s="3" t="s">
-        <v>717</v>
+        <v>709</v>
       </c>
     </row>
     <row r="34" spans="1:14">
@@ -4052,10 +4055,10 @@
         <v>206</v>
       </c>
       <c r="E34" s="4" t="s">
-        <v>586</v>
+        <v>578</v>
       </c>
       <c r="F34" s="3" t="s">
-        <v>648</v>
+        <v>640</v>
       </c>
       <c r="G34" s="2" t="s">
         <v>207</v>
@@ -4096,10 +4099,10 @@
         <v>213</v>
       </c>
       <c r="E35" s="4" t="s">
-        <v>587</v>
+        <v>579</v>
       </c>
       <c r="F35" s="3" t="s">
-        <v>649</v>
+        <v>641</v>
       </c>
       <c r="G35" s="2" t="s">
         <v>207</v>
@@ -4140,10 +4143,10 @@
         <v>222</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>570</v>
+        <v>562</v>
       </c>
       <c r="F36" s="3" t="s">
-        <v>638</v>
+        <v>630</v>
       </c>
       <c r="G36" s="2" t="s">
         <v>156</v>
@@ -4165,7 +4168,7 @@
         <v>0</v>
       </c>
       <c r="N36" s="3" t="s">
-        <v>563</v>
+        <v>555</v>
       </c>
     </row>
     <row r="37" spans="1:14">
@@ -4182,10 +4185,10 @@
         <v>222</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>570</v>
+        <v>562</v>
       </c>
       <c r="F37" s="3" t="s">
-        <v>638</v>
+        <v>630</v>
       </c>
       <c r="G37" s="2" t="s">
         <v>156</v>
@@ -4207,7 +4210,7 @@
         <v>0</v>
       </c>
       <c r="N37" s="3" t="s">
-        <v>563</v>
+        <v>555</v>
       </c>
     </row>
     <row r="38" spans="1:14">
@@ -4224,10 +4227,10 @@
         <v>227</v>
       </c>
       <c r="E38" s="4" t="s">
-        <v>588</v>
+        <v>580</v>
       </c>
       <c r="F38" s="3" t="s">
-        <v>639</v>
+        <v>631</v>
       </c>
       <c r="G38" s="2" t="s">
         <v>178</v>
@@ -4268,10 +4271,10 @@
         <v>232</v>
       </c>
       <c r="E39" s="4" t="s">
-        <v>589</v>
+        <v>581</v>
       </c>
       <c r="F39" s="3" t="s">
-        <v>640</v>
+        <v>632</v>
       </c>
       <c r="G39" s="2" t="s">
         <v>178</v>
@@ -4312,7 +4315,7 @@
         <v>236</v>
       </c>
       <c r="E40" s="4" t="s">
-        <v>590</v>
+        <v>582</v>
       </c>
       <c r="F40" s="3" t="s">
         <v>237</v>
@@ -4356,10 +4359,10 @@
         <v>244</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>590</v>
+        <v>582</v>
       </c>
       <c r="F41" s="3" t="s">
-        <v>688</v>
+        <v>680</v>
       </c>
       <c r="G41" s="2" t="s">
         <v>238</v>
@@ -4388,22 +4391,22 @@
     </row>
     <row r="42" spans="1:14">
       <c r="A42" s="2" t="s">
-        <v>555</v>
+        <v>549</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>556</v>
+        <v>550</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>557</v>
+        <v>551</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>558</v>
+        <v>552</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>715</v>
+        <v>707</v>
       </c>
       <c r="F42" s="2" t="s">
-        <v>559</v>
+        <v>553</v>
       </c>
       <c r="G42" s="2" t="s">
         <v>156</v>
@@ -4442,10 +4445,10 @@
         <v>254</v>
       </c>
       <c r="E43" s="4" t="s">
-        <v>591</v>
+        <v>583</v>
       </c>
       <c r="F43" s="3" t="s">
-        <v>660</v>
+        <v>652</v>
       </c>
       <c r="G43" s="2" t="s">
         <v>249</v>
@@ -4486,10 +4489,10 @@
         <v>248</v>
       </c>
       <c r="E44" s="4" t="s">
-        <v>712</v>
+        <v>704</v>
       </c>
       <c r="F44" s="3" t="s">
-        <v>661</v>
+        <v>653</v>
       </c>
       <c r="G44" s="2" t="s">
         <v>249</v>
@@ -4530,10 +4533,10 @@
         <v>259</v>
       </c>
       <c r="E45" s="4" t="s">
-        <v>592</v>
+        <v>584</v>
       </c>
       <c r="F45" s="3" t="s">
-        <v>689</v>
+        <v>681</v>
       </c>
       <c r="G45" s="2" t="s">
         <v>69</v>
@@ -4574,10 +4577,10 @@
         <v>270</v>
       </c>
       <c r="E46" s="4" t="s">
-        <v>593</v>
+        <v>585</v>
       </c>
       <c r="F46" s="3" t="s">
-        <v>650</v>
+        <v>642</v>
       </c>
       <c r="G46" s="2" t="s">
         <v>207</v>
@@ -4601,7 +4604,7 @@
         <v>1</v>
       </c>
       <c r="N46" s="3" t="s">
-        <v>564</v>
+        <v>556</v>
       </c>
     </row>
     <row r="47" spans="1:14">
@@ -4618,10 +4621,10 @@
         <v>265</v>
       </c>
       <c r="E47" s="4" t="s">
-        <v>594</v>
+        <v>586</v>
       </c>
       <c r="F47" s="3" t="s">
-        <v>651</v>
+        <v>643</v>
       </c>
       <c r="G47" s="2" t="s">
         <v>207</v>
@@ -4662,7 +4665,7 @@
         <v>274</v>
       </c>
       <c r="E48" s="4" t="s">
-        <v>595</v>
+        <v>587</v>
       </c>
       <c r="F48" s="2" t="s">
         <v>275</v>
@@ -4706,10 +4709,10 @@
         <v>283</v>
       </c>
       <c r="E49" s="4" t="s">
-        <v>596</v>
+        <v>588</v>
       </c>
       <c r="F49" s="3" t="s">
-        <v>671</v>
+        <v>663</v>
       </c>
       <c r="G49" s="2" t="s">
         <v>276</v>
@@ -4750,10 +4753,10 @@
         <v>293</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>596</v>
+        <v>588</v>
       </c>
       <c r="F50" s="3" t="s">
-        <v>672</v>
+        <v>664</v>
       </c>
       <c r="G50" s="2" t="s">
         <v>288</v>
@@ -4794,10 +4797,10 @@
         <v>287</v>
       </c>
       <c r="E51" s="4" t="s">
-        <v>597</v>
+        <v>589</v>
       </c>
       <c r="F51" s="3" t="s">
-        <v>673</v>
+        <v>665</v>
       </c>
       <c r="G51" s="2" t="s">
         <v>288</v>
@@ -4838,10 +4841,10 @@
         <v>298</v>
       </c>
       <c r="E52" s="4" t="s">
-        <v>713</v>
+        <v>705</v>
       </c>
       <c r="F52" s="3" t="s">
-        <v>674</v>
+        <v>666</v>
       </c>
       <c r="G52" s="2" t="s">
         <v>276</v>
@@ -4870,7 +4873,7 @@
     </row>
     <row r="53" spans="1:14">
       <c r="A53" s="3" t="s">
-        <v>566</v>
+        <v>558</v>
       </c>
       <c r="B53" s="2" t="s">
         <v>14</v>
@@ -4879,7 +4882,7 @@
         <v>435</v>
       </c>
       <c r="D53" s="3" t="s">
-        <v>567</v>
+        <v>559</v>
       </c>
       <c r="E53" s="4"/>
       <c r="F53" s="2"/>
@@ -4914,7 +4917,7 @@
         <v>304</v>
       </c>
       <c r="E54" s="4" t="s">
-        <v>598</v>
+        <v>590</v>
       </c>
       <c r="F54" s="2" t="s">
         <v>305</v>
@@ -4940,28 +4943,28 @@
       <c r="M54" s="2">
         <v>1</v>
       </c>
-      <c r="N54" s="2" t="s">
-        <v>307</v>
+      <c r="N54" s="3" t="s">
+        <v>716</v>
       </c>
     </row>
     <row r="55" spans="1:14">
       <c r="A55" s="2" t="s">
+        <v>307</v>
+      </c>
+      <c r="B55" s="2" t="s">
         <v>308</v>
       </c>
-      <c r="B55" s="2" t="s">
+      <c r="C55" s="1" t="s">
         <v>309</v>
       </c>
-      <c r="C55" s="1" t="s">
+      <c r="D55" s="1" t="s">
         <v>310</v>
       </c>
-      <c r="D55" s="1" t="s">
-        <v>311</v>
-      </c>
       <c r="E55" s="1" t="s">
-        <v>598</v>
+        <v>590</v>
       </c>
       <c r="F55" s="3" t="s">
-        <v>680</v>
+        <v>672</v>
       </c>
       <c r="G55" s="2" t="s">
         <v>89</v>
@@ -4984,28 +4987,28 @@
       <c r="M55" s="2">
         <v>1</v>
       </c>
-      <c r="N55" s="2" t="s">
-        <v>307</v>
+      <c r="N55" s="3" t="s">
+        <v>716</v>
       </c>
     </row>
     <row r="56" spans="1:14">
       <c r="A56" s="2" t="s">
+        <v>311</v>
+      </c>
+      <c r="B56" s="2" t="s">
         <v>312</v>
       </c>
-      <c r="B56" s="2" t="s">
+      <c r="C56" s="1" t="s">
         <v>313</v>
       </c>
-      <c r="C56" s="1" t="s">
+      <c r="D56" s="1" t="s">
         <v>314</v>
       </c>
-      <c r="D56" s="1" t="s">
+      <c r="E56" s="4" t="s">
+        <v>591</v>
+      </c>
+      <c r="F56" s="3" t="s">
         <v>315</v>
-      </c>
-      <c r="E56" s="4" t="s">
-        <v>599</v>
-      </c>
-      <c r="F56" s="3" t="s">
-        <v>316</v>
       </c>
       <c r="G56" s="2" t="s">
         <v>89</v>
@@ -5014,7 +5017,7 @@
         <v>36</v>
       </c>
       <c r="I56" s="2" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="J56" s="2" t="s">
         <v>36</v>
@@ -5028,28 +5031,28 @@
       <c r="M56" s="2">
         <v>1</v>
       </c>
-      <c r="N56" s="2" t="s">
-        <v>307</v>
+      <c r="N56" s="3" t="s">
+        <v>716</v>
       </c>
     </row>
     <row r="57" spans="1:14">
       <c r="A57" s="2" t="s">
+        <v>317</v>
+      </c>
+      <c r="B57" s="2" t="s">
         <v>318</v>
       </c>
-      <c r="B57" s="2" t="s">
+      <c r="C57" s="1" t="s">
         <v>319</v>
       </c>
-      <c r="C57" s="1" t="s">
+      <c r="D57" s="1" t="s">
         <v>320</v>
       </c>
-      <c r="D57" s="1" t="s">
-        <v>321</v>
-      </c>
       <c r="E57" s="4" t="s">
-        <v>600</v>
+        <v>592</v>
       </c>
       <c r="F57" s="3" t="s">
-        <v>681</v>
+        <v>673</v>
       </c>
       <c r="G57" s="2" t="s">
         <v>89</v>
@@ -5058,7 +5061,7 @@
         <v>36</v>
       </c>
       <c r="I57" s="2" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="J57" s="2" t="s">
         <v>36</v>
@@ -5072,43 +5075,43 @@
       <c r="M57" s="2">
         <v>0</v>
       </c>
-      <c r="N57" s="2" t="s">
-        <v>307</v>
+      <c r="N57" s="3" t="s">
+        <v>716</v>
       </c>
     </row>
     <row r="58" spans="1:14">
       <c r="A58" s="2" t="s">
+        <v>321</v>
+      </c>
+      <c r="B58" s="2" t="s">
         <v>322</v>
       </c>
-      <c r="B58" s="2" t="s">
+      <c r="C58" s="1" t="s">
         <v>323</v>
       </c>
-      <c r="C58" s="1" t="s">
+      <c r="D58" s="1" t="s">
         <v>324</v>
       </c>
-      <c r="D58" s="1" t="s">
+      <c r="E58" s="4" t="s">
+        <v>595</v>
+      </c>
+      <c r="F58" s="3" t="s">
+        <v>674</v>
+      </c>
+      <c r="G58" s="2" t="s">
         <v>325</v>
-      </c>
-      <c r="E58" s="4" t="s">
-        <v>603</v>
-      </c>
-      <c r="F58" s="3" t="s">
-        <v>682</v>
-      </c>
-      <c r="G58" s="2" t="s">
-        <v>326</v>
       </c>
       <c r="H58" s="2" t="s">
         <v>36</v>
       </c>
       <c r="I58" s="2" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="J58" s="2" t="s">
         <v>36</v>
       </c>
       <c r="K58" s="2" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="L58" s="2">
         <v>1</v>
@@ -5116,43 +5119,43 @@
       <c r="M58" s="2">
         <v>1</v>
       </c>
-      <c r="N58" s="2" t="s">
-        <v>327</v>
+      <c r="N58" s="3" t="s">
+        <v>717</v>
       </c>
     </row>
     <row r="59" spans="1:14">
       <c r="A59" s="2" t="s">
+        <v>326</v>
+      </c>
+      <c r="B59" s="2" t="s">
+        <v>327</v>
+      </c>
+      <c r="C59" s="1" t="s">
         <v>328</v>
       </c>
-      <c r="B59" s="2" t="s">
+      <c r="D59" s="1" t="s">
         <v>329</v>
       </c>
-      <c r="C59" s="1" t="s">
-        <v>330</v>
-      </c>
-      <c r="D59" s="1" t="s">
-        <v>331</v>
-      </c>
       <c r="E59" s="4" t="s">
-        <v>602</v>
+        <v>594</v>
       </c>
       <c r="F59" s="3" t="s">
-        <v>683</v>
+        <v>675</v>
       </c>
       <c r="G59" s="2" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="H59" s="2" t="s">
         <v>36</v>
       </c>
       <c r="I59" s="2" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="J59" s="2" t="s">
         <v>36</v>
       </c>
       <c r="K59" s="2" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="L59" s="2">
         <v>1</v>
@@ -5160,43 +5163,43 @@
       <c r="M59" s="2">
         <v>1</v>
       </c>
-      <c r="N59" s="2" t="s">
-        <v>332</v>
+      <c r="N59" s="3" t="s">
+        <v>715</v>
       </c>
     </row>
     <row r="60" spans="1:14">
       <c r="A60" s="2" t="s">
+        <v>330</v>
+      </c>
+      <c r="B60" s="2" t="s">
+        <v>331</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>332</v>
+      </c>
+      <c r="D60" s="1" t="s">
         <v>333</v>
       </c>
-      <c r="B60" s="2" t="s">
-        <v>334</v>
-      </c>
-      <c r="C60" s="1" t="s">
-        <v>335</v>
-      </c>
-      <c r="D60" s="1" t="s">
-        <v>336</v>
-      </c>
       <c r="E60" s="4" t="s">
-        <v>601</v>
+        <v>593</v>
       </c>
       <c r="F60" s="3" t="s">
-        <v>684</v>
+        <v>676</v>
       </c>
       <c r="G60" s="2" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="H60" s="2" t="s">
         <v>36</v>
       </c>
       <c r="I60" s="2" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="J60" s="2" t="s">
         <v>36</v>
       </c>
       <c r="K60" s="2" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="L60" s="2">
         <v>1</v>
@@ -5204,43 +5207,43 @@
       <c r="M60" s="2">
         <v>1</v>
       </c>
-      <c r="N60" s="2" t="s">
-        <v>338</v>
+      <c r="N60" s="3" t="s">
+        <v>713</v>
       </c>
     </row>
     <row r="61" spans="1:14">
       <c r="A61" s="2" t="s">
+        <v>335</v>
+      </c>
+      <c r="B61" s="2" t="s">
+        <v>336</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>337</v>
+      </c>
+      <c r="D61" s="1" t="s">
+        <v>338</v>
+      </c>
+      <c r="E61" s="4" t="s">
+        <v>596</v>
+      </c>
+      <c r="F61" s="3" t="s">
         <v>339</v>
       </c>
-      <c r="B61" s="2" t="s">
-        <v>340</v>
-      </c>
-      <c r="C61" s="1" t="s">
-        <v>341</v>
-      </c>
-      <c r="D61" s="1" t="s">
-        <v>342</v>
-      </c>
-      <c r="E61" s="4" t="s">
-        <v>604</v>
-      </c>
-      <c r="F61" s="3" t="s">
-        <v>343</v>
-      </c>
       <c r="G61" s="2" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="H61" s="2" t="s">
         <v>36</v>
       </c>
       <c r="I61" s="2" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="J61" s="2" t="s">
         <v>36</v>
       </c>
       <c r="K61" s="2" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="L61" s="2">
         <v>1</v>
@@ -5248,28 +5251,28 @@
       <c r="M61" s="2">
         <v>1</v>
       </c>
-      <c r="N61" s="2" t="s">
-        <v>338</v>
+      <c r="N61" s="3" t="s">
+        <v>713</v>
       </c>
     </row>
     <row r="62" spans="1:14">
       <c r="A62" s="2" t="s">
-        <v>344</v>
+        <v>340</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>345</v>
+        <v>341</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>347</v>
+        <v>343</v>
       </c>
       <c r="E62" s="4" t="s">
-        <v>605</v>
+        <v>597</v>
       </c>
       <c r="F62" s="3" t="s">
-        <v>662</v>
+        <v>654</v>
       </c>
       <c r="G62" s="2" t="s">
         <v>249</v>
@@ -5278,7 +5281,7 @@
         <v>58</v>
       </c>
       <c r="I62" s="2" t="s">
-        <v>348</v>
+        <v>344</v>
       </c>
       <c r="J62" s="2" t="s">
         <v>58</v>
@@ -5293,27 +5296,27 @@
         <v>1</v>
       </c>
       <c r="N62" s="2" t="s">
-        <v>349</v>
+        <v>345</v>
       </c>
     </row>
     <row r="63" spans="1:14">
       <c r="A63" s="2" t="s">
-        <v>350</v>
+        <v>346</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>351</v>
+        <v>347</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>707</v>
+        <v>699</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>352</v>
+        <v>348</v>
       </c>
       <c r="E63" s="1" t="s">
-        <v>605</v>
+        <v>597</v>
       </c>
       <c r="F63" s="3" t="s">
-        <v>353</v>
+        <v>349</v>
       </c>
       <c r="G63" s="2" t="s">
         <v>249</v>
@@ -5322,7 +5325,7 @@
         <v>58</v>
       </c>
       <c r="I63" s="2" t="s">
-        <v>348</v>
+        <v>344</v>
       </c>
       <c r="J63" s="2" t="s">
         <v>58</v>
@@ -5337,27 +5340,27 @@
         <v>1</v>
       </c>
       <c r="N63" s="2" t="s">
-        <v>349</v>
+        <v>345</v>
       </c>
     </row>
     <row r="64" spans="1:14">
       <c r="A64" s="2" t="s">
+        <v>350</v>
+      </c>
+      <c r="B64" s="2" t="s">
+        <v>351</v>
+      </c>
+      <c r="C64" s="1" t="s">
+        <v>352</v>
+      </c>
+      <c r="D64" s="1" t="s">
+        <v>353</v>
+      </c>
+      <c r="E64" s="4" t="s">
         <v>354</v>
       </c>
-      <c r="B64" s="2" t="s">
-        <v>355</v>
-      </c>
-      <c r="C64" s="1" t="s">
-        <v>356</v>
-      </c>
-      <c r="D64" s="1" t="s">
-        <v>357</v>
-      </c>
-      <c r="E64" s="4" t="s">
-        <v>358</v>
-      </c>
       <c r="F64" s="3" t="s">
-        <v>703</v>
+        <v>695</v>
       </c>
       <c r="G64" s="2" t="s">
         <v>185</v>
@@ -5366,13 +5369,13 @@
         <v>186</v>
       </c>
       <c r="I64" s="2" t="s">
-        <v>358</v>
+        <v>354</v>
       </c>
       <c r="J64" s="2" t="s">
         <v>188</v>
       </c>
       <c r="K64" s="2" t="s">
-        <v>358</v>
+        <v>354</v>
       </c>
       <c r="L64" s="2">
         <v>1</v>
@@ -5381,27 +5384,27 @@
         <v>1</v>
       </c>
       <c r="N64" s="2" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
     </row>
     <row r="65" spans="1:14">
       <c r="A65" s="2" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>361</v>
+        <v>357</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>362</v>
+        <v>358</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>363</v>
+        <v>359</v>
       </c>
       <c r="E65" s="4" t="s">
-        <v>606</v>
+        <v>598</v>
       </c>
       <c r="F65" s="3" t="s">
-        <v>641</v>
+        <v>633</v>
       </c>
       <c r="G65" s="2" t="s">
         <v>156</v>
@@ -5423,27 +5426,27 @@
         <v>0</v>
       </c>
       <c r="N65" s="3" t="s">
-        <v>562</v>
+        <v>554</v>
       </c>
     </row>
     <row r="66" spans="1:14">
       <c r="A66" s="2" t="s">
-        <v>369</v>
+        <v>365</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>370</v>
+        <v>366</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>371</v>
+        <v>367</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>372</v>
+        <v>368</v>
       </c>
       <c r="E66" s="4" t="s">
-        <v>607</v>
+        <v>599</v>
       </c>
       <c r="F66" s="3" t="s">
-        <v>690</v>
+        <v>682</v>
       </c>
       <c r="G66" s="2" t="s">
         <v>238</v>
@@ -5467,27 +5470,27 @@
         <v>1</v>
       </c>
       <c r="N66" s="2" t="s">
-        <v>373</v>
+        <v>369</v>
       </c>
     </row>
     <row r="67" spans="1:14">
       <c r="A67" s="2" t="s">
-        <v>364</v>
+        <v>360</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>365</v>
+        <v>361</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>367</v>
+        <v>363</v>
       </c>
       <c r="E67" s="4" t="s">
-        <v>608</v>
+        <v>600</v>
       </c>
       <c r="F67" s="3" t="s">
-        <v>691</v>
+        <v>683</v>
       </c>
       <c r="G67" s="2" t="s">
         <v>238</v>
@@ -5511,27 +5514,27 @@
         <v>1</v>
       </c>
       <c r="N67" s="2" t="s">
-        <v>368</v>
+        <v>364</v>
       </c>
     </row>
     <row r="68" spans="1:14">
       <c r="A68" s="2" t="s">
-        <v>374</v>
+        <v>370</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>375</v>
+        <v>371</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>376</v>
+        <v>372</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>377</v>
+        <v>373</v>
       </c>
       <c r="E68" s="4" t="s">
-        <v>609</v>
+        <v>601</v>
       </c>
       <c r="F68" s="3" t="s">
-        <v>642</v>
+        <v>634</v>
       </c>
       <c r="G68" s="2" t="s">
         <v>28</v>
@@ -5555,27 +5558,27 @@
         <v>1</v>
       </c>
       <c r="N68" s="3" t="s">
-        <v>560</v>
+        <v>711</v>
       </c>
     </row>
     <row r="69" spans="1:14">
       <c r="A69" s="2" t="s">
+        <v>374</v>
+      </c>
+      <c r="B69" s="2" t="s">
+        <v>375</v>
+      </c>
+      <c r="C69" s="1" t="s">
+        <v>376</v>
+      </c>
+      <c r="D69" s="1" t="s">
+        <v>377</v>
+      </c>
+      <c r="E69" s="4" t="s">
+        <v>602</v>
+      </c>
+      <c r="F69" s="3" t="s">
         <v>378</v>
-      </c>
-      <c r="B69" s="2" t="s">
-        <v>379</v>
-      </c>
-      <c r="C69" s="1" t="s">
-        <v>380</v>
-      </c>
-      <c r="D69" s="1" t="s">
-        <v>381</v>
-      </c>
-      <c r="E69" s="4" t="s">
-        <v>610</v>
-      </c>
-      <c r="F69" s="3" t="s">
-        <v>382</v>
       </c>
       <c r="G69" s="2" t="s">
         <v>28</v>
@@ -5599,27 +5602,27 @@
         <v>1</v>
       </c>
       <c r="N69" s="3" t="s">
-        <v>561</v>
+        <v>712</v>
       </c>
     </row>
     <row r="70" spans="1:14">
       <c r="A70" s="2" t="s">
-        <v>384</v>
+        <v>380</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>385</v>
+        <v>381</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>386</v>
+        <v>382</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>387</v>
+        <v>383</v>
       </c>
       <c r="E70" s="4" t="s">
-        <v>383</v>
+        <v>379</v>
       </c>
       <c r="F70" s="3" t="s">
-        <v>704</v>
+        <v>696</v>
       </c>
       <c r="G70" s="2" t="s">
         <v>186</v>
@@ -5628,7 +5631,7 @@
         <v>186</v>
       </c>
       <c r="I70" s="2" t="s">
-        <v>383</v>
+        <v>379</v>
       </c>
       <c r="J70" s="2" t="s">
         <v>188</v>
@@ -5643,27 +5646,27 @@
         <v>1</v>
       </c>
       <c r="N70" s="2" t="s">
-        <v>388</v>
+        <v>384</v>
       </c>
     </row>
     <row r="71" spans="1:14">
       <c r="A71" s="2" t="s">
-        <v>389</v>
+        <v>385</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>390</v>
+        <v>386</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>391</v>
+        <v>387</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>392</v>
+        <v>388</v>
       </c>
       <c r="E71" s="4" t="s">
-        <v>611</v>
+        <v>603</v>
       </c>
       <c r="F71" s="3" t="s">
-        <v>643</v>
+        <v>635</v>
       </c>
       <c r="G71" s="2" t="s">
         <v>28</v>
@@ -5685,27 +5688,27 @@
         <v>0</v>
       </c>
       <c r="N71" s="2" t="s">
-        <v>393</v>
+        <v>389</v>
       </c>
     </row>
     <row r="72" spans="1:14">
       <c r="A72" s="2" t="s">
-        <v>394</v>
+        <v>390</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>396</v>
+        <v>392</v>
       </c>
       <c r="D72" s="1" t="s">
-        <v>397</v>
+        <v>393</v>
       </c>
       <c r="E72" s="4" t="s">
-        <v>612</v>
+        <v>604</v>
       </c>
       <c r="F72" s="3" t="s">
-        <v>692</v>
+        <v>684</v>
       </c>
       <c r="G72" s="2" t="s">
         <v>49</v>
@@ -5728,28 +5731,28 @@
       <c r="M72" s="2">
         <v>1</v>
       </c>
-      <c r="N72" s="2" t="s">
-        <v>52</v>
+      <c r="N72" s="3" t="s">
+        <v>714</v>
       </c>
     </row>
     <row r="73" spans="1:14">
       <c r="A73" s="2" t="s">
-        <v>398</v>
+        <v>394</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>399</v>
+        <v>395</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>400</v>
+        <v>396</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>401</v>
+        <v>397</v>
       </c>
       <c r="E73" s="1" t="s">
-        <v>582</v>
+        <v>574</v>
       </c>
       <c r="F73" s="3" t="s">
-        <v>667</v>
+        <v>659</v>
       </c>
       <c r="G73" s="2" t="s">
         <v>20</v>
@@ -5773,27 +5776,27 @@
         <v>1</v>
       </c>
       <c r="N73" s="2" t="s">
-        <v>402</v>
+        <v>398</v>
       </c>
     </row>
     <row r="74" spans="1:14">
       <c r="A74" s="2" t="s">
-        <v>403</v>
+        <v>399</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>404</v>
+        <v>400</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>405</v>
+        <v>401</v>
       </c>
       <c r="D74" s="1" t="s">
-        <v>406</v>
+        <v>402</v>
       </c>
       <c r="E74" s="4" t="s">
-        <v>613</v>
+        <v>605</v>
       </c>
       <c r="F74" s="3" t="s">
-        <v>668</v>
+        <v>660</v>
       </c>
       <c r="G74" s="2" t="s">
         <v>20</v>
@@ -5817,27 +5820,27 @@
         <v>1</v>
       </c>
       <c r="N74" s="2" t="s">
-        <v>402</v>
+        <v>398</v>
       </c>
     </row>
     <row r="75" spans="1:14">
       <c r="A75" s="2" t="s">
-        <v>407</v>
+        <v>403</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>408</v>
+        <v>404</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>409</v>
+        <v>405</v>
       </c>
       <c r="D75" s="1" t="s">
-        <v>410</v>
+        <v>406</v>
       </c>
       <c r="E75" s="1" t="s">
         <v>49</v>
       </c>
       <c r="F75" s="3" t="s">
-        <v>693</v>
+        <v>685</v>
       </c>
       <c r="G75" s="2" t="s">
         <v>49</v>
@@ -5846,7 +5849,7 @@
         <v>50</v>
       </c>
       <c r="I75" s="2" t="s">
-        <v>411</v>
+        <v>407</v>
       </c>
       <c r="J75" s="2" t="s">
         <v>50</v>
@@ -5866,37 +5869,37 @@
     </row>
     <row r="76" spans="1:14">
       <c r="A76" s="2" t="s">
+        <v>408</v>
+      </c>
+      <c r="B76" s="2" t="s">
+        <v>409</v>
+      </c>
+      <c r="C76" s="1" t="s">
+        <v>410</v>
+      </c>
+      <c r="D76" s="1" t="s">
+        <v>411</v>
+      </c>
+      <c r="E76" s="4" t="s">
+        <v>606</v>
+      </c>
+      <c r="F76" s="3" t="s">
+        <v>686</v>
+      </c>
+      <c r="G76" s="2" t="s">
         <v>412</v>
       </c>
-      <c r="B76" s="2" t="s">
+      <c r="H76" s="2" t="s">
+        <v>412</v>
+      </c>
+      <c r="I76" s="2" t="s">
         <v>413</v>
-      </c>
-      <c r="C76" s="1" t="s">
-        <v>414</v>
-      </c>
-      <c r="D76" s="1" t="s">
-        <v>415</v>
-      </c>
-      <c r="E76" s="4" t="s">
-        <v>614</v>
-      </c>
-      <c r="F76" s="3" t="s">
-        <v>694</v>
-      </c>
-      <c r="G76" s="2" t="s">
-        <v>416</v>
-      </c>
-      <c r="H76" s="2" t="s">
-        <v>416</v>
-      </c>
-      <c r="I76" s="2" t="s">
-        <v>417</v>
       </c>
       <c r="J76" s="2" t="s">
         <v>188</v>
       </c>
       <c r="K76" s="2" t="s">
-        <v>416</v>
+        <v>412</v>
       </c>
       <c r="L76" s="2">
         <v>1</v>
@@ -5905,42 +5908,42 @@
         <v>1</v>
       </c>
       <c r="N76" s="2" t="s">
-        <v>418</v>
+        <v>414</v>
       </c>
     </row>
     <row r="77" spans="1:14">
       <c r="A77" s="2" t="s">
-        <v>419</v>
+        <v>415</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>420</v>
+        <v>416</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>421</v>
+        <v>417</v>
       </c>
       <c r="D77" s="1" t="s">
-        <v>422</v>
+        <v>418</v>
       </c>
       <c r="E77" s="4" t="s">
-        <v>615</v>
+        <v>607</v>
       </c>
       <c r="F77" s="3" t="s">
-        <v>695</v>
+        <v>687</v>
       </c>
       <c r="G77" s="2" t="s">
-        <v>416</v>
+        <v>412</v>
       </c>
       <c r="H77" s="2" t="s">
-        <v>416</v>
+        <v>412</v>
       </c>
       <c r="I77" s="2" t="s">
-        <v>417</v>
+        <v>413</v>
       </c>
       <c r="J77" s="2" t="s">
         <v>188</v>
       </c>
       <c r="K77" s="2" t="s">
-        <v>416</v>
+        <v>412</v>
       </c>
       <c r="L77" s="2">
         <v>1</v>
@@ -5949,42 +5952,42 @@
         <v>1</v>
       </c>
       <c r="N77" s="2" t="s">
-        <v>418</v>
+        <v>414</v>
       </c>
     </row>
     <row r="78" spans="1:14">
       <c r="A78" s="2" t="s">
+        <v>425</v>
+      </c>
+      <c r="B78" s="2" t="s">
+        <v>426</v>
+      </c>
+      <c r="C78" s="1" t="s">
+        <v>427</v>
+      </c>
+      <c r="D78" s="1" t="s">
+        <v>428</v>
+      </c>
+      <c r="E78" s="1" t="s">
+        <v>607</v>
+      </c>
+      <c r="F78" s="3" t="s">
         <v>429</v>
       </c>
-      <c r="B78" s="2" t="s">
-        <v>430</v>
-      </c>
-      <c r="C78" s="1" t="s">
-        <v>431</v>
-      </c>
-      <c r="D78" s="1" t="s">
-        <v>432</v>
-      </c>
-      <c r="E78" s="1" t="s">
-        <v>615</v>
-      </c>
-      <c r="F78" s="3" t="s">
-        <v>433</v>
-      </c>
       <c r="G78" s="2" t="s">
-        <v>416</v>
+        <v>412</v>
       </c>
       <c r="H78" s="2" t="s">
-        <v>416</v>
+        <v>412</v>
       </c>
       <c r="I78" s="2" t="s">
-        <v>427</v>
+        <v>423</v>
       </c>
       <c r="J78" s="2" t="s">
         <v>188</v>
       </c>
       <c r="K78" s="2" t="s">
-        <v>416</v>
+        <v>412</v>
       </c>
       <c r="L78" s="2">
         <v>1</v>
@@ -5993,42 +5996,42 @@
         <v>1</v>
       </c>
       <c r="N78" s="2" t="s">
-        <v>434</v>
+        <v>430</v>
       </c>
     </row>
     <row r="79" spans="1:14">
       <c r="A79" s="2" t="s">
+        <v>419</v>
+      </c>
+      <c r="B79" s="2" t="s">
+        <v>420</v>
+      </c>
+      <c r="C79" s="1" t="s">
+        <v>421</v>
+      </c>
+      <c r="D79" s="1" t="s">
+        <v>422</v>
+      </c>
+      <c r="E79" s="4" t="s">
+        <v>706</v>
+      </c>
+      <c r="F79" s="3" t="s">
+        <v>688</v>
+      </c>
+      <c r="G79" s="2" t="s">
+        <v>412</v>
+      </c>
+      <c r="H79" s="2" t="s">
+        <v>412</v>
+      </c>
+      <c r="I79" s="2" t="s">
         <v>423</v>
-      </c>
-      <c r="B79" s="2" t="s">
-        <v>424</v>
-      </c>
-      <c r="C79" s="1" t="s">
-        <v>425</v>
-      </c>
-      <c r="D79" s="1" t="s">
-        <v>426</v>
-      </c>
-      <c r="E79" s="4" t="s">
-        <v>714</v>
-      </c>
-      <c r="F79" s="3" t="s">
-        <v>696</v>
-      </c>
-      <c r="G79" s="2" t="s">
-        <v>416</v>
-      </c>
-      <c r="H79" s="2" t="s">
-        <v>416</v>
-      </c>
-      <c r="I79" s="2" t="s">
-        <v>427</v>
       </c>
       <c r="J79" s="2" t="s">
         <v>188</v>
       </c>
       <c r="K79" s="2" t="s">
-        <v>416</v>
+        <v>412</v>
       </c>
       <c r="L79" s="2">
         <v>1</v>
@@ -6037,42 +6040,42 @@
         <v>1</v>
       </c>
       <c r="N79" s="2" t="s">
-        <v>428</v>
+        <v>424</v>
       </c>
     </row>
     <row r="80" spans="1:14">
       <c r="A80" s="2" t="s">
+        <v>431</v>
+      </c>
+      <c r="B80" s="2" t="s">
+        <v>432</v>
+      </c>
+      <c r="C80" s="1" t="s">
+        <v>433</v>
+      </c>
+      <c r="D80" s="1" t="s">
+        <v>434</v>
+      </c>
+      <c r="E80" s="4" t="s">
+        <v>608</v>
+      </c>
+      <c r="F80" s="3" t="s">
+        <v>644</v>
+      </c>
+      <c r="G80" s="2" t="s">
         <v>435</v>
-      </c>
-      <c r="B80" s="2" t="s">
-        <v>436</v>
-      </c>
-      <c r="C80" s="1" t="s">
-        <v>437</v>
-      </c>
-      <c r="D80" s="1" t="s">
-        <v>438</v>
-      </c>
-      <c r="E80" s="4" t="s">
-        <v>616</v>
-      </c>
-      <c r="F80" s="3" t="s">
-        <v>652</v>
-      </c>
-      <c r="G80" s="2" t="s">
-        <v>439</v>
       </c>
       <c r="H80" s="2" t="s">
         <v>133</v>
       </c>
       <c r="I80" s="2" t="s">
-        <v>439</v>
+        <v>435</v>
       </c>
       <c r="J80" s="2" t="s">
         <v>133</v>
       </c>
       <c r="K80" s="2" t="s">
-        <v>439</v>
+        <v>435</v>
       </c>
       <c r="L80" s="2">
         <v>1</v>
@@ -6081,42 +6084,42 @@
         <v>1</v>
       </c>
       <c r="N80" s="2" t="s">
-        <v>440</v>
+        <v>436</v>
       </c>
     </row>
     <row r="81" spans="1:14">
       <c r="A81" s="2" t="s">
+        <v>437</v>
+      </c>
+      <c r="B81" s="2" t="s">
+        <v>438</v>
+      </c>
+      <c r="C81" s="1" t="s">
+        <v>439</v>
+      </c>
+      <c r="D81" s="1" t="s">
+        <v>440</v>
+      </c>
+      <c r="E81" s="4" t="s">
+        <v>608</v>
+      </c>
+      <c r="F81" s="3" t="s">
         <v>441</v>
       </c>
-      <c r="B81" s="2" t="s">
-        <v>442</v>
-      </c>
-      <c r="C81" s="1" t="s">
-        <v>443</v>
-      </c>
-      <c r="D81" s="1" t="s">
-        <v>444</v>
-      </c>
-      <c r="E81" s="4" t="s">
-        <v>616</v>
-      </c>
-      <c r="F81" s="3" t="s">
-        <v>445</v>
-      </c>
       <c r="G81" s="2" t="s">
-        <v>439</v>
+        <v>435</v>
       </c>
       <c r="H81" s="2" t="s">
         <v>133</v>
       </c>
       <c r="I81" s="2" t="s">
-        <v>439</v>
+        <v>435</v>
       </c>
       <c r="J81" s="2" t="s">
         <v>133</v>
       </c>
       <c r="K81" s="2" t="s">
-        <v>439</v>
+        <v>435</v>
       </c>
       <c r="L81" s="2">
         <v>1</v>
@@ -6125,42 +6128,42 @@
         <v>1</v>
       </c>
       <c r="N81" s="2" t="s">
-        <v>440</v>
+        <v>436</v>
       </c>
     </row>
     <row r="82" spans="1:14">
       <c r="A82" s="2" t="s">
-        <v>446</v>
+        <v>442</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>447</v>
+        <v>443</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>448</v>
+        <v>444</v>
       </c>
       <c r="D82" s="1" t="s">
-        <v>449</v>
+        <v>445</v>
       </c>
       <c r="E82" s="4" t="s">
-        <v>617</v>
+        <v>609</v>
       </c>
       <c r="F82" s="3" t="s">
-        <v>653</v>
+        <v>645</v>
       </c>
       <c r="G82" s="2" t="s">
-        <v>439</v>
+        <v>435</v>
       </c>
       <c r="H82" s="2" t="s">
         <v>133</v>
       </c>
       <c r="I82" s="2" t="s">
-        <v>439</v>
+        <v>435</v>
       </c>
       <c r="J82" s="2" t="s">
         <v>133</v>
       </c>
       <c r="K82" s="2" t="s">
-        <v>439</v>
+        <v>435</v>
       </c>
       <c r="L82" s="2">
         <v>1</v>
@@ -6169,27 +6172,27 @@
         <v>1</v>
       </c>
       <c r="N82" s="2" t="s">
-        <v>440</v>
+        <v>436</v>
       </c>
     </row>
     <row r="83" spans="1:14">
       <c r="A83" s="2" t="s">
-        <v>450</v>
+        <v>446</v>
       </c>
       <c r="B83" s="2" t="s">
-        <v>451</v>
+        <v>447</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>452</v>
+        <v>448</v>
       </c>
       <c r="D83" s="1" t="s">
-        <v>453</v>
+        <v>449</v>
       </c>
       <c r="E83" s="4" t="s">
         <v>168</v>
       </c>
       <c r="F83" s="3" t="s">
-        <v>654</v>
+        <v>646</v>
       </c>
       <c r="G83" s="2" t="s">
         <v>168</v>
@@ -6213,27 +6216,27 @@
         <v>1</v>
       </c>
       <c r="N83" s="2" t="s">
-        <v>454</v>
+        <v>450</v>
       </c>
     </row>
     <row r="84" spans="1:14">
       <c r="A84" s="2" t="s">
+        <v>451</v>
+      </c>
+      <c r="B84" s="2" t="s">
+        <v>452</v>
+      </c>
+      <c r="C84" s="1" t="s">
+        <v>453</v>
+      </c>
+      <c r="D84" s="1" t="s">
+        <v>454</v>
+      </c>
+      <c r="E84" s="4" t="s">
+        <v>610</v>
+      </c>
+      <c r="F84" s="3" t="s">
         <v>455</v>
-      </c>
-      <c r="B84" s="2" t="s">
-        <v>456</v>
-      </c>
-      <c r="C84" s="1" t="s">
-        <v>457</v>
-      </c>
-      <c r="D84" s="1" t="s">
-        <v>458</v>
-      </c>
-      <c r="E84" s="4" t="s">
-        <v>618</v>
-      </c>
-      <c r="F84" s="3" t="s">
-        <v>459</v>
       </c>
       <c r="G84" s="2" t="s">
         <v>168</v>
@@ -6257,42 +6260,42 @@
         <v>0</v>
       </c>
       <c r="N84" s="2" t="s">
-        <v>460</v>
+        <v>456</v>
       </c>
     </row>
     <row r="85" spans="1:14">
       <c r="A85" s="2" t="s">
+        <v>457</v>
+      </c>
+      <c r="B85" s="2" t="s">
+        <v>458</v>
+      </c>
+      <c r="C85" s="1" t="s">
+        <v>459</v>
+      </c>
+      <c r="D85" s="1" t="s">
+        <v>460</v>
+      </c>
+      <c r="E85" s="4" t="s">
+        <v>462</v>
+      </c>
+      <c r="F85" s="3" t="s">
+        <v>661</v>
+      </c>
+      <c r="G85" s="2" t="s">
         <v>461</v>
-      </c>
-      <c r="B85" s="2" t="s">
-        <v>462</v>
-      </c>
-      <c r="C85" s="1" t="s">
-        <v>463</v>
-      </c>
-      <c r="D85" s="1" t="s">
-        <v>464</v>
-      </c>
-      <c r="E85" s="4" t="s">
-        <v>466</v>
-      </c>
-      <c r="F85" s="3" t="s">
-        <v>669</v>
-      </c>
-      <c r="G85" s="2" t="s">
-        <v>465</v>
       </c>
       <c r="H85" s="2" t="s">
         <v>21</v>
       </c>
       <c r="I85" s="2" t="s">
-        <v>466</v>
+        <v>462</v>
       </c>
       <c r="J85" s="2" t="s">
         <v>21</v>
       </c>
       <c r="K85" s="2" t="s">
-        <v>465</v>
+        <v>461</v>
       </c>
       <c r="L85" s="2">
         <v>1</v>
@@ -6301,42 +6304,42 @@
         <v>1</v>
       </c>
       <c r="N85" s="2" t="s">
-        <v>467</v>
+        <v>463</v>
       </c>
     </row>
     <row r="86" spans="1:14">
       <c r="A86" s="2" t="s">
+        <v>464</v>
+      </c>
+      <c r="B86" s="2" t="s">
+        <v>465</v>
+      </c>
+      <c r="C86" s="1" t="s">
+        <v>466</v>
+      </c>
+      <c r="D86" s="1" t="s">
+        <v>467</v>
+      </c>
+      <c r="E86" s="4" t="s">
+        <v>703</v>
+      </c>
+      <c r="F86" s="3" t="s">
+        <v>667</v>
+      </c>
+      <c r="G86" s="2" t="s">
         <v>468</v>
-      </c>
-      <c r="B86" s="2" t="s">
-        <v>469</v>
-      </c>
-      <c r="C86" s="1" t="s">
-        <v>470</v>
-      </c>
-      <c r="D86" s="1" t="s">
-        <v>471</v>
-      </c>
-      <c r="E86" s="4" t="s">
-        <v>711</v>
-      </c>
-      <c r="F86" s="3" t="s">
-        <v>675</v>
-      </c>
-      <c r="G86" s="2" t="s">
-        <v>472</v>
       </c>
       <c r="H86" s="2" t="s">
         <v>277</v>
       </c>
       <c r="I86" s="2" t="s">
-        <v>472</v>
+        <v>468</v>
       </c>
       <c r="J86" s="2" t="s">
         <v>100</v>
       </c>
       <c r="K86" s="2" t="s">
-        <v>472</v>
+        <v>468</v>
       </c>
       <c r="L86" s="2">
         <v>1</v>
@@ -6345,42 +6348,42 @@
         <v>1</v>
       </c>
       <c r="N86" s="2" t="s">
-        <v>473</v>
+        <v>469</v>
       </c>
     </row>
     <row r="87" spans="1:14">
       <c r="A87" s="2" t="s">
-        <v>474</v>
+        <v>470</v>
       </c>
       <c r="B87" s="2" t="s">
-        <v>475</v>
+        <v>471</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>476</v>
+        <v>472</v>
       </c>
       <c r="D87" s="1" t="s">
-        <v>477</v>
+        <v>473</v>
       </c>
       <c r="E87" s="4" t="s">
-        <v>619</v>
+        <v>611</v>
       </c>
       <c r="F87" s="3" t="s">
-        <v>676</v>
+        <v>668</v>
       </c>
       <c r="G87" s="2" t="s">
-        <v>472</v>
-      </c>
-      <c r="H87" s="2" t="s">
+        <v>468</v>
+      </c>
+      <c r="H87" s="3" t="s">
         <v>277</v>
       </c>
       <c r="I87" s="2" t="s">
-        <v>472</v>
+        <v>468</v>
       </c>
       <c r="J87" s="2" t="s">
         <v>100</v>
       </c>
       <c r="K87" s="2" t="s">
-        <v>472</v>
+        <v>468</v>
       </c>
       <c r="L87" s="2">
         <v>1</v>
@@ -6389,42 +6392,42 @@
         <v>1</v>
       </c>
       <c r="N87" s="2" t="s">
-        <v>478</v>
+        <v>474</v>
       </c>
     </row>
     <row r="88" spans="1:14">
       <c r="A88" s="2" t="s">
+        <v>475</v>
+      </c>
+      <c r="B88" s="2" t="s">
+        <v>476</v>
+      </c>
+      <c r="C88" s="1" t="s">
+        <v>477</v>
+      </c>
+      <c r="D88" s="1" t="s">
+        <v>478</v>
+      </c>
+      <c r="E88" s="4" t="s">
+        <v>612</v>
+      </c>
+      <c r="F88" s="2" t="s">
         <v>479</v>
       </c>
-      <c r="B88" s="2" t="s">
-        <v>480</v>
-      </c>
-      <c r="C88" s="1" t="s">
-        <v>481</v>
-      </c>
-      <c r="D88" s="1" t="s">
-        <v>482</v>
-      </c>
-      <c r="E88" s="4" t="s">
-        <v>620</v>
-      </c>
-      <c r="F88" s="2" t="s">
-        <v>483</v>
-      </c>
       <c r="G88" s="2" t="s">
-        <v>465</v>
+        <v>461</v>
       </c>
       <c r="H88" s="2" t="s">
         <v>21</v>
       </c>
       <c r="I88" s="2" t="s">
-        <v>484</v>
+        <v>480</v>
       </c>
       <c r="J88" s="2" t="s">
         <v>21</v>
       </c>
       <c r="K88" s="2" t="s">
-        <v>465</v>
+        <v>461</v>
       </c>
       <c r="L88" s="2">
         <v>1</v>
@@ -6433,42 +6436,42 @@
         <v>1</v>
       </c>
       <c r="N88" s="2" t="s">
-        <v>485</v>
+        <v>481</v>
       </c>
     </row>
     <row r="89" spans="1:14">
       <c r="A89" s="2" t="s">
+        <v>482</v>
+      </c>
+      <c r="B89" s="2" t="s">
+        <v>483</v>
+      </c>
+      <c r="C89" s="1" t="s">
+        <v>484</v>
+      </c>
+      <c r="D89" s="1" t="s">
+        <v>485</v>
+      </c>
+      <c r="E89" s="4" t="s">
+        <v>612</v>
+      </c>
+      <c r="F89" s="2" t="s">
         <v>486</v>
       </c>
-      <c r="B89" s="2" t="s">
-        <v>487</v>
-      </c>
-      <c r="C89" s="1" t="s">
-        <v>488</v>
-      </c>
-      <c r="D89" s="1" t="s">
-        <v>489</v>
-      </c>
-      <c r="E89" s="4" t="s">
-        <v>620</v>
-      </c>
-      <c r="F89" s="2" t="s">
-        <v>490</v>
-      </c>
       <c r="G89" s="2" t="s">
-        <v>465</v>
+        <v>461</v>
       </c>
       <c r="H89" s="2" t="s">
         <v>21</v>
       </c>
       <c r="I89" s="2" t="s">
-        <v>491</v>
+        <v>487</v>
       </c>
       <c r="J89" s="2" t="s">
         <v>21</v>
       </c>
       <c r="K89" s="2" t="s">
-        <v>465</v>
+        <v>461</v>
       </c>
       <c r="L89" s="2">
         <v>1</v>
@@ -6477,42 +6480,42 @@
         <v>1</v>
       </c>
       <c r="N89" s="2" t="s">
-        <v>485</v>
+        <v>481</v>
       </c>
     </row>
     <row r="90" spans="1:14">
       <c r="A90" s="2" t="s">
-        <v>492</v>
+        <v>488</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>493</v>
+        <v>489</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>494</v>
+        <v>490</v>
       </c>
       <c r="D90" s="1" t="s">
-        <v>495</v>
+        <v>491</v>
       </c>
       <c r="E90" s="1" t="s">
-        <v>466</v>
+        <v>462</v>
       </c>
       <c r="F90" s="3" t="s">
-        <v>670</v>
+        <v>662</v>
       </c>
       <c r="G90" s="2" t="s">
-        <v>465</v>
+        <v>461</v>
       </c>
       <c r="H90" s="2" t="s">
         <v>21</v>
       </c>
       <c r="I90" s="2" t="s">
-        <v>491</v>
+        <v>487</v>
       </c>
       <c r="J90" s="2" t="s">
         <v>21</v>
       </c>
       <c r="K90" s="2" t="s">
-        <v>465</v>
+        <v>461</v>
       </c>
       <c r="L90" s="2">
         <v>1</v>
@@ -6521,42 +6524,42 @@
         <v>1</v>
       </c>
       <c r="N90" s="2" t="s">
-        <v>485</v>
+        <v>481</v>
       </c>
     </row>
     <row r="91" spans="1:14">
       <c r="A91" s="2" t="s">
+        <v>492</v>
+      </c>
+      <c r="B91" s="3" t="s">
+        <v>493</v>
+      </c>
+      <c r="C91" s="1" t="s">
+        <v>494</v>
+      </c>
+      <c r="D91" s="1" t="s">
+        <v>495</v>
+      </c>
+      <c r="E91" s="4" t="s">
+        <v>613</v>
+      </c>
+      <c r="F91" s="3" t="s">
+        <v>677</v>
+      </c>
+      <c r="G91" s="2" t="s">
         <v>496</v>
-      </c>
-      <c r="B91" s="3" t="s">
-        <v>497</v>
-      </c>
-      <c r="C91" s="1" t="s">
-        <v>498</v>
-      </c>
-      <c r="D91" s="1" t="s">
-        <v>499</v>
-      </c>
-      <c r="E91" s="4" t="s">
-        <v>621</v>
-      </c>
-      <c r="F91" s="3" t="s">
-        <v>685</v>
-      </c>
-      <c r="G91" s="2" t="s">
-        <v>500</v>
       </c>
       <c r="H91" s="2" t="s">
         <v>36</v>
       </c>
       <c r="I91" s="2" t="s">
-        <v>501</v>
+        <v>497</v>
       </c>
       <c r="J91" s="2" t="s">
         <v>36</v>
       </c>
       <c r="K91" s="2" t="s">
-        <v>500</v>
+        <v>496</v>
       </c>
       <c r="L91" s="2">
         <v>1</v>
@@ -6564,43 +6567,43 @@
       <c r="M91" s="2">
         <v>1</v>
       </c>
-      <c r="N91" s="2" t="s">
-        <v>502</v>
+      <c r="N91" s="3" t="s">
+        <v>718</v>
       </c>
     </row>
     <row r="92" spans="1:14">
       <c r="A92" s="2" t="s">
-        <v>503</v>
+        <v>498</v>
       </c>
       <c r="B92" s="2" t="s">
-        <v>504</v>
+        <v>499</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>505</v>
+        <v>500</v>
       </c>
       <c r="D92" s="1" t="s">
-        <v>506</v>
+        <v>501</v>
       </c>
       <c r="E92" s="4" t="s">
-        <v>622</v>
+        <v>614</v>
       </c>
       <c r="F92" s="3" t="s">
-        <v>507</v>
+        <v>502</v>
       </c>
       <c r="G92" s="2" t="s">
-        <v>500</v>
+        <v>496</v>
       </c>
       <c r="H92" s="2" t="s">
         <v>36</v>
       </c>
       <c r="I92" s="2" t="s">
-        <v>501</v>
+        <v>497</v>
       </c>
       <c r="J92" s="2" t="s">
         <v>36</v>
       </c>
       <c r="K92" s="2" t="s">
-        <v>500</v>
+        <v>496</v>
       </c>
       <c r="L92" s="2">
         <v>1</v>
@@ -6608,43 +6611,43 @@
       <c r="M92" s="2">
         <v>1</v>
       </c>
-      <c r="N92" s="2" t="s">
-        <v>508</v>
+      <c r="N92" s="3" t="s">
+        <v>719</v>
       </c>
     </row>
     <row r="93" spans="1:14">
       <c r="A93" s="2" t="s">
-        <v>509</v>
+        <v>503</v>
       </c>
       <c r="B93" s="2" t="s">
-        <v>510</v>
+        <v>504</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>511</v>
+        <v>505</v>
       </c>
       <c r="D93" s="1" t="s">
-        <v>512</v>
+        <v>506</v>
       </c>
       <c r="E93" s="4" t="s">
-        <v>621</v>
+        <v>613</v>
       </c>
       <c r="F93" s="3" t="s">
-        <v>686</v>
+        <v>678</v>
       </c>
       <c r="G93" s="2" t="s">
-        <v>500</v>
+        <v>496</v>
       </c>
       <c r="H93" s="2" t="s">
         <v>36</v>
       </c>
       <c r="I93" s="2" t="s">
-        <v>513</v>
+        <v>507</v>
       </c>
       <c r="J93" s="2" t="s">
         <v>36</v>
       </c>
       <c r="K93" s="2" t="s">
-        <v>500</v>
+        <v>496</v>
       </c>
       <c r="L93" s="2">
         <v>1</v>
@@ -6653,42 +6656,42 @@
         <v>1</v>
       </c>
       <c r="N93" s="2" t="s">
-        <v>514</v>
+        <v>508</v>
       </c>
     </row>
     <row r="94" spans="1:14">
       <c r="A94" s="3" t="s">
-        <v>628</v>
+        <v>620</v>
       </c>
       <c r="B94" s="3" t="s">
-        <v>531</v>
+        <v>525</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>630</v>
+        <v>622</v>
       </c>
       <c r="D94" s="1" t="s">
-        <v>631</v>
+        <v>623</v>
       </c>
       <c r="E94" s="4" t="s">
-        <v>625</v>
+        <v>617</v>
       </c>
       <c r="F94" s="3" t="s">
-        <v>697</v>
+        <v>689</v>
       </c>
       <c r="G94" s="2" t="s">
-        <v>517</v>
+        <v>511</v>
       </c>
       <c r="H94" s="2" t="s">
-        <v>416</v>
+        <v>412</v>
       </c>
       <c r="I94" s="2" t="s">
-        <v>518</v>
+        <v>512</v>
       </c>
       <c r="J94" s="2" t="s">
         <v>188</v>
       </c>
       <c r="K94" s="2" t="s">
-        <v>517</v>
+        <v>511</v>
       </c>
       <c r="L94" s="2">
         <v>1</v>
@@ -6697,42 +6700,42 @@
         <v>1</v>
       </c>
       <c r="N94" s="2" t="s">
-        <v>519</v>
+        <v>513</v>
       </c>
     </row>
     <row r="95" spans="1:14">
       <c r="A95" s="2" t="s">
-        <v>520</v>
+        <v>514</v>
       </c>
       <c r="B95" s="2" t="s">
-        <v>521</v>
+        <v>515</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>522</v>
+        <v>516</v>
       </c>
       <c r="D95" s="1" t="s">
-        <v>523</v>
+        <v>517</v>
       </c>
       <c r="E95" s="4" t="s">
-        <v>624</v>
+        <v>616</v>
       </c>
       <c r="F95" s="3" t="s">
-        <v>698</v>
+        <v>690</v>
       </c>
       <c r="G95" s="2" t="s">
-        <v>517</v>
+        <v>511</v>
       </c>
       <c r="H95" s="2" t="s">
-        <v>416</v>
+        <v>412</v>
       </c>
       <c r="I95" s="2" t="s">
-        <v>524</v>
+        <v>518</v>
       </c>
       <c r="J95" s="2" t="s">
         <v>188</v>
       </c>
       <c r="K95" s="2" t="s">
-        <v>517</v>
+        <v>511</v>
       </c>
       <c r="L95" s="2">
         <v>1</v>
@@ -6741,42 +6744,42 @@
         <v>1</v>
       </c>
       <c r="N95" s="2" t="s">
-        <v>525</v>
+        <v>519</v>
       </c>
     </row>
     <row r="96" spans="1:14">
       <c r="A96" s="2" t="s">
-        <v>526</v>
+        <v>520</v>
       </c>
       <c r="B96" s="2" t="s">
-        <v>527</v>
+        <v>521</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>528</v>
+        <v>522</v>
       </c>
       <c r="D96" s="1" t="s">
-        <v>529</v>
+        <v>523</v>
       </c>
       <c r="E96" s="1" t="s">
-        <v>623</v>
+        <v>615</v>
       </c>
       <c r="F96" s="3" t="s">
-        <v>699</v>
+        <v>691</v>
       </c>
       <c r="G96" s="2" t="s">
-        <v>517</v>
+        <v>511</v>
       </c>
       <c r="H96" s="2" t="s">
-        <v>416</v>
+        <v>412</v>
       </c>
       <c r="I96" s="2" t="s">
-        <v>524</v>
+        <v>518</v>
       </c>
       <c r="J96" s="2" t="s">
         <v>188</v>
       </c>
       <c r="K96" s="2" t="s">
-        <v>517</v>
+        <v>511</v>
       </c>
       <c r="L96" s="2">
         <v>1</v>
@@ -6785,42 +6788,42 @@
         <v>1</v>
       </c>
       <c r="N96" s="2" t="s">
-        <v>530</v>
+        <v>524</v>
       </c>
     </row>
     <row r="97" spans="1:14">
       <c r="A97" s="3" t="s">
-        <v>629</v>
+        <v>621</v>
       </c>
       <c r="B97" s="3" t="s">
-        <v>515</v>
+        <v>509</v>
       </c>
       <c r="C97" s="1" t="s">
-        <v>632</v>
+        <v>624</v>
       </c>
       <c r="D97" s="1" t="s">
-        <v>633</v>
+        <v>625</v>
       </c>
       <c r="E97" s="4" t="s">
-        <v>623</v>
+        <v>615</v>
       </c>
       <c r="F97" s="3" t="s">
-        <v>516</v>
+        <v>510</v>
       </c>
       <c r="G97" s="2" t="s">
-        <v>517</v>
+        <v>511</v>
       </c>
       <c r="H97" s="2" t="s">
-        <v>416</v>
+        <v>412</v>
       </c>
       <c r="I97" s="2" t="s">
-        <v>532</v>
+        <v>526</v>
       </c>
       <c r="J97" s="2" t="s">
         <v>188</v>
       </c>
       <c r="K97" s="2" t="s">
-        <v>517</v>
+        <v>511</v>
       </c>
       <c r="L97" s="2">
         <v>1</v>
@@ -6829,42 +6832,42 @@
         <v>1</v>
       </c>
       <c r="N97" s="3" t="s">
-        <v>718</v>
+        <v>710</v>
       </c>
     </row>
     <row r="98" spans="1:14">
       <c r="A98" s="2" t="s">
-        <v>533</v>
+        <v>527</v>
       </c>
       <c r="B98" s="2" t="s">
-        <v>534</v>
+        <v>528</v>
       </c>
       <c r="C98" s="1" t="s">
-        <v>535</v>
+        <v>529</v>
       </c>
       <c r="D98" s="1" t="s">
-        <v>536</v>
+        <v>530</v>
       </c>
       <c r="E98" s="4" t="s">
-        <v>708</v>
+        <v>700</v>
       </c>
       <c r="F98" s="3" t="s">
-        <v>700</v>
+        <v>692</v>
       </c>
       <c r="G98" s="2" t="s">
-        <v>537</v>
+        <v>531</v>
       </c>
       <c r="H98" s="2" t="s">
-        <v>416</v>
+        <v>412</v>
       </c>
       <c r="I98" s="2" t="s">
-        <v>537</v>
+        <v>531</v>
       </c>
       <c r="J98" s="2" t="s">
         <v>188</v>
       </c>
       <c r="K98" s="2" t="s">
-        <v>537</v>
+        <v>531</v>
       </c>
       <c r="L98" s="2">
         <v>1</v>
@@ -6873,71 +6876,71 @@
         <v>1</v>
       </c>
       <c r="N98" s="2" t="s">
-        <v>538</v>
+        <v>532</v>
       </c>
     </row>
     <row r="99" spans="1:14">
       <c r="A99" s="2" t="s">
-        <v>539</v>
+        <v>533</v>
       </c>
       <c r="B99" s="2" t="s">
-        <v>540</v>
+        <v>534</v>
       </c>
       <c r="C99" s="1" t="s">
-        <v>541</v>
+        <v>535</v>
       </c>
       <c r="D99" s="1" t="s">
-        <v>542</v>
+        <v>536</v>
       </c>
       <c r="E99" s="4" t="s">
-        <v>709</v>
+        <v>701</v>
       </c>
       <c r="F99" s="3" t="s">
-        <v>701</v>
+        <v>693</v>
       </c>
       <c r="G99" s="2" t="s">
-        <v>537</v>
+        <v>531</v>
       </c>
       <c r="H99" s="2" t="s">
-        <v>416</v>
+        <v>412</v>
       </c>
       <c r="I99" s="2" t="s">
-        <v>537</v>
+        <v>531</v>
       </c>
       <c r="J99" s="2" t="s">
         <v>188</v>
       </c>
       <c r="K99" s="2" t="s">
+        <v>531</v>
+      </c>
+      <c r="L99" s="2">
+        <v>1</v>
+      </c>
+      <c r="M99" s="2">
+        <v>1</v>
+      </c>
+      <c r="N99" s="2" t="s">
         <v>537</v>
-      </c>
-      <c r="L99" s="2">
-        <v>1</v>
-      </c>
-      <c r="M99" s="2">
-        <v>1</v>
-      </c>
-      <c r="N99" s="2" t="s">
-        <v>543</v>
       </c>
     </row>
     <row r="100" spans="1:14">
       <c r="A100" s="2" t="s">
-        <v>544</v>
+        <v>538</v>
       </c>
       <c r="B100" s="2" t="s">
-        <v>545</v>
+        <v>539</v>
       </c>
       <c r="C100" s="1" t="s">
-        <v>546</v>
+        <v>540</v>
       </c>
       <c r="D100" s="1" t="s">
-        <v>547</v>
+        <v>541</v>
       </c>
       <c r="E100" s="4" t="s">
-        <v>716</v>
+        <v>708</v>
       </c>
       <c r="F100" s="2" t="s">
-        <v>548</v>
+        <v>542</v>
       </c>
       <c r="G100" s="2" t="s">
         <v>186</v>
@@ -6961,27 +6964,27 @@
         <v>1</v>
       </c>
       <c r="N100" s="2" t="s">
-        <v>549</v>
+        <v>543</v>
       </c>
     </row>
     <row r="101" spans="1:14">
       <c r="A101" s="2" t="s">
-        <v>550</v>
+        <v>544</v>
       </c>
       <c r="B101" s="2" t="s">
-        <v>551</v>
+        <v>545</v>
       </c>
       <c r="C101" s="1" t="s">
-        <v>552</v>
+        <v>546</v>
       </c>
       <c r="D101" s="1" t="s">
-        <v>553</v>
+        <v>547</v>
       </c>
       <c r="E101" s="4" t="s">
-        <v>626</v>
+        <v>618</v>
       </c>
       <c r="F101" s="3" t="s">
-        <v>705</v>
+        <v>697</v>
       </c>
       <c r="G101" s="2" t="s">
         <v>186</v>
@@ -7005,7 +7008,7 @@
         <v>1</v>
       </c>
       <c r="N101" s="2" t="s">
-        <v>554</v>
+        <v>548</v>
       </c>
     </row>
     <row r="104" spans="1:14">

</xml_diff>

<commit_message>
Simplify config-loading; reminder texts specified in config file
</commit_message>
<xml_diff>
--- a/config/phone_list.xlsx
+++ b/config/phone_list.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11385"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11385" tabRatio="665"/>
   </bookViews>
   <sheets>
     <sheet name="PHONE_LIST" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">PHONE_LIST!$A$1:$O$101</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="152511" calcMode="manual" calcCompleted="0" calcOnSave="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -1607,9 +1607,6 @@
     <t>0972576574</t>
   </si>
   <si>
-    <t>S. Harvey / Hughes</t>
-  </si>
-  <si>
     <t>ZHUBEI</t>
   </si>
   <si>
@@ -2012,12 +2009,6 @@
     <t>E. Falck DL / Jensen</t>
   </si>
   <si>
-    <t>S. Fang / Huang</t>
-  </si>
-  <si>
-    <t>E. Byers / Puzey / Zhou</t>
-  </si>
-  <si>
     <t>S. LeFevre / Fenlaw STL</t>
   </si>
   <si>
@@ -2042,18 +2033,12 @@
     <t>E. Chia DL / Simonson</t>
   </si>
   <si>
-    <t>E. Griffin / Clegg</t>
-  </si>
-  <si>
     <t>S. Huntington / Erickson</t>
   </si>
   <si>
     <t>E. Dung DL / Sessions</t>
   </si>
   <si>
-    <t>S. Everett / Huang</t>
-  </si>
-  <si>
     <t>E. Sumsion / Mertz</t>
   </si>
   <si>
@@ -2259,6 +2244,21 @@
   </si>
   <si>
     <t>0965073051</t>
+  </si>
+  <si>
+    <t>E. Byers / Puzey</t>
+  </si>
+  <si>
+    <t>E. Griffin DL / Clegg</t>
+  </si>
+  <si>
+    <t>S. Harvey</t>
+  </si>
+  <si>
+    <t>S. Everett / Hughes</t>
+  </si>
+  <si>
+    <t>S. Huang / Hsiao</t>
   </si>
 </sst>
 </file>
@@ -2318,17 +2318,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1"/>
   </cellStyles>
-  <dxfs count="3">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="2">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -49764,10 +49754,10 @@
   <dimension ref="A1:O104"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B70" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B64" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="N88" sqref="N88"/>
+      <selection pane="bottomRight" activeCell="E73" sqref="E73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -49794,7 +49784,7 @@
         <v>3</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>4</v>
@@ -49821,7 +49811,7 @@
         <v>11</v>
       </c>
       <c r="N1" s="6" t="s">
-        <v>725</v>
+        <v>720</v>
       </c>
       <c r="O1" s="2" t="s">
         <v>12</v>
@@ -49829,7 +49819,7 @@
     </row>
     <row r="2" spans="1:15">
       <c r="A2" s="3" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>14</v>
@@ -49838,7 +49828,7 @@
         <v>435</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="E2" s="4"/>
       <c r="F2" s="2"/>
@@ -49856,7 +49846,7 @@
         <v>0</v>
       </c>
       <c r="N2" s="7" t="e">
-        <f>RIGHT(VLOOKUP(C2,[1]Sheet1!$V:$BT,51,FALSE),6)</f>
+        <f ca="1">RIGHT(VLOOKUP(C2,[1]Sheet1!$V:$BT,51,FALSE),6)</f>
         <v>#N/A</v>
       </c>
       <c r="O2" s="2" t="s">
@@ -49877,10 +49867,10 @@
         <v>19</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>654</v>
+        <v>723</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>20</v>
@@ -49904,7 +49894,7 @@
         <v>1</v>
       </c>
       <c r="N3" s="7" t="str">
-        <f>RIGHT(VLOOKUP(C3,[1]Sheet1!$V:$BT,51,FALSE),6)</f>
+        <f ca="1">RIGHT(VLOOKUP(C3,[1]Sheet1!$V:$BT,51,FALSE),6)</f>
         <v>545360</v>
       </c>
       <c r="O3" s="2" t="s">
@@ -49925,10 +49915,10 @@
         <v>27</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="G4" s="3" t="s">
         <v>28</v>
@@ -49950,11 +49940,11 @@
         <v>0</v>
       </c>
       <c r="N4" s="7" t="str">
-        <f>RIGHT(VLOOKUP(C4,[1]Sheet1!$V:$BT,51,FALSE),6)</f>
+        <f ca="1">RIGHT(VLOOKUP(C4,[1]Sheet1!$V:$BT,51,FALSE),6)</f>
         <v>455858</v>
       </c>
       <c r="O4" s="3" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
     </row>
     <row r="5" spans="1:15">
@@ -49971,10 +49961,10 @@
         <v>27</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>28</v>
@@ -49996,11 +49986,11 @@
         <v>0</v>
       </c>
       <c r="N5" s="7" t="str">
-        <f>RIGHT(VLOOKUP(C5,[1]Sheet1!$V:$BT,51,FALSE),6)</f>
+        <f ca="1">RIGHT(VLOOKUP(C5,[1]Sheet1!$V:$BT,51,FALSE),6)</f>
         <v>455858</v>
       </c>
       <c r="O5" s="3" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
     </row>
     <row r="6" spans="1:15">
@@ -50017,10 +50007,10 @@
         <v>34</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>668</v>
+        <v>663</v>
       </c>
       <c r="G6" s="2" t="s">
         <v>35</v>
@@ -50044,7 +50034,7 @@
         <v>1</v>
       </c>
       <c r="N6" s="7" t="str">
-        <f>RIGHT(VLOOKUP(C6,[1]Sheet1!$V:$BT,51,FALSE),6)</f>
+        <f ca="1">RIGHT(VLOOKUP(C6,[1]Sheet1!$V:$BT,51,FALSE),6)</f>
         <v>501091</v>
       </c>
       <c r="O6" s="2" t="s">
@@ -50065,7 +50055,7 @@
         <v>41</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="F7" s="3" t="s">
         <v>42</v>
@@ -50092,7 +50082,7 @@
         <v>1</v>
       </c>
       <c r="N7" s="7" t="str">
-        <f>RIGHT(VLOOKUP(C7,[1]Sheet1!$V:$BT,51,FALSE),6)</f>
+        <f ca="1">RIGHT(VLOOKUP(C7,[1]Sheet1!$V:$BT,51,FALSE),6)</f>
         <v>430545</v>
       </c>
       <c r="O7" s="2" t="s">
@@ -50113,10 +50103,10 @@
         <v>47</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>669</v>
+        <v>664</v>
       </c>
       <c r="G8" s="2" t="s">
         <v>35</v>
@@ -50140,7 +50130,7 @@
         <v>1</v>
       </c>
       <c r="N8" s="7" t="str">
-        <f>RIGHT(VLOOKUP(C8,[1]Sheet1!$V:$BT,51,FALSE),6)</f>
+        <f ca="1">RIGHT(VLOOKUP(C8,[1]Sheet1!$V:$BT,51,FALSE),6)</f>
         <v>497471</v>
       </c>
       <c r="O8" s="2" t="s">
@@ -50161,10 +50151,10 @@
         <v>56</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>649</v>
+        <v>646</v>
       </c>
       <c r="G9" s="2" t="s">
         <v>57</v>
@@ -50188,7 +50178,7 @@
         <v>1</v>
       </c>
       <c r="N9" s="7" t="str">
-        <f>RIGHT(VLOOKUP(C9,[1]Sheet1!$V:$BT,51,FALSE),6)</f>
+        <f ca="1">RIGHT(VLOOKUP(C9,[1]Sheet1!$V:$BT,51,FALSE),6)</f>
         <v>431834</v>
       </c>
       <c r="O9" s="2" t="s">
@@ -50209,7 +50199,7 @@
         <v>63</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="F10" s="3" t="s">
         <v>64</v>
@@ -50236,7 +50226,7 @@
         <v>1</v>
       </c>
       <c r="N10" s="7" t="str">
-        <f>RIGHT(VLOOKUP(C10,[1]Sheet1!$V:$BT,51,FALSE),6)</f>
+        <f ca="1">RIGHT(VLOOKUP(C10,[1]Sheet1!$V:$BT,51,FALSE),6)</f>
         <v>480454</v>
       </c>
       <c r="O10" s="2" t="s">
@@ -50257,10 +50247,10 @@
         <v>68</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>678</v>
+        <v>673</v>
       </c>
       <c r="G11" s="2" t="s">
         <v>69</v>
@@ -50284,7 +50274,7 @@
         <v>1</v>
       </c>
       <c r="N11" s="7" t="str">
-        <f>RIGHT(VLOOKUP(C11,[1]Sheet1!$V:$BT,51,FALSE),6)</f>
+        <f ca="1">RIGHT(VLOOKUP(C11,[1]Sheet1!$V:$BT,51,FALSE),6)</f>
         <v>500601</v>
       </c>
       <c r="O11" s="2" t="s">
@@ -50305,10 +50295,10 @@
         <v>75</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>650</v>
+        <v>647</v>
       </c>
       <c r="G12" s="2" t="s">
         <v>57</v>
@@ -50332,7 +50322,7 @@
         <v>1</v>
       </c>
       <c r="N12" s="7" t="str">
-        <f>RIGHT(VLOOKUP(C12,[1]Sheet1!$V:$BT,51,FALSE),6)</f>
+        <f ca="1">RIGHT(VLOOKUP(C12,[1]Sheet1!$V:$BT,51,FALSE),6)</f>
         <v>505612</v>
       </c>
       <c r="O12" s="2" t="s">
@@ -50353,7 +50343,7 @@
         <v>81</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="F13" s="2" t="s">
         <v>82</v>
@@ -50380,7 +50370,7 @@
         <v>1</v>
       </c>
       <c r="N13" s="7" t="str">
-        <f>RIGHT(VLOOKUP(C13,[1]Sheet1!$V:$BT,51,FALSE),6)</f>
+        <f ca="1">RIGHT(VLOOKUP(C13,[1]Sheet1!$V:$BT,51,FALSE),6)</f>
         <v>444608</v>
       </c>
       <c r="O13" s="2" t="s">
@@ -50428,7 +50418,7 @@
         <v>1</v>
       </c>
       <c r="N14" s="7" t="str">
-        <f>RIGHT(VLOOKUP(C14,[1]Sheet1!$V:$BT,51,FALSE),6)</f>
+        <f ca="1">RIGHT(VLOOKUP(C14,[1]Sheet1!$V:$BT,51,FALSE),6)</f>
         <v>451630</v>
       </c>
       <c r="O14" s="2" t="s">
@@ -50449,7 +50439,7 @@
         <v>95</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="F15" s="3" t="s">
         <v>96</v>
@@ -50476,7 +50466,7 @@
         <v>1</v>
       </c>
       <c r="N15" s="7" t="str">
-        <f>RIGHT(VLOOKUP(C15,[1]Sheet1!$V:$BT,51,FALSE),6)</f>
+        <f ca="1">RIGHT(VLOOKUP(C15,[1]Sheet1!$V:$BT,51,FALSE),6)</f>
         <v>480807</v>
       </c>
       <c r="O15" s="2" t="s">
@@ -50497,10 +50487,10 @@
         <v>105</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>701</v>
+        <v>696</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>646</v>
+        <v>643</v>
       </c>
       <c r="G16" s="2" t="s">
         <v>97</v>
@@ -50524,7 +50514,7 @@
         <v>1</v>
       </c>
       <c r="N16" s="7" t="str">
-        <f>RIGHT(VLOOKUP(C16,[1]Sheet1!$V:$BT,51,FALSE),6)</f>
+        <f ca="1">RIGHT(VLOOKUP(C16,[1]Sheet1!$V:$BT,51,FALSE),6)</f>
         <v>486563</v>
       </c>
       <c r="O16" s="2" t="s">
@@ -50545,7 +50535,7 @@
         <v>109</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="F17" s="2" t="s">
         <v>110</v>
@@ -50572,7 +50562,7 @@
         <v>1</v>
       </c>
       <c r="N17" s="7" t="str">
-        <f>RIGHT(VLOOKUP(C17,[1]Sheet1!$V:$BT,51,FALSE),6)</f>
+        <f ca="1">RIGHT(VLOOKUP(C17,[1]Sheet1!$V:$BT,51,FALSE),6)</f>
         <v>535098</v>
       </c>
       <c r="O17" s="2" t="s">
@@ -50593,7 +50583,7 @@
         <v>116</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="F18" s="2" t="s">
         <v>117</v>
@@ -50620,7 +50610,7 @@
         <v>0</v>
       </c>
       <c r="N18" s="7" t="str">
-        <f>RIGHT(VLOOKUP(C18,[1]Sheet1!$V:$BT,51,FALSE),6)</f>
+        <f ca="1">RIGHT(VLOOKUP(C18,[1]Sheet1!$V:$BT,51,FALSE),6)</f>
         <v>434073</v>
       </c>
       <c r="O18" s="2" t="s">
@@ -50641,10 +50631,10 @@
         <v>122</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>647</v>
+        <v>644</v>
       </c>
       <c r="G19" s="2" t="s">
         <v>98</v>
@@ -50668,7 +50658,7 @@
         <v>0</v>
       </c>
       <c r="N19" s="7" t="str">
-        <f>RIGHT(VLOOKUP(C19,[1]Sheet1!$V:$BT,51,FALSE),6)</f>
+        <f ca="1">RIGHT(VLOOKUP(C19,[1]Sheet1!$V:$BT,51,FALSE),6)</f>
         <v>506345</v>
       </c>
       <c r="O19" s="2" t="s">
@@ -50689,10 +50679,10 @@
         <v>127</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>701</v>
+        <v>696</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>648</v>
+        <v>645</v>
       </c>
       <c r="G20" s="2" t="s">
         <v>98</v>
@@ -50716,7 +50706,7 @@
         <v>1</v>
       </c>
       <c r="N20" s="7" t="str">
-        <f>RIGHT(VLOOKUP(C20,[1]Sheet1!$V:$BT,51,FALSE),6)</f>
+        <f ca="1">RIGHT(VLOOKUP(C20,[1]Sheet1!$V:$BT,51,FALSE),6)</f>
         <v>458154</v>
       </c>
       <c r="O20" s="2" t="s">
@@ -50725,22 +50715,22 @@
     </row>
     <row r="21" spans="1:15">
       <c r="A21" s="1" t="s">
-        <v>723</v>
+        <v>718</v>
       </c>
       <c r="B21" s="5" t="s">
+        <v>714</v>
+      </c>
+      <c r="C21" s="1" t="s">
         <v>719</v>
       </c>
-      <c r="C21" s="1" t="s">
-        <v>724</v>
-      </c>
       <c r="D21" s="1" t="s">
-        <v>720</v>
+        <v>715</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>721</v>
+        <v>716</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>722</v>
+        <v>717</v>
       </c>
       <c r="G21" s="2" t="s">
         <v>97</v>
@@ -50764,7 +50754,7 @@
         <v>1</v>
       </c>
       <c r="N21" s="7" t="e">
-        <f>RIGHT(VLOOKUP(C21,[1]Sheet1!$V:$BT,51,FALSE),6)</f>
+        <f ca="1">RIGHT(VLOOKUP(C21,[1]Sheet1!$V:$BT,51,FALSE),6)</f>
         <v>#N/A</v>
       </c>
     </row>
@@ -50785,7 +50775,7 @@
         <v>132</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="G22" s="2" t="s">
         <v>132</v>
@@ -50809,7 +50799,7 @@
         <v>1</v>
       </c>
       <c r="N22" s="7" t="str">
-        <f>RIGHT(VLOOKUP(C22,[1]Sheet1!$V:$BT,51,FALSE),6)</f>
+        <f ca="1">RIGHT(VLOOKUP(C22,[1]Sheet1!$V:$BT,51,FALSE),6)</f>
         <v>421056</v>
       </c>
       <c r="O22" s="2" t="s">
@@ -50833,7 +50823,7 @@
         <v>132</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="G23" s="2" t="s">
         <v>132</v>
@@ -50857,7 +50847,7 @@
         <v>1</v>
       </c>
       <c r="N23" s="7" t="str">
-        <f>RIGHT(VLOOKUP(C23,[1]Sheet1!$V:$BT,51,FALSE),6)</f>
+        <f ca="1">RIGHT(VLOOKUP(C23,[1]Sheet1!$V:$BT,51,FALSE),6)</f>
         <v>447116</v>
       </c>
       <c r="O23" s="2" t="s">
@@ -50878,10 +50868,10 @@
         <v>150</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="F24" s="3" t="s">
-        <v>655</v>
+        <v>651</v>
       </c>
       <c r="G24" s="2" t="s">
         <v>145</v>
@@ -50905,7 +50895,7 @@
         <v>1</v>
       </c>
       <c r="N24" s="7" t="str">
-        <f>RIGHT(VLOOKUP(C24,[1]Sheet1!$V:$BT,51,FALSE),6)</f>
+        <f ca="1">RIGHT(VLOOKUP(C24,[1]Sheet1!$V:$BT,51,FALSE),6)</f>
         <v>527470</v>
       </c>
       <c r="O24" s="2" t="s">
@@ -50926,7 +50916,7 @@
         <v>143</v>
       </c>
       <c r="E25" s="4" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="F25" s="2" t="s">
         <v>144</v>
@@ -50953,7 +50943,7 @@
         <v>1</v>
       </c>
       <c r="N25" s="7" t="str">
-        <f>RIGHT(VLOOKUP(C25,[1]Sheet1!$V:$BT,51,FALSE),6)</f>
+        <f ca="1">RIGHT(VLOOKUP(C25,[1]Sheet1!$V:$BT,51,FALSE),6)</f>
         <v>440276</v>
       </c>
       <c r="O25" s="2" t="s">
@@ -50974,7 +50964,7 @@
         <v>154</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="F26" s="2" t="s">
         <v>155</v>
@@ -51001,11 +50991,11 @@
         <v>0</v>
       </c>
       <c r="N26" s="7" t="str">
-        <f>RIGHT(VLOOKUP(C26,[1]Sheet1!$V:$BT,51,FALSE),6)</f>
+        <f ca="1">RIGHT(VLOOKUP(C26,[1]Sheet1!$V:$BT,51,FALSE),6)</f>
         <v>543498</v>
       </c>
       <c r="O26" s="3" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
     </row>
     <row r="27" spans="1:15">
@@ -51022,10 +51012,10 @@
         <v>217</v>
       </c>
       <c r="E27" s="4" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="F27" s="3" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="G27" s="2" t="s">
         <v>156</v>
@@ -51049,7 +51039,7 @@
         <v>1</v>
       </c>
       <c r="N27" s="7" t="str">
-        <f>RIGHT(VLOOKUP(C27,[1]Sheet1!$V:$BT,51,FALSE),6)</f>
+        <f ca="1">RIGHT(VLOOKUP(C27,[1]Sheet1!$V:$BT,51,FALSE),6)</f>
         <v>471198</v>
       </c>
       <c r="O27" s="3" t="s">
@@ -51073,7 +51063,7 @@
         <v>162</v>
       </c>
       <c r="F28" s="3" t="s">
-        <v>670</v>
+        <v>665</v>
       </c>
       <c r="G28" s="2" t="s">
         <v>35</v>
@@ -51097,7 +51087,7 @@
         <v>1</v>
       </c>
       <c r="N28" s="7" t="str">
-        <f>RIGHT(VLOOKUP(C28,[1]Sheet1!$V:$BT,51,FALSE),6)</f>
+        <f ca="1">RIGHT(VLOOKUP(C28,[1]Sheet1!$V:$BT,51,FALSE),6)</f>
         <v>526167</v>
       </c>
       <c r="O28" s="2" t="s">
@@ -51118,10 +51108,10 @@
         <v>167</v>
       </c>
       <c r="E29" s="4" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="F29" s="3" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="G29" s="2" t="s">
         <v>168</v>
@@ -51145,7 +51135,7 @@
         <v>1</v>
       </c>
       <c r="N29" s="7" t="str">
-        <f>RIGHT(VLOOKUP(C29,[1]Sheet1!$V:$BT,51,FALSE),6)</f>
+        <f ca="1">RIGHT(VLOOKUP(C29,[1]Sheet1!$V:$BT,51,FALSE),6)</f>
         <v>541123</v>
       </c>
       <c r="O29" s="2" t="s">
@@ -51166,10 +51156,10 @@
         <v>173</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="F30" s="3" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="G30" s="2" t="s">
         <v>168</v>
@@ -51193,7 +51183,7 @@
         <v>1</v>
       </c>
       <c r="N30" s="7" t="str">
-        <f>RIGHT(VLOOKUP(C30,[1]Sheet1!$V:$BT,51,FALSE),6)</f>
+        <f ca="1">RIGHT(VLOOKUP(C30,[1]Sheet1!$V:$BT,51,FALSE),6)</f>
         <v>460396</v>
       </c>
       <c r="O30" s="2" t="s">
@@ -51214,10 +51204,10 @@
         <v>177</v>
       </c>
       <c r="E31" s="4" t="s">
-        <v>697</v>
+        <v>692</v>
       </c>
       <c r="F31" s="3" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="G31" s="2" t="s">
         <v>178</v>
@@ -51241,7 +51231,7 @@
         <v>1</v>
       </c>
       <c r="N31" s="7" t="str">
-        <f>RIGHT(VLOOKUP(C31,[1]Sheet1!$V:$BT,51,FALSE),6)</f>
+        <f ca="1">RIGHT(VLOOKUP(C31,[1]Sheet1!$V:$BT,51,FALSE),6)</f>
         <v>468445</v>
       </c>
       <c r="O31" s="2" t="s">
@@ -51262,10 +51252,10 @@
         <v>184</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>697</v>
+        <v>692</v>
       </c>
       <c r="F32" s="3" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="G32" s="2" t="s">
         <v>178</v>
@@ -51289,7 +51279,7 @@
         <v>1</v>
       </c>
       <c r="N32" s="7" t="str">
-        <f>RIGHT(VLOOKUP(C32,[1]Sheet1!$V:$BT,51,FALSE),6)</f>
+        <f ca="1">RIGHT(VLOOKUP(C32,[1]Sheet1!$V:$BT,51,FALSE),6)</f>
         <v>429128</v>
       </c>
       <c r="O32" s="2" t="s">
@@ -51313,7 +51303,7 @@
         <v>187</v>
       </c>
       <c r="F33" s="3" t="s">
-        <v>693</v>
+        <v>688</v>
       </c>
       <c r="G33" s="2" t="s">
         <v>185</v>
@@ -51337,7 +51327,7 @@
         <v>1</v>
       </c>
       <c r="N33" s="7" t="str">
-        <f>RIGHT(VLOOKUP(C33,[1]Sheet1!$V:$BT,51,FALSE),6)</f>
+        <f ca="1">RIGHT(VLOOKUP(C33,[1]Sheet1!$V:$BT,51,FALSE),6)</f>
         <v>531318</v>
       </c>
       <c r="O33" s="2" t="s">
@@ -51358,10 +51348,10 @@
         <v>197</v>
       </c>
       <c r="E34" s="4" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="F34" s="3" t="s">
-        <v>656</v>
+        <v>652</v>
       </c>
       <c r="G34" s="2" t="s">
         <v>145</v>
@@ -51385,11 +51375,11 @@
         <v>1</v>
       </c>
       <c r="N34" s="7" t="str">
-        <f>RIGHT(VLOOKUP(C34,[1]Sheet1!$V:$BT,51,FALSE),6)</f>
+        <f ca="1">RIGHT(VLOOKUP(C34,[1]Sheet1!$V:$BT,51,FALSE),6)</f>
         <v>536947</v>
       </c>
       <c r="O34" s="3" t="s">
-        <v>708</v>
+        <v>703</v>
       </c>
     </row>
     <row r="35" spans="1:15">
@@ -51406,10 +51396,10 @@
         <v>202</v>
       </c>
       <c r="E35" s="4" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="F35" s="3" t="s">
-        <v>657</v>
+        <v>725</v>
       </c>
       <c r="G35" s="2" t="s">
         <v>145</v>
@@ -51433,11 +51423,11 @@
         <v>1</v>
       </c>
       <c r="N35" s="7" t="str">
-        <f>RIGHT(VLOOKUP(C35,[1]Sheet1!$V:$BT,51,FALSE),6)</f>
+        <f ca="1">RIGHT(VLOOKUP(C35,[1]Sheet1!$V:$BT,51,FALSE),6)</f>
         <v>485908</v>
       </c>
       <c r="O35" s="3" t="s">
-        <v>708</v>
+        <v>703</v>
       </c>
     </row>
     <row r="36" spans="1:15">
@@ -51454,10 +51444,10 @@
         <v>206</v>
       </c>
       <c r="E36" s="4" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="F36" s="3" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="G36" s="2" t="s">
         <v>207</v>
@@ -51481,7 +51471,7 @@
         <v>1</v>
       </c>
       <c r="N36" s="7" t="str">
-        <f>RIGHT(VLOOKUP(C36,[1]Sheet1!$V:$BT,51,FALSE),6)</f>
+        <f ca="1">RIGHT(VLOOKUP(C36,[1]Sheet1!$V:$BT,51,FALSE),6)</f>
         <v>502447</v>
       </c>
       <c r="O36" s="2" t="s">
@@ -51502,10 +51492,10 @@
         <v>213</v>
       </c>
       <c r="E37" s="4" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="F37" s="3" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
       <c r="G37" s="2" t="s">
         <v>207</v>
@@ -51529,7 +51519,7 @@
         <v>1</v>
       </c>
       <c r="N37" s="7" t="str">
-        <f>RIGHT(VLOOKUP(C37,[1]Sheet1!$V:$BT,51,FALSE),6)</f>
+        <f ca="1">RIGHT(VLOOKUP(C37,[1]Sheet1!$V:$BT,51,FALSE),6)</f>
         <v>437988</v>
       </c>
       <c r="O37" s="2" t="s">
@@ -51550,10 +51540,10 @@
         <v>222</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="F38" s="3" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="G38" s="2" t="s">
         <v>156</v>
@@ -51575,11 +51565,11 @@
         <v>0</v>
       </c>
       <c r="N38" s="7" t="str">
-        <f>RIGHT(VLOOKUP(C38,[1]Sheet1!$V:$BT,51,FALSE),6)</f>
+        <f ca="1">RIGHT(VLOOKUP(C38,[1]Sheet1!$V:$BT,51,FALSE),6)</f>
         <v>446606</v>
       </c>
       <c r="O38" s="3" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
     </row>
     <row r="39" spans="1:15">
@@ -51596,10 +51586,10 @@
         <v>222</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="F39" s="3" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="G39" s="2" t="s">
         <v>156</v>
@@ -51621,11 +51611,11 @@
         <v>0</v>
       </c>
       <c r="N39" s="7" t="str">
-        <f>RIGHT(VLOOKUP(C39,[1]Sheet1!$V:$BT,51,FALSE),6)</f>
+        <f ca="1">RIGHT(VLOOKUP(C39,[1]Sheet1!$V:$BT,51,FALSE),6)</f>
         <v>446606</v>
       </c>
       <c r="O39" s="3" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
     </row>
     <row r="40" spans="1:15">
@@ -51642,10 +51632,10 @@
         <v>227</v>
       </c>
       <c r="E40" s="4" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="F40" s="3" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="G40" s="2" t="s">
         <v>178</v>
@@ -51669,7 +51659,7 @@
         <v>1</v>
       </c>
       <c r="N40" s="7" t="str">
-        <f>RIGHT(VLOOKUP(C40,[1]Sheet1!$V:$BT,51,FALSE),6)</f>
+        <f ca="1">RIGHT(VLOOKUP(C40,[1]Sheet1!$V:$BT,51,FALSE),6)</f>
         <v>466715</v>
       </c>
       <c r="O40" s="2" t="s">
@@ -51690,10 +51680,10 @@
         <v>232</v>
       </c>
       <c r="E41" s="4" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="F41" s="3" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="G41" s="2" t="s">
         <v>178</v>
@@ -51717,7 +51707,7 @@
         <v>1</v>
       </c>
       <c r="N41" s="7" t="str">
-        <f>RIGHT(VLOOKUP(C41,[1]Sheet1!$V:$BT,51,FALSE),6)</f>
+        <f ca="1">RIGHT(VLOOKUP(C41,[1]Sheet1!$V:$BT,51,FALSE),6)</f>
         <v>513235</v>
       </c>
       <c r="O41" s="2" t="s">
@@ -51738,7 +51728,7 @@
         <v>236</v>
       </c>
       <c r="E42" s="4" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="F42" s="3" t="s">
         <v>237</v>
@@ -51765,7 +51755,7 @@
         <v>1</v>
       </c>
       <c r="N42" s="7" t="str">
-        <f>RIGHT(VLOOKUP(C42,[1]Sheet1!$V:$BT,51,FALSE),6)</f>
+        <f ca="1">RIGHT(VLOOKUP(C42,[1]Sheet1!$V:$BT,51,FALSE),6)</f>
         <v>509288</v>
       </c>
       <c r="O42" s="2" t="s">
@@ -51786,10 +51776,10 @@
         <v>244</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="F43" s="3" t="s">
-        <v>679</v>
+        <v>674</v>
       </c>
       <c r="G43" s="2" t="s">
         <v>238</v>
@@ -51813,7 +51803,7 @@
         <v>1</v>
       </c>
       <c r="N43" s="7" t="str">
-        <f>RIGHT(VLOOKUP(C43,[1]Sheet1!$V:$BT,51,FALSE),6)</f>
+        <f ca="1">RIGHT(VLOOKUP(C43,[1]Sheet1!$V:$BT,51,FALSE),6)</f>
         <v>447492</v>
       </c>
       <c r="O43" s="2" t="s">
@@ -51822,22 +51812,22 @@
     </row>
     <row r="44" spans="1:15">
       <c r="A44" s="2" t="s">
+        <v>547</v>
+      </c>
+      <c r="B44" s="2" t="s">
         <v>548</v>
       </c>
-      <c r="B44" s="2" t="s">
+      <c r="C44" s="1" t="s">
         <v>549</v>
       </c>
-      <c r="C44" s="1" t="s">
+      <c r="D44" s="1" t="s">
         <v>550</v>
       </c>
-      <c r="D44" s="1" t="s">
+      <c r="E44" s="1" t="s">
+        <v>701</v>
+      </c>
+      <c r="F44" s="2" t="s">
         <v>551</v>
-      </c>
-      <c r="E44" s="1" t="s">
-        <v>706</v>
-      </c>
-      <c r="F44" s="2" t="s">
-        <v>552</v>
       </c>
       <c r="G44" s="2" t="s">
         <v>156</v>
@@ -51861,7 +51851,7 @@
         <v>1</v>
       </c>
       <c r="N44" s="7" t="str">
-        <f>RIGHT(VLOOKUP(C44,[1]Sheet1!$V:$BT,51,FALSE),6)</f>
+        <f ca="1">RIGHT(VLOOKUP(C44,[1]Sheet1!$V:$BT,51,FALSE),6)</f>
         <v>532885</v>
       </c>
       <c r="O44" s="2"/>
@@ -51880,10 +51870,10 @@
         <v>254</v>
       </c>
       <c r="E45" s="4" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="F45" s="3" t="s">
-        <v>651</v>
+        <v>648</v>
       </c>
       <c r="G45" s="2" t="s">
         <v>249</v>
@@ -51907,7 +51897,7 @@
         <v>1</v>
       </c>
       <c r="N45" s="7" t="str">
-        <f>RIGHT(VLOOKUP(C45,[1]Sheet1!$V:$BT,51,FALSE),6)</f>
+        <f ca="1">RIGHT(VLOOKUP(C45,[1]Sheet1!$V:$BT,51,FALSE),6)</f>
         <v>475247</v>
       </c>
       <c r="O45" s="2" t="s">
@@ -51928,10 +51918,10 @@
         <v>248</v>
       </c>
       <c r="E46" s="4" t="s">
-        <v>703</v>
+        <v>698</v>
       </c>
       <c r="F46" s="3" t="s">
-        <v>652</v>
+        <v>649</v>
       </c>
       <c r="G46" s="2" t="s">
         <v>249</v>
@@ -51955,7 +51945,7 @@
         <v>1</v>
       </c>
       <c r="N46" s="7" t="str">
-        <f>RIGHT(VLOOKUP(C46,[1]Sheet1!$V:$BT,51,FALSE),6)</f>
+        <f ca="1">RIGHT(VLOOKUP(C46,[1]Sheet1!$V:$BT,51,FALSE),6)</f>
         <v>480156</v>
       </c>
       <c r="O46" s="2" t="s">
@@ -51976,10 +51966,10 @@
         <v>259</v>
       </c>
       <c r="E47" s="4" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="F47" s="3" t="s">
-        <v>680</v>
+        <v>675</v>
       </c>
       <c r="G47" s="2" t="s">
         <v>69</v>
@@ -52003,7 +51993,7 @@
         <v>1</v>
       </c>
       <c r="N47" s="7" t="str">
-        <f>RIGHT(VLOOKUP(C47,[1]Sheet1!$V:$BT,51,FALSE),6)</f>
+        <f ca="1">RIGHT(VLOOKUP(C47,[1]Sheet1!$V:$BT,51,FALSE),6)</f>
         <v>428329</v>
       </c>
       <c r="O47" s="2" t="s">
@@ -52024,10 +52014,10 @@
         <v>270</v>
       </c>
       <c r="E48" s="4" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="F48" s="3" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="G48" s="2" t="s">
         <v>207</v>
@@ -52051,11 +52041,11 @@
         <v>1</v>
       </c>
       <c r="N48" s="7" t="str">
-        <f>RIGHT(VLOOKUP(C48,[1]Sheet1!$V:$BT,51,FALSE),6)</f>
+        <f ca="1">RIGHT(VLOOKUP(C48,[1]Sheet1!$V:$BT,51,FALSE),6)</f>
         <v>485123</v>
       </c>
       <c r="O48" s="3" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
     </row>
     <row r="49" spans="1:15">
@@ -52072,10 +52062,10 @@
         <v>265</v>
       </c>
       <c r="E49" s="4" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="F49" s="3" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
       <c r="G49" s="2" t="s">
         <v>207</v>
@@ -52099,7 +52089,7 @@
         <v>1</v>
       </c>
       <c r="N49" s="7" t="str">
-        <f>RIGHT(VLOOKUP(C49,[1]Sheet1!$V:$BT,51,FALSE),6)</f>
+        <f ca="1">RIGHT(VLOOKUP(C49,[1]Sheet1!$V:$BT,51,FALSE),6)</f>
         <v>451966</v>
       </c>
       <c r="O49" s="2" t="s">
@@ -52120,7 +52110,7 @@
         <v>274</v>
       </c>
       <c r="E50" s="4" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="F50" s="2" t="s">
         <v>275</v>
@@ -52147,7 +52137,7 @@
         <v>1</v>
       </c>
       <c r="N50" s="7" t="str">
-        <f>RIGHT(VLOOKUP(C50,[1]Sheet1!$V:$BT,51,FALSE),6)</f>
+        <f ca="1">RIGHT(VLOOKUP(C50,[1]Sheet1!$V:$BT,51,FALSE),6)</f>
         <v>500406</v>
       </c>
       <c r="O50" s="2" t="s">
@@ -52168,10 +52158,10 @@
         <v>283</v>
       </c>
       <c r="E51" s="4" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="F51" s="3" t="s">
-        <v>662</v>
+        <v>657</v>
       </c>
       <c r="G51" s="2" t="s">
         <v>276</v>
@@ -52195,7 +52185,7 @@
         <v>1</v>
       </c>
       <c r="N51" s="7" t="str">
-        <f>RIGHT(VLOOKUP(C51,[1]Sheet1!$V:$BT,51,FALSE),6)</f>
+        <f ca="1">RIGHT(VLOOKUP(C51,[1]Sheet1!$V:$BT,51,FALSE),6)</f>
         <v>504878</v>
       </c>
       <c r="O51" s="2" t="s">
@@ -52216,10 +52206,10 @@
         <v>293</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="F52" s="3" t="s">
-        <v>663</v>
+        <v>658</v>
       </c>
       <c r="G52" s="2" t="s">
         <v>288</v>
@@ -52243,7 +52233,7 @@
         <v>1</v>
       </c>
       <c r="N52" s="7" t="str">
-        <f>RIGHT(VLOOKUP(C52,[1]Sheet1!$V:$BT,51,FALSE),6)</f>
+        <f ca="1">RIGHT(VLOOKUP(C52,[1]Sheet1!$V:$BT,51,FALSE),6)</f>
         <v>471114</v>
       </c>
       <c r="O52" s="2" t="s">
@@ -52264,10 +52254,10 @@
         <v>287</v>
       </c>
       <c r="E53" s="4" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="F53" s="3" t="s">
-        <v>664</v>
+        <v>659</v>
       </c>
       <c r="G53" s="2" t="s">
         <v>288</v>
@@ -52291,7 +52281,7 @@
         <v>0</v>
       </c>
       <c r="N53" s="7" t="str">
-        <f>RIGHT(VLOOKUP(C53,[1]Sheet1!$V:$BT,51,FALSE),6)</f>
+        <f ca="1">RIGHT(VLOOKUP(C53,[1]Sheet1!$V:$BT,51,FALSE),6)</f>
         <v>438385</v>
       </c>
       <c r="O53" s="2" t="s">
@@ -52312,10 +52302,10 @@
         <v>298</v>
       </c>
       <c r="E54" s="4" t="s">
-        <v>704</v>
+        <v>699</v>
       </c>
       <c r="F54" s="3" t="s">
-        <v>665</v>
+        <v>660</v>
       </c>
       <c r="G54" s="2" t="s">
         <v>276</v>
@@ -52339,7 +52329,7 @@
         <v>1</v>
       </c>
       <c r="N54" s="7" t="str">
-        <f>RIGHT(VLOOKUP(C54,[1]Sheet1!$V:$BT,51,FALSE),6)</f>
+        <f ca="1">RIGHT(VLOOKUP(C54,[1]Sheet1!$V:$BT,51,FALSE),6)</f>
         <v>468705</v>
       </c>
       <c r="O54" s="2" t="s">
@@ -52360,7 +52350,7 @@
         <v>304</v>
       </c>
       <c r="E55" s="4" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="F55" s="2" t="s">
         <v>305</v>
@@ -52387,11 +52377,11 @@
         <v>1</v>
       </c>
       <c r="N55" s="7" t="str">
-        <f>RIGHT(VLOOKUP(C55,[1]Sheet1!$V:$BT,51,FALSE),6)</f>
+        <f ca="1">RIGHT(VLOOKUP(C55,[1]Sheet1!$V:$BT,51,FALSE),6)</f>
         <v>437917</v>
       </c>
       <c r="O55" s="3" t="s">
-        <v>715</v>
+        <v>710</v>
       </c>
     </row>
     <row r="56" spans="1:15">
@@ -52408,10 +52398,10 @@
         <v>310</v>
       </c>
       <c r="E56" s="1" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="F56" s="3" t="s">
-        <v>671</v>
+        <v>666</v>
       </c>
       <c r="G56" s="2" t="s">
         <v>89</v>
@@ -52435,11 +52425,11 @@
         <v>1</v>
       </c>
       <c r="N56" s="7" t="str">
-        <f>RIGHT(VLOOKUP(C56,[1]Sheet1!$V:$BT,51,FALSE),6)</f>
+        <f ca="1">RIGHT(VLOOKUP(C56,[1]Sheet1!$V:$BT,51,FALSE),6)</f>
         <v>508872</v>
       </c>
       <c r="O56" s="3" t="s">
-        <v>715</v>
+        <v>710</v>
       </c>
     </row>
     <row r="57" spans="1:15">
@@ -52456,7 +52446,7 @@
         <v>314</v>
       </c>
       <c r="E57" s="4" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="F57" s="3" t="s">
         <v>315</v>
@@ -52483,11 +52473,11 @@
         <v>1</v>
       </c>
       <c r="N57" s="7" t="str">
-        <f>RIGHT(VLOOKUP(C57,[1]Sheet1!$V:$BT,51,FALSE),6)</f>
+        <f ca="1">RIGHT(VLOOKUP(C57,[1]Sheet1!$V:$BT,51,FALSE),6)</f>
         <v>475892</v>
       </c>
       <c r="O57" s="3" t="s">
-        <v>715</v>
+        <v>710</v>
       </c>
     </row>
     <row r="58" spans="1:15">
@@ -52504,10 +52494,10 @@
         <v>320</v>
       </c>
       <c r="E58" s="4" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="F58" s="3" t="s">
-        <v>672</v>
+        <v>667</v>
       </c>
       <c r="G58" s="2" t="s">
         <v>89</v>
@@ -52531,11 +52521,11 @@
         <v>0</v>
       </c>
       <c r="N58" s="7" t="str">
-        <f>RIGHT(VLOOKUP(C58,[1]Sheet1!$V:$BT,51,FALSE),6)</f>
+        <f ca="1">RIGHT(VLOOKUP(C58,[1]Sheet1!$V:$BT,51,FALSE),6)</f>
         <v>539132</v>
       </c>
       <c r="O58" s="3" t="s">
-        <v>715</v>
+        <v>710</v>
       </c>
     </row>
     <row r="59" spans="1:15">
@@ -52552,10 +52542,10 @@
         <v>324</v>
       </c>
       <c r="E59" s="4" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="F59" s="3" t="s">
-        <v>673</v>
+        <v>668</v>
       </c>
       <c r="G59" s="2" t="s">
         <v>325</v>
@@ -52579,11 +52569,11 @@
         <v>1</v>
       </c>
       <c r="N59" s="7" t="str">
-        <f>RIGHT(VLOOKUP(C59,[1]Sheet1!$V:$BT,51,FALSE),6)</f>
+        <f ca="1">RIGHT(VLOOKUP(C59,[1]Sheet1!$V:$BT,51,FALSE),6)</f>
         <v>497961</v>
       </c>
       <c r="O59" s="3" t="s">
-        <v>716</v>
+        <v>711</v>
       </c>
     </row>
     <row r="60" spans="1:15">
@@ -52600,10 +52590,10 @@
         <v>329</v>
       </c>
       <c r="E60" s="4" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="F60" s="3" t="s">
-        <v>674</v>
+        <v>669</v>
       </c>
       <c r="G60" s="2" t="s">
         <v>325</v>
@@ -52627,11 +52617,11 @@
         <v>1</v>
       </c>
       <c r="N60" s="7" t="str">
-        <f>RIGHT(VLOOKUP(C60,[1]Sheet1!$V:$BT,51,FALSE),6)</f>
+        <f ca="1">RIGHT(VLOOKUP(C60,[1]Sheet1!$V:$BT,51,FALSE),6)</f>
         <v>482011</v>
       </c>
       <c r="O60" s="3" t="s">
-        <v>714</v>
+        <v>709</v>
       </c>
     </row>
     <row r="61" spans="1:15">
@@ -52648,10 +52638,10 @@
         <v>333</v>
       </c>
       <c r="E61" s="4" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="F61" s="3" t="s">
-        <v>675</v>
+        <v>670</v>
       </c>
       <c r="G61" s="2" t="s">
         <v>325</v>
@@ -52675,11 +52665,11 @@
         <v>1</v>
       </c>
       <c r="N61" s="7" t="str">
-        <f>RIGHT(VLOOKUP(C61,[1]Sheet1!$V:$BT,51,FALSE),6)</f>
+        <f ca="1">RIGHT(VLOOKUP(C61,[1]Sheet1!$V:$BT,51,FALSE),6)</f>
         <v>478441</v>
       </c>
       <c r="O61" s="3" t="s">
-        <v>712</v>
+        <v>707</v>
       </c>
     </row>
     <row r="62" spans="1:15">
@@ -52696,7 +52686,7 @@
         <v>338</v>
       </c>
       <c r="E62" s="4" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="F62" s="3" t="s">
         <v>339</v>
@@ -52723,11 +52713,11 @@
         <v>1</v>
       </c>
       <c r="N62" s="7" t="str">
-        <f>RIGHT(VLOOKUP(C62,[1]Sheet1!$V:$BT,51,FALSE),6)</f>
+        <f ca="1">RIGHT(VLOOKUP(C62,[1]Sheet1!$V:$BT,51,FALSE),6)</f>
         <v>460887</v>
       </c>
       <c r="O62" s="3" t="s">
-        <v>712</v>
+        <v>707</v>
       </c>
     </row>
     <row r="63" spans="1:15">
@@ -52744,10 +52734,10 @@
         <v>343</v>
       </c>
       <c r="E63" s="4" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="F63" s="3" t="s">
-        <v>653</v>
+        <v>650</v>
       </c>
       <c r="G63" s="2" t="s">
         <v>249</v>
@@ -52771,7 +52761,7 @@
         <v>1</v>
       </c>
       <c r="N63" s="7" t="str">
-        <f>RIGHT(VLOOKUP(C63,[1]Sheet1!$V:$BT,51,FALSE),6)</f>
+        <f ca="1">RIGHT(VLOOKUP(C63,[1]Sheet1!$V:$BT,51,FALSE),6)</f>
         <v>511753</v>
       </c>
       <c r="O63" s="2" t="s">
@@ -52786,13 +52776,13 @@
         <v>347</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>698</v>
+        <v>693</v>
       </c>
       <c r="D64" s="1" t="s">
         <v>348</v>
       </c>
       <c r="E64" s="1" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="F64" s="3" t="s">
         <v>349</v>
@@ -52819,7 +52809,7 @@
         <v>1</v>
       </c>
       <c r="N64" s="7" t="str">
-        <f>RIGHT(VLOOKUP(C64,[1]Sheet1!$V:$BT,51,FALSE),6)</f>
+        <f ca="1">RIGHT(VLOOKUP(C64,[1]Sheet1!$V:$BT,51,FALSE),6)</f>
         <v>442846</v>
       </c>
       <c r="O64" s="2" t="s">
@@ -52843,7 +52833,7 @@
         <v>354</v>
       </c>
       <c r="F65" s="3" t="s">
-        <v>694</v>
+        <v>689</v>
       </c>
       <c r="G65" s="2" t="s">
         <v>185</v>
@@ -52867,7 +52857,7 @@
         <v>1</v>
       </c>
       <c r="N65" s="7" t="str">
-        <f>RIGHT(VLOOKUP(C65,[1]Sheet1!$V:$BT,51,FALSE),6)</f>
+        <f ca="1">RIGHT(VLOOKUP(C65,[1]Sheet1!$V:$BT,51,FALSE),6)</f>
         <v>450676</v>
       </c>
       <c r="O65" s="2" t="s">
@@ -52888,10 +52878,10 @@
         <v>359</v>
       </c>
       <c r="E66" s="4" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="F66" s="3" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="G66" s="2" t="s">
         <v>156</v>
@@ -52913,11 +52903,11 @@
         <v>0</v>
       </c>
       <c r="N66" s="7" t="str">
-        <f>RIGHT(VLOOKUP(C66,[1]Sheet1!$V:$BT,51,FALSE),6)</f>
+        <f ca="1">RIGHT(VLOOKUP(C66,[1]Sheet1!$V:$BT,51,FALSE),6)</f>
         <v>549999</v>
       </c>
       <c r="O66" s="3" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
     </row>
     <row r="67" spans="1:15">
@@ -52934,10 +52924,10 @@
         <v>368</v>
       </c>
       <c r="E67" s="4" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="F67" s="3" t="s">
-        <v>681</v>
+        <v>676</v>
       </c>
       <c r="G67" s="2" t="s">
         <v>238</v>
@@ -52961,7 +52951,7 @@
         <v>1</v>
       </c>
       <c r="N67" s="7" t="str">
-        <f>RIGHT(VLOOKUP(C67,[1]Sheet1!$V:$BT,51,FALSE),6)</f>
+        <f ca="1">RIGHT(VLOOKUP(C67,[1]Sheet1!$V:$BT,51,FALSE),6)</f>
         <v>531462</v>
       </c>
       <c r="O67" s="2" t="s">
@@ -52982,10 +52972,10 @@
         <v>363</v>
       </c>
       <c r="E68" s="4" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="F68" s="3" t="s">
-        <v>682</v>
+        <v>677</v>
       </c>
       <c r="G68" s="2" t="s">
         <v>238</v>
@@ -53009,7 +52999,7 @@
         <v>1</v>
       </c>
       <c r="N68" s="7" t="str">
-        <f>RIGHT(VLOOKUP(C68,[1]Sheet1!$V:$BT,51,FALSE),6)</f>
+        <f ca="1">RIGHT(VLOOKUP(C68,[1]Sheet1!$V:$BT,51,FALSE),6)</f>
         <v>439915</v>
       </c>
       <c r="O68" s="2" t="s">
@@ -53030,10 +53020,10 @@
         <v>373</v>
       </c>
       <c r="E69" s="4" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="F69" s="3" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="G69" s="2" t="s">
         <v>28</v>
@@ -53057,11 +53047,11 @@
         <v>1</v>
       </c>
       <c r="N69" s="7" t="str">
-        <f>RIGHT(VLOOKUP(C69,[1]Sheet1!$V:$BT,51,FALSE),6)</f>
+        <f ca="1">RIGHT(VLOOKUP(C69,[1]Sheet1!$V:$BT,51,FALSE),6)</f>
         <v>514485</v>
       </c>
       <c r="O69" s="3" t="s">
-        <v>710</v>
+        <v>705</v>
       </c>
     </row>
     <row r="70" spans="1:15">
@@ -53078,7 +53068,7 @@
         <v>377</v>
       </c>
       <c r="E70" s="4" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="F70" s="3" t="s">
         <v>378</v>
@@ -53105,11 +53095,11 @@
         <v>1</v>
       </c>
       <c r="N70" s="7" t="str">
-        <f>RIGHT(VLOOKUP(C70,[1]Sheet1!$V:$BT,51,FALSE),6)</f>
+        <f ca="1">RIGHT(VLOOKUP(C70,[1]Sheet1!$V:$BT,51,FALSE),6)</f>
         <v>477261</v>
       </c>
       <c r="O70" s="3" t="s">
-        <v>711</v>
+        <v>706</v>
       </c>
     </row>
     <row r="71" spans="1:15">
@@ -53129,7 +53119,7 @@
         <v>379</v>
       </c>
       <c r="F71" s="3" t="s">
-        <v>695</v>
+        <v>690</v>
       </c>
       <c r="G71" s="2" t="s">
         <v>186</v>
@@ -53153,7 +53143,7 @@
         <v>1</v>
       </c>
       <c r="N71" s="7" t="str">
-        <f>RIGHT(VLOOKUP(C71,[1]Sheet1!$V:$BT,51,FALSE),6)</f>
+        <f ca="1">RIGHT(VLOOKUP(C71,[1]Sheet1!$V:$BT,51,FALSE),6)</f>
         <v>455008</v>
       </c>
       <c r="O71" s="2" t="s">
@@ -53174,10 +53164,10 @@
         <v>388</v>
       </c>
       <c r="E72" s="4" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="F72" s="3" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="G72" s="2" t="s">
         <v>28</v>
@@ -53199,7 +53189,7 @@
         <v>0</v>
       </c>
       <c r="N72" s="7" t="str">
-        <f>RIGHT(VLOOKUP(C72,[1]Sheet1!$V:$BT,51,FALSE),6)</f>
+        <f ca="1">RIGHT(VLOOKUP(C72,[1]Sheet1!$V:$BT,51,FALSE),6)</f>
         <v>536702</v>
       </c>
       <c r="O72" s="2" t="s">
@@ -53220,10 +53210,10 @@
         <v>393</v>
       </c>
       <c r="E73" s="4" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="F73" s="3" t="s">
-        <v>683</v>
+        <v>678</v>
       </c>
       <c r="G73" s="2" t="s">
         <v>49</v>
@@ -53247,11 +53237,11 @@
         <v>1</v>
       </c>
       <c r="N73" s="7" t="str">
-        <f>RIGHT(VLOOKUP(C73,[1]Sheet1!$V:$BT,51,FALSE),6)</f>
+        <f ca="1">RIGHT(VLOOKUP(C73,[1]Sheet1!$V:$BT,51,FALSE),6)</f>
         <v>496168</v>
       </c>
       <c r="O73" s="3" t="s">
-        <v>713</v>
+        <v>708</v>
       </c>
     </row>
     <row r="74" spans="1:15">
@@ -53268,10 +53258,10 @@
         <v>397</v>
       </c>
       <c r="E74" s="1" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="F74" s="3" t="s">
-        <v>658</v>
+        <v>653</v>
       </c>
       <c r="G74" s="2" t="s">
         <v>20</v>
@@ -53295,7 +53285,7 @@
         <v>1</v>
       </c>
       <c r="N74" s="7" t="str">
-        <f>RIGHT(VLOOKUP(C74,[1]Sheet1!$V:$BT,51,FALSE),6)</f>
+        <f ca="1">RIGHT(VLOOKUP(C74,[1]Sheet1!$V:$BT,51,FALSE),6)</f>
         <v>440308</v>
       </c>
       <c r="O74" s="2" t="s">
@@ -53316,10 +53306,10 @@
         <v>402</v>
       </c>
       <c r="E75" s="4" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="F75" s="3" t="s">
-        <v>659</v>
+        <v>654</v>
       </c>
       <c r="G75" s="2" t="s">
         <v>20</v>
@@ -53343,7 +53333,7 @@
         <v>1</v>
       </c>
       <c r="N75" s="7" t="str">
-        <f>RIGHT(VLOOKUP(C75,[1]Sheet1!$V:$BT,51,FALSE),6)</f>
+        <f ca="1">RIGHT(VLOOKUP(C75,[1]Sheet1!$V:$BT,51,FALSE),6)</f>
         <v>494954</v>
       </c>
       <c r="O75" s="2" t="s">
@@ -53367,7 +53357,7 @@
         <v>49</v>
       </c>
       <c r="F76" s="3" t="s">
-        <v>684</v>
+        <v>679</v>
       </c>
       <c r="G76" s="2" t="s">
         <v>49</v>
@@ -53391,7 +53381,7 @@
         <v>1</v>
       </c>
       <c r="N76" s="7" t="str">
-        <f>RIGHT(VLOOKUP(C76,[1]Sheet1!$V:$BT,51,FALSE),6)</f>
+        <f ca="1">RIGHT(VLOOKUP(C76,[1]Sheet1!$V:$BT,51,FALSE),6)</f>
         <v>541429</v>
       </c>
       <c r="O76" s="2" t="s">
@@ -53412,10 +53402,10 @@
         <v>411</v>
       </c>
       <c r="E77" s="4" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="F77" s="3" t="s">
-        <v>685</v>
+        <v>680</v>
       </c>
       <c r="G77" s="2" t="s">
         <v>412</v>
@@ -53439,7 +53429,7 @@
         <v>1</v>
       </c>
       <c r="N77" s="7" t="str">
-        <f>RIGHT(VLOOKUP(C77,[1]Sheet1!$V:$BT,51,FALSE),6)</f>
+        <f ca="1">RIGHT(VLOOKUP(C77,[1]Sheet1!$V:$BT,51,FALSE),6)</f>
         <v>504586</v>
       </c>
       <c r="O77" s="2" t="s">
@@ -53460,10 +53450,10 @@
         <v>418</v>
       </c>
       <c r="E78" s="4" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="F78" s="3" t="s">
-        <v>686</v>
+        <v>681</v>
       </c>
       <c r="G78" s="2" t="s">
         <v>412</v>
@@ -53487,7 +53477,7 @@
         <v>1</v>
       </c>
       <c r="N78" s="7" t="str">
-        <f>RIGHT(VLOOKUP(C78,[1]Sheet1!$V:$BT,51,FALSE),6)</f>
+        <f ca="1">RIGHT(VLOOKUP(C78,[1]Sheet1!$V:$BT,51,FALSE),6)</f>
         <v>485585</v>
       </c>
       <c r="O78" s="2" t="s">
@@ -53508,7 +53498,7 @@
         <v>428</v>
       </c>
       <c r="E79" s="1" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="F79" s="3" t="s">
         <v>429</v>
@@ -53535,7 +53525,7 @@
         <v>1</v>
       </c>
       <c r="N79" s="7" t="str">
-        <f>RIGHT(VLOOKUP(C79,[1]Sheet1!$V:$BT,51,FALSE),6)</f>
+        <f ca="1">RIGHT(VLOOKUP(C79,[1]Sheet1!$V:$BT,51,FALSE),6)</f>
         <v>473091</v>
       </c>
       <c r="O79" s="2" t="s">
@@ -53556,10 +53546,10 @@
         <v>422</v>
       </c>
       <c r="E80" s="4" t="s">
-        <v>705</v>
+        <v>700</v>
       </c>
       <c r="F80" s="3" t="s">
-        <v>687</v>
+        <v>682</v>
       </c>
       <c r="G80" s="2" t="s">
         <v>412</v>
@@ -53583,7 +53573,7 @@
         <v>1</v>
       </c>
       <c r="N80" s="7" t="str">
-        <f>RIGHT(VLOOKUP(C80,[1]Sheet1!$V:$BT,51,FALSE),6)</f>
+        <f ca="1">RIGHT(VLOOKUP(C80,[1]Sheet1!$V:$BT,51,FALSE),6)</f>
         <v>435798</v>
       </c>
       <c r="O80" s="2" t="s">
@@ -53604,10 +53594,10 @@
         <v>434</v>
       </c>
       <c r="E81" s="4" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="F81" s="3" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="G81" s="2" t="s">
         <v>435</v>
@@ -53631,7 +53621,7 @@
         <v>1</v>
       </c>
       <c r="N81" s="7" t="str">
-        <f>RIGHT(VLOOKUP(C81,[1]Sheet1!$V:$BT,51,FALSE),6)</f>
+        <f ca="1">RIGHT(VLOOKUP(C81,[1]Sheet1!$V:$BT,51,FALSE),6)</f>
         <v>495289</v>
       </c>
       <c r="O81" s="2" t="s">
@@ -53652,7 +53642,7 @@
         <v>440</v>
       </c>
       <c r="E82" s="4" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="F82" s="3" t="s">
         <v>441</v>
@@ -53679,7 +53669,7 @@
         <v>1</v>
       </c>
       <c r="N82" s="7" t="str">
-        <f>RIGHT(VLOOKUP(C82,[1]Sheet1!$V:$BT,51,FALSE),6)</f>
+        <f ca="1">RIGHT(VLOOKUP(C82,[1]Sheet1!$V:$BT,51,FALSE),6)</f>
         <v>430862</v>
       </c>
       <c r="O82" s="2" t="s">
@@ -53700,10 +53690,10 @@
         <v>445</v>
       </c>
       <c r="E83" s="4" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="F83" s="3" t="s">
-        <v>644</v>
+        <v>726</v>
       </c>
       <c r="G83" s="2" t="s">
         <v>435</v>
@@ -53727,7 +53717,7 @@
         <v>1</v>
       </c>
       <c r="N83" s="7" t="str">
-        <f>RIGHT(VLOOKUP(C83,[1]Sheet1!$V:$BT,51,FALSE),6)</f>
+        <f ca="1">RIGHT(VLOOKUP(C83,[1]Sheet1!$V:$BT,51,FALSE),6)</f>
         <v>546441</v>
       </c>
       <c r="O83" s="2" t="s">
@@ -53751,7 +53741,7 @@
         <v>168</v>
       </c>
       <c r="F84" s="3" t="s">
-        <v>645</v>
+        <v>722</v>
       </c>
       <c r="G84" s="2" t="s">
         <v>168</v>
@@ -53775,7 +53765,7 @@
         <v>1</v>
       </c>
       <c r="N84" s="7" t="str">
-        <f>RIGHT(VLOOKUP(C84,[1]Sheet1!$V:$BT,51,FALSE),6)</f>
+        <f ca="1">RIGHT(VLOOKUP(C84,[1]Sheet1!$V:$BT,51,FALSE),6)</f>
         <v>501570</v>
       </c>
       <c r="O84" s="2" t="s">
@@ -53796,7 +53786,7 @@
         <v>454</v>
       </c>
       <c r="E85" s="4" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="F85" s="3" t="s">
         <v>455</v>
@@ -53823,7 +53813,7 @@
         <v>0</v>
       </c>
       <c r="N85" s="7" t="str">
-        <f>RIGHT(VLOOKUP(C85,[1]Sheet1!$V:$BT,51,FALSE),6)</f>
+        <f ca="1">RIGHT(VLOOKUP(C85,[1]Sheet1!$V:$BT,51,FALSE),6)</f>
         <v>468966</v>
       </c>
       <c r="O85" s="2" t="s">
@@ -53847,7 +53837,7 @@
         <v>462</v>
       </c>
       <c r="F86" s="3" t="s">
-        <v>660</v>
+        <v>655</v>
       </c>
       <c r="G86" s="2" t="s">
         <v>461</v>
@@ -53871,7 +53861,7 @@
         <v>1</v>
       </c>
       <c r="N86" s="7" t="str">
-        <f>RIGHT(VLOOKUP(C86,[1]Sheet1!$V:$BT,51,FALSE),6)</f>
+        <f ca="1">RIGHT(VLOOKUP(C86,[1]Sheet1!$V:$BT,51,FALSE),6)</f>
         <v>464361</v>
       </c>
       <c r="O86" s="2" t="s">
@@ -53883,7 +53873,7 @@
         <v>464</v>
       </c>
       <c r="B87" s="3" t="s">
-        <v>726</v>
+        <v>721</v>
       </c>
       <c r="C87" s="1" t="s">
         <v>465</v>
@@ -53892,10 +53882,10 @@
         <v>466</v>
       </c>
       <c r="E87" s="4" t="s">
-        <v>702</v>
+        <v>697</v>
       </c>
       <c r="F87" s="3" t="s">
-        <v>666</v>
+        <v>661</v>
       </c>
       <c r="G87" s="2" t="s">
         <v>467</v>
@@ -53919,7 +53909,7 @@
         <v>1</v>
       </c>
       <c r="N87" s="7" t="str">
-        <f>RIGHT(VLOOKUP(C87,[1]Sheet1!$V:$BT,51,FALSE),6)</f>
+        <f ca="1">RIGHT(VLOOKUP(C87,[1]Sheet1!$V:$BT,51,FALSE),6)</f>
         <v>509792</v>
       </c>
       <c r="O87" s="2" t="s">
@@ -53940,10 +53930,10 @@
         <v>472</v>
       </c>
       <c r="E88" s="4" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="F88" s="3" t="s">
-        <v>667</v>
+        <v>662</v>
       </c>
       <c r="G88" s="2" t="s">
         <v>467</v>
@@ -53967,7 +53957,7 @@
         <v>1</v>
       </c>
       <c r="N88" s="7" t="str">
-        <f>RIGHT(VLOOKUP(C88,[1]Sheet1!$V:$BT,51,FALSE),6)</f>
+        <f ca="1">RIGHT(VLOOKUP(C88,[1]Sheet1!$V:$BT,51,FALSE),6)</f>
         <v>532846</v>
       </c>
       <c r="O88" s="2" t="s">
@@ -53988,7 +53978,7 @@
         <v>477</v>
       </c>
       <c r="E89" s="4" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="F89" s="2" t="s">
         <v>478</v>
@@ -54015,7 +54005,7 @@
         <v>1</v>
       </c>
       <c r="N89" s="7" t="str">
-        <f>RIGHT(VLOOKUP(C89,[1]Sheet1!$V:$BT,51,FALSE),6)</f>
+        <f ca="1">RIGHT(VLOOKUP(C89,[1]Sheet1!$V:$BT,51,FALSE),6)</f>
         <v>500117</v>
       </c>
       <c r="O89" s="2" t="s">
@@ -54036,7 +54026,7 @@
         <v>484</v>
       </c>
       <c r="E90" s="4" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="F90" s="2" t="s">
         <v>485</v>
@@ -54063,7 +54053,7 @@
         <v>1</v>
       </c>
       <c r="N90" s="7" t="str">
-        <f>RIGHT(VLOOKUP(C90,[1]Sheet1!$V:$BT,51,FALSE),6)</f>
+        <f ca="1">RIGHT(VLOOKUP(C90,[1]Sheet1!$V:$BT,51,FALSE),6)</f>
         <v>489681</v>
       </c>
       <c r="O90" s="2" t="s">
@@ -54087,7 +54077,7 @@
         <v>462</v>
       </c>
       <c r="F91" s="3" t="s">
-        <v>661</v>
+        <v>656</v>
       </c>
       <c r="G91" s="2" t="s">
         <v>461</v>
@@ -54111,7 +54101,7 @@
         <v>1</v>
       </c>
       <c r="N91" s="7" t="str">
-        <f>RIGHT(VLOOKUP(C91,[1]Sheet1!$V:$BT,51,FALSE),6)</f>
+        <f ca="1">RIGHT(VLOOKUP(C91,[1]Sheet1!$V:$BT,51,FALSE),6)</f>
         <v>500317</v>
       </c>
       <c r="O91" s="2" t="s">
@@ -54132,10 +54122,10 @@
         <v>494</v>
       </c>
       <c r="E92" s="4" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="F92" s="3" t="s">
-        <v>676</v>
+        <v>671</v>
       </c>
       <c r="G92" s="2" t="s">
         <v>495</v>
@@ -54159,11 +54149,11 @@
         <v>1</v>
       </c>
       <c r="N92" s="7" t="str">
-        <f>RIGHT(VLOOKUP(C92,[1]Sheet1!$V:$BT,51,FALSE),6)</f>
+        <f ca="1">RIGHT(VLOOKUP(C92,[1]Sheet1!$V:$BT,51,FALSE),6)</f>
         <v>497949</v>
       </c>
       <c r="O92" s="3" t="s">
-        <v>717</v>
+        <v>712</v>
       </c>
     </row>
     <row r="93" spans="1:15">
@@ -54180,7 +54170,7 @@
         <v>500</v>
       </c>
       <c r="E93" s="4" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="F93" s="3" t="s">
         <v>501</v>
@@ -54207,11 +54197,11 @@
         <v>1</v>
       </c>
       <c r="N93" s="7" t="str">
-        <f>RIGHT(VLOOKUP(C93,[1]Sheet1!$V:$BT,51,FALSE),6)</f>
+        <f ca="1">RIGHT(VLOOKUP(C93,[1]Sheet1!$V:$BT,51,FALSE),6)</f>
         <v>539630</v>
       </c>
       <c r="O93" s="3" t="s">
-        <v>718</v>
+        <v>713</v>
       </c>
     </row>
     <row r="94" spans="1:15">
@@ -54228,10 +54218,10 @@
         <v>505</v>
       </c>
       <c r="E94" s="4" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="F94" s="3" t="s">
-        <v>677</v>
+        <v>672</v>
       </c>
       <c r="G94" s="2" t="s">
         <v>495</v>
@@ -54255,7 +54245,7 @@
         <v>1</v>
       </c>
       <c r="N94" s="7" t="str">
-        <f>RIGHT(VLOOKUP(C94,[1]Sheet1!$V:$BT,51,FALSE),6)</f>
+        <f ca="1">RIGHT(VLOOKUP(C94,[1]Sheet1!$V:$BT,51,FALSE),6)</f>
         <v>498827</v>
       </c>
       <c r="O94" s="2" t="s">
@@ -54264,37 +54254,37 @@
     </row>
     <row r="95" spans="1:15">
       <c r="A95" s="3" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="B95" s="3" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="C95" s="1" t="s">
+        <v>620</v>
+      </c>
+      <c r="D95" s="1" t="s">
         <v>621</v>
       </c>
-      <c r="D95" s="1" t="s">
-        <v>622</v>
-      </c>
       <c r="E95" s="4" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="F95" s="3" t="s">
-        <v>688</v>
+        <v>683</v>
       </c>
       <c r="G95" s="2" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="H95" s="2" t="s">
         <v>412</v>
       </c>
       <c r="I95" s="2" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="J95" s="2" t="s">
         <v>188</v>
       </c>
       <c r="K95" s="2" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="L95" s="2">
         <v>1</v>
@@ -54303,46 +54293,46 @@
         <v>1</v>
       </c>
       <c r="N95" s="7" t="str">
-        <f>RIGHT(VLOOKUP(C95,[1]Sheet1!$V:$BT,51,FALSE),6)</f>
+        <f ca="1">RIGHT(VLOOKUP(C95,[1]Sheet1!$V:$BT,51,FALSE),6)</f>
         <v>497726</v>
       </c>
       <c r="O95" s="2" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
     </row>
     <row r="96" spans="1:15">
       <c r="A96" s="2" t="s">
+        <v>512</v>
+      </c>
+      <c r="B96" s="2" t="s">
         <v>513</v>
       </c>
-      <c r="B96" s="2" t="s">
+      <c r="C96" s="1" t="s">
         <v>514</v>
       </c>
-      <c r="C96" s="1" t="s">
+      <c r="D96" s="1" t="s">
         <v>515</v>
       </c>
-      <c r="D96" s="1" t="s">
-        <v>516</v>
-      </c>
       <c r="E96" s="4" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="F96" s="3" t="s">
-        <v>689</v>
+        <v>684</v>
       </c>
       <c r="G96" s="2" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="H96" s="2" t="s">
         <v>412</v>
       </c>
       <c r="I96" s="2" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="J96" s="2" t="s">
         <v>188</v>
       </c>
       <c r="K96" s="2" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="L96" s="2">
         <v>1</v>
@@ -54351,46 +54341,46 @@
         <v>1</v>
       </c>
       <c r="N96" s="7" t="str">
-        <f>RIGHT(VLOOKUP(C96,[1]Sheet1!$V:$BT,51,FALSE),6)</f>
+        <f ca="1">RIGHT(VLOOKUP(C96,[1]Sheet1!$V:$BT,51,FALSE),6)</f>
         <v>504366</v>
       </c>
       <c r="O96" s="2" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
     </row>
     <row r="97" spans="1:15">
       <c r="A97" s="2" t="s">
+        <v>518</v>
+      </c>
+      <c r="B97" s="2" t="s">
         <v>519</v>
       </c>
-      <c r="B97" s="2" t="s">
+      <c r="C97" s="1" t="s">
         <v>520</v>
       </c>
-      <c r="C97" s="1" t="s">
+      <c r="D97" s="1" t="s">
         <v>521</v>
       </c>
-      <c r="D97" s="1" t="s">
-        <v>522</v>
-      </c>
       <c r="E97" s="1" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="F97" s="3" t="s">
-        <v>690</v>
+        <v>685</v>
       </c>
       <c r="G97" s="2" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="H97" s="2" t="s">
         <v>412</v>
       </c>
       <c r="I97" s="2" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="J97" s="2" t="s">
         <v>188</v>
       </c>
       <c r="K97" s="2" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="L97" s="2">
         <v>1</v>
@@ -54399,46 +54389,46 @@
         <v>1</v>
       </c>
       <c r="N97" s="7" t="str">
-        <f>RIGHT(VLOOKUP(C97,[1]Sheet1!$V:$BT,51,FALSE),6)</f>
+        <f ca="1">RIGHT(VLOOKUP(C97,[1]Sheet1!$V:$BT,51,FALSE),6)</f>
         <v>468799</v>
       </c>
       <c r="O97" s="2" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
     </row>
     <row r="98" spans="1:15">
       <c r="A98" s="3" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="B98" s="3" t="s">
         <v>508</v>
       </c>
       <c r="C98" s="1" t="s">
+        <v>622</v>
+      </c>
+      <c r="D98" s="1" t="s">
         <v>623</v>
       </c>
-      <c r="D98" s="1" t="s">
-        <v>624</v>
-      </c>
       <c r="E98" s="4" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="F98" s="3" t="s">
+        <v>724</v>
+      </c>
+      <c r="G98" s="2" t="s">
         <v>509</v>
-      </c>
-      <c r="G98" s="2" t="s">
-        <v>510</v>
       </c>
       <c r="H98" s="2" t="s">
         <v>412</v>
       </c>
       <c r="I98" s="2" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="J98" s="2" t="s">
         <v>188</v>
       </c>
       <c r="K98" s="2" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="L98" s="2">
         <v>1</v>
@@ -54447,46 +54437,46 @@
         <v>1</v>
       </c>
       <c r="N98" s="7" t="str">
-        <f>RIGHT(VLOOKUP(C98,[1]Sheet1!$V:$BT,51,FALSE),6)</f>
+        <f ca="1">RIGHT(VLOOKUP(C98,[1]Sheet1!$V:$BT,51,FALSE),6)</f>
         <v>457613</v>
       </c>
       <c r="O98" s="3" t="s">
-        <v>709</v>
+        <v>704</v>
       </c>
     </row>
     <row r="99" spans="1:15">
       <c r="A99" s="2" t="s">
+        <v>525</v>
+      </c>
+      <c r="B99" s="2" t="s">
         <v>526</v>
       </c>
-      <c r="B99" s="2" t="s">
+      <c r="C99" s="1" t="s">
         <v>527</v>
       </c>
-      <c r="C99" s="1" t="s">
+      <c r="D99" s="1" t="s">
         <v>528</v>
       </c>
-      <c r="D99" s="1" t="s">
+      <c r="E99" s="4" t="s">
+        <v>694</v>
+      </c>
+      <c r="F99" s="3" t="s">
+        <v>686</v>
+      </c>
+      <c r="G99" s="2" t="s">
         <v>529</v>
-      </c>
-      <c r="E99" s="4" t="s">
-        <v>699</v>
-      </c>
-      <c r="F99" s="3" t="s">
-        <v>691</v>
-      </c>
-      <c r="G99" s="2" t="s">
-        <v>530</v>
       </c>
       <c r="H99" s="2" t="s">
         <v>412</v>
       </c>
       <c r="I99" s="2" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="J99" s="2" t="s">
         <v>188</v>
       </c>
       <c r="K99" s="2" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="L99" s="2">
         <v>1</v>
@@ -54495,46 +54485,46 @@
         <v>1</v>
       </c>
       <c r="N99" s="7" t="str">
-        <f>RIGHT(VLOOKUP(C99,[1]Sheet1!$V:$BT,51,FALSE),6)</f>
+        <f ca="1">RIGHT(VLOOKUP(C99,[1]Sheet1!$V:$BT,51,FALSE),6)</f>
         <v>504642</v>
       </c>
       <c r="O99" s="2" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
     </row>
     <row r="100" spans="1:15">
       <c r="A100" s="2" t="s">
+        <v>531</v>
+      </c>
+      <c r="B100" s="2" t="s">
         <v>532</v>
       </c>
-      <c r="B100" s="2" t="s">
+      <c r="C100" s="1" t="s">
         <v>533</v>
       </c>
-      <c r="C100" s="1" t="s">
+      <c r="D100" s="1" t="s">
         <v>534</v>
       </c>
-      <c r="D100" s="1" t="s">
-        <v>535</v>
-      </c>
       <c r="E100" s="4" t="s">
-        <v>700</v>
+        <v>695</v>
       </c>
       <c r="F100" s="3" t="s">
-        <v>692</v>
+        <v>687</v>
       </c>
       <c r="G100" s="2" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="H100" s="2" t="s">
         <v>412</v>
       </c>
       <c r="I100" s="2" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="J100" s="2" t="s">
         <v>188</v>
       </c>
       <c r="K100" s="2" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="L100" s="2">
         <v>1</v>
@@ -54543,31 +54533,31 @@
         <v>1</v>
       </c>
       <c r="N100" s="7" t="str">
-        <f>RIGHT(VLOOKUP(C100,[1]Sheet1!$V:$BT,51,FALSE),6)</f>
+        <f ca="1">RIGHT(VLOOKUP(C100,[1]Sheet1!$V:$BT,51,FALSE),6)</f>
         <v>472242</v>
       </c>
       <c r="O100" s="2" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
     </row>
     <row r="101" spans="1:15">
       <c r="A101" s="2" t="s">
+        <v>536</v>
+      </c>
+      <c r="B101" s="2" t="s">
         <v>537</v>
       </c>
-      <c r="B101" s="2" t="s">
+      <c r="C101" s="1" t="s">
         <v>538</v>
       </c>
-      <c r="C101" s="1" t="s">
+      <c r="D101" s="1" t="s">
         <v>539</v>
       </c>
-      <c r="D101" s="1" t="s">
+      <c r="E101" s="4" t="s">
+        <v>702</v>
+      </c>
+      <c r="F101" s="2" t="s">
         <v>540</v>
-      </c>
-      <c r="E101" s="4" t="s">
-        <v>707</v>
-      </c>
-      <c r="F101" s="2" t="s">
-        <v>541</v>
       </c>
       <c r="G101" s="2" t="s">
         <v>186</v>
@@ -54591,31 +54581,31 @@
         <v>1</v>
       </c>
       <c r="N101" s="7" t="str">
-        <f>RIGHT(VLOOKUP(C101,[1]Sheet1!$V:$BT,51,FALSE),6)</f>
+        <f ca="1">RIGHT(VLOOKUP(C101,[1]Sheet1!$V:$BT,51,FALSE),6)</f>
         <v>515987</v>
       </c>
       <c r="O101" s="2" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
     </row>
     <row r="102" spans="1:15">
       <c r="A102" s="2" t="s">
+        <v>542</v>
+      </c>
+      <c r="B102" s="2" t="s">
         <v>543</v>
       </c>
-      <c r="B102" s="2" t="s">
+      <c r="C102" s="1" t="s">
         <v>544</v>
       </c>
-      <c r="C102" s="1" t="s">
+      <c r="D102" s="1" t="s">
         <v>545</v>
       </c>
-      <c r="D102" s="1" t="s">
-        <v>546</v>
-      </c>
       <c r="E102" s="4" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="F102" s="3" t="s">
-        <v>696</v>
+        <v>691</v>
       </c>
       <c r="G102" s="2" t="s">
         <v>186</v>
@@ -54639,11 +54629,11 @@
         <v>1</v>
       </c>
       <c r="N102" s="7" t="str">
-        <f>RIGHT(VLOOKUP(C102,[1]Sheet1!$V:$BT,51,FALSE),6)</f>
+        <f ca="1">RIGHT(VLOOKUP(C102,[1]Sheet1!$V:$BT,51,FALSE),6)</f>
         <v>451701</v>
       </c>
       <c r="O102" s="2" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
     </row>
     <row r="104" spans="1:15">
@@ -54659,10 +54649,10 @@
     <sortCondition ref="A82"/>
   </sortState>
   <conditionalFormatting sqref="B1:B101">
-    <cfRule type="duplicateValues" dxfId="2" priority="12"/>
+    <cfRule type="duplicateValues" dxfId="1" priority="12"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="N2:N102">
-    <cfRule type="duplicateValues" dxfId="1" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Add Vatchers to phone list
</commit_message>
<xml_diff>
--- a/config/phone_list.xlsx
+++ b/config/phone_list.xlsx
@@ -5,7 +5,7 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="J:\arps\config\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="J:\ARPS\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1199" uniqueCount="721">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1215" uniqueCount="731">
   <si>
     <t>AREA_NAME</t>
   </si>
@@ -2190,6 +2190,36 @@
   </si>
   <si>
     <t>E. Bezzant DL / McPherson</t>
+  </si>
+  <si>
+    <t>0905388991</t>
+  </si>
+  <si>
+    <t>0905388992</t>
+  </si>
+  <si>
+    <t>屈長老</t>
+  </si>
+  <si>
+    <t>屈姐妹</t>
+  </si>
+  <si>
+    <t>DAAN_FUXING_COUPLE</t>
+  </si>
+  <si>
+    <t>E. Vatcher</t>
+  </si>
+  <si>
+    <t>S. Vatcher</t>
+  </si>
+  <si>
+    <t>VATCHER_E</t>
+  </si>
+  <si>
+    <t>VATCHER_S</t>
+  </si>
+  <si>
+    <t>0</t>
   </si>
 </sst>
 </file>
@@ -2235,7 +2265,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
@@ -2243,6 +2273,8 @@
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2536,13 +2568,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:N103"/>
+  <dimension ref="A1:O103"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B83" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B74" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="S87" sqref="S87"/>
+      <selection pane="bottomRight" activeCell="L89" sqref="L89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2555,7 +2587,7 @@
     <col min="15" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14">
+    <row r="1" spans="1:15">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -2598,8 +2630,9 @@
       <c r="N1" s="2" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="2" spans="1:14">
+      <c r="O1" s="8"/>
+    </row>
+    <row r="2" spans="1:15">
       <c r="A2" s="2" t="s">
         <v>199</v>
       </c>
@@ -2643,7 +2676,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="3" spans="1:14">
+    <row r="3" spans="1:15">
       <c r="A3" s="2" t="s">
         <v>204</v>
       </c>
@@ -2685,7 +2718,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="4" spans="1:14">
+    <row r="4" spans="1:15">
       <c r="A4" s="2" t="s">
         <v>204</v>
       </c>
@@ -2727,7 +2760,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="5" spans="1:14">
+    <row r="5" spans="1:15">
       <c r="A5" s="2" t="s">
         <v>515</v>
       </c>
@@ -2769,7 +2802,7 @@
       </c>
       <c r="N5" s="2"/>
     </row>
-    <row r="6" spans="1:14">
+    <row r="6" spans="1:15">
       <c r="A6" s="2" t="s">
         <v>335</v>
       </c>
@@ -2811,7 +2844,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="7" spans="1:14">
+    <row r="7" spans="1:15">
       <c r="A7" s="2" t="s">
         <v>159</v>
       </c>
@@ -2855,7 +2888,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="8" spans="1:14">
+    <row r="8" spans="1:15">
       <c r="A8" s="2" t="s">
         <v>166</v>
       </c>
@@ -2899,7 +2932,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="9" spans="1:14">
+    <row r="9" spans="1:15">
       <c r="A9" s="2" t="s">
         <v>209</v>
       </c>
@@ -2943,7 +2976,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="10" spans="1:14">
+    <row r="10" spans="1:15">
       <c r="A10" s="2" t="s">
         <v>214</v>
       </c>
@@ -2987,7 +3020,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="11" spans="1:14">
+    <row r="11" spans="1:15">
       <c r="A11" s="2" t="s">
         <v>24</v>
       </c>
@@ -3029,7 +3062,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="12" spans="1:14">
+    <row r="12" spans="1:15">
       <c r="A12" s="2" t="s">
         <v>24</v>
       </c>
@@ -3071,7 +3104,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="13" spans="1:14">
+    <row r="13" spans="1:15">
       <c r="A13" s="2" t="s">
         <v>349</v>
       </c>
@@ -3115,7 +3148,7 @@
         <v>634</v>
       </c>
     </row>
-    <row r="14" spans="1:14">
+    <row r="14" spans="1:15">
       <c r="A14" s="2" t="s">
         <v>353</v>
       </c>
@@ -3159,7 +3192,7 @@
         <v>635</v>
       </c>
     </row>
-    <row r="15" spans="1:14">
+    <row r="15" spans="1:15">
       <c r="A15" s="2" t="s">
         <v>363</v>
       </c>
@@ -3201,7 +3234,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="16" spans="1:14">
+    <row r="16" spans="1:15">
       <c r="A16" s="2" t="s">
         <v>121</v>
       </c>
@@ -6970,8 +7003,57 @@
         <v>514</v>
       </c>
     </row>
+    <row r="102" spans="1:14">
+      <c r="A102" s="7" t="s">
+        <v>728</v>
+      </c>
+      <c r="B102" s="7" t="s">
+        <v>721</v>
+      </c>
+      <c r="C102" s="7" t="s">
+        <v>726</v>
+      </c>
+      <c r="D102" s="7" t="s">
+        <v>723</v>
+      </c>
+      <c r="E102" s="7" t="s">
+        <v>725</v>
+      </c>
+      <c r="F102" s="7" t="s">
+        <v>726</v>
+      </c>
+      <c r="L102" s="7" t="s">
+        <v>730</v>
+      </c>
+      <c r="M102" s="7" t="s">
+        <v>730</v>
+      </c>
+    </row>
     <row r="103" spans="1:14">
-      <c r="E103" s="2"/>
+      <c r="A103" s="7" t="s">
+        <v>729</v>
+      </c>
+      <c r="B103" s="7" t="s">
+        <v>722</v>
+      </c>
+      <c r="C103" s="7" t="s">
+        <v>727</v>
+      </c>
+      <c r="D103" s="7" t="s">
+        <v>724</v>
+      </c>
+      <c r="E103" s="7" t="s">
+        <v>725</v>
+      </c>
+      <c r="F103" s="7" t="s">
+        <v>727</v>
+      </c>
+      <c r="L103" s="7" t="s">
+        <v>730</v>
+      </c>
+      <c r="M103" s="7" t="s">
+        <v>730</v>
+      </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:N100">

</xml_diff>

<commit_message>
Update phone list with changes in English teaching
</commit_message>
<xml_diff>
--- a/config/phone_list.xlsx
+++ b/config/phone_list.xlsx
@@ -5,7 +5,7 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="J:\arps\config\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="J:\ARPS\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -17,7 +17,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">PHONE_LIST!$A$1:$N$100</definedName>
   </definedNames>
-  <calcPr calcId="152511" calcMode="manual"/>
+  <calcPr calcId="152511" calcMode="manual" calcOnSave="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1215" uniqueCount="731">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1216" uniqueCount="731">
   <si>
     <t>AREA_NAME</t>
   </si>
@@ -2571,10 +2571,10 @@
   <dimension ref="A1:O103"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B40" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G13" sqref="G13"/>
+      <selection pane="bottomRight" activeCell="M58" sqref="M58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5072,8 +5072,8 @@
       <c r="L57" s="2">
         <v>1</v>
       </c>
-      <c r="M57" s="2">
-        <v>1</v>
+      <c r="M57" s="1" t="s">
+        <v>725</v>
       </c>
       <c r="N57" s="2" t="s">
         <v>283</v>

</xml_diff>

<commit_message>
Add ADDRESS column to phone list
</commit_message>
<xml_diff>
--- a/config/phone_list.xlsx
+++ b/config/phone_list.xlsx
@@ -14,10 +14,13 @@
   <sheets>
     <sheet name="PHONE_LIST" sheetId="1" r:id="rId1"/>
   </sheets>
+  <externalReferences>
+    <externalReference r:id="rId2"/>
+  </externalReferences>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">PHONE_LIST!$A$1:$N$100</definedName>
   </definedNames>
-  <calcPr calcId="152511" calcMode="manual" calcOnSave="0"/>
+  <calcPr calcId="152511" calcMode="manual" calcCompleted="0" calcOnSave="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -27,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1216" uniqueCount="731">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1217" uniqueCount="732">
   <si>
     <t>AREA_NAME</t>
   </si>
@@ -1712,9 +1715,6 @@
     <t>LUZHU_XINGZHONG</t>
   </si>
   <si>
-    <t>LUZHU_ZHONGZHENG</t>
-  </si>
-  <si>
     <t>SHILIN_YUSHENG</t>
   </si>
   <si>
@@ -2220,6 +2220,12 @@
   </si>
   <si>
     <t>DAAN,NEW_TAIPEI,大安區,新北市,大安,ENGLISH_WARD,ENGLISH,ENGLISHWARD,英文,英文支會</t>
+  </si>
+  <si>
+    <t>LUZHU_NANPING</t>
+  </si>
+  <si>
+    <t>ADDRESS</t>
   </si>
 </sst>
 </file>
@@ -2244,12 +2250,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -2265,7 +2277,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
@@ -2274,7 +2286,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2293,6 +2307,11 @@
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFFFF99"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -2302,6 +2321,2033 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="CONTROLS"/>
+      <sheetName val="COMP_LIST"/>
+      <sheetName val="APARTMENTS"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0"/>
+      <sheetData sheetId="1"/>
+      <sheetData sheetId="2">
+        <row r="1">
+          <cell r="A1" t="str">
+            <v>Apartment Name</v>
+          </cell>
+          <cell r="C1" t="str">
+            <v>Companionship</v>
+          </cell>
+          <cell r="E1" t="str">
+            <v>Zone</v>
+          </cell>
+          <cell r="F1" t="str">
+            <v>District</v>
+          </cell>
+          <cell r="G1" t="str">
+            <v>Address</v>
+          </cell>
+        </row>
+        <row r="2">
+          <cell r="A2" t="str">
+            <v>English</v>
+          </cell>
+          <cell r="B2" t="str">
+            <v>Chinese</v>
+          </cell>
+          <cell r="C2">
+            <v>1</v>
+          </cell>
+          <cell r="D2">
+            <v>2</v>
+          </cell>
+        </row>
+        <row r="3">
+          <cell r="A3" t="str">
+            <v>BANQIAO</v>
+          </cell>
+          <cell r="B3" t="str">
+            <v>板橋</v>
+          </cell>
+          <cell r="C3" t="str">
+            <v>XINPU_E</v>
+          </cell>
+          <cell r="D3" t="str">
+            <v/>
+          </cell>
+          <cell r="E3" t="str">
+            <v>WEST</v>
+          </cell>
+          <cell r="F3" t="str">
+            <v>BANQIAO</v>
+          </cell>
+          <cell r="G3" t="str">
+            <v>新北市板橋區民生路三段281巷2弄7號4樓</v>
+          </cell>
+        </row>
+        <row r="4">
+          <cell r="A4" t="str">
+            <v>BEITOU_WENQUAN</v>
+          </cell>
+          <cell r="B4" t="str">
+            <v>北投溫泉</v>
+          </cell>
+          <cell r="C4" t="str">
+            <v>BEITOU_E</v>
+          </cell>
+          <cell r="D4" t="str">
+            <v/>
+          </cell>
+          <cell r="E4" t="str">
+            <v>NORTH</v>
+          </cell>
+          <cell r="F4" t="str">
+            <v>BEITOU</v>
+          </cell>
+          <cell r="G4" t="str">
+            <v>台北市北投區溫泉路65巷16號7樓之14</v>
+          </cell>
+        </row>
+        <row r="5">
+          <cell r="A5" t="str">
+            <v>BEITOU_ZHONGYANG</v>
+          </cell>
+          <cell r="B5" t="str">
+            <v>北投中央</v>
+          </cell>
+          <cell r="C5" t="str">
+            <v>BEITOU_S</v>
+          </cell>
+          <cell r="D5" t="str">
+            <v/>
+          </cell>
+          <cell r="E5" t="str">
+            <v>NORTH</v>
+          </cell>
+          <cell r="F5" t="str">
+            <v>BEITOU</v>
+          </cell>
+          <cell r="G5" t="str">
+            <v>臺北市北投區中央北路二段181號4樓之3</v>
+          </cell>
+        </row>
+        <row r="6">
+          <cell r="A6" t="str">
+            <v>DAAN_HEPING</v>
+          </cell>
+          <cell r="B6" t="str">
+            <v>大安和平</v>
+          </cell>
+          <cell r="C6" t="str">
+            <v>XINAN_S</v>
+          </cell>
+          <cell r="D6" t="str">
+            <v/>
+          </cell>
+          <cell r="E6" t="str">
+            <v>CENTRAL</v>
+          </cell>
+          <cell r="F6" t="str">
+            <v>XINAN</v>
+          </cell>
+          <cell r="G6" t="str">
+            <v>台北市大安區和平東路二段96巷20弄12號3樓</v>
+          </cell>
+        </row>
+        <row r="7">
+          <cell r="A7" t="str">
+            <v>DAAN_JINAN_COUPLE</v>
+          </cell>
+          <cell r="B7" t="str">
+            <v>大安濟南夫婦</v>
+          </cell>
+          <cell r="C7" t="str">
+            <v/>
+          </cell>
+          <cell r="D7" t="str">
+            <v/>
+          </cell>
+          <cell r="E7" t="str">
+            <v/>
+          </cell>
+          <cell r="F7" t="str">
+            <v/>
+          </cell>
+          <cell r="G7" t="str">
+            <v>台北市大安區濟南路二段31-42號11樓之D</v>
+          </cell>
+        </row>
+        <row r="8">
+          <cell r="A8" t="str">
+            <v>DAAN_JINHUA</v>
+          </cell>
+          <cell r="B8" t="str">
+            <v>大安金華</v>
+          </cell>
+          <cell r="C8" t="str">
+            <v>TOUR_S</v>
+          </cell>
+          <cell r="D8" t="str">
+            <v/>
+          </cell>
+          <cell r="E8" t="str">
+            <v>CENTRAL</v>
+          </cell>
+          <cell r="F8" t="str">
+            <v>JINHUA</v>
+          </cell>
+          <cell r="G8" t="str">
+            <v>台北市大安區金華街102巷5號4樓</v>
+          </cell>
+        </row>
+        <row r="9">
+          <cell r="A9" t="str">
+            <v>DAAN_YONGKANG</v>
+          </cell>
+          <cell r="B9" t="str">
+            <v>大案永康</v>
+          </cell>
+          <cell r="C9" t="str">
+            <v>OFFICE_E</v>
+          </cell>
+          <cell r="D9" t="str">
+            <v>OFFICE_E</v>
+          </cell>
+          <cell r="E9" t="str">
+            <v>CENTRAL</v>
+          </cell>
+          <cell r="F9" t="str">
+            <v>JINHUA</v>
+          </cell>
+          <cell r="G9" t="str">
+            <v>台北市大安區永康街47巷12號4F</v>
+          </cell>
+        </row>
+        <row r="10">
+          <cell r="A10" t="str">
+            <v>DAAN_YONGKANG_COUPLE</v>
+          </cell>
+          <cell r="B10" t="str">
+            <v>大安永康夫婦</v>
+          </cell>
+          <cell r="C10" t="str">
+            <v/>
+          </cell>
+          <cell r="D10" t="str">
+            <v/>
+          </cell>
+          <cell r="E10" t="str">
+            <v/>
+          </cell>
+          <cell r="F10" t="str">
+            <v/>
+          </cell>
+          <cell r="G10" t="str">
+            <v>臺北市大安區永康街14巷1-4號</v>
+          </cell>
+        </row>
+        <row r="11">
+          <cell r="A11" t="str">
+            <v>DANSHUI_MINQUAN</v>
+          </cell>
+          <cell r="B11" t="str">
+            <v>淡水民權</v>
+          </cell>
+          <cell r="C11" t="str">
+            <v>DANSHUI_A_E</v>
+          </cell>
+          <cell r="D11" t="str">
+            <v/>
+          </cell>
+          <cell r="E11" t="str">
+            <v>NORTH</v>
+          </cell>
+          <cell r="F11" t="str">
+            <v>BEITOU</v>
+          </cell>
+          <cell r="G11" t="str">
+            <v>新北市淡水區民權路173巷7號3樓-13</v>
+          </cell>
+        </row>
+        <row r="12">
+          <cell r="A12" t="str">
+            <v>DANSHUI_YINGZHUAN</v>
+          </cell>
+          <cell r="B12" t="str">
+            <v>淡水英專</v>
+          </cell>
+          <cell r="C12" t="str">
+            <v>DANSHUI_B_E</v>
+          </cell>
+          <cell r="D12" t="str">
+            <v/>
+          </cell>
+          <cell r="E12" t="str">
+            <v>NORTH</v>
+          </cell>
+          <cell r="F12" t="str">
+            <v>BEITOU</v>
+          </cell>
+          <cell r="G12" t="str">
+            <v>新北市淡水區英專路90之2號3樓</v>
+          </cell>
+        </row>
+        <row r="13">
+          <cell r="A13" t="str">
+            <v>DATONG</v>
+          </cell>
+          <cell r="B13" t="str">
+            <v>大同</v>
+          </cell>
+          <cell r="C13" t="str">
+            <v>WANDA_S</v>
+          </cell>
+          <cell r="D13" t="str">
+            <v/>
+          </cell>
+          <cell r="E13" t="str">
+            <v>CENTRAL</v>
+          </cell>
+          <cell r="F13" t="str">
+            <v>XINAN</v>
+          </cell>
+          <cell r="G13" t="str">
+            <v>台北市大同區南京西路103號10樓之10</v>
+          </cell>
+        </row>
+        <row r="14">
+          <cell r="A14" t="str">
+            <v>DAXI_QIAOAI_34</v>
+          </cell>
+          <cell r="B14" t="str">
+            <v>大溪僑愛34</v>
+          </cell>
+          <cell r="C14" t="str">
+            <v>BADE_S</v>
+          </cell>
+          <cell r="D14" t="str">
+            <v/>
+          </cell>
+          <cell r="E14" t="str">
+            <v>TAOYUAN</v>
+          </cell>
+          <cell r="F14" t="str">
+            <v>BADE</v>
+          </cell>
+          <cell r="G14" t="str">
+            <v>桃園市大溪鎮僑愛一街34巷7號8樓</v>
+          </cell>
+        </row>
+        <row r="15">
+          <cell r="A15" t="str">
+            <v>DAXI_QIAOAI_35</v>
+          </cell>
+          <cell r="B15" t="str">
+            <v>大溪僑愛35</v>
+          </cell>
+          <cell r="C15" t="str">
+            <v>BADE_A_E</v>
+          </cell>
+          <cell r="D15" t="str">
+            <v/>
+          </cell>
+          <cell r="E15" t="str">
+            <v>TAOYUAN</v>
+          </cell>
+          <cell r="F15" t="str">
+            <v>BADE</v>
+          </cell>
+          <cell r="G15" t="str">
+            <v>桃園市大溪鎮僑愛一街35巷20弄10號9樓</v>
+          </cell>
+        </row>
+        <row r="16">
+          <cell r="A16" t="str">
+            <v>GUISHAN</v>
+          </cell>
+          <cell r="B16" t="str">
+            <v>龜山</v>
+          </cell>
+          <cell r="C16" t="str">
+            <v>GUISHAN_E</v>
+          </cell>
+          <cell r="D16" t="str">
+            <v/>
+          </cell>
+          <cell r="E16" t="str">
+            <v>TAOYUAN</v>
+          </cell>
+          <cell r="F16" t="str">
+            <v>TAOYUAN_1_2</v>
+          </cell>
+          <cell r="G16" t="str">
+            <v>桃園市龜山區自強東路226號3樓</v>
+          </cell>
+        </row>
+        <row r="17">
+          <cell r="A17" t="str">
+            <v>HUALIAN_BEICHANG</v>
+          </cell>
+          <cell r="B17" t="str">
+            <v>花蓮北昌</v>
+          </cell>
+          <cell r="C17" t="str">
+            <v>HUALIAN_3_E</v>
+          </cell>
+          <cell r="D17" t="str">
+            <v/>
+          </cell>
+          <cell r="E17" t="str">
+            <v>HUALIAN</v>
+          </cell>
+          <cell r="F17" t="str">
+            <v>HUALIAN</v>
+          </cell>
+          <cell r="G17" t="str">
+            <v>花蓮縣吉安鄉北昌五街102號2樓</v>
+          </cell>
+        </row>
+        <row r="18">
+          <cell r="A18" t="str">
+            <v>HUALIAN_CHANGAN_COUPLE</v>
+          </cell>
+          <cell r="B18" t="str">
+            <v>花蓮長安夫婦</v>
+          </cell>
+          <cell r="C18" t="str">
+            <v>HUALIAN_COUPLE</v>
+          </cell>
+          <cell r="D18" t="str">
+            <v/>
+          </cell>
+          <cell r="E18" t="str">
+            <v>HUALIAN</v>
+          </cell>
+          <cell r="F18" t="str">
+            <v>JIAN</v>
+          </cell>
+          <cell r="G18" t="str">
+            <v>花蓮縣花蓮市長安街26號13樓之9</v>
+          </cell>
+        </row>
+        <row r="19">
+          <cell r="A19" t="str">
+            <v>HUALIAN_DEAN</v>
+          </cell>
+          <cell r="B19" t="str">
+            <v>花蓮德安</v>
+          </cell>
+          <cell r="C19" t="str">
+            <v>HUALIAN_2_E</v>
+          </cell>
+          <cell r="D19" t="str">
+            <v>HUALIAN_2_ZL</v>
+          </cell>
+          <cell r="E19" t="str">
+            <v>HUALIAN</v>
+          </cell>
+          <cell r="F19" t="str">
+            <v>JIAN</v>
+          </cell>
+          <cell r="G19" t="str">
+            <v>花蓮縣花蓮市德安一街291號5F之3</v>
+          </cell>
+        </row>
+        <row r="20">
+          <cell r="A20" t="str">
+            <v>HUALIAN_ZHONGHE</v>
+          </cell>
+          <cell r="B20" t="str">
+            <v>花蓮中和</v>
+          </cell>
+          <cell r="C20" t="str">
+            <v>HUALIAN_3_S</v>
+          </cell>
+          <cell r="D20" t="str">
+            <v>HUALIAN_1_S</v>
+          </cell>
+          <cell r="E20" t="str">
+            <v>HUALIAN</v>
+          </cell>
+          <cell r="F20" t="str">
+            <v>HUALIAN</v>
+          </cell>
+          <cell r="G20" t="str">
+            <v>花蓮縣花蓮市中和街217號10樓之1</v>
+          </cell>
+        </row>
+        <row r="21">
+          <cell r="A21" t="str">
+            <v>HUALIAN_ZHONGMEI</v>
+          </cell>
+          <cell r="B21" t="str">
+            <v>花蓮中美</v>
+          </cell>
+          <cell r="C21" t="str">
+            <v>HUALIAN_1_E</v>
+          </cell>
+          <cell r="D21" t="str">
+            <v/>
+          </cell>
+          <cell r="E21" t="str">
+            <v>HUALIAN</v>
+          </cell>
+          <cell r="F21" t="str">
+            <v>JIAN</v>
+          </cell>
+          <cell r="G21" t="str">
+            <v>花蓮縣花蓮市中美13街78號2F之12</v>
+          </cell>
+        </row>
+        <row r="22">
+          <cell r="A22" t="str">
+            <v>JILONG</v>
+          </cell>
+          <cell r="B22" t="str">
+            <v>基隆</v>
+          </cell>
+          <cell r="C22" t="str">
+            <v>JILONG_A_E</v>
+          </cell>
+          <cell r="D22" t="str">
+            <v>JILONG_B_E</v>
+          </cell>
+          <cell r="E22" t="str">
+            <v>EAST</v>
+          </cell>
+          <cell r="F22" t="str">
+            <v>JILONG</v>
+          </cell>
+          <cell r="G22" t="str">
+            <v>基隆市中正區義一路186號2樓</v>
+          </cell>
+        </row>
+        <row r="23">
+          <cell r="A23" t="str">
+            <v>LONGTAN</v>
+          </cell>
+          <cell r="B23" t="str">
+            <v>龍潭</v>
+          </cell>
+          <cell r="C23" t="str">
+            <v>LONGTAN_E</v>
+          </cell>
+          <cell r="D23" t="str">
+            <v/>
+          </cell>
+          <cell r="E23" t="str">
+            <v>TAOYUAN</v>
+          </cell>
+          <cell r="F23" t="str">
+            <v>BADE</v>
+          </cell>
+          <cell r="G23" t="str">
+            <v>桃園市龍潭區龍星村大同路207號10樓</v>
+          </cell>
+        </row>
+        <row r="24">
+          <cell r="A24" t="str">
+            <v>LUODONG_GONGZHENG</v>
+          </cell>
+          <cell r="B24" t="str">
+            <v>羅東公正</v>
+          </cell>
+          <cell r="C24" t="str">
+            <v>LUODONG_A_E</v>
+          </cell>
+          <cell r="D24" t="str">
+            <v>LUODONG_B_E</v>
+          </cell>
+          <cell r="E24" t="str">
+            <v>EAST</v>
+          </cell>
+          <cell r="F24" t="str">
+            <v>YILAN</v>
+          </cell>
+          <cell r="G24" t="str">
+            <v>宜蘭縣羅東鎮公正路289之3號8樓</v>
+          </cell>
+        </row>
+        <row r="25">
+          <cell r="A25" t="str">
+            <v>LUODONG_ZHANDONG</v>
+          </cell>
+          <cell r="B25" t="str">
+            <v>羅東站東</v>
+          </cell>
+          <cell r="C25" t="str">
+            <v>YILAN_S</v>
+          </cell>
+          <cell r="D25" t="str">
+            <v/>
+          </cell>
+          <cell r="E25" t="str">
+            <v>EAST</v>
+          </cell>
+          <cell r="F25" t="str">
+            <v>YILAN</v>
+          </cell>
+          <cell r="G25" t="str">
+            <v>宜蘭縣羅東鎮站東路108號C棟2樓</v>
+          </cell>
+        </row>
+        <row r="26">
+          <cell r="A26" t="str">
+            <v>LUZHOU_XINYI</v>
+          </cell>
+          <cell r="B26" t="str">
+            <v>瀘州信義</v>
+          </cell>
+          <cell r="C26" t="str">
+            <v>LUZHOU_A_E</v>
+          </cell>
+          <cell r="D26" t="str">
+            <v>LUZHOU_B_E</v>
+          </cell>
+          <cell r="E26" t="str">
+            <v>CENTRAL</v>
+          </cell>
+          <cell r="F26" t="str">
+            <v>SANCHONG</v>
+          </cell>
+          <cell r="G26" t="str">
+            <v>新北市瀘州區信義路222巷35號9樓之3</v>
+          </cell>
+        </row>
+        <row r="27">
+          <cell r="A27" t="str">
+            <v>LUZHU_XINGZHONG</v>
+          </cell>
+          <cell r="B27" t="str">
+            <v>蘆竹興中</v>
+          </cell>
+          <cell r="C27" t="str">
+            <v>TAO_3_E</v>
+          </cell>
+          <cell r="D27" t="str">
+            <v/>
+          </cell>
+          <cell r="E27" t="str">
+            <v>TAOYUAN</v>
+          </cell>
+          <cell r="F27" t="str">
+            <v>TAOYUAN_3</v>
+          </cell>
+          <cell r="G27" t="str">
+            <v>桃園市蘆竹區興中街55號4樓之1</v>
+          </cell>
+        </row>
+        <row r="28">
+          <cell r="A28" t="str">
+            <v>LUZHU_ZHONGZHENG</v>
+          </cell>
+          <cell r="B28" t="str">
+            <v>蘆竹中正</v>
+          </cell>
+          <cell r="C28" t="str">
+            <v>TAO_4_S</v>
+          </cell>
+          <cell r="D28" t="str">
+            <v/>
+          </cell>
+          <cell r="E28" t="str">
+            <v>TAOYUAN</v>
+          </cell>
+          <cell r="F28" t="str">
+            <v>TAOYUAN_3</v>
+          </cell>
+          <cell r="G28" t="str">
+            <v>桃園市蘆竹區中正路27號23樓之1</v>
+          </cell>
+        </row>
+        <row r="29">
+          <cell r="A29" t="str">
+            <v>LUZHU_NANPING</v>
+          </cell>
+          <cell r="B29" t="str">
+            <v>蘆竹南平</v>
+          </cell>
+          <cell r="C29" t="str">
+            <v/>
+          </cell>
+          <cell r="D29" t="str">
+            <v/>
+          </cell>
+          <cell r="E29" t="str">
+            <v/>
+          </cell>
+          <cell r="F29" t="str">
+            <v/>
+          </cell>
+          <cell r="G29" t="str">
+            <v>桃園市蘆竹區南平街7號2樓之三</v>
+          </cell>
+        </row>
+        <row r="30">
+          <cell r="A30" t="str">
+            <v>MIAOLI</v>
+          </cell>
+          <cell r="B30" t="str">
+            <v>苗栗</v>
+          </cell>
+          <cell r="C30" t="str">
+            <v>MIAOLI_E</v>
+          </cell>
+          <cell r="D30" t="str">
+            <v/>
+          </cell>
+          <cell r="E30" t="str">
+            <v>ZHUNAN</v>
+          </cell>
+          <cell r="F30" t="str">
+            <v>TOUFEN_MIAOLI</v>
+          </cell>
+          <cell r="G30" t="str">
+            <v>苗栗縣苗栗市嘉福街177巷7號4F.5F</v>
+          </cell>
+        </row>
+        <row r="31">
+          <cell r="A31" t="str">
+            <v>NEIHU_JINHU</v>
+          </cell>
+          <cell r="B31" t="str">
+            <v>內湖金湖</v>
+          </cell>
+          <cell r="C31" t="str">
+            <v>NEIHU_S</v>
+          </cell>
+          <cell r="D31" t="str">
+            <v/>
+          </cell>
+          <cell r="E31" t="str">
+            <v>EAST</v>
+          </cell>
+          <cell r="F31" t="str">
+            <v>SONGSHAN</v>
+          </cell>
+          <cell r="G31" t="str">
+            <v>臺北市內湖區金湖路326巷45號5樓之2</v>
+          </cell>
+        </row>
+        <row r="32">
+          <cell r="A32" t="str">
+            <v>NEIHU_NEIHU</v>
+          </cell>
+          <cell r="B32" t="str">
+            <v>內湖内湖</v>
+          </cell>
+          <cell r="C32" t="str">
+            <v>NEIHU_E</v>
+          </cell>
+          <cell r="D32" t="str">
+            <v/>
+          </cell>
+          <cell r="E32" t="str">
+            <v>EAST</v>
+          </cell>
+          <cell r="F32" t="str">
+            <v>SONGSHAN</v>
+          </cell>
+          <cell r="G32" t="str">
+            <v>臺北市內湖區內湖路1段411巷5號4樓</v>
+          </cell>
+        </row>
+        <row r="33">
+          <cell r="A33" t="str">
+            <v>SANCHONG_CHENGGONG_5</v>
+          </cell>
+          <cell r="B33" t="str">
+            <v>三重成功5</v>
+          </cell>
+          <cell r="C33" t="str">
+            <v>SANCHONG_S</v>
+          </cell>
+          <cell r="D33" t="str">
+            <v/>
+          </cell>
+          <cell r="E33" t="str">
+            <v>CENTRAL</v>
+          </cell>
+          <cell r="F33" t="str">
+            <v>SANCHONG</v>
+          </cell>
+          <cell r="G33" t="str">
+            <v>新北市三重區成功路100號9樓之5</v>
+          </cell>
+        </row>
+        <row r="34">
+          <cell r="A34" t="str">
+            <v>SANCHONG_CHENGGONG_6</v>
+          </cell>
+          <cell r="B34" t="str">
+            <v>三重成功6</v>
+          </cell>
+          <cell r="C34" t="str">
+            <v>SANCHONG_E</v>
+          </cell>
+          <cell r="D34" t="str">
+            <v/>
+          </cell>
+          <cell r="E34" t="str">
+            <v>CENTRAL</v>
+          </cell>
+          <cell r="F34" t="str">
+            <v>SANCHONG</v>
+          </cell>
+          <cell r="G34" t="str">
+            <v>新北市三重區成功路100號9樓之6</v>
+          </cell>
+        </row>
+        <row r="35">
+          <cell r="A35" t="str">
+            <v>SHILIN_DABEI</v>
+          </cell>
+          <cell r="B35" t="str">
+            <v>士林仁勇</v>
+          </cell>
+          <cell r="C35" t="str">
+            <v>SHILIN_ZL</v>
+          </cell>
+          <cell r="D35" t="str">
+            <v/>
+          </cell>
+          <cell r="E35" t="str">
+            <v>NORTH</v>
+          </cell>
+          <cell r="F35" t="str">
+            <v>SHILIN</v>
+          </cell>
+          <cell r="G35" t="str">
+            <v>臺北市士林區大北路100號3樓</v>
+          </cell>
+        </row>
+        <row r="36">
+          <cell r="A36" t="str">
+            <v>SHILIN_SHUANGXI</v>
+          </cell>
+          <cell r="B36" t="str">
+            <v>士林雙溪</v>
+          </cell>
+          <cell r="C36" t="str">
+            <v>SHILIN_S</v>
+          </cell>
+          <cell r="D36" t="str">
+            <v/>
+          </cell>
+          <cell r="E36" t="str">
+            <v>NORTH</v>
+          </cell>
+          <cell r="F36" t="str">
+            <v>SHILIN</v>
+          </cell>
+          <cell r="G36" t="str">
+            <v>臺北市士林區雙溪街106號2樓之1</v>
+          </cell>
+        </row>
+        <row r="37">
+          <cell r="A37" t="str">
+            <v>SHILIN_YUSHENG</v>
+          </cell>
+          <cell r="B37" t="str">
+            <v>士林雨聲</v>
+          </cell>
+          <cell r="C37" t="str">
+            <v>TIANMU_A_E</v>
+          </cell>
+          <cell r="D37" t="str">
+            <v>TIANMU_B_E</v>
+          </cell>
+          <cell r="E37" t="str">
+            <v>NORTH</v>
+          </cell>
+          <cell r="F37" t="str">
+            <v>SHILIN</v>
+          </cell>
+          <cell r="G37" t="str">
+            <v>臺北市士林區雨聲街83巷5號3樓</v>
+          </cell>
+        </row>
+        <row r="38">
+          <cell r="A38" t="str">
+            <v>SHULIN</v>
+          </cell>
+          <cell r="B38" t="str">
+            <v>樹林</v>
+          </cell>
+          <cell r="C38" t="str">
+            <v>SANXIA_A_E</v>
+          </cell>
+          <cell r="D38" t="str">
+            <v>SANXIA_B_E</v>
+          </cell>
+          <cell r="E38" t="str">
+            <v>WEST</v>
+          </cell>
+          <cell r="F38" t="str">
+            <v>TUCHENG</v>
+          </cell>
+          <cell r="G38" t="str">
+            <v>新北市樹林區佳園路3段452號8樓</v>
+          </cell>
+        </row>
+        <row r="39">
+          <cell r="A39" t="str">
+            <v>SONGSHAN_BADE</v>
+          </cell>
+          <cell r="B39" t="str">
+            <v>松山八德</v>
+          </cell>
+          <cell r="C39" t="str">
+            <v>SONGSHAN_S</v>
+          </cell>
+          <cell r="D39" t="str">
+            <v/>
+          </cell>
+          <cell r="E39" t="str">
+            <v>EAST</v>
+          </cell>
+          <cell r="F39" t="str">
+            <v>SONGSHAN</v>
+          </cell>
+          <cell r="G39" t="str">
+            <v>臺北市松山區八德路4段262號4樓</v>
+          </cell>
+        </row>
+        <row r="40">
+          <cell r="A40" t="str">
+            <v>SONGSHAN_NANJING</v>
+          </cell>
+          <cell r="B40" t="str">
+            <v>松山南京</v>
+          </cell>
+          <cell r="C40" t="str">
+            <v>SONGSHAN_ZL</v>
+          </cell>
+          <cell r="D40" t="str">
+            <v/>
+          </cell>
+          <cell r="E40" t="str">
+            <v>EAST</v>
+          </cell>
+          <cell r="F40" t="str">
+            <v>SONGSHAN</v>
+          </cell>
+          <cell r="G40" t="str">
+            <v>臺北市松山區南京東路5段328號6樓之1</v>
+          </cell>
+        </row>
+        <row r="41">
+          <cell r="A41" t="str">
+            <v>TAIDONG_CHANGSHA_2</v>
+          </cell>
+          <cell r="B41" t="str">
+            <v>台東長沙2</v>
+          </cell>
+          <cell r="C41" t="str">
+            <v>TAIDONG_1_S</v>
+          </cell>
+          <cell r="D41" t="str">
+            <v>TAIDONG_2_S</v>
+          </cell>
+          <cell r="E41" t="str">
+            <v>TAIDONG</v>
+          </cell>
+          <cell r="F41" t="str">
+            <v>TAIDONG_1_3</v>
+          </cell>
+          <cell r="G41" t="str">
+            <v>臺東縣臺東市長沙街206巷17弄2號2樓</v>
+          </cell>
+        </row>
+        <row r="42">
+          <cell r="A42" t="str">
+            <v>TAIDONG_CHANGSHA_8</v>
+          </cell>
+          <cell r="B42" t="str">
+            <v>台東長沙8</v>
+          </cell>
+          <cell r="C42" t="str">
+            <v>TAIDONG_2_ZL</v>
+          </cell>
+          <cell r="D42" t="str">
+            <v/>
+          </cell>
+          <cell r="E42" t="str">
+            <v>TAIDONG</v>
+          </cell>
+          <cell r="F42" t="str">
+            <v>TAIDONG_2</v>
+          </cell>
+          <cell r="G42" t="str">
+            <v>臺東縣臺東市長沙街206巷15弄8號2樓</v>
+          </cell>
+        </row>
+        <row r="43">
+          <cell r="A43" t="str">
+            <v>TAIDONG_KAIFENG</v>
+          </cell>
+          <cell r="B43" t="str">
+            <v>台東開封</v>
+          </cell>
+          <cell r="C43" t="str">
+            <v>TAIDONG_1_E</v>
+          </cell>
+          <cell r="D43" t="str">
+            <v/>
+          </cell>
+          <cell r="E43" t="str">
+            <v>TAIDONG</v>
+          </cell>
+          <cell r="F43" t="str">
+            <v>TAIDONG_1_3</v>
+          </cell>
+          <cell r="G43" t="str">
+            <v>臺東縣臺東市開封街439號4樓之4</v>
+          </cell>
+        </row>
+        <row r="44">
+          <cell r="A44" t="str">
+            <v>TAIDONG_GENGSHENG</v>
+          </cell>
+          <cell r="B44" t="str">
+            <v>台東南王</v>
+          </cell>
+          <cell r="C44" t="str">
+            <v>TAIDONG_3_E</v>
+          </cell>
+          <cell r="D44" t="str">
+            <v/>
+          </cell>
+          <cell r="E44" t="str">
+            <v>TAIDONG</v>
+          </cell>
+          <cell r="F44" t="str">
+            <v>TAIDONG_1_3</v>
+          </cell>
+          <cell r="G44" t="str">
+            <v>臺東縣臺東市更生北路674巷22號</v>
+          </cell>
+        </row>
+        <row r="45">
+          <cell r="A45" t="str">
+            <v>TAOYUAN_DAYOU</v>
+          </cell>
+          <cell r="B45" t="str">
+            <v>桃園大有</v>
+          </cell>
+          <cell r="C45" t="str">
+            <v>TAO_1_A</v>
+          </cell>
+          <cell r="D45" t="str">
+            <v>TAO_1_B</v>
+          </cell>
+          <cell r="E45" t="str">
+            <v>TAOYUAN</v>
+          </cell>
+          <cell r="F45" t="str">
+            <v>TAOYUAN_1_2</v>
+          </cell>
+          <cell r="G45" t="str">
+            <v>桃園市桃園區大有路630之11號20樓</v>
+          </cell>
+        </row>
+        <row r="46">
+          <cell r="A46" t="str">
+            <v>TAOYUAN_GUODING</v>
+          </cell>
+          <cell r="B46" t="str">
+            <v>桃園國鼎</v>
+          </cell>
+          <cell r="C46" t="str">
+            <v>TAO_2_E</v>
+          </cell>
+          <cell r="D46" t="str">
+            <v/>
+          </cell>
+          <cell r="E46" t="str">
+            <v>TAOYUAN</v>
+          </cell>
+          <cell r="F46" t="str">
+            <v>TAOYUAN_1_2</v>
+          </cell>
+          <cell r="G46" t="str">
+            <v>桃園市桃園區國鼎一街3號12樓之2</v>
+          </cell>
+        </row>
+        <row r="47">
+          <cell r="A47" t="str">
+            <v>TAOYUAN_GUOJI</v>
+          </cell>
+          <cell r="B47" t="str">
+            <v>桃園國際</v>
+          </cell>
+          <cell r="C47" t="str">
+            <v>TAO_2_S</v>
+          </cell>
+          <cell r="D47" t="str">
+            <v/>
+          </cell>
+          <cell r="E47" t="str">
+            <v>TAOYUAN</v>
+          </cell>
+          <cell r="F47" t="str">
+            <v>TAOYUAN_1_2</v>
+          </cell>
+          <cell r="G47" t="str">
+            <v>桃園市桃園區國際路1段1191號16樓之4</v>
+          </cell>
+        </row>
+        <row r="48">
+          <cell r="A48" t="str">
+            <v>TAOYUAN_MINYOU</v>
+          </cell>
+          <cell r="B48" t="str">
+            <v>桃園民有</v>
+          </cell>
+          <cell r="C48" t="str">
+            <v>TAO_4_E</v>
+          </cell>
+          <cell r="D48" t="str">
+            <v/>
+          </cell>
+          <cell r="E48" t="str">
+            <v>TAOYUAN</v>
+          </cell>
+          <cell r="F48" t="str">
+            <v>TAOYUAN_3</v>
+          </cell>
+          <cell r="G48" t="str">
+            <v>桃園市桃園區民有十二街66號9樓</v>
+          </cell>
+        </row>
+        <row r="49">
+          <cell r="A49" t="str">
+            <v>TAOYUAN_ZHONGPU</v>
+          </cell>
+          <cell r="B49" t="str">
+            <v>桃園中埔</v>
+          </cell>
+          <cell r="C49" t="str">
+            <v>TAO_3_E_ZL</v>
+          </cell>
+          <cell r="D49" t="str">
+            <v/>
+          </cell>
+          <cell r="E49" t="str">
+            <v>TAOYUAN</v>
+          </cell>
+          <cell r="F49" t="str">
+            <v>TAOYUAN_3</v>
+          </cell>
+          <cell r="G49" t="str">
+            <v>桃園市桃園區中埔二街83號13樓</v>
+          </cell>
+        </row>
+        <row r="50">
+          <cell r="A50" t="str">
+            <v>TOUFEN</v>
+          </cell>
+          <cell r="B50" t="str">
+            <v>頭分</v>
+          </cell>
+          <cell r="C50" t="str">
+            <v>TOUFEN_E</v>
+          </cell>
+          <cell r="D50" t="str">
+            <v/>
+          </cell>
+          <cell r="E50" t="str">
+            <v>ZHUNAN</v>
+          </cell>
+          <cell r="F50" t="str">
+            <v>TOUFEN_MIAOLI</v>
+          </cell>
+          <cell r="G50" t="str">
+            <v>苗栗縣頭份鎮節約街88號7樓</v>
+          </cell>
+        </row>
+        <row r="51">
+          <cell r="A51" t="str">
+            <v>TUCHENG_YUMIN</v>
+          </cell>
+          <cell r="B51" t="str">
+            <v>土城裕民</v>
+          </cell>
+          <cell r="C51" t="str">
+            <v>TUCHENG_ZL</v>
+          </cell>
+          <cell r="D51" t="str">
+            <v/>
+          </cell>
+          <cell r="E51" t="str">
+            <v>WEST</v>
+          </cell>
+          <cell r="F51" t="str">
+            <v>TUCHENG</v>
+          </cell>
+          <cell r="G51" t="str">
+            <v>新北市土城區裕民路92巷5弄6號8樓</v>
+          </cell>
+        </row>
+        <row r="52">
+          <cell r="A52" t="str">
+            <v>TUCHENG_ZHONGYANG</v>
+          </cell>
+          <cell r="B52" t="str">
+            <v>土城中央</v>
+          </cell>
+          <cell r="C52" t="str">
+            <v>TUCHENG_S</v>
+          </cell>
+          <cell r="D52" t="str">
+            <v/>
+          </cell>
+          <cell r="E52" t="str">
+            <v>WEST</v>
+          </cell>
+          <cell r="F52" t="str">
+            <v>TUCHENG</v>
+          </cell>
+          <cell r="G52" t="str">
+            <v>新北市土城區中央路1段88號16樓</v>
+          </cell>
+        </row>
+        <row r="53">
+          <cell r="A53" t="str">
+            <v>WANHUA</v>
+          </cell>
+          <cell r="B53" t="str">
+            <v>萬華</v>
+          </cell>
+          <cell r="C53" t="str">
+            <v>WANDA_E</v>
+          </cell>
+          <cell r="D53" t="str">
+            <v/>
+          </cell>
+          <cell r="E53" t="str">
+            <v>CENTRAL</v>
+          </cell>
+          <cell r="F53" t="str">
+            <v>XINAN</v>
+          </cell>
+          <cell r="G53" t="str">
+            <v>臺北市萬華區國興路58號2樓</v>
+          </cell>
+        </row>
+        <row r="54">
+          <cell r="A54" t="str">
+            <v>WENSHAN_MUZHA</v>
+          </cell>
+          <cell r="B54" t="str">
+            <v>文山木柵</v>
+          </cell>
+          <cell r="C54" t="str">
+            <v>MUZHA_E</v>
+          </cell>
+          <cell r="D54" t="str">
+            <v/>
+          </cell>
+          <cell r="E54" t="str">
+            <v>SOUTH</v>
+          </cell>
+          <cell r="F54" t="str">
+            <v>JINGXIN</v>
+          </cell>
+          <cell r="G54" t="str">
+            <v>臺北市文山區木柵路3段85巷29號2樓</v>
+          </cell>
+        </row>
+        <row r="55">
+          <cell r="A55" t="str">
+            <v>WENSHAN_WANSHOU</v>
+          </cell>
+          <cell r="B55" t="str">
+            <v>文山萬壽</v>
+          </cell>
+          <cell r="C55" t="str">
+            <v>MUZHA_S</v>
+          </cell>
+          <cell r="D55" t="str">
+            <v/>
+          </cell>
+          <cell r="E55" t="str">
+            <v>SOUTH</v>
+          </cell>
+          <cell r="F55" t="str">
+            <v>JINGXIN</v>
+          </cell>
+          <cell r="G55" t="str">
+            <v>臺北市文山區萬壽路17巷1號7樓之2</v>
+          </cell>
+        </row>
+        <row r="56">
+          <cell r="A56" t="str">
+            <v>XIANGSHAN</v>
+          </cell>
+          <cell r="B56" t="str">
+            <v>香山</v>
+          </cell>
+          <cell r="C56" t="str">
+            <v>XIANGSHAN_E</v>
+          </cell>
+          <cell r="D56" t="str">
+            <v/>
+          </cell>
+          <cell r="E56" t="str">
+            <v>ZHUNAN</v>
+          </cell>
+          <cell r="F56" t="str">
+            <v>ZHUNAN</v>
+          </cell>
+          <cell r="G56" t="str">
+            <v>新竹市香山區牛埔東路247號12樓之4</v>
+          </cell>
+        </row>
+        <row r="57">
+          <cell r="A57" t="str">
+            <v>XINDIAN_ANKANG</v>
+          </cell>
+          <cell r="B57" t="str">
+            <v>新店安康</v>
+          </cell>
+          <cell r="C57" t="str">
+            <v>ANKANG_E</v>
+          </cell>
+          <cell r="D57" t="str">
+            <v/>
+          </cell>
+          <cell r="E57" t="str">
+            <v>SOUTH</v>
+          </cell>
+          <cell r="F57" t="str">
+            <v>XINDIAN</v>
+          </cell>
+          <cell r="G57" t="str">
+            <v>新北市新店區安康路2段159巷5號12樓</v>
+          </cell>
+        </row>
+        <row r="58">
+          <cell r="A58" t="str">
+            <v>XINDIAN_BINLANG</v>
+          </cell>
+          <cell r="B58" t="str">
+            <v>新店檳榔</v>
+          </cell>
+          <cell r="C58" t="str">
+            <v>JINGXIN_ZL</v>
+          </cell>
+          <cell r="D58" t="str">
+            <v>XINDIAN_E</v>
+          </cell>
+          <cell r="E58" t="str">
+            <v>SOUTH</v>
+          </cell>
+          <cell r="F58" t="str">
+            <v>JINGXIN</v>
+          </cell>
+          <cell r="G58" t="str">
+            <v>新北市新店區檳榔路53巷2號6樓</v>
+          </cell>
+        </row>
+        <row r="59">
+          <cell r="A59" t="str">
+            <v>XINDIAN_ZHONGYANG</v>
+          </cell>
+          <cell r="B59" t="str">
+            <v>新店中央</v>
+          </cell>
+          <cell r="C59" t="str">
+            <v>JINGXIN_S</v>
+          </cell>
+          <cell r="D59" t="str">
+            <v>XINDIAN_S</v>
+          </cell>
+          <cell r="E59" t="str">
+            <v>SOUTH</v>
+          </cell>
+          <cell r="F59" t="str">
+            <v>JINGXIN</v>
+          </cell>
+          <cell r="G59" t="str">
+            <v>新北市新店區中央八街68號4樓</v>
+          </cell>
+        </row>
+        <row r="60">
+          <cell r="A60" t="str">
+            <v>XINFENG</v>
+          </cell>
+          <cell r="B60" t="str">
+            <v>新豐</v>
+          </cell>
+          <cell r="C60" t="str">
+            <v>ZHUBEI_2_E</v>
+          </cell>
+          <cell r="D60" t="str">
+            <v/>
+          </cell>
+          <cell r="E60" t="str">
+            <v>XINZHU</v>
+          </cell>
+          <cell r="F60" t="str">
+            <v>ZHUBEI</v>
+          </cell>
+          <cell r="G60" t="str">
+            <v>新竹縣新豐鄉明新街426巷20號2樓之1</v>
+          </cell>
+        </row>
+        <row r="61">
+          <cell r="A61" t="str">
+            <v>XINZHU_1_3_S</v>
+          </cell>
+          <cell r="B61" t="str">
+            <v>新竹一+三姐妹</v>
+          </cell>
+          <cell r="C61" t="str">
+            <v/>
+          </cell>
+          <cell r="D61" t="str">
+            <v/>
+          </cell>
+          <cell r="E61" t="str">
+            <v/>
+          </cell>
+          <cell r="F61" t="str">
+            <v/>
+          </cell>
+          <cell r="G61" t="str">
+            <v>新竹市北區東大路2段186號2樓之2</v>
+          </cell>
+        </row>
+        <row r="62">
+          <cell r="A62" t="str">
+            <v>XINZHU_BEIDA</v>
+          </cell>
+          <cell r="B62" t="str">
+            <v>新竹北大</v>
+          </cell>
+          <cell r="C62" t="str">
+            <v>XINZHU_1_E</v>
+          </cell>
+          <cell r="D62" t="str">
+            <v/>
+          </cell>
+          <cell r="E62" t="str">
+            <v>XINZHU</v>
+          </cell>
+          <cell r="F62" t="str">
+            <v>XINZHU</v>
+          </cell>
+          <cell r="G62" t="str">
+            <v>新竹市北區北大路166巷28號8樓之4</v>
+          </cell>
+        </row>
+        <row r="63">
+          <cell r="A63" t="str">
+            <v>XINZHU_DONGDA</v>
+          </cell>
+          <cell r="B63" t="str">
+            <v>新竹東大</v>
+          </cell>
+          <cell r="C63" t="str">
+            <v>XINZHU_1_S</v>
+          </cell>
+          <cell r="D63" t="str">
+            <v>XINZHU_3_S</v>
+          </cell>
+          <cell r="E63" t="str">
+            <v>XINZHU</v>
+          </cell>
+          <cell r="F63" t="str">
+            <v>XINZHU</v>
+          </cell>
+          <cell r="G63" t="str">
+            <v>新竹市東區東大路2段232巷11號6樓</v>
+          </cell>
+        </row>
+        <row r="64">
+          <cell r="A64" t="str">
+            <v>XINZHU_SHIPIN</v>
+          </cell>
+          <cell r="B64" t="str">
+            <v>新竹綠水</v>
+          </cell>
+          <cell r="C64" t="str">
+            <v>XINZHU_3_ZL</v>
+          </cell>
+          <cell r="D64" t="str">
+            <v/>
+          </cell>
+          <cell r="E64" t="str">
+            <v>XINZHU</v>
+          </cell>
+          <cell r="F64" t="str">
+            <v>XINZHU</v>
+          </cell>
+          <cell r="G64" t="str">
+            <v>新竹市東區食品路27號3樓之33(1301室)</v>
+          </cell>
+        </row>
+        <row r="65">
+          <cell r="A65" t="str">
+            <v>XINZHUANG_QINGSHAN</v>
+          </cell>
+          <cell r="B65" t="str">
+            <v>新莊青山</v>
+          </cell>
+          <cell r="C65" t="str">
+            <v>DANFENG_E</v>
+          </cell>
+          <cell r="D65" t="str">
+            <v/>
+          </cell>
+          <cell r="E65" t="str">
+            <v>WEST</v>
+          </cell>
+          <cell r="F65" t="str">
+            <v>XINZHUANG</v>
+          </cell>
+          <cell r="G65" t="str">
+            <v>新北市新莊區青山路1段64之3號10樓</v>
+          </cell>
+        </row>
+        <row r="66">
+          <cell r="A66" t="str">
+            <v>XINZHUANG_ZHONGZHENG</v>
+          </cell>
+          <cell r="B66" t="str">
+            <v>新莊中正</v>
+          </cell>
+          <cell r="C66" t="str">
+            <v>SIYUAN_E</v>
+          </cell>
+          <cell r="D66" t="str">
+            <v/>
+          </cell>
+          <cell r="E66" t="str">
+            <v>WEST</v>
+          </cell>
+          <cell r="F66" t="str">
+            <v>XINZHUANG</v>
+          </cell>
+          <cell r="G66" t="str">
+            <v>新北市新莊區中正路370號4樓</v>
+          </cell>
+        </row>
+        <row r="67">
+          <cell r="A67" t="str">
+            <v>XIZHI_LIANXING</v>
+          </cell>
+          <cell r="B67" t="str">
+            <v>汐止連興</v>
+          </cell>
+          <cell r="C67" t="str">
+            <v>XIZHI_S</v>
+          </cell>
+          <cell r="D67" t="str">
+            <v/>
+          </cell>
+          <cell r="E67" t="str">
+            <v>EAST</v>
+          </cell>
+          <cell r="F67" t="str">
+            <v>XIZHI</v>
+          </cell>
+          <cell r="G67" t="str">
+            <v>新北市汐止區連興街42號22樓</v>
+          </cell>
+        </row>
+        <row r="68">
+          <cell r="A68" t="str">
+            <v>XIZHI_LONGAN</v>
+          </cell>
+          <cell r="B68" t="str">
+            <v>汐止龍安</v>
+          </cell>
+          <cell r="C68" t="str">
+            <v>XIZHI_A_E</v>
+          </cell>
+          <cell r="D68" t="str">
+            <v>XIZHI_B_E</v>
+          </cell>
+          <cell r="E68" t="str">
+            <v>EAST</v>
+          </cell>
+          <cell r="F68" t="str">
+            <v>XIZHI</v>
+          </cell>
+          <cell r="G68" t="str">
+            <v>新北市汐止區龍安路28巷6號4樓之1</v>
+          </cell>
+        </row>
+        <row r="69">
+          <cell r="A69" t="str">
+            <v>YILAN</v>
+          </cell>
+          <cell r="B69" t="str">
+            <v>宜蘭</v>
+          </cell>
+          <cell r="C69" t="str">
+            <v>YILAN_E</v>
+          </cell>
+          <cell r="D69" t="str">
+            <v/>
+          </cell>
+          <cell r="E69" t="str">
+            <v>EAST</v>
+          </cell>
+          <cell r="F69" t="str">
+            <v>YILAN</v>
+          </cell>
+          <cell r="G69" t="str">
+            <v>宜蘭縣宜蘭市新興路20號3樓</v>
+          </cell>
+        </row>
+        <row r="70">
+          <cell r="A70" t="str">
+            <v>YINGGE</v>
+          </cell>
+          <cell r="B70" t="str">
+            <v>鶯歌</v>
+          </cell>
+          <cell r="C70" t="str">
+            <v>BADE_B_E</v>
+          </cell>
+          <cell r="D70" t="str">
+            <v/>
+          </cell>
+          <cell r="E70" t="str">
+            <v>TAOYUAN</v>
+          </cell>
+          <cell r="F70" t="str">
+            <v>BADE</v>
+          </cell>
+          <cell r="G70" t="str">
+            <v>新北市鶯歌區光明街126號12樓</v>
+          </cell>
+        </row>
+        <row r="71">
+          <cell r="A71" t="str">
+            <v>YONGHE</v>
+          </cell>
+          <cell r="B71" t="str">
+            <v>永和</v>
+          </cell>
+          <cell r="C71" t="str">
+            <v>YONGHE_S</v>
+          </cell>
+          <cell r="D71" t="str">
+            <v>ZHONGHE_2_S</v>
+          </cell>
+          <cell r="E71" t="str">
+            <v>SOUTH</v>
+          </cell>
+          <cell r="F71" t="str">
+            <v>SHUANGHE</v>
+          </cell>
+          <cell r="G71" t="str">
+            <v>新北市永和區水源街45巷16號5樓</v>
+          </cell>
+        </row>
+        <row r="72">
+          <cell r="A72" t="str">
+            <v>YULI_GUANGFU</v>
+          </cell>
+          <cell r="B72" t="str">
+            <v>玉里光復</v>
+          </cell>
+          <cell r="C72" t="str">
+            <v>YULI_S</v>
+          </cell>
+          <cell r="D72" t="str">
+            <v/>
+          </cell>
+          <cell r="E72" t="str">
+            <v>TAIDONG</v>
+          </cell>
+          <cell r="F72" t="str">
+            <v>YULI</v>
+          </cell>
+          <cell r="G72" t="str">
+            <v>花蓮縣玉里鎮光復路82巷10號4樓</v>
+          </cell>
+        </row>
+        <row r="73">
+          <cell r="A73" t="str">
+            <v>YULI_XINGGUO</v>
+          </cell>
+          <cell r="B73" t="str">
+            <v>玉里啓模</v>
+          </cell>
+          <cell r="C73" t="str">
+            <v>YULI_E</v>
+          </cell>
+          <cell r="D73" t="str">
+            <v/>
+          </cell>
+          <cell r="E73" t="str">
+            <v>TAIDONG</v>
+          </cell>
+          <cell r="F73" t="str">
+            <v>YULI</v>
+          </cell>
+          <cell r="G73" t="str">
+            <v>花蓮縣玉里鎮興國路2段128巷8號</v>
+          </cell>
+        </row>
+        <row r="74">
+          <cell r="A74" t="str">
+            <v>ZHONGHE_JUGUANG</v>
+          </cell>
+          <cell r="B74" t="str">
+            <v>中和莒光</v>
+          </cell>
+          <cell r="C74" t="str">
+            <v>XINBAN_E</v>
+          </cell>
+          <cell r="D74" t="str">
+            <v/>
+          </cell>
+          <cell r="E74" t="str">
+            <v>WEST</v>
+          </cell>
+          <cell r="F74" t="str">
+            <v>BANQIAO</v>
+          </cell>
+          <cell r="G74" t="str">
+            <v>新北市中和區莒光路120巷34號3樓</v>
+          </cell>
+        </row>
+        <row r="75">
+          <cell r="A75" t="str">
+            <v>ZHONGHE_YUANTONG</v>
+          </cell>
+          <cell r="B75" t="str">
+            <v>中和圓通</v>
+          </cell>
+          <cell r="C75" t="str">
+            <v>ZHONGHE_1_E</v>
+          </cell>
+          <cell r="D75" t="str">
+            <v>ZHONGHE_2_E</v>
+          </cell>
+          <cell r="E75" t="str">
+            <v>SOUTH</v>
+          </cell>
+          <cell r="F75" t="str">
+            <v>SHUANGHE</v>
+          </cell>
+          <cell r="G75" t="str">
+            <v>新北市中和區圓通路141巷41之4號4樓</v>
+          </cell>
+        </row>
+        <row r="76">
+          <cell r="A76" t="str">
+            <v>ZHONGLI_JIUHE</v>
+          </cell>
+          <cell r="B76" t="str">
+            <v>中壢九和</v>
+          </cell>
+          <cell r="C76" t="str">
+            <v>ZHONGLI_1_A_E</v>
+          </cell>
+          <cell r="D76" t="str">
+            <v>ZHONGLI_2_E</v>
+          </cell>
+          <cell r="E76" t="str">
+            <v>TAOYUAN</v>
+          </cell>
+          <cell r="F76" t="str">
+            <v>ZHONGLI</v>
+          </cell>
+          <cell r="G76" t="str">
+            <v>桃園市中壢區九和一街57號7樓之3B棟</v>
+          </cell>
+        </row>
+        <row r="77">
+          <cell r="A77" t="str">
+            <v>ZHONGLI_ZHONGBEI</v>
+          </cell>
+          <cell r="B77" t="str">
+            <v>中壢中北</v>
+          </cell>
+          <cell r="C77" t="str">
+            <v>ZHONGLI_1_B_E</v>
+          </cell>
+          <cell r="D77" t="str">
+            <v/>
+          </cell>
+          <cell r="E77" t="str">
+            <v>TAOYUAN</v>
+          </cell>
+          <cell r="F77" t="str">
+            <v>ZHONGLI</v>
+          </cell>
+          <cell r="G77" t="str">
+            <v>桃園市中壢區中北路2段208巷13號6F</v>
+          </cell>
+        </row>
+        <row r="78">
+          <cell r="A78" t="str">
+            <v>ZHONGSHAN</v>
+          </cell>
+          <cell r="B78" t="str">
+            <v>中山</v>
+          </cell>
+          <cell r="C78" t="str">
+            <v>JINHUA_ZL</v>
+          </cell>
+          <cell r="D78" t="str">
+            <v/>
+          </cell>
+          <cell r="E78" t="str">
+            <v>CENTRAL</v>
+          </cell>
+          <cell r="F78" t="str">
+            <v>JINHUA</v>
+          </cell>
+          <cell r="G78" t="str">
+            <v>臺北市中山區龍江路1號4樓之6</v>
+          </cell>
+        </row>
+        <row r="79">
+          <cell r="A79" t="str">
+            <v>ZHONGZHENG_NANCHANG_1_COUPLE</v>
+          </cell>
+          <cell r="B79" t="str">
+            <v>中正南昌1夫婦</v>
+          </cell>
+          <cell r="C79" t="str">
+            <v/>
+          </cell>
+          <cell r="D79" t="str">
+            <v/>
+          </cell>
+          <cell r="E79" t="str">
+            <v/>
+          </cell>
+          <cell r="F79" t="str">
+            <v/>
+          </cell>
+          <cell r="G79" t="str">
+            <v>臺北市中正區南昌路1段123號4樓之5</v>
+          </cell>
+        </row>
+        <row r="80">
+          <cell r="A80" t="str">
+            <v>ZHONGZHENG_NANCHANG_2_COUPLE</v>
+          </cell>
+          <cell r="B80" t="str">
+            <v>中正南昌2夫婦</v>
+          </cell>
+          <cell r="C80" t="str">
+            <v>SENIOR_COUPLE</v>
+          </cell>
+          <cell r="D80" t="str">
+            <v/>
+          </cell>
+          <cell r="E80" t="str">
+            <v>CENTRAL</v>
+          </cell>
+          <cell r="F80" t="str">
+            <v>JINHUA</v>
+          </cell>
+          <cell r="G80" t="str">
+            <v>臺北市中正區南昌路2段142之1號12樓</v>
+          </cell>
+        </row>
+        <row r="81">
+          <cell r="A81" t="str">
+            <v>ZHUBEI_BOAI</v>
+          </cell>
+          <cell r="B81" t="str">
+            <v>竹北博愛</v>
+          </cell>
+          <cell r="C81" t="str">
+            <v>ZHUBEI_1_E</v>
+          </cell>
+          <cell r="D81" t="str">
+            <v/>
+          </cell>
+          <cell r="E81" t="str">
+            <v>XINZHU</v>
+          </cell>
+          <cell r="F81" t="str">
+            <v>ZHUBEI</v>
+          </cell>
+          <cell r="G81" t="str">
+            <v>新竹縣竹北市博愛街486巷1號3樓</v>
+          </cell>
+        </row>
+        <row r="82">
+          <cell r="A82" t="str">
+            <v>ZHUBEI_XINTAI</v>
+          </cell>
+          <cell r="B82" t="str">
+            <v>竹北新泰</v>
+          </cell>
+          <cell r="C82" t="str">
+            <v>ZHUBEI_2_S</v>
+          </cell>
+          <cell r="D82" t="str">
+            <v>ZHUBEI_3_S</v>
+          </cell>
+          <cell r="E82" t="str">
+            <v>XINZHU</v>
+          </cell>
+          <cell r="F82" t="str">
+            <v>ZHUBEI</v>
+          </cell>
+          <cell r="G82" t="str">
+            <v>新竹縣竹北市新泰路118號4樓之7</v>
+          </cell>
+        </row>
+        <row r="83">
+          <cell r="A83" t="str">
+            <v>ZHUDONG_XINGFU_1</v>
+          </cell>
+          <cell r="B83" t="str">
+            <v>竹東幸福1</v>
+          </cell>
+          <cell r="C83" t="str">
+            <v>ZHUDONG_E</v>
+          </cell>
+          <cell r="D83" t="str">
+            <v/>
+          </cell>
+          <cell r="E83" t="str">
+            <v>XINZHU</v>
+          </cell>
+          <cell r="F83" t="str">
+            <v>ZHUDONG</v>
+          </cell>
+          <cell r="G83" t="str">
+            <v>新竹縣竹東鎮幸福路121巷1號13樓</v>
+          </cell>
+        </row>
+        <row r="84">
+          <cell r="A84" t="str">
+            <v>ZHUDONG_XINGFU_21</v>
+          </cell>
+          <cell r="B84" t="str">
+            <v>竹東幸福21</v>
+          </cell>
+          <cell r="C84" t="str">
+            <v>ZHUDONG_S</v>
+          </cell>
+          <cell r="D84" t="str">
+            <v/>
+          </cell>
+          <cell r="E84" t="str">
+            <v>XINZHU</v>
+          </cell>
+          <cell r="F84" t="str">
+            <v>ZHUDONG</v>
+          </cell>
+          <cell r="G84" t="str">
+            <v>新竹縣竹東鎮幸福路121巷21號11樓</v>
+          </cell>
+        </row>
+        <row r="85">
+          <cell r="A85" t="str">
+            <v>ZHUNAN_YANPING</v>
+          </cell>
+          <cell r="B85" t="str">
+            <v>竹南延平</v>
+          </cell>
+          <cell r="C85" t="str">
+            <v>ZHUNAN_ZL</v>
+          </cell>
+          <cell r="D85" t="str">
+            <v/>
+          </cell>
+          <cell r="E85" t="str">
+            <v>ZHUNAN</v>
+          </cell>
+          <cell r="F85" t="str">
+            <v>ZHUNAN</v>
+          </cell>
+          <cell r="G85" t="str">
+            <v>苗栗縣竹南鎮延平路110號6樓之3</v>
+          </cell>
+        </row>
+        <row r="86">
+          <cell r="A86" t="str">
+            <v>ZHUNAN_ZHONGZHENG</v>
+          </cell>
+          <cell r="B86" t="str">
+            <v>竹南中正</v>
+          </cell>
+          <cell r="C86" t="str">
+            <v>ZHUNAN_S</v>
+          </cell>
+          <cell r="D86" t="str">
+            <v/>
+          </cell>
+          <cell r="E86" t="str">
+            <v>ZHUNAN</v>
+          </cell>
+          <cell r="F86" t="str">
+            <v>ZHUNAN</v>
+          </cell>
+          <cell r="G86" t="str">
+            <v>苗栗縣竹南鎮中正路215巷2號4樓</v>
+          </cell>
+        </row>
+        <row r="87">
+          <cell r="A87" t="str">
+            <v>ZHUNAN_BOAI</v>
+          </cell>
+          <cell r="B87" t="str">
+            <v>竹南博愛</v>
+          </cell>
+          <cell r="C87" t="str">
+            <v/>
+          </cell>
+          <cell r="D87" t="str">
+            <v/>
+          </cell>
+          <cell r="E87" t="str">
+            <v/>
+          </cell>
+          <cell r="F87" t="str">
+            <v/>
+          </cell>
+          <cell r="G87" t="str">
+            <v>苗栗縣竹南鎮博愛街313巷9號12樓</v>
+          </cell>
+        </row>
+        <row r="88">
+          <cell r="A88" t="str">
+            <v>DAAN_FUXING_COUPLE</v>
+          </cell>
+          <cell r="B88" t="str">
+            <v>大安復興夫婦</v>
+          </cell>
+          <cell r="C88" t="str">
+            <v/>
+          </cell>
+          <cell r="D88" t="str">
+            <v/>
+          </cell>
+          <cell r="E88" t="str">
+            <v/>
+          </cell>
+          <cell r="F88" t="str">
+            <v/>
+          </cell>
+          <cell r="G88" t="str">
+            <v>臺北市大安區復興南路1段295巷13弄8號2樓</v>
+          </cell>
+        </row>
+      </sheetData>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2571,10 +4617,10 @@
   <dimension ref="A1:O103"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B40" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="M58" sqref="M58"/>
+      <selection pane="bottomRight" activeCell="O6" sqref="O6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2584,7 +4630,8 @@
     <col min="5" max="5" width="26.42578125" style="4" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="28.140625" style="4" bestFit="1" customWidth="1"/>
     <col min="7" max="14" width="9.140625" style="4"/>
-    <col min="15" max="16384" width="9.140625" style="3"/>
+    <col min="15" max="15" width="43.42578125" style="10" bestFit="1" customWidth="1"/>
+    <col min="16" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15">
@@ -2630,7 +4677,9 @@
       <c r="N1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="O1" s="8"/>
+      <c r="O1" s="9" t="s">
+        <v>731</v>
+      </c>
     </row>
     <row r="2" spans="1:15">
       <c r="A2" s="2" t="s">
@@ -2649,7 +4698,7 @@
         <v>540</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="G2" s="2" t="s">
         <v>143</v>
@@ -2674,6 +4723,10 @@
       </c>
       <c r="N2" s="2" t="s">
         <v>203</v>
+      </c>
+      <c r="O2" s="10" t="str">
+        <f ca="1">VLOOKUP(E2,[1]APARTMENTS!$A:$G,7,FALSE)</f>
+        <v>臺北市中山區龍江路1號4樓之6</v>
       </c>
     </row>
     <row r="3" spans="1:15">
@@ -2693,7 +4746,7 @@
         <v>527</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>143</v>
@@ -2716,6 +4769,10 @@
       </c>
       <c r="N3" s="2" t="s">
         <v>521</v>
+      </c>
+      <c r="O3" s="10" t="str">
+        <f ca="1">VLOOKUP(E3,[1]APARTMENTS!$A:$G,7,FALSE)</f>
+        <v>台北市大安區永康街47巷12號4F</v>
       </c>
     </row>
     <row r="4" spans="1:15">
@@ -2735,7 +4792,7 @@
         <v>527</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="G4" s="2" t="s">
         <v>143</v>
@@ -2758,6 +4815,10 @@
       </c>
       <c r="N4" s="2" t="s">
         <v>521</v>
+      </c>
+      <c r="O4" s="10" t="str">
+        <f ca="1">VLOOKUP(E4,[1]APARTMENTS!$A:$G,7,FALSE)</f>
+        <v>台北市大安區永康街47巷12號4F</v>
       </c>
     </row>
     <row r="5" spans="1:15">
@@ -2774,7 +4835,7 @@
         <v>518</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="F5" s="2" t="s">
         <v>519</v>
@@ -2801,6 +4862,10 @@
         <v>1</v>
       </c>
       <c r="N5" s="2"/>
+      <c r="O5" s="10" t="str">
+        <f ca="1">VLOOKUP(E5,[1]APARTMENTS!$A:$G,7,FALSE)</f>
+        <v>臺北市中正區南昌路2段142之1號12樓</v>
+      </c>
     </row>
     <row r="6" spans="1:15">
       <c r="A6" s="2" t="s">
@@ -2816,10 +4881,10 @@
         <v>338</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="G6" s="2" t="s">
         <v>143</v>
@@ -2842,6 +4907,10 @@
       </c>
       <c r="N6" s="2" t="s">
         <v>520</v>
+      </c>
+      <c r="O6" s="10" t="str">
+        <f ca="1">VLOOKUP(E6,[1]APARTMENTS!$A:$G,7,FALSE)</f>
+        <v>台北市大安區金華街102巷5號4樓</v>
       </c>
     </row>
     <row r="7" spans="1:15">
@@ -2858,10 +4927,10 @@
         <v>162</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
       <c r="G7" s="2" t="s">
         <v>163</v>
@@ -2886,6 +4955,10 @@
       </c>
       <c r="N7" s="2" t="s">
         <v>165</v>
+      </c>
+      <c r="O7" s="10" t="str">
+        <f ca="1">VLOOKUP(E7,[1]APARTMENTS!$A:$G,7,FALSE)</f>
+        <v>新北市瀘州區信義路222巷35號9樓之3</v>
       </c>
     </row>
     <row r="8" spans="1:15">
@@ -2902,10 +4975,10 @@
         <v>169</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
       <c r="G8" s="2" t="s">
         <v>163</v>
@@ -2930,6 +5003,10 @@
       </c>
       <c r="N8" s="2" t="s">
         <v>165</v>
+      </c>
+      <c r="O8" s="10" t="str">
+        <f ca="1">VLOOKUP(E8,[1]APARTMENTS!$A:$G,7,FALSE)</f>
+        <v>新北市瀘州區信義路222巷35號9樓之3</v>
       </c>
     </row>
     <row r="9" spans="1:15">
@@ -2949,7 +5026,7 @@
         <v>545</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
       <c r="G9" s="2" t="s">
         <v>163</v>
@@ -2974,6 +5051,10 @@
       </c>
       <c r="N9" s="2" t="s">
         <v>213</v>
+      </c>
+      <c r="O9" s="10" t="str">
+        <f ca="1">VLOOKUP(E9,[1]APARTMENTS!$A:$G,7,FALSE)</f>
+        <v>新北市三重區成功路100號9樓之6</v>
       </c>
     </row>
     <row r="10" spans="1:15">
@@ -2993,7 +5074,7 @@
         <v>546</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
       <c r="G10" s="2" t="s">
         <v>163</v>
@@ -3018,6 +5099,10 @@
       </c>
       <c r="N10" s="2" t="s">
         <v>213</v>
+      </c>
+      <c r="O10" s="10" t="str">
+        <f ca="1">VLOOKUP(E10,[1]APARTMENTS!$A:$G,7,FALSE)</f>
+        <v>新北市三重區成功路100號9樓之5</v>
       </c>
     </row>
     <row r="11" spans="1:15">
@@ -3037,7 +5122,7 @@
         <v>527</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="G11" s="2" t="s">
         <v>28</v>
@@ -3059,7 +5144,11 @@
         <v>0</v>
       </c>
       <c r="N11" s="1" t="s">
-        <v>730</v>
+        <v>729</v>
+      </c>
+      <c r="O11" s="10" t="str">
+        <f ca="1">VLOOKUP(E11,[1]APARTMENTS!$A:$G,7,FALSE)</f>
+        <v>台北市大安區永康街47巷12號4F</v>
       </c>
     </row>
     <row r="12" spans="1:15">
@@ -3079,7 +5168,7 @@
         <v>527</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="G12" s="2" t="s">
         <v>28</v>
@@ -3101,7 +5190,11 @@
         <v>0</v>
       </c>
       <c r="N12" s="1" t="s">
-        <v>730</v>
+        <v>729</v>
+      </c>
+      <c r="O12" s="10" t="str">
+        <f ca="1">VLOOKUP(E12,[1]APARTMENTS!$A:$G,7,FALSE)</f>
+        <v>台北市大安區永康街47巷12號4F</v>
       </c>
     </row>
     <row r="13" spans="1:15">
@@ -3118,10 +5211,10 @@
         <v>352</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="G13" s="2" t="s">
         <v>28</v>
@@ -3145,7 +5238,11 @@
         <v>0</v>
       </c>
       <c r="N13" s="2" t="s">
-        <v>633</v>
+        <v>632</v>
+      </c>
+      <c r="O13" s="10" t="str">
+        <f ca="1">VLOOKUP(E13,[1]APARTMENTS!$A:$G,7,FALSE)</f>
+        <v>臺北市萬華區國興路58號2樓</v>
       </c>
     </row>
     <row r="14" spans="1:15">
@@ -3162,10 +5259,10 @@
         <v>356</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="G14" s="2" t="s">
         <v>28</v>
@@ -3189,7 +5286,11 @@
         <v>1</v>
       </c>
       <c r="N14" s="1" t="s">
-        <v>729</v>
+        <v>728</v>
+      </c>
+      <c r="O14" s="10" t="str">
+        <f ca="1">VLOOKUP(E14,[1]APARTMENTS!$A:$G,7,FALSE)</f>
+        <v>台北市大同區南京西路103號10樓之10</v>
       </c>
     </row>
     <row r="15" spans="1:15">
@@ -3206,10 +5307,10 @@
         <v>366</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="G15" s="2" t="s">
         <v>28</v>
@@ -3232,6 +5333,10 @@
       </c>
       <c r="N15" s="2" t="s">
         <v>367</v>
+      </c>
+      <c r="O15" s="10" t="str">
+        <f ca="1">VLOOKUP(E15,[1]APARTMENTS!$A:$G,7,FALSE)</f>
+        <v>台北市大安區和平東路二段96巷20弄12號3樓</v>
       </c>
     </row>
     <row r="16" spans="1:15">
@@ -3251,7 +5356,7 @@
         <v>125</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="G16" s="2" t="s">
         <v>125</v>
@@ -3277,8 +5382,12 @@
       <c r="N16" s="2" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="17" spans="1:14">
+      <c r="O16" s="10" t="str">
+        <f ca="1">VLOOKUP(E16,[1]APARTMENTS!$A:$G,7,FALSE)</f>
+        <v>基隆市中正區義一路186號2樓</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15">
       <c r="A17" s="2" t="s">
         <v>128</v>
       </c>
@@ -3295,7 +5404,7 @@
         <v>125</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="G17" s="2" t="s">
         <v>125</v>
@@ -3321,8 +5430,12 @@
       <c r="N17" s="2" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="18" spans="1:14">
+      <c r="O17" s="10" t="str">
+        <f ca="1">VLOOKUP(E17,[1]APARTMENTS!$A:$G,7,FALSE)</f>
+        <v>基隆市中正區義一路186號2樓</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15">
       <c r="A18" s="2" t="s">
         <v>188</v>
       </c>
@@ -3339,7 +5452,7 @@
         <v>543</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>715</v>
+        <v>714</v>
       </c>
       <c r="G18" s="2" t="s">
         <v>192</v>
@@ -3365,8 +5478,12 @@
       <c r="N18" s="2" t="s">
         <v>194</v>
       </c>
-    </row>
-    <row r="19" spans="1:14">
+      <c r="O18" s="10" t="str">
+        <f ca="1">VLOOKUP(E18,[1]APARTMENTS!$A:$G,7,FALSE)</f>
+        <v>臺北市內湖區內湖路1段411巷5號4樓</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15">
       <c r="A19" s="2" t="s">
         <v>195</v>
       </c>
@@ -3383,7 +5500,7 @@
         <v>544</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="G19" s="2" t="s">
         <v>192</v>
@@ -3409,8 +5526,12 @@
       <c r="N19" s="2" t="s">
         <v>194</v>
       </c>
-    </row>
-    <row r="20" spans="1:14">
+      <c r="O19" s="10" t="str">
+        <f ca="1">VLOOKUP(E19,[1]APARTMENTS!$A:$G,7,FALSE)</f>
+        <v>臺北市內湖區金湖路326巷45號5樓之2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15">
       <c r="A20" s="2" t="s">
         <v>251</v>
       </c>
@@ -3427,7 +5548,7 @@
         <v>550</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="G20" s="2" t="s">
         <v>192</v>
@@ -3453,8 +5574,12 @@
       <c r="N20" s="2" t="s">
         <v>522</v>
       </c>
-    </row>
-    <row r="21" spans="1:14">
+      <c r="O20" s="10" t="str">
+        <f ca="1">VLOOKUP(E20,[1]APARTMENTS!$A:$G,7,FALSE)</f>
+        <v>臺北市松山區八德路4段262號4樓</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15">
       <c r="A21" s="2" t="s">
         <v>246</v>
       </c>
@@ -3471,7 +5596,7 @@
         <v>551</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="G21" s="2" t="s">
         <v>192</v>
@@ -3497,8 +5622,12 @@
       <c r="N21" s="2" t="s">
         <v>250</v>
       </c>
-    </row>
-    <row r="22" spans="1:14">
+      <c r="O21" s="10" t="str">
+        <f ca="1">VLOOKUP(E21,[1]APARTMENTS!$A:$G,7,FALSE)</f>
+        <v>臺北市松山區南京東路5段328號6樓之1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15">
       <c r="A22" s="2" t="s">
         <v>408</v>
       </c>
@@ -3512,10 +5641,10 @@
         <v>411</v>
       </c>
       <c r="E22" s="5" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="G22" s="2" t="s">
         <v>412</v>
@@ -3541,8 +5670,12 @@
       <c r="N22" s="2" t="s">
         <v>413</v>
       </c>
-    </row>
-    <row r="23" spans="1:14">
+      <c r="O22" s="10" t="str">
+        <f ca="1">VLOOKUP(E22,[1]APARTMENTS!$A:$G,7,FALSE)</f>
+        <v>新北市汐止區龍安路28巷6號4樓之1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15">
       <c r="A23" s="2" t="s">
         <v>414</v>
       </c>
@@ -3556,7 +5689,7 @@
         <v>417</v>
       </c>
       <c r="E23" s="5" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="F23" s="2" t="s">
         <v>418</v>
@@ -3585,8 +5718,12 @@
       <c r="N23" s="2" t="s">
         <v>413</v>
       </c>
-    </row>
-    <row r="24" spans="1:14">
+      <c r="O23" s="10" t="str">
+        <f ca="1">VLOOKUP(E23,[1]APARTMENTS!$A:$G,7,FALSE)</f>
+        <v>新北市汐止區龍安路28巷6號4樓之1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15">
       <c r="A24" s="2" t="s">
         <v>419</v>
       </c>
@@ -3600,10 +5737,10 @@
         <v>422</v>
       </c>
       <c r="E24" s="5" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
       <c r="G24" s="2" t="s">
         <v>412</v>
@@ -3629,8 +5766,12 @@
       <c r="N24" s="2" t="s">
         <v>413</v>
       </c>
-    </row>
-    <row r="25" spans="1:14">
+      <c r="O24" s="10" t="str">
+        <f ca="1">VLOOKUP(E24,[1]APARTMENTS!$A:$G,7,FALSE)</f>
+        <v>新北市汐止區連興街42號22樓</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15">
       <c r="A25" s="2" t="s">
         <v>151</v>
       </c>
@@ -3644,10 +5785,10 @@
         <v>154</v>
       </c>
       <c r="E25" s="5" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="G25" s="2" t="s">
         <v>155</v>
@@ -3673,8 +5814,12 @@
       <c r="N25" s="2" t="s">
         <v>156</v>
       </c>
-    </row>
-    <row r="26" spans="1:14">
+      <c r="O25" s="10" t="str">
+        <f ca="1">VLOOKUP(E25,[1]APARTMENTS!$A:$G,7,FALSE)</f>
+        <v>宜蘭縣羅東鎮公正路289之3號8樓</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15">
       <c r="A26" s="2" t="s">
         <v>157</v>
       </c>
@@ -3682,16 +5827,16 @@
         <v>158</v>
       </c>
       <c r="C26" s="4" t="s">
+        <v>692</v>
+      </c>
+      <c r="D26" s="4" t="s">
         <v>693</v>
       </c>
-      <c r="D26" s="4" t="s">
-        <v>694</v>
-      </c>
       <c r="E26" s="4" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="G26" s="2" t="s">
         <v>155</v>
@@ -3717,8 +5862,12 @@
       <c r="N26" s="2" t="s">
         <v>156</v>
       </c>
-    </row>
-    <row r="27" spans="1:14">
+      <c r="O26" s="10" t="str">
+        <f ca="1">VLOOKUP(E26,[1]APARTMENTS!$A:$G,7,FALSE)</f>
+        <v>宜蘭縣羅東鎮公正路289之3號8樓</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15">
       <c r="A27" s="2" t="s">
         <v>423</v>
       </c>
@@ -3735,7 +5884,7 @@
         <v>155</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="G27" s="2" t="s">
         <v>155</v>
@@ -3761,8 +5910,12 @@
       <c r="N27" s="2" t="s">
         <v>427</v>
       </c>
-    </row>
-    <row r="28" spans="1:14">
+      <c r="O27" s="10" t="str">
+        <f ca="1">VLOOKUP(E27,[1]APARTMENTS!$A:$G,7,FALSE)</f>
+        <v>宜蘭縣宜蘭市新興路20號3樓</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15">
       <c r="A28" s="2" t="s">
         <v>428</v>
       </c>
@@ -3776,10 +5929,10 @@
         <v>431</v>
       </c>
       <c r="E28" s="5" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
       <c r="G28" s="2" t="s">
         <v>155</v>
@@ -3805,8 +5958,12 @@
       <c r="N28" s="2" t="s">
         <v>432</v>
       </c>
-    </row>
-    <row r="29" spans="1:14">
+      <c r="O28" s="10" t="str">
+        <f ca="1">VLOOKUP(E28,[1]APARTMENTS!$A:$G,7,FALSE)</f>
+        <v>宜蘭縣羅東鎮站東路108號C棟2樓</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15">
       <c r="A29" s="2" t="s">
         <v>112</v>
       </c>
@@ -3823,7 +5980,7 @@
         <v>538</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="G29" s="2" t="s">
         <v>93</v>
@@ -3849,8 +6006,12 @@
       <c r="N29" s="2" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="30" spans="1:14">
+      <c r="O29" s="10" t="str">
+        <f ca="1">VLOOKUP(E29,[1]APARTMENTS!$A:$G,7,FALSE)</f>
+        <v>花蓮縣吉安鄉北昌五街102號2樓</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15">
       <c r="A30" s="2" t="s">
         <v>117</v>
       </c>
@@ -3864,10 +6025,10 @@
         <v>120</v>
       </c>
       <c r="E30" s="4" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
       <c r="G30" s="2" t="s">
         <v>93</v>
@@ -3893,8 +6054,12 @@
       <c r="N30" s="2" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="31" spans="1:14">
+      <c r="O30" s="10" t="str">
+        <f ca="1">VLOOKUP(E30,[1]APARTMENTS!$A:$G,7,FALSE)</f>
+        <v>花蓮縣花蓮市中和街217號10樓之1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15">
       <c r="A31" s="2" t="s">
         <v>88</v>
       </c>
@@ -3911,7 +6076,7 @@
         <v>536</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
       <c r="G31" s="2" t="s">
         <v>92</v>
@@ -3937,8 +6102,12 @@
       <c r="N31" s="2" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="32" spans="1:14">
+      <c r="O31" s="10" t="str">
+        <f ca="1">VLOOKUP(E31,[1]APARTMENTS!$A:$G,7,FALSE)</f>
+        <v>花蓮縣花蓮市中美13街78號2F之12</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15">
       <c r="A32" s="2" t="s">
         <v>97</v>
       </c>
@@ -3952,10 +6121,10 @@
         <v>100</v>
       </c>
       <c r="E32" s="5" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="G32" s="2" t="s">
         <v>92</v>
@@ -3981,8 +6150,12 @@
       <c r="N32" s="2" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="33" spans="1:14">
+      <c r="O32" s="10" t="str">
+        <f ca="1">VLOOKUP(E32,[1]APARTMENTS!$A:$G,7,FALSE)</f>
+        <v>花蓮縣花蓮市中和街217號10樓之1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:15">
       <c r="A33" s="2" t="s">
         <v>101</v>
       </c>
@@ -3999,7 +6172,7 @@
         <v>537</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
       <c r="G33" s="2" t="s">
         <v>92</v>
@@ -4025,8 +6198,12 @@
       <c r="N33" s="2" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="34" spans="1:14">
+      <c r="O33" s="10" t="str">
+        <f ca="1">VLOOKUP(E33,[1]APARTMENTS!$A:$G,7,FALSE)</f>
+        <v>花蓮縣花蓮市德安一街291號5F之3</v>
+      </c>
+    </row>
+    <row r="34" spans="1:15">
       <c r="A34" s="2" t="s">
         <v>107</v>
       </c>
@@ -4043,7 +6220,7 @@
         <v>537</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
       <c r="G34" s="2" t="s">
         <v>92</v>
@@ -4069,25 +6246,29 @@
       <c r="N34" s="2" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="35" spans="1:14">
+      <c r="O34" s="10" t="str">
+        <f ca="1">VLOOKUP(E34,[1]APARTMENTS!$A:$G,7,FALSE)</f>
+        <v>花蓮縣花蓮市德安一街291號5F之3</v>
+      </c>
+    </row>
+    <row r="35" spans="1:15">
       <c r="A35" s="4" t="s">
+        <v>644</v>
+      </c>
+      <c r="B35" s="6" t="s">
+        <v>640</v>
+      </c>
+      <c r="C35" s="4" t="s">
         <v>645</v>
       </c>
-      <c r="B35" s="6" t="s">
+      <c r="D35" s="4" t="s">
         <v>641</v>
       </c>
-      <c r="C35" s="4" t="s">
-        <v>646</v>
-      </c>
-      <c r="D35" s="4" t="s">
+      <c r="E35" s="4" t="s">
         <v>642</v>
       </c>
-      <c r="E35" s="4" t="s">
+      <c r="F35" s="4" t="s">
         <v>643</v>
-      </c>
-      <c r="F35" s="4" t="s">
-        <v>644</v>
       </c>
       <c r="G35" s="2" t="s">
         <v>92</v>
@@ -4110,8 +6291,12 @@
       <c r="M35" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="36" spans="1:14">
+      <c r="O35" s="10" t="str">
+        <f ca="1">VLOOKUP(E35,[1]APARTMENTS!$A:$G,7,FALSE)</f>
+        <v>花蓮縣花蓮市長安街26號13樓之9</v>
+      </c>
+    </row>
+    <row r="36" spans="1:15">
       <c r="A36" s="2" t="s">
         <v>52</v>
       </c>
@@ -4128,7 +6313,7 @@
         <v>531</v>
       </c>
       <c r="F36" s="2" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="G36" s="2" t="s">
         <v>56</v>
@@ -4154,8 +6339,12 @@
       <c r="N36" s="2" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="37" spans="1:14">
+      <c r="O36" s="10" t="str">
+        <f ca="1">VLOOKUP(E36,[1]APARTMENTS!$A:$G,7,FALSE)</f>
+        <v>台北市北投區溫泉路65巷16號7樓之14</v>
+      </c>
+    </row>
+    <row r="37" spans="1:15">
       <c r="A37" s="2" t="s">
         <v>59</v>
       </c>
@@ -4172,7 +6361,7 @@
         <v>532</v>
       </c>
       <c r="F37" s="2" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="G37" s="2" t="s">
         <v>56</v>
@@ -4198,8 +6387,12 @@
       <c r="N37" s="2" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="38" spans="1:14">
+      <c r="O37" s="10" t="str">
+        <f ca="1">VLOOKUP(E37,[1]APARTMENTS!$A:$G,7,FALSE)</f>
+        <v>臺北市北投區中央北路二段181號4樓之3</v>
+      </c>
+    </row>
+    <row r="38" spans="1:15">
       <c r="A38" s="2" t="s">
         <v>70</v>
       </c>
@@ -4216,7 +6409,7 @@
         <v>534</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="G38" s="2" t="s">
         <v>56</v>
@@ -4242,8 +6435,12 @@
       <c r="N38" s="2" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="39" spans="1:14">
+      <c r="O38" s="10" t="str">
+        <f ca="1">VLOOKUP(E38,[1]APARTMENTS!$A:$G,7,FALSE)</f>
+        <v>新北市淡水區民權路173巷7號3樓-13</v>
+      </c>
+    </row>
+    <row r="39" spans="1:15">
       <c r="A39" s="2" t="s">
         <v>76</v>
       </c>
@@ -4260,7 +6457,7 @@
         <v>535</v>
       </c>
       <c r="F39" s="2" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="G39" s="2" t="s">
         <v>56</v>
@@ -4286,8 +6483,12 @@
       <c r="N39" s="2" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="40" spans="1:14">
+      <c r="O39" s="10" t="str">
+        <f ca="1">VLOOKUP(E39,[1]APARTMENTS!$A:$G,7,FALSE)</f>
+        <v>新北市淡水區英專路90之2號3樓</v>
+      </c>
+    </row>
+    <row r="40" spans="1:15">
       <c r="A40" s="2" t="s">
         <v>235</v>
       </c>
@@ -4304,7 +6505,7 @@
         <v>548</v>
       </c>
       <c r="F40" s="2" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="G40" s="2" t="s">
         <v>233</v>
@@ -4330,8 +6531,12 @@
       <c r="N40" s="2" t="s">
         <v>239</v>
       </c>
-    </row>
-    <row r="41" spans="1:14">
+      <c r="O40" s="10" t="str">
+        <f ca="1">VLOOKUP(E40,[1]APARTMENTS!$A:$G,7,FALSE)</f>
+        <v>臺北市士林區雙溪街106號2樓之1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:15">
       <c r="A41" s="2" t="s">
         <v>229</v>
       </c>
@@ -4345,10 +6550,10 @@
         <v>232</v>
       </c>
       <c r="E41" s="5" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="F41" s="2" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="G41" s="2" t="s">
         <v>233</v>
@@ -4374,8 +6579,12 @@
       <c r="N41" s="2" t="s">
         <v>234</v>
       </c>
-    </row>
-    <row r="42" spans="1:14">
+      <c r="O41" s="10" t="str">
+        <f ca="1">VLOOKUP(E41,[1]APARTMENTS!$A:$G,7,FALSE)</f>
+        <v>臺北市士林區大北路100號3樓</v>
+      </c>
+    </row>
+    <row r="42" spans="1:15">
       <c r="A42" s="2" t="s">
         <v>320</v>
       </c>
@@ -4389,10 +6598,10 @@
         <v>323</v>
       </c>
       <c r="E42" s="5" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="F42" s="2" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="G42" s="2" t="s">
         <v>233</v>
@@ -4418,8 +6627,12 @@
       <c r="N42" s="2" t="s">
         <v>325</v>
       </c>
-    </row>
-    <row r="43" spans="1:14">
+      <c r="O42" s="10" t="str">
+        <f ca="1">VLOOKUP(E42,[1]APARTMENTS!$A:$G,7,FALSE)</f>
+        <v>臺北市士林區雨聲街83巷5號3樓</v>
+      </c>
+    </row>
+    <row r="43" spans="1:15">
       <c r="A43" s="2" t="s">
         <v>326</v>
       </c>
@@ -4427,16 +6640,16 @@
         <v>327</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="D43" s="4" t="s">
         <v>328</v>
       </c>
       <c r="E43" s="4" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="F43" s="2" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
       <c r="G43" s="2" t="s">
         <v>233</v>
@@ -4462,8 +6675,12 @@
       <c r="N43" s="2" t="s">
         <v>325</v>
       </c>
-    </row>
-    <row r="44" spans="1:14">
+      <c r="O43" s="10" t="str">
+        <f ca="1">VLOOKUP(E43,[1]APARTMENTS!$A:$G,7,FALSE)</f>
+        <v>臺北市士林區雨聲街83巷5號3樓</v>
+      </c>
+    </row>
+    <row r="44" spans="1:15">
       <c r="A44" s="2" t="s">
         <v>139</v>
       </c>
@@ -4477,10 +6694,10 @@
         <v>142</v>
       </c>
       <c r="E44" s="4" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="F44" s="2" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="G44" s="2" t="s">
         <v>137</v>
@@ -4506,8 +6723,12 @@
       <c r="N44" s="2" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="45" spans="1:14">
+      <c r="O44" s="10" t="str">
+        <f ca="1">VLOOKUP(E44,[1]APARTMENTS!$A:$G,7,FALSE)</f>
+        <v>新北市新店區中央八街68號4樓</v>
+      </c>
+    </row>
+    <row r="45" spans="1:15">
       <c r="A45" s="2" t="s">
         <v>133</v>
       </c>
@@ -4524,7 +6745,7 @@
         <v>539</v>
       </c>
       <c r="F45" s="2" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="G45" s="2" t="s">
         <v>137</v>
@@ -4550,8 +6771,12 @@
       <c r="N45" s="2" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="46" spans="1:14">
+      <c r="O45" s="10" t="str">
+        <f ca="1">VLOOKUP(E45,[1]APARTMENTS!$A:$G,7,FALSE)</f>
+        <v>新北市新店區檳榔路53巷2號6樓</v>
+      </c>
+    </row>
+    <row r="46" spans="1:15">
       <c r="A46" s="2" t="s">
         <v>179</v>
       </c>
@@ -4568,7 +6793,7 @@
         <v>541</v>
       </c>
       <c r="F46" s="2" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="G46" s="2" t="s">
         <v>137</v>
@@ -4592,10 +6817,14 @@
         <v>1</v>
       </c>
       <c r="N46" s="2" t="s">
-        <v>631</v>
-      </c>
-    </row>
-    <row r="47" spans="1:14">
+        <v>630</v>
+      </c>
+      <c r="O46" s="10" t="str">
+        <f ca="1">VLOOKUP(E46,[1]APARTMENTS!$A:$G,7,FALSE)</f>
+        <v>臺北市文山區木柵路3段85巷29號2樓</v>
+      </c>
+    </row>
+    <row r="47" spans="1:15">
       <c r="A47" s="2" t="s">
         <v>184</v>
       </c>
@@ -4612,7 +6841,7 @@
         <v>542</v>
       </c>
       <c r="F47" s="2" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
       <c r="G47" s="2" t="s">
         <v>137</v>
@@ -4636,10 +6865,14 @@
         <v>1</v>
       </c>
       <c r="N47" s="2" t="s">
-        <v>631</v>
-      </c>
-    </row>
-    <row r="48" spans="1:14">
+        <v>630</v>
+      </c>
+      <c r="O47" s="10" t="str">
+        <f ca="1">VLOOKUP(E47,[1]APARTMENTS!$A:$G,7,FALSE)</f>
+        <v>臺北市文山區萬壽路17巷1號7樓之2</v>
+      </c>
+    </row>
+    <row r="48" spans="1:15">
       <c r="A48" s="2" t="s">
         <v>433</v>
       </c>
@@ -4656,7 +6889,7 @@
         <v>438</v>
       </c>
       <c r="F48" s="2" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="G48" s="2" t="s">
         <v>437</v>
@@ -4682,8 +6915,12 @@
       <c r="N48" s="2" t="s">
         <v>439</v>
       </c>
-    </row>
-    <row r="49" spans="1:14">
+      <c r="O48" s="10" t="str">
+        <f ca="1">VLOOKUP(E48,[1]APARTMENTS!$A:$G,7,FALSE)</f>
+        <v>新北市永和區水源街45巷16號5樓</v>
+      </c>
+    </row>
+    <row r="49" spans="1:15">
       <c r="A49" s="2" t="s">
         <v>450</v>
       </c>
@@ -4697,10 +6934,10 @@
         <v>453</v>
       </c>
       <c r="E49" s="5" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="F49" s="2" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
       <c r="G49" s="2" t="s">
         <v>437</v>
@@ -4726,8 +6963,12 @@
       <c r="N49" s="2" t="s">
         <v>455</v>
       </c>
-    </row>
-    <row r="50" spans="1:14">
+      <c r="O49" s="10" t="str">
+        <f ca="1">VLOOKUP(E49,[1]APARTMENTS!$A:$G,7,FALSE)</f>
+        <v>新北市中和區圓通路141巷41之4號4樓</v>
+      </c>
+    </row>
+    <row r="50" spans="1:15">
       <c r="A50" s="2" t="s">
         <v>456</v>
       </c>
@@ -4741,10 +6982,10 @@
         <v>459</v>
       </c>
       <c r="E50" s="5" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="F50" s="2" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
       <c r="G50" s="2" t="s">
         <v>437</v>
@@ -4770,8 +7011,12 @@
       <c r="N50" s="2" t="s">
         <v>455</v>
       </c>
-    </row>
-    <row r="51" spans="1:14">
+      <c r="O50" s="10" t="str">
+        <f ca="1">VLOOKUP(E50,[1]APARTMENTS!$A:$G,7,FALSE)</f>
+        <v>新北市中和區圓通路141巷41之4號4樓</v>
+      </c>
+    </row>
+    <row r="51" spans="1:15">
       <c r="A51" s="2" t="s">
         <v>461</v>
       </c>
@@ -4788,7 +7033,7 @@
         <v>438</v>
       </c>
       <c r="F51" s="2" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
       <c r="G51" s="2" t="s">
         <v>437</v>
@@ -4814,8 +7059,12 @@
       <c r="N51" s="2" t="s">
         <v>455</v>
       </c>
-    </row>
-    <row r="52" spans="1:14">
+      <c r="O51" s="10" t="str">
+        <f ca="1">VLOOKUP(E51,[1]APARTMENTS!$A:$G,7,FALSE)</f>
+        <v>新北市永和區水源街45巷16號5樓</v>
+      </c>
+    </row>
+    <row r="52" spans="1:15">
       <c r="A52" s="2" t="s">
         <v>16</v>
       </c>
@@ -4832,7 +7081,7 @@
         <v>526</v>
       </c>
       <c r="F52" s="2" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="G52" s="2" t="s">
         <v>20</v>
@@ -4858,8 +7107,12 @@
       <c r="N52" s="2" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="53" spans="1:14">
+      <c r="O52" s="10" t="str">
+        <f ca="1">VLOOKUP(E52,[1]APARTMENTS!$A:$G,7,FALSE)</f>
+        <v>新北市新店區安康路2段159巷5號12樓</v>
+      </c>
+    </row>
+    <row r="53" spans="1:15">
       <c r="A53" s="2" t="s">
         <v>372</v>
       </c>
@@ -4876,7 +7129,7 @@
         <v>539</v>
       </c>
       <c r="F53" s="2" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="G53" s="2" t="s">
         <v>20</v>
@@ -4902,8 +7155,12 @@
       <c r="N53" s="2" t="s">
         <v>376</v>
       </c>
-    </row>
-    <row r="54" spans="1:14">
+      <c r="O53" s="10" t="str">
+        <f ca="1">VLOOKUP(E53,[1]APARTMENTS!$A:$G,7,FALSE)</f>
+        <v>新北市新店區檳榔路53巷2號6樓</v>
+      </c>
+    </row>
+    <row r="54" spans="1:15">
       <c r="A54" s="2" t="s">
         <v>377</v>
       </c>
@@ -4917,10 +7174,10 @@
         <v>380</v>
       </c>
       <c r="E54" s="5" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="F54" s="2" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="G54" s="2" t="s">
         <v>20</v>
@@ -4946,8 +7203,12 @@
       <c r="N54" s="2" t="s">
         <v>376</v>
       </c>
-    </row>
-    <row r="55" spans="1:14">
+      <c r="O54" s="10" t="str">
+        <f ca="1">VLOOKUP(E54,[1]APARTMENTS!$A:$G,7,FALSE)</f>
+        <v>新北市新店區中央八街68號4樓</v>
+      </c>
+    </row>
+    <row r="55" spans="1:15">
       <c r="A55" s="2" t="s">
         <v>255</v>
       </c>
@@ -4964,7 +7225,7 @@
         <v>552</v>
       </c>
       <c r="F55" s="2" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="G55" s="2" t="s">
         <v>259</v>
@@ -4990,8 +7251,12 @@
       <c r="N55" s="2" t="s">
         <v>262</v>
       </c>
-    </row>
-    <row r="56" spans="1:14">
+      <c r="O55" s="10" t="str">
+        <f ca="1">VLOOKUP(E55,[1]APARTMENTS!$A:$G,7,FALSE)</f>
+        <v>臺東縣臺東市開封街439號4樓之4</v>
+      </c>
+    </row>
+    <row r="56" spans="1:15">
       <c r="A56" s="2" t="s">
         <v>263</v>
       </c>
@@ -5008,7 +7273,7 @@
         <v>553</v>
       </c>
       <c r="F56" s="2" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="G56" s="2" t="s">
         <v>259</v>
@@ -5034,8 +7299,12 @@
       <c r="N56" s="2" t="s">
         <v>262</v>
       </c>
-    </row>
-    <row r="57" spans="1:14">
+      <c r="O56" s="10" t="str">
+        <f ca="1">VLOOKUP(E56,[1]APARTMENTS!$A:$G,7,FALSE)</f>
+        <v>臺東縣臺東市長沙街206巷17弄2號2樓</v>
+      </c>
+    </row>
+    <row r="57" spans="1:15">
       <c r="A57" s="2" t="s">
         <v>278</v>
       </c>
@@ -5049,10 +7318,10 @@
         <v>281</v>
       </c>
       <c r="E57" s="5" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="F57" s="2" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="G57" s="2" t="s">
         <v>259</v>
@@ -5073,13 +7342,17 @@
         <v>1</v>
       </c>
       <c r="M57" s="1" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
       <c r="N57" s="2" t="s">
         <v>283</v>
       </c>
-    </row>
-    <row r="58" spans="1:14">
+      <c r="O57" s="10" t="str">
+        <f ca="1">VLOOKUP(E57,[1]APARTMENTS!$A:$G,7,FALSE)</f>
+        <v>臺東縣臺東市更生北路674巷22號</v>
+      </c>
+    </row>
+    <row r="58" spans="1:15">
       <c r="A58" s="2" t="s">
         <v>273</v>
       </c>
@@ -5096,7 +7369,7 @@
         <v>553</v>
       </c>
       <c r="F58" s="2" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
       <c r="G58" s="2" t="s">
         <v>271</v>
@@ -5122,8 +7395,12 @@
       <c r="N58" s="2" t="s">
         <v>277</v>
       </c>
-    </row>
-    <row r="59" spans="1:14">
+      <c r="O58" s="10" t="str">
+        <f ca="1">VLOOKUP(E58,[1]APARTMENTS!$A:$G,7,FALSE)</f>
+        <v>臺東縣臺東市長沙街206巷17弄2號2樓</v>
+      </c>
+    </row>
+    <row r="59" spans="1:15">
       <c r="A59" s="2" t="s">
         <v>267</v>
       </c>
@@ -5140,7 +7417,7 @@
         <v>554</v>
       </c>
       <c r="F59" s="2" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
       <c r="G59" s="2" t="s">
         <v>271</v>
@@ -5166,13 +7443,17 @@
       <c r="N59" s="2" t="s">
         <v>272</v>
       </c>
-    </row>
-    <row r="60" spans="1:14">
+      <c r="O59" s="10" t="str">
+        <f ca="1">VLOOKUP(E59,[1]APARTMENTS!$A:$G,7,FALSE)</f>
+        <v>臺東縣臺東市長沙街206巷15弄8號2樓</v>
+      </c>
+    </row>
+    <row r="60" spans="1:15">
       <c r="A60" s="2" t="s">
         <v>440</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="C60" s="4" t="s">
         <v>441</v>
@@ -5181,10 +7462,10 @@
         <v>442</v>
       </c>
       <c r="E60" s="5" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="F60" s="2" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
       <c r="G60" s="2" t="s">
         <v>443</v>
@@ -5210,8 +7491,12 @@
       <c r="N60" s="2" t="s">
         <v>444</v>
       </c>
-    </row>
-    <row r="61" spans="1:14">
+      <c r="O60" s="10" t="str">
+        <f ca="1">VLOOKUP(E60,[1]APARTMENTS!$A:$G,7,FALSE)</f>
+        <v>花蓮縣玉里鎮興國路2段128巷8號</v>
+      </c>
+    </row>
+    <row r="61" spans="1:15">
       <c r="A61" s="2" t="s">
         <v>445</v>
       </c>
@@ -5225,10 +7510,10 @@
         <v>448</v>
       </c>
       <c r="E61" s="5" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="F61" s="2" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
       <c r="G61" s="2" t="s">
         <v>443</v>
@@ -5254,8 +7539,12 @@
       <c r="N61" s="2" t="s">
         <v>449</v>
       </c>
-    </row>
-    <row r="62" spans="1:14">
+      <c r="O61" s="10" t="str">
+        <f ca="1">VLOOKUP(E61,[1]APARTMENTS!$A:$G,7,FALSE)</f>
+        <v>花蓮縣玉里鎮光復路82巷10號4樓</v>
+      </c>
+    </row>
+    <row r="62" spans="1:15">
       <c r="A62" s="2" t="s">
         <v>523</v>
       </c>
@@ -5286,8 +7575,12 @@
       <c r="N62" s="2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="63" spans="1:14">
+      <c r="O62" s="10" t="e">
+        <f ca="1">VLOOKUP(E62,[1]APARTMENTS!$A:$G,7,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="63" spans="1:15">
       <c r="A63" s="2" t="s">
         <v>31</v>
       </c>
@@ -5304,7 +7597,7 @@
         <v>528</v>
       </c>
       <c r="F63" s="2" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
       <c r="G63" s="2" t="s">
         <v>35</v>
@@ -5330,8 +7623,12 @@
       <c r="N63" s="2" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="64" spans="1:14">
+      <c r="O63" s="10" t="str">
+        <f ca="1">VLOOKUP(E63,[1]APARTMENTS!$A:$G,7,FALSE)</f>
+        <v>桃園市大溪鎮僑愛一街35巷20弄10號9樓</v>
+      </c>
+    </row>
+    <row r="64" spans="1:15">
       <c r="A64" s="2" t="s">
         <v>38</v>
       </c>
@@ -5348,7 +7645,7 @@
         <v>529</v>
       </c>
       <c r="F64" s="2" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
       <c r="G64" s="2" t="s">
         <v>35</v>
@@ -5374,8 +7671,12 @@
       <c r="N64" s="2" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="65" spans="1:14">
+      <c r="O64" s="10" t="str">
+        <f ca="1">VLOOKUP(E64,[1]APARTMENTS!$A:$G,7,FALSE)</f>
+        <v>新北市鶯歌區光明街126號12樓</v>
+      </c>
+    </row>
+    <row r="65" spans="1:15">
       <c r="A65" s="2" t="s">
         <v>43</v>
       </c>
@@ -5392,7 +7693,7 @@
         <v>530</v>
       </c>
       <c r="F65" s="2" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
       <c r="G65" s="2" t="s">
         <v>35</v>
@@ -5418,8 +7719,12 @@
       <c r="N65" s="2" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="66" spans="1:14">
+      <c r="O65" s="10" t="str">
+        <f ca="1">VLOOKUP(E65,[1]APARTMENTS!$A:$G,7,FALSE)</f>
+        <v>桃園市大溪鎮僑愛一街34巷7號8樓</v>
+      </c>
+    </row>
+    <row r="66" spans="1:15">
       <c r="A66" s="2" t="s">
         <v>145</v>
       </c>
@@ -5436,7 +7741,7 @@
         <v>149</v>
       </c>
       <c r="F66" s="2" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="G66" s="2" t="s">
         <v>35</v>
@@ -5462,8 +7767,12 @@
       <c r="N66" s="2" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="67" spans="1:14">
+      <c r="O66" s="10" t="str">
+        <f ca="1">VLOOKUP(E66,[1]APARTMENTS!$A:$G,7,FALSE)</f>
+        <v>桃園市龍潭區龍星村大同路207號10樓</v>
+      </c>
+    </row>
+    <row r="67" spans="1:15">
       <c r="A67" s="2" t="s">
         <v>81</v>
       </c>
@@ -5480,7 +7789,7 @@
         <v>86</v>
       </c>
       <c r="F67" s="1" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
       <c r="G67" s="2" t="s">
         <v>85</v>
@@ -5506,8 +7815,12 @@
       <c r="N67" s="2" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="68" spans="1:14">
+      <c r="O67" s="10" t="str">
+        <f ca="1">VLOOKUP(E67,[1]APARTMENTS!$A:$G,7,FALSE)</f>
+        <v>桃園市龜山區自強東路226號3樓</v>
+      </c>
+    </row>
+    <row r="68" spans="1:15">
       <c r="A68" s="2" t="s">
         <v>284</v>
       </c>
@@ -5524,7 +7837,7 @@
         <v>555</v>
       </c>
       <c r="F68" s="1" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
       <c r="G68" s="2" t="s">
         <v>85</v>
@@ -5548,10 +7861,14 @@
         <v>1</v>
       </c>
       <c r="N68" s="2" t="s">
-        <v>637</v>
-      </c>
-    </row>
-    <row r="69" spans="1:14">
+        <v>636</v>
+      </c>
+      <c r="O68" s="10" t="str">
+        <f ca="1">VLOOKUP(E68,[1]APARTMENTS!$A:$G,7,FALSE)</f>
+        <v>桃園市桃園區大有路630之11號20樓</v>
+      </c>
+    </row>
+    <row r="69" spans="1:15">
       <c r="A69" s="2" t="s">
         <v>289</v>
       </c>
@@ -5568,7 +7885,7 @@
         <v>555</v>
       </c>
       <c r="F69" s="2" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="G69" s="2" t="s">
         <v>85</v>
@@ -5592,10 +7909,14 @@
         <v>1</v>
       </c>
       <c r="N69" s="2" t="s">
-        <v>637</v>
-      </c>
-    </row>
-    <row r="70" spans="1:14">
+        <v>636</v>
+      </c>
+      <c r="O69" s="10" t="str">
+        <f ca="1">VLOOKUP(E69,[1]APARTMENTS!$A:$G,7,FALSE)</f>
+        <v>桃園市桃園區大有路630之11號20樓</v>
+      </c>
+    </row>
+    <row r="70" spans="1:15">
       <c r="A70" s="2" t="s">
         <v>293</v>
       </c>
@@ -5612,7 +7933,7 @@
         <v>556</v>
       </c>
       <c r="F70" s="1" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
       <c r="G70" s="2" t="s">
         <v>85</v>
@@ -5636,10 +7957,14 @@
         <v>1</v>
       </c>
       <c r="N70" s="2" t="s">
-        <v>637</v>
-      </c>
-    </row>
-    <row r="71" spans="1:14">
+        <v>636</v>
+      </c>
+      <c r="O70" s="10" t="str">
+        <f ca="1">VLOOKUP(E70,[1]APARTMENTS!$A:$G,7,FALSE)</f>
+        <v>桃園市桃園區國鼎一街3號12樓之2</v>
+      </c>
+    </row>
+    <row r="71" spans="1:15">
       <c r="A71" s="2" t="s">
         <v>298</v>
       </c>
@@ -5656,7 +7981,7 @@
         <v>557</v>
       </c>
       <c r="F71" s="2" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="G71" s="2" t="s">
         <v>85</v>
@@ -5680,10 +8005,14 @@
         <v>0</v>
       </c>
       <c r="N71" s="2" t="s">
-        <v>637</v>
-      </c>
-    </row>
-    <row r="72" spans="1:14">
+        <v>636</v>
+      </c>
+      <c r="O71" s="10" t="str">
+        <f ca="1">VLOOKUP(E71,[1]APARTMENTS!$A:$G,7,FALSE)</f>
+        <v>桃園市桃園區國際路1段1191號16樓之4</v>
+      </c>
+    </row>
+    <row r="72" spans="1:15">
       <c r="A72" s="2" t="s">
         <v>302</v>
       </c>
@@ -5700,7 +8029,7 @@
         <v>560</v>
       </c>
       <c r="F72" s="2" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="G72" s="2" t="s">
         <v>306</v>
@@ -5724,10 +8053,14 @@
         <v>1</v>
       </c>
       <c r="N72" s="2" t="s">
-        <v>638</v>
-      </c>
-    </row>
-    <row r="73" spans="1:14">
+        <v>637</v>
+      </c>
+      <c r="O72" s="10" t="str">
+        <f ca="1">VLOOKUP(E72,[1]APARTMENTS!$A:$G,7,FALSE)</f>
+        <v>桃園市蘆竹區興中街55號4樓之1</v>
+      </c>
+    </row>
+    <row r="73" spans="1:15">
       <c r="A73" s="2" t="s">
         <v>307</v>
       </c>
@@ -5744,7 +8077,7 @@
         <v>559</v>
       </c>
       <c r="F73" s="2" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="G73" s="2" t="s">
         <v>306</v>
@@ -5768,10 +8101,14 @@
         <v>1</v>
       </c>
       <c r="N73" s="2" t="s">
-        <v>636</v>
-      </c>
-    </row>
-    <row r="74" spans="1:14">
+        <v>635</v>
+      </c>
+      <c r="O73" s="10" t="str">
+        <f ca="1">VLOOKUP(E73,[1]APARTMENTS!$A:$G,7,FALSE)</f>
+        <v>桃園市桃園區中埔二街83號13樓</v>
+      </c>
+    </row>
+    <row r="74" spans="1:15">
       <c r="A74" s="2" t="s">
         <v>311</v>
       </c>
@@ -5788,7 +8125,7 @@
         <v>558</v>
       </c>
       <c r="F74" s="2" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="G74" s="2" t="s">
         <v>306</v>
@@ -5812,10 +8149,14 @@
         <v>1</v>
       </c>
       <c r="N74" s="2" t="s">
-        <v>634</v>
-      </c>
-    </row>
-    <row r="75" spans="1:14">
+        <v>633</v>
+      </c>
+      <c r="O74" s="10" t="str">
+        <f ca="1">VLOOKUP(E74,[1]APARTMENTS!$A:$G,7,FALSE)</f>
+        <v>桃園市桃園區民有十二街66號9樓</v>
+      </c>
+    </row>
+    <row r="75" spans="1:15">
       <c r="A75" s="2" t="s">
         <v>316</v>
       </c>
@@ -5828,11 +8169,11 @@
       <c r="D75" s="4" t="s">
         <v>319</v>
       </c>
-      <c r="E75" s="5" t="s">
-        <v>561</v>
+      <c r="E75" s="8" t="s">
+        <v>730</v>
       </c>
       <c r="F75" s="2" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
       <c r="G75" s="2" t="s">
         <v>306</v>
@@ -5856,27 +8197,31 @@
         <v>1</v>
       </c>
       <c r="N75" s="2" t="s">
-        <v>634</v>
-      </c>
-    </row>
-    <row r="76" spans="1:14">
+        <v>633</v>
+      </c>
+      <c r="O75" s="10" t="str">
+        <f ca="1">VLOOKUP(E75,[1]APARTMENTS!$A:$G,7,FALSE)</f>
+        <v>桃園市蘆竹區南平街7號2樓之三</v>
+      </c>
+    </row>
+    <row r="76" spans="1:15">
       <c r="A76" s="2" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
       <c r="B76" s="2" t="s">
         <v>465</v>
       </c>
       <c r="C76" s="4" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
       <c r="D76" s="4" t="s">
         <v>466</v>
       </c>
       <c r="E76" s="5" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="F76" s="1" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
       <c r="G76" s="2" t="s">
         <v>467</v>
@@ -5900,27 +8245,31 @@
         <v>1</v>
       </c>
       <c r="N76" s="2" t="s">
-        <v>639</v>
-      </c>
-    </row>
-    <row r="77" spans="1:14">
+        <v>638</v>
+      </c>
+      <c r="O76" s="10" t="str">
+        <f ca="1">VLOOKUP(E76,[1]APARTMENTS!$A:$G,7,FALSE)</f>
+        <v>桃園市中壢區九和一街57號7樓之3B棟</v>
+      </c>
+    </row>
+    <row r="77" spans="1:15">
       <c r="A77" s="2" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
       <c r="B77" s="2" t="s">
         <v>469</v>
       </c>
       <c r="C77" s="4" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
       <c r="D77" s="4" t="s">
         <v>470</v>
       </c>
       <c r="E77" s="5" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="F77" s="1" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
       <c r="G77" s="2" t="s">
         <v>467</v>
@@ -5944,10 +8293,14 @@
         <v>1</v>
       </c>
       <c r="N77" s="2" t="s">
-        <v>640</v>
-      </c>
-    </row>
-    <row r="78" spans="1:14">
+        <v>639</v>
+      </c>
+      <c r="O77" s="10" t="str">
+        <f ca="1">VLOOKUP(E77,[1]APARTMENTS!$A:$G,7,FALSE)</f>
+        <v>桃園市中壢區中北路2段208巷13號6F</v>
+      </c>
+    </row>
+    <row r="78" spans="1:15">
       <c r="A78" s="2" t="s">
         <v>471</v>
       </c>
@@ -5961,10 +8314,10 @@
         <v>474</v>
       </c>
       <c r="E78" s="5" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="F78" s="1" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
       <c r="G78" s="2" t="s">
         <v>467</v>
@@ -5990,8 +8343,12 @@
       <c r="N78" s="2" t="s">
         <v>476</v>
       </c>
-    </row>
-    <row r="79" spans="1:14">
+      <c r="O78" s="10" t="str">
+        <f ca="1">VLOOKUP(E78,[1]APARTMENTS!$A:$G,7,FALSE)</f>
+        <v>桃園市中壢區九和一街57號7樓之3B棟</v>
+      </c>
+    </row>
+    <row r="79" spans="1:15">
       <c r="A79" s="2" t="s">
         <v>368</v>
       </c>
@@ -6005,10 +8362,10 @@
         <v>371</v>
       </c>
       <c r="E79" s="5" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="F79" s="1" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
       <c r="G79" s="2" t="s">
         <v>48</v>
@@ -6032,10 +8389,14 @@
         <v>1</v>
       </c>
       <c r="N79" s="2" t="s">
-        <v>635</v>
-      </c>
-    </row>
-    <row r="80" spans="1:14">
+        <v>634</v>
+      </c>
+      <c r="O79" s="10" t="str">
+        <f ca="1">VLOOKUP(E79,[1]APARTMENTS!$A:$G,7,FALSE)</f>
+        <v>新北市中和區莒光路120巷34號3樓</v>
+      </c>
+    </row>
+    <row r="80" spans="1:15">
       <c r="A80" s="2" t="s">
         <v>381</v>
       </c>
@@ -6052,7 +8413,7 @@
         <v>48</v>
       </c>
       <c r="F80" s="1" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="G80" s="2" t="s">
         <v>48</v>
@@ -6078,8 +8439,12 @@
       <c r="N80" s="2" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="81" spans="1:14">
+      <c r="O80" s="10" t="str">
+        <f ca="1">VLOOKUP(E80,[1]APARTMENTS!$A:$G,7,FALSE)</f>
+        <v>新北市板橋區民生路三段281巷2弄7號4樓</v>
+      </c>
+    </row>
+    <row r="81" spans="1:15">
       <c r="A81" s="2" t="s">
         <v>218</v>
       </c>
@@ -6096,7 +8461,7 @@
         <v>547</v>
       </c>
       <c r="F81" s="1" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="G81" s="2" t="s">
         <v>222</v>
@@ -6122,8 +8487,12 @@
       <c r="N81" s="2" t="s">
         <v>224</v>
       </c>
-    </row>
-    <row r="82" spans="1:14">
+      <c r="O81" s="10" t="str">
+        <f ca="1">VLOOKUP(E81,[1]APARTMENTS!$A:$G,7,FALSE)</f>
+        <v>新北市樹林區佳園路3段452號8樓</v>
+      </c>
+    </row>
+    <row r="82" spans="1:15">
       <c r="A82" s="2" t="s">
         <v>225</v>
       </c>
@@ -6140,7 +8509,7 @@
         <v>547</v>
       </c>
       <c r="F82" s="1" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="G82" s="2" t="s">
         <v>222</v>
@@ -6166,8 +8535,12 @@
       <c r="N82" s="2" t="s">
         <v>224</v>
       </c>
-    </row>
-    <row r="83" spans="1:14">
+      <c r="O82" s="10" t="str">
+        <f ca="1">VLOOKUP(E82,[1]APARTMENTS!$A:$G,7,FALSE)</f>
+        <v>新北市樹林區佳園路3段452號8樓</v>
+      </c>
+    </row>
+    <row r="83" spans="1:15">
       <c r="A83" s="2" t="s">
         <v>344</v>
       </c>
@@ -6181,10 +8554,10 @@
         <v>347</v>
       </c>
       <c r="E83" s="5" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="F83" s="1" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
       <c r="G83" s="2" t="s">
         <v>222</v>
@@ -6210,8 +8583,12 @@
       <c r="N83" s="2" t="s">
         <v>348</v>
       </c>
-    </row>
-    <row r="84" spans="1:14">
+      <c r="O83" s="10" t="str">
+        <f ca="1">VLOOKUP(E83,[1]APARTMENTS!$A:$G,7,FALSE)</f>
+        <v>新北市土城區中央路1段88號16樓</v>
+      </c>
+    </row>
+    <row r="84" spans="1:15">
       <c r="A84" s="2" t="s">
         <v>339</v>
       </c>
@@ -6225,10 +8602,10 @@
         <v>342</v>
       </c>
       <c r="E84" s="5" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="F84" s="2" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="G84" s="2" t="s">
         <v>222</v>
@@ -6254,8 +8631,12 @@
       <c r="N84" s="2" t="s">
         <v>343</v>
       </c>
-    </row>
-    <row r="85" spans="1:14">
+      <c r="O84" s="10" t="str">
+        <f ca="1">VLOOKUP(E84,[1]APARTMENTS!$A:$G,7,FALSE)</f>
+        <v>新北市土城區裕民路92巷5弄6號8樓</v>
+      </c>
+    </row>
+    <row r="85" spans="1:15">
       <c r="A85" s="2" t="s">
         <v>63</v>
       </c>
@@ -6272,7 +8653,7 @@
         <v>533</v>
       </c>
       <c r="F85" s="1" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="G85" s="2" t="s">
         <v>67</v>
@@ -6298,8 +8679,12 @@
       <c r="N85" s="2" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="86" spans="1:14">
+      <c r="O85" s="10" t="str">
+        <f ca="1">VLOOKUP(E85,[1]APARTMENTS!$A:$G,7,FALSE)</f>
+        <v>新北市新莊區青山路1段64之3號10樓</v>
+      </c>
+    </row>
+    <row r="86" spans="1:15">
       <c r="A86" s="2" t="s">
         <v>240</v>
       </c>
@@ -6316,7 +8701,7 @@
         <v>549</v>
       </c>
       <c r="F86" s="2" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="G86" s="2" t="s">
         <v>67</v>
@@ -6342,8 +8727,12 @@
       <c r="N86" s="2" t="s">
         <v>245</v>
       </c>
-    </row>
-    <row r="87" spans="1:14">
+      <c r="O86" s="10" t="str">
+        <f ca="1">VLOOKUP(E86,[1]APARTMENTS!$A:$G,7,FALSE)</f>
+        <v>新北市新莊區中正路370號4樓</v>
+      </c>
+    </row>
+    <row r="87" spans="1:15">
       <c r="A87" s="2" t="s">
         <v>386</v>
       </c>
@@ -6357,10 +8746,10 @@
         <v>389</v>
       </c>
       <c r="E87" s="5" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="F87" s="1" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
       <c r="G87" s="2" t="s">
         <v>390</v>
@@ -6386,8 +8775,12 @@
       <c r="N87" s="2" t="s">
         <v>392</v>
       </c>
-    </row>
-    <row r="88" spans="1:14">
+      <c r="O87" s="10" t="str">
+        <f ca="1">VLOOKUP(E87,[1]APARTMENTS!$A:$G,7,FALSE)</f>
+        <v>新竹市北區北大路166巷28號8樓之4</v>
+      </c>
+    </row>
+    <row r="88" spans="1:15">
       <c r="A88" s="2" t="s">
         <v>393</v>
       </c>
@@ -6401,10 +8794,10 @@
         <v>396</v>
       </c>
       <c r="E88" s="5" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="F88" s="1" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
       <c r="G88" s="2" t="s">
         <v>390</v>
@@ -6430,8 +8823,12 @@
       <c r="N88" s="2" t="s">
         <v>392</v>
       </c>
-    </row>
-    <row r="89" spans="1:14">
+      <c r="O88" s="10" t="str">
+        <f ca="1">VLOOKUP(E88,[1]APARTMENTS!$A:$G,7,FALSE)</f>
+        <v>新竹市東區東大路2段232巷11號6樓</v>
+      </c>
+    </row>
+    <row r="89" spans="1:15">
       <c r="A89" s="2" t="s">
         <v>403</v>
       </c>
@@ -6445,10 +8842,10 @@
         <v>406</v>
       </c>
       <c r="E89" s="4" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="F89" s="1" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
       <c r="G89" s="2" t="s">
         <v>390</v>
@@ -6474,8 +8871,12 @@
       <c r="N89" s="2" t="s">
         <v>407</v>
       </c>
-    </row>
-    <row r="90" spans="1:14">
+      <c r="O89" s="10" t="str">
+        <f ca="1">VLOOKUP(E89,[1]APARTMENTS!$A:$G,7,FALSE)</f>
+        <v>新竹市東區東大路2段232巷11號6樓</v>
+      </c>
+    </row>
+    <row r="90" spans="1:15">
       <c r="A90" s="2" t="s">
         <v>397</v>
       </c>
@@ -6489,10 +8890,10 @@
         <v>400</v>
       </c>
       <c r="E90" s="5" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="F90" s="2" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="G90" s="2" t="s">
         <v>390</v>
@@ -6518,25 +8919,29 @@
       <c r="N90" s="2" t="s">
         <v>402</v>
       </c>
-    </row>
-    <row r="91" spans="1:14">
+      <c r="O90" s="10" t="str">
+        <f ca="1">VLOOKUP(E90,[1]APARTMENTS!$A:$G,7,FALSE)</f>
+        <v>新竹市東區食品路27號3樓之33(1301室)</v>
+      </c>
+    </row>
+    <row r="91" spans="1:15">
       <c r="A91" s="2" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="B91" s="2" t="s">
         <v>492</v>
       </c>
       <c r="C91" s="4" t="s">
+        <v>586</v>
+      </c>
+      <c r="D91" s="4" t="s">
         <v>587</v>
       </c>
-      <c r="D91" s="4" t="s">
-        <v>588</v>
-      </c>
       <c r="E91" s="5" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="F91" s="1" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
       <c r="G91" s="2" t="s">
         <v>478</v>
@@ -6562,8 +8967,12 @@
       <c r="N91" s="2" t="s">
         <v>480</v>
       </c>
-    </row>
-    <row r="92" spans="1:14">
+      <c r="O91" s="10" t="str">
+        <f ca="1">VLOOKUP(E91,[1]APARTMENTS!$A:$G,7,FALSE)</f>
+        <v>新竹縣竹北市博愛街486巷1號3樓</v>
+      </c>
+    </row>
+    <row r="92" spans="1:15">
       <c r="A92" s="2" t="s">
         <v>481</v>
       </c>
@@ -6577,10 +8986,10 @@
         <v>484</v>
       </c>
       <c r="E92" s="5" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="F92" s="1" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="G92" s="2" t="s">
         <v>478</v>
@@ -6606,8 +9015,12 @@
       <c r="N92" s="2" t="s">
         <v>486</v>
       </c>
-    </row>
-    <row r="93" spans="1:14">
+      <c r="O92" s="10" t="str">
+        <f ca="1">VLOOKUP(E92,[1]APARTMENTS!$A:$G,7,FALSE)</f>
+        <v>新竹縣新豐鄉明新街426巷20號2樓之1</v>
+      </c>
+    </row>
+    <row r="93" spans="1:15">
       <c r="A93" s="2" t="s">
         <v>487</v>
       </c>
@@ -6621,10 +9034,10 @@
         <v>490</v>
       </c>
       <c r="E93" s="4" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="F93" s="1" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="G93" s="2" t="s">
         <v>478</v>
@@ -6650,25 +9063,29 @@
       <c r="N93" s="2" t="s">
         <v>491</v>
       </c>
-    </row>
-    <row r="94" spans="1:14">
+      <c r="O93" s="10" t="str">
+        <f ca="1">VLOOKUP(E93,[1]APARTMENTS!$A:$G,7,FALSE)</f>
+        <v>新竹縣竹北市新泰路118號4樓之7</v>
+      </c>
+    </row>
+    <row r="94" spans="1:15">
       <c r="A94" s="2" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="B94" s="2" t="s">
         <v>477</v>
       </c>
       <c r="C94" s="4" t="s">
+        <v>588</v>
+      </c>
+      <c r="D94" s="4" t="s">
         <v>589</v>
       </c>
-      <c r="D94" s="4" t="s">
-        <v>590</v>
-      </c>
       <c r="E94" s="5" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="F94" s="1" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
       <c r="G94" s="2" t="s">
         <v>478</v>
@@ -6692,10 +9109,14 @@
         <v>1</v>
       </c>
       <c r="N94" s="2" t="s">
-        <v>632</v>
-      </c>
-    </row>
-    <row r="95" spans="1:14">
+        <v>631</v>
+      </c>
+      <c r="O94" s="10" t="str">
+        <f ca="1">VLOOKUP(E94,[1]APARTMENTS!$A:$G,7,FALSE)</f>
+        <v>新竹縣竹北市新泰路118號4樓之7</v>
+      </c>
+    </row>
+    <row r="95" spans="1:15">
       <c r="A95" s="2" t="s">
         <v>494</v>
       </c>
@@ -6709,10 +9130,10 @@
         <v>497</v>
       </c>
       <c r="E95" s="5" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="F95" s="2" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="G95" s="2" t="s">
         <v>498</v>
@@ -6738,8 +9159,12 @@
       <c r="N95" s="2" t="s">
         <v>499</v>
       </c>
-    </row>
-    <row r="96" spans="1:14">
+      <c r="O95" s="10" t="str">
+        <f ca="1">VLOOKUP(E95,[1]APARTMENTS!$A:$G,7,FALSE)</f>
+        <v>新竹縣竹東鎮幸福路121巷1號13樓</v>
+      </c>
+    </row>
+    <row r="96" spans="1:15">
       <c r="A96" s="2" t="s">
         <v>500</v>
       </c>
@@ -6753,10 +9178,10 @@
         <v>503</v>
       </c>
       <c r="E96" s="5" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="F96" s="1" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
       <c r="G96" s="2" t="s">
         <v>498</v>
@@ -6782,8 +9207,12 @@
       <c r="N96" s="2" t="s">
         <v>504</v>
       </c>
-    </row>
-    <row r="97" spans="1:14">
+      <c r="O96" s="10" t="str">
+        <f ca="1">VLOOKUP(E96,[1]APARTMENTS!$A:$G,7,FALSE)</f>
+        <v>新竹縣竹東鎮幸福路121巷21號11樓</v>
+      </c>
+    </row>
+    <row r="97" spans="1:15">
       <c r="A97" s="2" t="s">
         <v>174</v>
       </c>
@@ -6800,7 +9229,7 @@
         <v>172</v>
       </c>
       <c r="F97" s="1" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
       <c r="G97" s="2" t="s">
         <v>170</v>
@@ -6826,8 +9255,12 @@
       <c r="N97" s="2" t="s">
         <v>178</v>
       </c>
-    </row>
-    <row r="98" spans="1:14">
+      <c r="O97" s="10" t="str">
+        <f ca="1">VLOOKUP(E97,[1]APARTMENTS!$A:$G,7,FALSE)</f>
+        <v>苗栗縣苗栗市嘉福街177巷7號4F.5F</v>
+      </c>
+    </row>
+    <row r="98" spans="1:15">
       <c r="A98" s="2" t="s">
         <v>329</v>
       </c>
@@ -6844,7 +9277,7 @@
         <v>333</v>
       </c>
       <c r="F98" s="1" t="s">
-        <v>712</v>
+        <v>711</v>
       </c>
       <c r="G98" s="2" t="s">
         <v>170</v>
@@ -6870,8 +9303,12 @@
       <c r="N98" s="2" t="s">
         <v>334</v>
       </c>
-    </row>
-    <row r="99" spans="1:14">
+      <c r="O98" s="10" t="str">
+        <f ca="1">VLOOKUP(E98,[1]APARTMENTS!$A:$G,7,FALSE)</f>
+        <v>苗栗縣頭份鎮節約街88號7樓</v>
+      </c>
+    </row>
+    <row r="99" spans="1:15">
       <c r="A99" s="2" t="s">
         <v>358</v>
       </c>
@@ -6888,7 +9325,7 @@
         <v>357</v>
       </c>
       <c r="F99" s="1" t="s">
-        <v>713</v>
+        <v>712</v>
       </c>
       <c r="G99" s="2" t="s">
         <v>171</v>
@@ -6914,8 +9351,12 @@
       <c r="N99" s="1" t="s">
         <v>362</v>
       </c>
-    </row>
-    <row r="100" spans="1:14">
+      <c r="O99" s="10" t="str">
+        <f ca="1">VLOOKUP(E99,[1]APARTMENTS!$A:$G,7,FALSE)</f>
+        <v>新竹市香山區牛埔東路247號12樓之4</v>
+      </c>
+    </row>
+    <row r="100" spans="1:15">
       <c r="A100" s="2" t="s">
         <v>505</v>
       </c>
@@ -6929,10 +9370,10 @@
         <v>508</v>
       </c>
       <c r="E100" s="5" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="F100" s="1" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
       <c r="G100" s="2" t="s">
         <v>171</v>
@@ -6958,8 +9399,12 @@
       <c r="N100" s="2" t="s">
         <v>509</v>
       </c>
-    </row>
-    <row r="101" spans="1:14">
+      <c r="O100" s="10" t="str">
+        <f ca="1">VLOOKUP(E100,[1]APARTMENTS!$A:$G,7,FALSE)</f>
+        <v>苗栗縣竹南鎮中正路215巷2號4樓</v>
+      </c>
+    </row>
+    <row r="101" spans="1:15">
       <c r="A101" s="2" t="s">
         <v>510</v>
       </c>
@@ -6973,10 +9418,10 @@
         <v>513</v>
       </c>
       <c r="E101" s="5" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="F101" s="2" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="G101" s="2" t="s">
         <v>171</v>
@@ -7002,57 +9447,69 @@
       <c r="N101" s="2" t="s">
         <v>514</v>
       </c>
-    </row>
-    <row r="102" spans="1:14">
+      <c r="O101" s="10" t="str">
+        <f ca="1">VLOOKUP(E101,[1]APARTMENTS!$A:$G,7,FALSE)</f>
+        <v>苗栗縣竹南鎮延平路110號6樓之3</v>
+      </c>
+    </row>
+    <row r="102" spans="1:15">
       <c r="A102" s="7" t="s">
+        <v>722</v>
+      </c>
+      <c r="B102" s="7" t="s">
+        <v>715</v>
+      </c>
+      <c r="C102" s="7" t="s">
+        <v>720</v>
+      </c>
+      <c r="D102" s="7" t="s">
+        <v>717</v>
+      </c>
+      <c r="E102" s="7" t="s">
+        <v>719</v>
+      </c>
+      <c r="F102" s="7" t="s">
+        <v>720</v>
+      </c>
+      <c r="L102" s="7" t="s">
+        <v>724</v>
+      </c>
+      <c r="M102" s="7" t="s">
+        <v>724</v>
+      </c>
+      <c r="O102" s="10" t="str">
+        <f ca="1">VLOOKUP(E102,[1]APARTMENTS!$A:$G,7,FALSE)</f>
+        <v>臺北市大安區復興南路1段295巷13弄8號2樓</v>
+      </c>
+    </row>
+    <row r="103" spans="1:15">
+      <c r="A103" s="7" t="s">
         <v>723</v>
       </c>
-      <c r="B102" s="7" t="s">
+      <c r="B103" s="7" t="s">
         <v>716</v>
       </c>
-      <c r="C102" s="7" t="s">
+      <c r="C103" s="7" t="s">
         <v>721</v>
       </c>
-      <c r="D102" s="7" t="s">
+      <c r="D103" s="7" t="s">
         <v>718</v>
       </c>
-      <c r="E102" s="7" t="s">
-        <v>720</v>
-      </c>
-      <c r="F102" s="7" t="s">
+      <c r="E103" s="7" t="s">
+        <v>719</v>
+      </c>
+      <c r="F103" s="7" t="s">
         <v>721</v>
       </c>
-      <c r="L102" s="7" t="s">
-        <v>725</v>
-      </c>
-      <c r="M102" s="7" t="s">
-        <v>725</v>
-      </c>
-    </row>
-    <row r="103" spans="1:14">
-      <c r="A103" s="7" t="s">
+      <c r="L103" s="7" t="s">
         <v>724</v>
       </c>
-      <c r="B103" s="7" t="s">
-        <v>717</v>
-      </c>
-      <c r="C103" s="7" t="s">
-        <v>722</v>
-      </c>
-      <c r="D103" s="7" t="s">
-        <v>719</v>
-      </c>
-      <c r="E103" s="7" t="s">
-        <v>720</v>
-      </c>
-      <c r="F103" s="7" t="s">
-        <v>722</v>
-      </c>
-      <c r="L103" s="7" t="s">
-        <v>725</v>
-      </c>
       <c r="M103" s="7" t="s">
-        <v>725</v>
+        <v>724</v>
+      </c>
+      <c r="O103" s="10" t="str">
+        <f ca="1">VLOOKUP(E103,[1]APARTMENTS!$A:$G,7,FALSE)</f>
+        <v>臺北市大安區復興南路1段295巷13弄8號2樓</v>
       </c>
     </row>
   </sheetData>

</xml_diff>